<commit_message>
updated for functional programming paradigm
</commit_message>
<xml_diff>
--- a/VBPO.xlsx
+++ b/VBPO.xlsx
@@ -438,7 +438,7 @@
   <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D2" sqref="D2:I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -514,22 +514,22 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>TACTGGCTGGTCGCGTTTAACTGTCGCGTCGCGCACGGACTTCTGCGGTTGCGCGACCGCCGCCCGGGATAGTTGGGCGGATTAGTTCGTTTACCCCTACTTGTCGGAATGCTTAGACGTTTGATACGATACAGAAAATGGTTTCCGAACCTATTATTGTGCTGGTGCCCAGACTAGCTTGTCAGTCCTCTAAAACTTCGGAAAGGAAGACGCTAACTATTGCCCAAGCGTCTTCTGAAGTGCGCGTTGCACCGCCACGGCGGACGACTTGGAGCGGCGTTCAACCTCCGGGGCTGGCGTCCGTGTCACATACTTAACGTTCCAGGTCTAGGCGTTCGGCACTGATAGGGTGGGCGGGGCCGAGACACGAGACTACTTGAATGGAAGCTTTACCGACTTCACATGCTTAACCGCGAGAACGGACTGGACGGTAAATTGCGTAAACAGCGACCGCCCCCGAGTCGGCGTGACCGCCTAAGTTGACGTGCTGAATTGAGCGACCGAATACGAGTTCTGCCAAAGTTGGCGGCCGGCGCGTGCTGTTTGAGCAGGTTGGTCAACCTGCGCGTCTGGCATAAGGGACCAAGAAGAGGCCCACACCTAGTTCCAGGGATGAACAGCGTCAAATACGACTAGCCTTTACGTAGAGGCAGGCTCCCCTAATGGGGACTTGTCCCCAAATAATTAAAGCCACGCGTCGCGTATCTAGTCGCCCATGACCTTCGTGGAGTTGTTCTGCTAATATACTACTTTAACCTACTAAACTTGGGACATGTCGTTCCGATACTTCAAGGACGACTAGCCAAGCTAGGCACGTTTAGAAGACCAGGTCCTGTCCGGAAATGCCCGGTCGCGGCGAAGTAGTTGTGCGGGGCGCTAAACCGTTGGATGCATTTACAACTACGTGACATAGTCCGCATAGACTTGCGTACAGAAGACAATGAGCCGTTACCGTGTCGTAAACTGGGCCCCAAGCTGGACGACAGTCCGCCGCCGCTTCCAGAGAACTTACTAGGCCGGCCGCCGGTTTTTCACGGCGACTTGCGACCACCGAAGCGTAATAACCCACCGGGCTTGCAGGACAGCGACCACTGCCTCCACCGATGAGCGCCAGACTTTCGACATGGAATGGTCTTCAAATTGTTGTTAGATGGAGACGGAGGCCTTCGGGAACGTCGCGGATAGCTTTTCCGTGTCCTCTAGCTTAGGGCGAAAGGCTGCTAAACACCGACGAAAAGACTTTACCGTAGACTGGACGTTGTCCAGCACCTAGATTAAGCCTTGTTGTTAGTCAGGAACCGTCCACTTCGCTGGCGGGAGGAAGGTTACCGCAAACGGCTTCCGAGGGGCTACTTGGGACGGATACCACGTCCCTTGCGTTGCCAACGCCCGCGGACACATTGCTAGAATTTCCGCAAAAAGTTATGAAGGCGGGAAAAACACTTTTAATTGCTGCAACGTCCAAAGTTGAGATTTGTCTTGTAGGATCGCGGAAATTTTACACCCCTGAGGCAACTCCGCCCACGCATAGTCCTTTGGCTAACACCCTTCGCGGACCTTAAGCTTGCGACACCGAGAAAGTTAGACTATCTTCCCTTTATGCGCTGGAAGTTCGGCCTACCGTTTTGATTAGTTAGAACGACGGGCGACTGGGACCTTCCGCTTGAATTGTTTGAACGACGTTTGTAGAGATAACCCGCGTTGTACCGGCCGCATTTAATGAAGAGCCTAATAATGCTAAGGGAGGGATACCCGCTTCTCTAACGTTAGCCATAAGACCTCCTTGTCCGAGACACAATATTTTGACTAGGAAAGCAAGACAGACAAGGCTGCAAGCTACCACTACACGGAGGATAGCCCGTTGGA</t>
+          <t>TACTGCCTAGTCGGATTCGACTGACGGGTCGGACATGGACTCCTACGCTTGCGGGAACGTCGGCCAGGATAGTTGGGCGGATTAGTCCGGTTGCCTCTACTCGTCGCGATACTTAGGCGGTTAATGCGGTACAGAAAGTGGTTTCCGGACCTATTGTTGTGCTGGTGGCCAGAGTATCTTGTCAGACCGCTAAAACTTCGAAAAGCGAGACGTTAACTGTTACCGAAACGGCTTCTGAAGTGAGCGTTGCATCGACAGGGTGCCCGACTCGGCGCGGCGTTTAACCTCCGGGGATGCCGGCCTTGCCACATACTTGACGTCCCCGGCCTAGGTGTCCGGCAGTGGTAAGGAGGGCGCGGACGGAACACGAGGCTGCTTGAATGAAAACTCTACCGTCTTCACATACTTGACCGCGACGACGCGCTGAACGGCAAGTTGCGGAAACAGCGCCCGCCACCAAGCCGTCGCGACCGGCTGAGATGACGCGCTGAATTGAGAGAGCGCATACGGGTTCTACCAAAGTTAGCGGCCGGTGGATGCTGGTTGAGGAGATTGGTCGACCTGCGAGTCTGACAAAAAGCGCCGAGAAGGGGCCCACAGCTAGTTCCAGGCATAGACAGCGTCAAGTACGACTAGCCGTTACGCAGAGGAAGACTTCCATAGTGGGGCCTCGTCCCCAAGTAATTGAAGCCGCGAGTCGCGTAACTAGTCGCGCATGACCTTCGGGCGGTTGTCCTACTAATGTACTACTTTAACCTACTAAACTTGGGACAAGTTGTCCCAATACTTCATGGACGTCTAGGAAAACTGGGCACGTTCAGGAGGCCAGGCCCGGTCCGTAAGTGACCCGTCGGAGGAAAGTAATTGTGCGGTGGACTAGACCGCTGGATACACTTGCACCTGCGAGACATGGTCCGGATAGACTTACGAACGGACAACGATAACCCATTGCCGTGGCGGAAACTGGGCCCTAAACTGGACGACAGACCACCGCCCCTTCCCAACGACTTACTAGGACGGCCGCCGGTCTTTCAAGGCGACTTGCGCCCACCCAAGCGGGACAACCCGCCAGGTTTGCAAGATAGCGATCAATGCCTCCAACGATGGGGACCTGACTTCCGACACGGAATGGTCTTCAAGTTATTGTTGGAGGCCAACGGAGGGCTCCGGGACCGGCGTGCGTAACTTTTTCGCGTCCTTTAACTTAGAGCGAAGGGCTGTTAAACGCCAACGAAGAGCCTTTACCGAAGACTAAATGTCGTCCAACAACTGAATTAGGGATTATTGTTGGTTAGCGACCGTCCGCTTCGGTGGCGAGACGACGGCTACCGCAAACGACTTCCAAGTGGCTACTTGGGTCGAATACCGCGCCCGTTACGCTGGCACCGGCCGCGGACGCACTGCTAAGACTTTCGGAAAAAATTGTGGAGCCGTGACAAGCACTTTTAATTGCTACAACGCCCGAAATTGAGCTTCGTCTTGTAAGACCGGGGAGAGTTTACGCCACTGAGACACCTTCGTCCCCGCATAGTCCTCTGACTGACGCCATTTGCGGAACTTAAGCTTGGAACACCAAGTAAATTGGACTATCTTCCGTTTATGCGGTGGAAGTTTGGCCTGCCTTTCTGCTTGGTTAGAACAACAGGGGATTGGAATCTTCCACTTGACTTGTTCGACCGCCGCTTGTAAAGGTAGCCAGGATTATACCGCCCACAGTTGATGAAAAGTCTAATAATACTAAGAGATGGATACCCTCTTCTTTAGCGATAACCGTAGGACCTTCTTGTCCGAGAAACAATATTTTGGCTGGGTAAGCACGACAGGCACGGCTGTAAGCTACCACTACACGGAGGATAACCAGTTGCG</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>ATGACCGACCAGCGCAAATTGACAGCGCAGCGCGTGCCTGAAGACGCCAACGCGCTGGCGGCGGGCCCTATCAACCCGCCTAATCAAGCAAATGGGGATGAACAGCCTTACGAATCTGCAAACTATGCTATGTCTTTTACCAAAGGCTTGGATAATAACACGACCACGGGTCTGATCGAACAGTCAGGAGATTTTGAAGCCTTTCCTTCTGCGATTGATAACGGGTTCGCAGAAGACTTCACGCGCAACGTGGCGGTGCCGCCTGCTGAACCTCGCCGCAAGTTGGAGGCCCCGACCGCAGGCACAGTGTATGAATTGCAAGGTCCAGATCCGCAAGCCGTGACTATCCCACCCGCCCCGGCTCTGTGCTCTGATGAACTTACCTTCGAAATGGCTGAAGTGTACGAATTGGCGCTCTTGCCTGACCTGCCATTTAACGCATTTGTCGCTGGCGGGGGCTCAGCCGCACTGGCGGATTCAACTGCACGACTTAACTCGCTGGCTTATGCTCAAGACGGTTTCAACCGCCGGCCGCGCACGACAAACTCGTCCAACCAGTTGGACGCGCAGACCGTATTCCCTGGTTCTTCTCCGGGTGTGGATCAAGGTCCCTACTTGTCGCAGTTTATGCTGATCGGAAATGCATCTCCGTCCGAGGGGATTACCCCTGAACAGGGGTTTATTAATTTCGGTGCGCAGCGCATAGATCAGCGGGTACTGGAAGCACCTCAACAAGACGATTATATGATGAAATTGGATGATTTGAACCCTGTACAGCAAGGCTATGAAGTTCCTGCTGATCGGTTCGATCCGTGCAAATCTTCTGGTCCAGGACAGGCCTTTACGGGCCAGCGCCGCTTCATCAACACGCCCCGCGATTTGGCAACCTACGTAAATGTTGATGCACTGTATCAGGCGTATCTGAACGCATGTCTTCTGTTACTCGGCAATGGCACAGCATTTGACCCGGGGTTCGACCTGCTGTCAGGCGGCGGCGAAGGTCTCTTGAATGATCCGGCCGGCGGCCAAAAAGTGCCGCTGAACGCTGGTGGCTTCGCATTATTGGGTGGCCCGAACGTCCTGTCGCTGGTGACGGAGGTGGCTACTCGCGGTCTGAAAGCTGTACCTTACCAGAAGTTTAACAACAATCTACCTCTGCCTCCGGAAGCCCTTGCAGCGCCTATCGAAAAGGCACAGGAGATCGAATCCCGCTTTCCGACGATTTGTGGCTGCTTTTCTGAAATGGCATCTGACCTGCAACAGGTCGTGGATCTAATTCGGAACAACAATCAGTCCTTGGCAGGTGAAGCGACCGCCCTCCTTCCAATGGCGTTTGCCGAAGGCTCCCCGATGAACCCTGCCTATGGTGCAGGGAACGCAACGGTTGCGGGCGCCTGTGTAACGATCTTAAAGGCGTTTTTCAATACTTCCGCCCTTTTTGTGAAAATTAACGACGTTGCAGGTTTCAACTCTAAACAGAACATCCTAGCGCCTTTAAAATGTGGGGACTCCGTTGAGGCGGGTGCGTATCAGGAAACCGATTGTGGGAAGCGCCTGGAATTCGAACGCTGTGGCTCTTTCAATCTGATAGAAGGGAAATACGCGACCTTCAAGCCGGATGGCAAAACTAATCAATCTTGCTGCCCGCTGACCCTGGAAGGCGAACTTAACAAACTTGCTGCAAACATCTCTATTGGGCGCAACATGGCCGGCGTAAATTACTTCTCGGATTATTACGATTCCCTCCCTATGGGCGAAGAGATTGCAATCGGTATTCTGGAGGAACAGGCTCTGTGTTATAAAACTGATCCTTTCGTTCTGTCTGTTCCGACGTTCGATGGTGATGTGCCTCCTATCGGGCAACCT</t>
+          <t>ATGACGGATCAGCCTAAGCTGACTGCCCAGCCTGTACCTGAGGATGCGAACGCCCTTGCAGCCGGTCCTATCAACCCGCCTAATCAGGCCAACGGAGATGAGCAGCGCTATGAATCCGCCAATTACGCCATGTCTTTCACCAAAGGCCTGGATAACAACACGACCACCGGTCTCATAGAACAGTCTGGCGATTTTGAAGCTTTTCGCTCTGCAATTGACAATGGCTTTGCCGAAGACTTCACTCGCAACGTAGCTGTCCCACGGGCTGAGCCGCGCCGCAAATTGGAGGCCCCTACGGCCGGAACGGTGTATGAACTGCAGGGGCCGGATCCACAGGCCGTCACCATTCCTCCCGCGCCTGCCTTGTGCTCCGACGAACTTACTTTTGAGATGGCAGAAGTGTATGAACTGGCGCTGCTGCGCGACTTGCCGTTCAACGCCTTTGTCGCGGGCGGTGGTTCGGCAGCGCTGGCCGACTCTACTGCGCGACTTAACTCTCTCGCGTATGCCCAAGATGGTTTCAATCGCCGGCCACCTACGACCAACTCCTCTAACCAGCTGGACGCTCAGACTGTTTTTCGCGGCTCTTCCCCGGGTGTCGATCAAGGTCCGTATCTGTCGCAGTTCATGCTGATCGGCAATGCGTCTCCTTCTGAAGGTATCACCCCGGAGCAGGGGTTCATTAACTTCGGCGCTCAGCGCATTGATCAGCGCGTACTGGAAGCCCGCCAACAGGATGATTACATGATGAAATTGGATGATTTGAACCCTGTTCAACAGGGTTATGAAGTACCTGCAGATCCTTTTGACCCGTGCAAGTCCTCCGGTCCGGGCCAGGCATTCACTGGGCAGCCTCCTTTCATTAACACGCCACCTGATCTGGCGACCTATGTGAACGTGGACGCTCTGTACCAGGCCTATCTGAATGCTTGCCTGTTGCTATTGGGTAACGGCACCGCCTTTGACCCGGGATTTGACCTGCTGTCTGGTGGCGGGGAAGGGTTGCTGAATGATCCTGCCGGCGGCCAGAAAGTTCCGCTGAACGCGGGTGGGTTCGCCCTGTTGGGCGGTCCAAACGTTCTATCGCTAGTTACGGAGGTTGCTACCCCTGGACTGAAGGCTGTGCCTTACCAGAAGTTCAATAACAACCTCCGGTTGCCTCCCGAGGCCCTGGCCGCACGCATTGAAAAAGCGCAGGAAATTGAATCTCGCTTCCCGACAATTTGCGGTTGCTTCTCGGAAATGGCTTCTGATTTACAGCAGGTTGTTGACTTAATCCCTAATAACAACCAATCGCTGGCAGGCGAAGCCACCGCTCTGCTGCCGATGGCGTTTGCTGAAGGTTCACCGATGAACCCAGCTTATGGCGCGGGCAATGCGACCGTGGCCGGCGCCTGCGTGACGATTCTGAAAGCCTTTTTTAACACCTCGGCACTGTTCGTGAAAATTAACGATGTTGCGGGCTTTAACTCGAAGCAGAACATTCTGGCCCCTCTCAAATGCGGTGACTCTGTGGAAGCAGGGGCGTATCAGGAGACTGACTGCGGTAAACGCCTTGAATTCGAACCTTGTGGTTCATTTAACCTGATAGAAGGCAAATACGCCACCTTCAAACCGGACGGAAAGACGAACCAATCTTGTTGTCCCCTAACCTTAGAAGGTGAACTGAACAAGCTGGCGGCGAACATTTCCATCGGTCCTAATATGGCGGGTGTCAACTACTTTTCAGATTATTATGATTCTCTACCTATGGGAGAAGAAATCGCTATTGGCATCCTGGAAGAACAGGCTCTTTGTTATAAAACCGACCCATTCGTGCTGTCCGTGCCGACATTCGATGGTGATGTGCCTCCTATTGGTCAACGC</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>ATGACCGACCAGC</t>
+          <t>ATGACGGATCAGCCT</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>AGGTTGCCCGATA</t>
+          <t>GCGTTGACCAATAGGA</t>
         </is>
       </c>
     </row>
@@ -556,22 +556,22 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>TACTGTCTAGTCGGATTTGACTGCCGCGTCGCGCAAGCGCTTCTGCGTTTGCGAGACCGGCGGCCGGGACAAGTCGGCGTTTTGGTCCGCTTGCCACTACTCGTCGGAATACTTAGACGGAGAATAGGGTACAGTAAATGGTTTCCAGACCTATTATTGTGTTGATGCCCAGACCAGCTCGTCAGTCCACTAAAGCTCCGCAAGGCTAGCCGATAACTATTACCAAAGCGGCTCCTAAAGTGAGCGGTTCAAGGCCAGGGATTGCGTCTTGGCGCCGCGTTTAACCTTCGTGGCTGGCGCCCGTGGCACATGCTTGAGGTCCCAGGCCTGGGTGTTCGCCAATGATATGGCGGCCGCGGCCGGGACACAAGTCTACTTGACTGGAAGCTTTAACGGCTCCACATGCTTAATCGGAATAATGCGCTAAATGGTAAGTTGCGGAAGCACCGCCCACCACCCAGCCGACGTGACCGACTAAGGTGACGGGCGGAGTTATTAGACCGCATACGCGTCCTACCGAAATTGAGGGGAGGTGCGTTTTGCTTAAGTAGATTCGTCAACCTACGAGTCTGTCAAAAGGCGCCGAGTAGAGGCCCACAACTCGGACCCGGCATGAATAGCGTCAAGTACGAATAACCGTTGCGCAGTGGCAGTCTTCCGTAATGCGGTCTAGTCCCAAAGTATTTAAAACCCCGTGTCGCCTAGCTAGTCGGACAGGAGCTTCGCGGAGTCGTCCTACTAATATACTACTTCAACCTACTAAACTTGGCCCACCTTGTCCCGATGCTTCAGGCGCCCCTAGGAAAGCTGGGTACATTTAGCAGCCCGGGGCCGGTCCGTAAATGGCCGGTCGGAGGAAAATAGTTATGTGGCGGACTGGACCGATGTATACAATTACATCTACGGGAGATGGTTCGCATAGAGTTGCGAACAGACGAAGACGACCCCTTGCCATGGGGGAAACTGGGCCCAAAGCTGGAGAACAGTCCACCGCCGCTCCCAAACGACTTACTAGGCCGCAGACCGGTTTTCCATGGCGAATTACGCCCCCCGAAACGTGAGAACCCCCCAGGTTTGCACGACAGGGACCACTGGCTCCAACGATGGGGACCCGACTTTCGCCAGGGAATAGTCTTTAAATTGTTATTGGACGGAGACGCGGGCCTTCGCAACCGTCGGGCCTAGCTCTTTCGCGTCCTTTAGCTCAGAGGAAAAGGCCTTTAGACGCCCACGAAAAGACTTTACCGCAGCCTGGACGTCGTTTGGCATCTGGAATAGGCGTTGTTATTGGTTAGAGAACGCCCACTACGTTGGCGCGAAGAGGGCTACCGTAAGCGGCTTCCAAGTGGCTACTTGGGCCGGATACCACGGCCATTACGCTGGCATCGGCCTCGGACGCAATGCTAGAACTTTCGGAAAAAGTTGTGGAGACGAGACAAGCACTTTTATTTGCTAGACCGCCCTAAGATGAGTTTTGTCTTATAGGAACTAGCGGAATTTACACCACTAAGACAGCTTCGCCCACGTATGGTCCACTGGCTGACGCCGTTTGGAAATCTTAAGCTTGCCACACCGAGTAAATTGGACTAACTTCCGTTTCTACGCTGAAAATTTGGCCTACCTTGGTGTTTGTTTAGAACAACGGGAGACTGCGACCTCCCGCTTAACTTGTTTAATCGCCGGTTGTAAAGATAACCTGCGTTGTACCGTCCACACTTAATGAAAAGGCTGATAATGCTGAGGGACGCTTACCCGCTTCTTTAACGGTAACCATAAGAACTCCTTGTCCGCGATACAATGTTTTGCCTAGGAAAGCACGACAGGCACGGTTGGAAACTGCCTCTACATGGAGCGTAACCAGTCGGA</t>
+          <t>TACTGCCTAGTCGGATTCGACTGGCGTGTCGGACACGGACTTCTACGTTTGCGCAACCGGCGCCCTGCGCATGTCGGAGTCTTGGTCCGGTTACCACTACTCGTCGCGATACTTAGGCGTAGAATAGGATACAGGAAGTGCTTCCCCGACCTATTATTGTGCTGCTGGCCTGACCAGCTCGTTAGGCCGCTAAAACTTCGGAAGGCGAGTCGGTAACTATTGCCGAAGCGACTCCTGAAATGCGGAGTCCACGGCCAAGGTTTACGCCTCGGCGGAGCGTTCAACCTTCGAGGATGGCGGCCATGCCAGATACTTGACGTTCCTGGCCTAGGTGTTCGGCACTGGTAGGGGGGCCGCGGCCGCAATACGAGCCTGCTTGACTGTAAGCTTTAGCGCCTCCACATGCTTGAACGGGACGACGGACTAGACGGCAAATTACGCAAACAGCGGCCGCCCCCAAGGCGACGGAACCGCCTGAGTTGACGCGGAGACTTATTAGACCGAATACGAGTTCTACCGAAATTGAGGGCGGGTGCGTTTTGATTGAGTAGGTTTGTCGACCTACGAGTCTGGCACAAAGCGCCAAGGAGCGGCCCGCAGCTCGCCCCAGGGATAGACAGTGTCAAGTACGACTAGCCATTGCGTAGAGGAAGGCTTCCGTATTGGGGCCTAGTCCCCAAATAGTTGAAACCCCGCGTCGGATAACTGGTTGCGCAGGACCTTCGCGGAGTCGTCCTACTAATGTACTACTTTAACCTACTGAACTTAGCGCACCTCGTCCCAATGCTTCACGCGCCGCTGGCCAAGCTGGGTACGTTTAGGAGTCCAGGGCCGGTTCGCAAGTGACCGGTCGGAGGAAAGTAATTATGCGGTGCGCTAGAGCGTTGCATGCACTTACAGCTACGGGACATAGTCCGCATAGACTTACGCACAGAAGATAACGAACCGTTGCCATGCGGCAAACTAGGCCCGAAGCTAGACGACAGGCCGCCACCGCTCCCAGACGACTTACTGGGACGAAGACCGGTCTTTCACGGTGACTTACGGCCACCAAAACGAGACAACCCACCAGGTTTGCACGACAGTGACCAATGGCTTCAACGCTGGGGACCCGAATTTCGGCAGGCCATAGTCTTTAAGTTGTTATTAAACGGAGACGCGGGCCTTCGTGACCGCCGGGCCTAACTTTTCCGGGTTCTTTAACTCAGAGGAAAAGGCCTTTAAACGCCGACGAAAAGACTTTACCGAAGCCTGGACGTCGTCTGGCATCTGGATTATGCCTTATTGTTGGTCAGCGACCGCCCGCTACGGTGGCGCGACGACGGATACCGCAAACGGCTTCCGAGGGGCTACTTAGGCCGGATACCGCGTCCCTTGCGCTGTCAACGTCCCCGTACGCAATGATAGGAGTTCCGGAAAAAGTTGTGGAGACGTAATAAGCATTTTTAGTTGCTGGACCGGCCGAAAATAAGATTTGTTTTGTAAGAGCTGGCGAATTTTACGCCGCTGAGACAGCTTCGCCCCCGAATGGTTCACTGGCTGACACCATTTGGAAATCTTAAGCTTGCTACGCCAAGGAAATTAGACTAGCTTCCGTTCCTACGTTGGAAATTTGGCCTGCCGTGGTGATTGTTTAGTACAACGGGAGACTGGGACCTTCCGCTTGACTTATTTAACCGCCGATTGTAAAGGTAACCGGCGTTGTACCGACCGCAATTGATGAAGAGCCTGATGATGCTAAGGGACGGATACCCACTTCTTTAGCGCTAGCCATAAGACCTCCTTGTCCGCGACACGATGTTTTGGCTGGGAAAACAAAACAGTCACGGCTGCAAACTGCCCCTACAAGGAGGATAACCAGTCGCC</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>ATGACAGATCAGCCTAAACTGACGGCGCAGCGCGTTCGCGAAGACGCAAACGCTCTGGCCGCCGGCCCTGTTCAGCCGCAAAACCAGGCGAACGGTGATGAGCAGCCTTATGAATCTGCCTCTTATCCCATGTCATTTACCAAAGGTCTGGATAATAACACAACTACGGGTCTGGTCGAGCAGTCAGGTGATTTCGAGGCGTTCCGATCGGCTATTGATAATGGTTTCGCCGAGGATTTCACTCGCCAAGTTCCGGTCCCTAACGCAGAACCGCGGCGCAAATTGGAAGCACCGACCGCGGGCACCGTGTACGAACTCCAGGGTCCGGACCCACAAGCGGTTACTATACCGCCGGCGCCGGCCCTGTGTTCAGATGAACTGACCTTCGAAATTGCCGAGGTGTACGAATTAGCCTTATTACGCGATTTACCATTCAACGCCTTCGTGGCGGGTGGTGGGTCGGCTGCACTGGCTGATTCCACTGCCCGCCTCAATAATCTGGCGTATGCGCAGGATGGCTTTAACTCCCCTCCACGCAAAACGAATTCATCTAAGCAGTTGGATGCTCAGACAGTTTTCCGCGGCTCATCTCCGGGTGTTGAGCCTGGGCCGTACTTATCGCAGTTCATGCTTATTGGCAACGCGTCACCGTCAGAAGGCATTACGCCAGATCAGGGTTTCATAAATTTTGGGGCACAGCGGATCGATCAGCCTGTCCTCGAAGCGCCTCAGCAGGATGATTATATGATGAAGTTGGATGATTTGAACCGGGTGGAACAGGGCTACGAAGTCCGCGGGGATCCTTTCGACCCATGTAAATCGTCGGGCCCCGGCCAGGCATTTACCGGCCAGCCTCCTTTTATCAATACACCGCCTGACCTGGCTACATATGTTAATGTAGATGCCCTCTACCAAGCGTATCTCAACGCTTGTCTGCTTCTGCTGGGGAACGGTACCCCCTTTGACCCGGGTTTCGACCTCTTGTCAGGTGGCGGCGAGGGTTTGCTGAATGATCCGGCGTCTGGCCAAAAGGTACCGCTTAATGCGGGGGGCTTTGCACTCTTGGGGGGTCCAAACGTGCTGTCCCTGGTGACCGAGGTTGCTACCCCTGGGCTGAAAGCGGTCCCTTATCAGAAATTTAACAATAACCTGCCTCTGCGCCCGGAAGCGTTGGCAGCCCGGATCGAGAAAGCGCAGGAAATCGAGTCTCCTTTTCCGGAAATCTGCGGGTGCTTTTCTGAAATGGCGTCGGACCTGCAGCAAACCGTAGACCTTATCCGCAACAATAACCAATCTCTTGCGGGTGATGCAACCGCGCTTCTCCCGATGGCATTCGCCGAAGGTTCACCGATGAACCCGGCCTATGGTGCCGGTAATGCGACCGTAGCCGGAGCCTGCGTTACGATCTTGAAAGCCTTTTTCAACACCTCTGCTCTGTTCGTGAAAATAAACGATCTGGCGGGATTCTACTCAAAACAGAATATCCTTGATCGCCTTAAATGTGGTGATTCTGTCGAAGCGGGTGCATACCAGGTGACCGACTGCGGCAAACCTTTAGAATTCGAACGGTGTGGCTCATTTAACCTGATTGAAGGCAAAGATGCGACTTTTAAACCGGATGGAACCACAAACAAATCTTGTTGCCCTCTGACGCTGGAGGGCGAATTGAACAAATTAGCGGCCAACATTTCTATTGGACGCAACATGGCAGGTGTGAATTACTTTTCCGACTATTACGACTCCCTGCGAATGGGCGAAGAAATTGCCATTGGTATTCTTGAGGAACAGGCGCTATGTTACAAAACGGATCCTTTCGTGCTGTCCGTGCCAACCTTTGACGGAGATGTACCTCGCATTGGTCAGCCT</t>
+          <t>ATGACGGATCAGCCTAAGCTGACCGCACAGCCTGTGCCTGAAGATGCAAACGCGTTGGCCGCGGGACGCGTACAGCCTCAGAACCAGGCCAATGGTGATGAGCAGCGCTATGAATCCGCATCTTATCCTATGTCCTTCACGAAGGGGCTGGATAATAACACGACGACCGGACTGGTCGAGCAATCCGGCGATTTTGAAGCCTTCCGCTCAGCCATTGATAACGGCTTCGCTGAGGACTTTACGCCTCAGGTGCCGGTTCCAAATGCGGAGCCGCCTCGCAAGTTGGAAGCTCCTACCGCCGGTACGGTCTATGAACTGCAAGGACCGGATCCACAAGCCGTGACCATCCCCCCGGCGCCGGCGTTATGCTCGGACGAACTGACATTCGAAATCGCGGAGGTGTACGAACTTGCCCTGCTGCCTGATCTGCCGTTTAATGCGTTTGTCGCCGGCGGGGGTTCCGCTGCCTTGGCGGACTCAACTGCGCCTCTGAATAATCTGGCTTATGCTCAAGATGGCTTTAACTCCCGCCCACGCAAAACTAACTCATCCAAACAGCTGGATGCTCAGACCGTGTTTCGCGGTTCCTCGCCGGGCGTCGAGCGGGGTCCCTATCTGTCACAGTTCATGCTGATCGGTAACGCATCTCCTTCCGAAGGCATAACCCCGGATCAGGGGTTTATCAACTTTGGGGCGCAGCCTATTGACCAACGCGTCCTGGAAGCGCCTCAGCAGGATGATTACATGATGAAATTGGATGACTTGAATCGCGTGGAGCAGGGTTACGAAGTGCGCGGCGACCGGTTCGACCCATGCAAATCCTCAGGTCCCGGCCAAGCGTTCACTGGCCAGCCTCCTTTCATTAATACGCCACGCGATCTCGCAACGTACGTGAATGTCGATGCCCTGTATCAGGCGTATCTGAATGCGTGTCTTCTATTGCTTGGCAACGGTACGCCGTTTGATCCGGGCTTCGATCTGCTGTCCGGCGGTGGCGAGGGTCTGCTGAATGACCCTGCTTCTGGCCAGAAAGTGCCACTGAATGCCGGTGGTTTTGCTCTGTTGGGTGGTCCAAACGTGCTGTCACTGGTTACCGAAGTTGCGACCCCTGGGCTTAAAGCCGTCCGGTATCAGAAATTCAACAATAATTTGCCTCTGCGCCCGGAAGCACTGGCGGCCCGGATTGAAAAGGCCCAAGAAATTGAGTCTCCTTTTCCGGAAATTTGCGGCTGCTTTTCTGAAATGGCTTCGGACCTGCAGCAGACCGTAGACCTAATACGGAATAACAACCAGTCGCTGGCGGGCGATGCCACCGCGCTGCTGCCTATGGCGTTTGCCGAAGGCTCCCCGATGAATCCGGCCTATGGCGCAGGGAACGCGACAGTTGCAGGGGCATGCGTTACTATCCTCAAGGCCTTTTTCAACACCTCTGCATTATTCGTAAAAATCAACGACCTGGCCGGCTTTTATTCTAAACAAAACATTCTCGACCGCTTAAAATGCGGCGACTCTGTCGAAGCGGGGGCTTACCAAGTGACCGACTGTGGTAAACCTTTAGAATTCGAACGATGCGGTTCCTTTAATCTGATCGAAGGCAAGGATGCAACCTTTAAACCGGACGGCACCACTAACAAATCATGTTGCCCTCTGACCCTGGAAGGCGAACTGAATAAATTGGCGGCTAACATTTCCATTGGCCGCAACATGGCTGGCGTTAACTACTTCTCGGACTACTACGATTCCCTGCCTATGGGTGAAGAAATCGCGATCGGTATTCTGGAGGAACAGGCGCTGTGCTACAAAACCGACCCTTTTGTTTTGTCAGTGCCGACGTTTGACGGGGATGTTCCTCCTATTGGTCAGCGG</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>ATGACAGATCAGCCTAAA</t>
+          <t>ATGACGGATCAGCCT</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>AGGCTGACCAATGC</t>
+          <t>CCGCTGACCAATAGG</t>
         </is>
       </c>
     </row>
@@ -598,22 +598,22 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>TACGCGCTTGCGAGGGTCTTTAGAATGAGCTAAGGACACCTACGTCGGCTTGACCGGGCGAGTGCGGTCTTAGGATAATTGCTTCGGTTGCCACTACTTGTCGGAATACCGCCACTGTTTATAAAATACAGGAAATGGTTTCCAGACTAATTATTGGGCTTATGACCCGACAACCTTCTAGGCGGACTAAAACACCTTAAAGGAGGACGTTAACTATTACCAAAGTAACTAGGCAAGTGACTAGCGCAAGCGTTACCGCGCTTCATGTTTCAATTACTAGTCCCATTATAGCATCTCCTTCTATTGGGGGTCCTGGACCTAAAAGGAGTTAACCTTCGTGGCTGGCGCCCGCACCAATTGCTTAACCTTCCAGGGCTACGAGTCCGACAATGGTAGGGAGGTCGTGGGGGAGACGACCTGAGTTGAGCTTTATGGTTGGGACTTGAGTAAAAACTTTACCGGCTCCACATACTTAACCGTTAGGACGCCCTGCACGGAAACTTGTTAAAGCTATTGTTTTTATGCTGTCTACTTGAATGGCGAAGATAACGGGCGGACTTATTGGACCTAATGCATTTGTTGGTCTTGCCGGCCGGCGCGTTCCAATTGGTTCGCCCACTTGACCTGGACGTTTGACACAAAGCCCCCAGGAGTGGCCCGCATCTTCACCCGGGAATAGACAGTGTTAAAGACGAATAACCTTTGTTTCCACATTTACCACACCTGTTGTGCTGGTGCCCGGGATAGCGGATACCGCATGTCGTCTATCTAGTCGGACAGGGCCACCGCAGACAAGTCTTGATATACTGGGTCAACCTTTTAATACAGGGACACGTCGCGCCGTAGTTTGTTCTTGCGCTCTGGATACACCTTCCGTTACCCAGCTTAGGAAAGTAGATATGGGGCGGACTGGACCGGTGGATACAATTGATACTACGCGACATAGTTCGCATGGACTTGCGGACGAAGTAGGACGAACCATACCCGTGCGGCAAACTGGGAAGGAAACTATTGGAGAGACCGCCACCGCTTCGGCGGTTTCTGGGCTTTTGAGCCGGATTGCGTCCACCAAAGCGCAACATGCGCCCTGGCTTGTAAGACTGGAACCAATGACTTCATCGGTGAGCGCGAGACTTTCGATAGGGAAAGGTCTTTAAGTTGTTGTTATAAGGAGACGCGGGACTTCGGGACCGACGAGCGTAACTAGAGCACGGAGGATTTTTGTTACCGCTTTAGGTCCTTAGGAATTAGGGCGTCCGCGACAGTGTCATACACTTGCCAAAATAGCTATTCGACCCAAGTTTGCCTATGCCAAGGAATTGATGGAGGTGCGACCCGGCGTATCGCTTTTAGCGTCTTAGGAGGATGGATGACGGTTACCGGAAGGGTCTTCCGAGAGGGTACTTAGGCCGTATGCCGCGTCCGTTGCGGTGGCATCGACCACGTACGCACTGTTAAAACTTTCGTAAAAAACTATGGAGATGACAGGACTAGTTTCTAAGGTTGTTGCTTATATTCAAATTTTTGGTCCTTCGAGTCCTAGTCAAATAGCGCAAGGGATGGTTAAGTAGGCCCTGCCTAAACTAGTGTCTTCTGTAGTTGTTATAGAGACTCCGGGACTGCGAACTCCCCCTCGACTTATTTAATCGCCGTTTGTAGAGGTAGCCTGCGTTATACCGACCACAGTTAATGAAAAGCCTGATAATACTGAGTTAAGGATACCCGCTCGTCTAGCGATAACCGTAGGACGTTCTTGTCCGCGACTGAATAAGATGTCTGGGAAAGCAGTACAGCCACGGATGAAAGCTGCCATTATAGCAAGGATAACCTATA</t>
+          <t>TACGCCCTCGGAAGTGTCTTTAGGATGAGTTATGGACAACTGCGCCGGCTTGACCGCGGAAGCGGAGTTTTGGGTTAATTGCTCCGCTTGCCCCTGCTCGTCGGAATGCCCCCGCTATTCATGAAGTACAGGAAGTGGTTTCCTAACTAGTTGTTGGGATTATGGCCGGACGACCTTCTAGGTGCGCTGAAGCAGCTCAAAGGAGCGCGATAGCTGTTGCCAAAGTAGCTAGGCAAATGACTAGGACAAGCGTTACCTCGTTTTATATTTCAATTGCTAGTCCCGTTGTAGCACCTTCTTCTATTGGGTGTCCTAGAGCTGAAAGCGGTTAACCTTCGGGGTTGTCGGCCGCAGCACTTGCTTGAGCTCCCGGGTCTACGTGTCCGCCACTGATAAGGCGGCCGTGGCGGGAACGAGCTGAGCTGCGCGTTATGGTTGGGCCTCGAGTAAAAGCTTTACCGCCTTCACATGCTTGAGCGTTAAAACGCGCTACAAGGCGAATTATTAAAGCTGTTGTTTTTATGGTGCCTGCTTGACTGTCGGAGGTAACGAGGAAATTTGTTGGACCTAATGCACTTGTTAGTCTTGCCGGGAGGAGCGTTTCACTTAGTCCGTCCACTTGACCTGGACGTCTGCCACAAAGCGCCAAGAAGGGGTCCACACCTTCACCCAGGCATGGACAGTGTCAAAGACGAGTAACCATTATTTCCACAGTTGCCCCACCTGTTATGGTGATGTCCCGGATAACGAATACCACACGTCGTTTAGCTAGTCGCGCAAGGTCAGCGCAGGCATGTCTTGATGTACTGGGTCAACCTCTTGATACACGCGCAGGTCGCGCCATAGTTTGTTCTTGCGCTTTGCATGCAGCTCCCGTTGCCGAGATTAGCCAAATAAATGTGCGGTGCGCTAGACCGTTGGATACAGTTGATACTACGGGACATAGTTCGTATGAACTTGCGGACAAAGTAGGACAACCCATACCCCTGTGGCAAACTGGGAAGAAAACTATTGGACAGCCCGCCACCGCTTCGCCGCTTTCTGGGATTCTGGGCGGGTTTGCGACCGCCAAAACGTGACATACGCCCAGGCTTATAAGAATGTGACCATTGCCTTCAGCGCTGGGGACGCGACTTTCGATAAGGAAAGGTCTTTAAATTGTTGTTGTAGGCTAACGGAGGACTCCGAGAACGACGTGCGTAACTGGACCACGCGGGATTTTTGTTGCCACTCTAAGTTCTCAGAGACTAGGGTGTCCGGGACAGGGTCATACACTTACCAAAGTAGCTATTTGACCCAAGATTACCAATACCCAGTGACTGGTGGAGATGAGACCCCGCGTAACGTTTTTATCGGCTCAGTAGGATGGAAGAGGGATACCGTAAAGGACTCCCGAGTGGCTACTTAGGGCGAATGCCCCGGCCATTGCGGTGCCACCGGCCACGTACGCACTGTTAAGAGTTTCGGAAAAAGCTATGGAGGTGGCATGACTAATTTCTGAGGTTATTGCTTATATTCAAATTCTTGGTCCTTCGCGTCCTGGTCAAGTAGCGAAAGGCGTGCTTGAGCAGACCTTGGCTAAATTATTGGCTTCTGTATTTATTATAGAGTCTCCGGGACTGGGACCTTCCTCTTGAGTTGTTTGACCGGCGCTTGTAAAGTTAACCCGGATTGTACCGGCCGCATTTGATGAAGAGGCTAATAATACTAAGCTAAGGATACCCGCTTGTCTAACGATATCCATAAGATGTCCTTGTCCGCGAGTGGATAAGATGTCTAGGAAAGCAATACAGGCAAGGTTGGAAACTACCATTATAGCATGCCTAACCAATG</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>ATGCGCGAACGCTCCCAGAAATCTTACTCGATTCCTGTGGATGCAGCCGAACTGGCCCGCTCACGCCAGAATCCTATTAACGAAGCCAACGGTGATGAACAGCCTTATGGCGGTGACAAATATTTTATGTCCTTTACCAAAGGTCTGATTAATAACCCGAATACTGGGCTGTTGGAAGATCCGCCTGATTTTGTGGAATTTCCTCCTGCAATTGATAATGGTTTCATTGATCCGTTCACTGATCGCGTTCGCAATGGCGCGAAGTACAAAGTTAATGATCAGGGTAATATCGTAGAGGAAGATAACCCCCAGGACCTGGATTTTCCTCAATTGGAAGCACCGACCGCGGGCGTGGTTAACGAATTGGAAGGTCCCGATGCTCAGGCTGTTACCATCCCTCCAGCACCCCCTCTGCTGGACTCAACTCGAAATACCAACCCTGAACTCATTTTTGAAATGGCCGAGGTGTATGAATTGGCAATCCTGCGGGACGTGCCTTTGAACAATTTCGATAACAAAAATACGACAGATGAACTTACCGCTTCTATTGCCCGCCTGAATAACCTGGATTACGTAAACAACCAGAACGGCCGGCCGCGCAAGGTTAACCAAGCGGGTGAACTGGACCTGCAAACTGTGTTTCGGGGGTCCTCACCGGGCGTAGAAGTGGGCCCTTATCTGTCACAATTTCTGCTTATTGGAAACAAAGGTGTAAATGGTGTGGACAACACGACCACGGGCCCTATCGCCTATGGCGTACAGCAGATAGATCAGCCTGTCCCGGTGGCGTCTGTTCAGAACTATATGACCCAGTTGGAAAATTATGTCCCTGTGCAGCGCGGCATCAAACAAGAACGCGAGACCTATGTGGAAGGCAATGGGTCGAATCCTTTCATCTATACCCCGCCTGACCTGGCCACCTATGTTAACTATGATGCGCTGTATCAAGCGTACCTGAACGCCTGCTTCATCCTGCTTGGTATGGGCACGCCGTTTGACCCTTCCTTTGATAACCTCTCTGGCGGTGGCGAAGCCGCCAAAGACCCGAAAACTCGGCCTAACGCAGGTGGTTTCGCGTTGTACGCGGGACCGAACATTCTGACCTTGGTTACTGAAGTAGCCACTCGCGCTCTGAAAGCTATCCCTTTCCAGAAATTCAACAACAATATTCCTCTGCGCCCTGAAGCCCTGGCTGCTCGCATTGATCTCGTGCCTCCTAAAAACAATGGCGAAATCCAGGAATCCTTAATCCCGCAGGCGCTGTCACAGTATGTGAACGGTTTTATCGATAAGCTGGGTTCAAACGGATACGGTTCCTTAACTACCTCCACGCTGGGCCGCATAGCGAAAATCGCAGAATCCTCCTACCTACTGCCAATGGCCTTCCCAGAAGGCTCTCCCATGAATCCGGCATACGGCGCAGGCAACGCCACCGTAGCTGGTGCATGCGTGACAATTTTGAAAGCATTTTTTGATACCTCTACTGTCCTGATCAAAGATTCCAACAACGAATATAAGTTTAAAAACCAGGAAGCTCAGGATCAGTTTATCGCGTTCCCTACCAATTCATCCGGGACGGATTTGATCACAGAAGACATCAACAATATCTCTGAGGCCCTGACGCTTGAGGGGGAGCTGAATAAATTAGCGGCAAACATCTCCATCGGACGCAATATGGCTGGTGTCAATTACTTTTCGGACTATTATGACTCAATTCCTATGGGCGAGCAGATCGCTATTGGCATCCTGCAAGAACAGGCGCTGACTTATTCTACAGACCCTTTCGTCATGTCGGTGCCTACTTTCGACGGTAATATCGTTCCTATTGGATAT</t>
+          <t>ATGCGGGAGCCTTCACAGAAATCCTACTCAATACCTGTTGACGCGGCCGAACTGGCGCCTTCGCCTCAAAACCCAATTAACGAGGCGAACGGGGACGAGCAGCCTTACGGGGGCGATAAGTACTTCATGTCCTTCACCAAAGGATTGATCAACAACCCTAATACCGGCCTGCTGGAAGATCCACGCGACTTCGTCGAGTTTCCTCGCGCTATCGACAACGGTTTCATCGATCCGTTTACTGATCCTGTTCGCAATGGAGCAAAATATAAAGTTAACGATCAGGGCAACATCGTGGAAGAAGATAACCCACAGGATCTCGACTTTCGCCAATTGGAAGCCCCAACAGCCGGCGTCGTGAACGAACTCGAGGGCCCAGATGCACAGGCGGTGACTATTCCGCCGGCACCGCCCTTGCTCGACTCGACGCGCAATACCAACCCGGAGCTCATTTTCGAAATGGCGGAAGTGTACGAACTCGCAATTTTGCGCGATGTTCCGCTTAATAATTTCGACAACAAAAATACCACGGACGAACTGACAGCCTCCATTGCTCCTTTAAACAACCTGGATTACGTGAACAATCAGAACGGCCCTCCTCGCAAAGTGAATCAGGCAGGTGAACTGGACCTGCAGACGGTGTTTCGCGGTTCTTCCCCAGGTGTGGAAGTGGGTCCGTACCTGTCACAGTTTCTGCTCATTGGTAATAAAGGTGTCAACGGGGTGGACAATACCACTACAGGGCCTATTGCTTATGGTGTGCAGCAAATCGATCAGCGCGTTCCAGTCGCGTCCGTACAGAACTACATGACCCAGTTGGAGAACTATGTGCGCGTCCAGCGCGGTATCAAACAAGAACGCGAAACGTACGTCGAGGGCAACGGCTCTAATCGGTTTATTTACACGCCACGCGATCTGGCAACCTATGTCAACTATGATGCCCTGTATCAAGCATACTTGAACGCCTGTTTCATCCTGTTGGGTATGGGGACACCGTTTGACCCTTCTTTTGATAACCTGTCGGGCGGTGGCGAAGCGGCGAAAGACCCTAAGACCCGCCCAAACGCTGGCGGTTTTGCACTGTATGCGGGTCCGAATATTCTTACACTGGTAACGGAAGTCGCGACCCCTGCGCTGAAAGCTATTCCTTTCCAGAAATTTAACAACAACATCCGATTGCCTCCTGAGGCTCTTGCTGCACGCATTGACCTGGTGCGCCCTAAAAACAACGGTGAGATTCAAGAGTCTCTGATCCCACAGGCCCTGTCCCAGTATGTGAATGGTTTCATCGATAAACTGGGTTCTAATGGTTATGGGTCACTGACCACCTCTACTCTGGGGCGCATTGCAAAAATAGCCGAGTCATCCTACCTTCTCCCTATGGCATTTCCTGAGGGCTCACCGATGAATCCCGCTTACGGGGCCGGTAACGCCACGGTGGCCGGTGCATGCGTGACAATTCTCAAAGCCTTTTTCGATACCTCCACCGTACTGATTAAAGACTCCAATAACGAATATAAGTTTAAGAACCAGGAAGCGCAGGACCAGTTCATCGCTTTCCGCACGAACTCGTCTGGAACCGATTTAATAACCGAAGACATAAATAATATCTCAGAGGCCCTGACCCTGGAAGGAGAACTCAACAAACTGGCCGCGAACATTTCAATTGGGCCTAACATGGCCGGCGTAAACTACTTCTCCGATTATTATGATTCGATTCCTATGGGCGAACAGATTGCTATAGGTATTCTACAGGAACAGGCGCTCACCTATTCTACAGATCCTTTCGTTATGTCCGTTCCAACCTTTGATGGTAATATCGTACGGATTGGTTAC</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>ATGCGCGAACGCT</t>
+          <t>ATGCGGGAGCCTT</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>ATATCCAATAGGAACGATATTAC</t>
+          <t>GTAACCAATCCGTACGAT</t>
         </is>
       </c>
     </row>
@@ -640,22 +640,22 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>TACTTGTGGGGAGGAGTCGTCCGCGTCTTGTAGGGATTGTTGCGCCGCCTTGACCGCCGATTAGCGGGCTTGGGCGTCTTGTAATTGTTGTTTCTTCTTATACTCATAGGAGCCGGTTTTTTTCTGCCGTTACTTGGTAGCTTATAACGTTTGAAGTGATTTCCGGATGGCTTGCTACTTTTGTGGCCTGACGATGACTTGAGTCGGCTGATACTGGTCAAACAAGACCCATAAGTTAGGCCGCTGTGGTGGCTAAAGCGAGCTTGGGGCGACCCAGGCCGACTCGACGGCTTTCATTTACCTACGGACAGCTTTGTCTTTTAACTAACGCTGCTGCTATTAGCCAGTCCGAAGAACTTTAGCGTCTAGCGCGTCCCACGGCGGCCGCCACTACCACGATTTGACGGACGTAACCTCAGCCGTCCCCGGCCAGACCAAAAGCTGGACCTTCCTGGCCTGCGAGTTCGCCAATGGTACGGAGGACGCGGCGGAGACCTTAGTGGCCTTGACTGGAGGCTTTAGCGGCTTCAGATAAGCGTCCGTGACGAGGCGCTATATTTGAAGAGTGTCGACGCGCTGGGCCCAGACCCGCTGGTTCAGTTACGTACGCTAAGAACGGGCTGCGTCGACAGGTAAATGCTCCGCTAACTGTAGGACTTGTGGCACGTTTAGCTTCCTGTCTTGAACAAAAGACGATTAACGACGCTAGACTGTCTGCTGCTTGTCCGGGGAGTCGCCGGCGACCAATGGGCGGTCTTATAAAAGGCGCCATAGCGGGGCCCACTACTGCAACCGGGCATGGAAAGGGTCAAGAACGACTAGCCGTTGTTACGTGAGCCACCGCCTCACAAGCCGGTCCTTCGTCCATTATAACCAATACCACGCTAAGGATAGCTGGTCGCGCAGGGATTTCGTTGCGGCACATTTCTAAAGTACTGGTTGAAACTTTGCAACGATCTGCACGTCTTGCCCCGGCTAGACGGACCAAATCTTTGCATGCAACTACGCCTGGGCCCATTCACGGCGCTTAAGGGGCGGATGGGACACTAATGATGGGGGGGACTAAATCGGTGCATACACTTAATACTACGCAATATACTTCGAATGGACTTGCGTACAGACTAAAATGACCCATACCCGCGAGGCAAACTAGGCCCTTAAGGAAAGGTCTTTGGCCTGCAGCTTCTATTCGTTGTTCCAAAGCGCTTGAAACCTCCTGGCGTCTAAGAATGAGACCAAACGCTTCGACGATGGGGACCGGACTTTCGACAAGGAAAGGTCTTTAAATTACAATTGGGAGCGGACGGAGGCCTTCGAAATCCGCCAGAGCATCTAGCGATGTTTTTACCATTTCCGCGACCACTACTTAACTTCGGGCATCGCCGAGAACACCTCCGTGAGCTTTTACAGCCGGACGACAGTTTTCAACAGCGATTGTTAGTTGACGTCTTGGTCTTAGATCTGGGAAGGCCCCTAGGCAGGAGCCGGCCACTGTTGATGAAAGACGGCTACCGCAAGGGTCTTCCAAGCGGCTACTTGGGAAGGATGCCTCGGCCTTTGCGCTGGCACCGGCCACGGACACAGTGGTACGACTTTCGCAAGAAGCTATTGCCAAACGTCGACTTGGAGCCATACCGCTTGCCGTTTATGTAAAGAATACTTGGCTTGGTTCTGCCGAGAAGAAATGTCGTCCAGGACAACCTAACGGGAGACTGGCACCTCCCGCTTGACTTGTTTTAACGCCGCTTGTAAAGGTAACCAGCGCTGAACCGTCCACAATTGATAAAATGGCTAATGTAACTCAGAGAGGCGGAGCCACTCTTTTAGCGTTAGCCGTAAGACCTTCTTGTTTTTGACTGGATGCCGCTCTTGAAATGTTACTGCCAGGGTGAGATACTACCCCCAAGTTAAGTCTAA</t>
+          <t>TACTTGTGCGCGGCGGTCGTCCGTGTCTTGTAGGCGTTATTGCGGCGGCTTGACCGACGTTTAGGAGGTTTGGGAGTCTTATAATTGTTATTTCTCCTTATGCTTATAGCCGCGGGATTTTTTCTGCCGTTACTTGGTAGGTTATAGCGCTTAAAATGATTTCCGGACGGTTTGCTACTCTTGTGGCCTGACGACGACTTGAGGCGTCTAATGCTGGTTAAGCACAATCCATAAGTCAGTCCGCTATGGTGACTGAAGCGAGGATGGGGCGACCCTGGCCGGCTCAACGGATTTCAATTGCCCACAAACAGCTTTGTCTTTTAGCTAACACTACTACTATTAGCCAGCCCGAAGAACTTTAGGGTTTAACGTGTTCCGCGCCGCCCGCCACTGCCGCGATTTGACGCGCGTAACCTTAGTCGCCCGCGCCCGAATCAAAAGCTGGAACTTCCAGGGCTACGCGTTCGACATTGGTACGGCGGCCGTGGCGGAGACCTTAGGGGACTTGAGTGTAGTCTCTAACGCCTCCAAATAAGAGTTCGTGAAGACGGACTATAATTGAAAAGAGTTAACGGACTGGGCCCAGACCCGCTAGTCCATTTACGGACACTAAGGACAGGCTGCGTTGACAGATAAATACTTCGGTAACTATAAGAATTATGGCATGTTTAACTCCCAGTCTTGAACAAAAGTCGGTTGACGACACTAAATTGCCTGCTGCTTGTCCGTGCGGTCGCGGGCGACCATTGTGGAGTCTTGTAAAAGGGACCGTAGCGAGGTCCTCTACTACATCCGGGAATAGATAGAGTTAAAGAGGACTAGCCCTTGTTGCGCAACCCGCCGCCGCAAAAACCCGTCCTTCGTCCGTTGTAACCAATACCACGGTAGGCGTAACTAGTCGGACACGCCTTCCGTTGGGGTACATTTCTAAAGTACTGGTTGAAGCTCTGGAACGACCTGCATGTCTTACCACGTCTAGACGCGCCGGACCTTTGTATGCAACTGCGGCTGGGACCGTTTACAGGACTTAAGGGACGCATAGCGCACTAATGGTGCGGTGGACTGGAACGGTGAATACAGTTAATACTACGGGAAATGCTCCGTATAGACTTGCGGACAGAGTAGGACGACCCATACCCCCGTGGCAAACTAGGCCCCTAAGGCAAAGTTTTTGGTCTGCAGCTTCTATTTGTCGTTCCGAAGCGGTTAAAGCCACCTGGCGTTTAGGACTGCAACCACACACTCCGCCGCTGCGCGCCGAATTTTCGACAGGCCAAGGTCTTCAAGTTGCAGTTGGCGGGAGACGGAGGGCTCCGGGACCCGCCAGACCACCTGGGAATATTTTTGCCATTCCCACGACCCCTACTTGACTTTGGCCACCGGCGCAACCACCTTCGGGATCTCTTACATCCCAACGACAGATTTCACCAGCGCTTGTTAGTCAACGTCTTAGTCTTGAACCTGGCGAGCCCGCTAGGCAGAAGACGACCACTATTAATAAAAGAGGGCTACCGTAAAGGCCTTCCAAGAGGCTACTTGGGAAGAATACCACGGCCATTGCGGTGGCAACGGCCACGCACACAGTGGTACAATTTCCGCAAGAAACTATTACCAAACGTCAACTTAGACCCTTACCGTTTGCCGTTTATGTAGAGAATGCTTGGCTTAGTCCTGCCGAGAAGTAACGTCGTCCAGGACAATCTAACGGGCAATTGGCATCTTCCGCTTGAATTATTTTAGCGGCGCTTATATAGGTAACCGGCGCTAAACCGGCCGCACTTGATAAAATGGCTGATGTAGCTTAGGAACGCCAACCCGCTTTTTTAACGATAACCATAAGACCTTCTCGTCTTTGAATGAATACCACTTTTAAAATGCTACTGACACGGTGACATGCTGCCCCCGAGGTAAGTCTAA</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>ATGAACACCCCTCCTCAGCAGGCGCAGAACATCCCTAACAACGCGGCGGAACTGGCGGCTAATCGCCCGAACCCGCAGAACATTAACAACAAAGAAGAATATGAGTATCCTCGGCCAAAAAAAGACGGCAATGAACCATCGAATATTGCAAACTTCACTAAAGGCCTACCGAACGATGAAAACACCGGACTGCTACTGAACTCAGCCGACTATGACCAGTTTGTTCTGGGTATTCAATCCGGCGACACCACCGATTTCGCTCGAACCCCGCTGGGTCCGGCTGAGCTGCCGAAAGTAAATGGATGCCTGTCGAAACAGAAAATTGATTGCGACGACGATAATCGGTCAGGCTTCTTGAAATCGCAGATCGCGCAGGGTGCCGCCGGCGGTGATGGTGCTAAACTGCCTGCATTGGAGTCGGCAGGGGCCGGTCTGGTTTTCGACCTGGAAGGACCGGACGCTCAAGCGGTTACCATGCCTCCTGCGCCGCCTCTGGAATCACCGGAACTGACCTCCGAAATCGCCGAAGTCTATTCGCAGGCACTGCTCCGCGATATAAACTTCTCACAGCTGCGCGACCCGGGTCTGGGCGACCAAGTCAATGCATGCGATTCTTGCCCGACGCAGCTGTCCATTTACGAGGCGATTGACATCCTGAACACCGTGCAAATCGAAGGACAGAACTTGTTTTCTGCTAATTGCTGCGATCTGACAGACGACGAACAGGCCCCTCAGCGGCCGCTGGTTACCCGCCAGAATATTTTCCGCGGTATCGCCCCGGGTGATGACGTTGGCCCGTACCTTTCCCAGTTCTTGCTGATCGGCAACAATGCACTCGGTGGCGGAGTGTTCGGCCAGGAAGCAGGTAATATTGGTTATGGTGCGATTCCTATCGACCAGCGCGTCCCTAAAGCAACGCCGTGTAAAGATTTCATGACCAACTTTGAAACGTTGCTAGACGTGCAGAACGGGGCCGATCTGCCTGGTTTAGAAACGTACGTTGATGCGGACCCGGGTAAGTGCCGCGAATTCCCCGCCTACCCTGTGATTACTACCCCCCCTGATTTAGCCACGTATGTGAATTATGATGCGTTATATGAAGCTTACCTGAACGCATGTCTGATTTTACTGGGTATGGGCGCTCCGTTTGATCCGGGAATTCCTTTCCAGAAACCGGACGTCGAAGATAAGCAACAAGGTTTCGCGAACTTTGGAGGACCGCAGATTCTTACTCTGGTTTGCGAAGCTGCTACCCCTGGCCTGAAAGCTGTTCCTTTCCAGAAATTTAATGTTAACCCTCGCCTGCCTCCGGAAGCTTTAGGCGGTCTCGTAGATCGCTACAAAAATGGTAAAGGCGCTGGTGATGAATTGAAGCCCGTAGCGGCTCTTGTGGAGGCACTCGAAAATGTCGGCCTGCTGTCAAAAGTTGTCGCTAACAATCAACTGCAGAACCAGAATCTAGACCCTTCCGGGGATCCGTCCTCGGCCGGTGACAACTACTTTCTGCCGATGGCGTTCCCAGAAGGTTCGCCGATGAACCCTTCCTACGGAGCCGGAAACGCGACCGTGGCCGGTGCCTGTGTCACCATGCTGAAAGCGTTCTTCGATAACGGTTTGCAGCTGAACCTCGGTATGGCGAACGGCAAATACATTTCTTATGAACCGAACCAAGACGGCTCTTCTTTACAGCAGGTCCTGTTGGATTGCCCTCTGACCGTGGAGGGCGAACTGAACAAAATTGCGGCGAACATTTCCATTGGTCGCGACTTGGCAGGTGTTAACTATTTTACCGATTACATTGAGTCTCTCCGCCTCGGTGAGAAAATCGCAATCGGCATTCTGGAAGAACAAAAACTGACCTACGGCGAGAACTTTACAATGACGGTCCCACTCTATGATGGGGGTTCAATTCAGATT</t>
+          <t>ATGAACACGCGCCGCCAGCAGGCACAGAACATCCGCAATAACGCCGCCGAACTGGCTGCAAATCCTCCAAACCCTCAGAATATTAACAATAAAGAGGAATACGAATATCGGCGCCCTAAAAAAGACGGCAATGAACCATCCAATATCGCGAATTTTACTAAAGGCCTGCCAAACGATGAGAACACCGGACTGCTGCTGAACTCCGCAGATTACGACCAATTCGTGTTAGGTATTCAGTCAGGCGATACCACTGACTTCGCTCCTACCCCGCTGGGACCGGCCGAGTTGCCTAAAGTTAACGGGTGTTTGTCGAAACAGAAAATCGATTGTGATGATGATAATCGGTCGGGCTTCTTGAAATCCCAAATTGCACAAGGCGCGGCGGGCGGTGACGGCGCTAAACTGCGCGCATTGGAATCAGCGGGCGCGGGCTTAGTTTTCGACCTTGAAGGTCCCGATGCGCAAGCTGTAACCATGCCGCCGGCACCGCCTCTGGAATCCCCTGAACTCACATCAGAGATTGCGGAGGTTTATTCTCAAGCACTTCTGCCTGATATTAACTTTTCTCAATTGCCTGACCCGGGTCTGGGCGATCAGGTAAATGCCTGTGATTCCTGTCCGACGCAACTGTCTATTTATGAAGCCATTGATATTCTTAATACCGTACAAATTGAGGGTCAGAACTTGTTTTCAGCCAACTGCTGTGATTTAACGGACGACGAACAGGCACGCCAGCGCCCGCTGGTAACACCTCAGAACATTTTCCCTGGCATCGCTCCAGGAGATGATGTAGGCCCTTATCTATCTCAATTTCTCCTGATCGGGAACAACGCGTTGGGCGGCGGCGTTTTTGGGCAGGAAGCAGGCAACATTGGTTATGGTGCCATCCGCATTGATCAGCCTGTGCGGAAGGCAACCCCATGTAAAGATTTCATGACCAACTTCGAGACCTTGCTGGACGTACAGAATGGTGCAGATCTGCGCGGCCTGGAAACATACGTTGACGCCGACCCTGGCAAATGTCCTGAATTCCCTGCGTATCGCGTGATTACCACGCCACCTGACCTTGCCACTTATGTCAATTATGATGCCCTTTACGAGGCATATCTGAACGCCTGTCTCATCCTGCTGGGTATGGGGGCACCGTTTGATCCGGGGATTCCGTTTCAAAAACCAGACGTCGAAGATAAACAGCAAGGCTTCGCCAATTTCGGTGGACCGCAAATCCTGACGTTGGTGTGTGAGGCGGCGACGCGCGGCTTAAAAGCTGTCCGGTTCCAGAAGTTCAACGTCAACCGCCCTCTGCCTCCCGAGGCCCTGGGCGGTCTGGTGGACCCTTATAAAAACGGTAAGGGTGCTGGGGATGAACTGAAACCGGTGGCCGCGTTGGTGGAAGCCCTAGAGAATGTAGGGTTGCTGTCTAAAGTGGTCGCGAACAATCAGTTGCAGAATCAGAACTTGGACCGCTCGGGCGATCCGTCTTCTGCTGGTGATAATTATTTTCTCCCGATGGCATTTCCGGAAGGTTCTCCGATGAACCCTTCTTATGGTGCCGGTAACGCCACCGTTGCCGGTGCGTGTGTCACCATGTTAAAGGCGTTCTTTGATAATGGTTTGCAGTTGAATCTGGGAATGGCAAACGGCAAATACATCTCTTACGAACCGAATCAGGACGGCTCTTCATTGCAGCAGGTCCTGTTAGATTGCCCGTTAACCGTAGAAGGCGAACTTAATAAAATCGCCGCGAATATATCCATTGGCCGCGATTTGGCCGGCGTGAACTATTTTACCGACTACATCGAATCCTTGCGGTTGGGCGAAAAAATTGCTATTGGTATTCTGGAAGAGCAGAAACTTACTTATGGTGAAAATTTTACGATGACTGTGCCACTGTACGACGGGGGCTCCATTCAGATT</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>ATGAACACCCCTCC</t>
+          <t>ATGAACACGCGCC</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>AATCTGAATTGAACCCC</t>
+          <t>AATCTGAATGGAGCCC</t>
         </is>
       </c>
     </row>
@@ -682,22 +682,22 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>TACTTTCTCGGAGGAGTCTTCAGGAAGAGGCATGGACAACTTCGCCGCCTTGACCGTTTTAGTGGAGTTATGGGCAGCTTGGTTCGTTTGCCACTGCTTGTTGCCATACGCCCACCGCTGGCGATAAAGTACAGGAAATGGTTCCCAGACTAATTGTTGCTATTTTGGCCGGACAATCTCCTAGGGGGACTAAAGCACCTCAAAGGAGGACGTTAGCTACTACCGAAGTAACTGGGCAAATGACTATTTCACGGATTGCCACGCTTTATGGTCCAGCACTTGCCGTTTTAATTTCTACTTTTTCTGGGGTTCTTTGAACCACTAAAGGCGGTCAACCTTCGCGGCTGGCGCCCACACCATTTGCTTGACCTTCCCGGCCTAGGCGTCCGACACTGGTACGGCGGCCGTGGCGGGGAGGACCTACGATGCCCATTGTGCTTGGGACTCGACTAAAAACTCTACCGACTTCACATGCTCGACCGGTAGTAGGGACTAGAGGGCGACTTAAGTAAGCTTTTATTGCCATGTCGACTACGCTTCGACGTTCCGAGATAGCTCGGAAATTTAGTCAATCTGATGTAGTTTCTTGTCTTGCCAGGAGGCGCGTTTCACTTGGGCTAGCCATTTGACCTGCGGGTCTGTCACAAGGCGCCGAGCAGGGGCCCTCAGCTTCACCCGGGCATGGACAGGGTCAAGGACAATTAGCCATTATTTAGCTAGTTACCACTCCAATTGCACCTTCTACCGTTTTAATGGATGCCCCACGACCTTTAGTTGGTCTTTCACGGTTAGCGCTGGGGCTTCGACCTAATGTACTGGTTTGACCTACTAATGCAACTACACGTTGCCCCGTAGGTCGTCGGTGGACTCCGGATGCTACGTCCAAATGCGAAATAAATGTGGGGAGGACTGAACCGGTGCATACAGTTGATGCTACGGGACATGGTTCGGATAGACTTACGGACAGACTAGGACGACCCTTACCCGTGGGGCAAGCTGGGCCCCAAACTGTTGGACAGCCCACCGCCACACCGCCGCCCGCTAGGCGTCTGGGCGGCGTTACGTTTGCCCAAGCGTGACATGCCGCCAGGCTTGTAAGATTTGGACCACTGCCTTCAGCGCTGGGCGCGAAATTTTCGGCAAGGAAAAGTCTTTAAGTTGTTGTTGGAAGCGGACGGAGGCCTCCGTGACCGGCGAGCGCATCTGGACCACGGAGGATTCTTACTAACGGTCTAGGTCCTCCTTTAGGGATTCCGCGAGAGCGTCATGCAAGTCCAAAAATAACTATTTGACTGGCGGTTAGTTCCCGTCACGGTCGACAGCTGCGACCTGCTTTAGACACGGTAACGCTTGTTGAGCATAAACAATGGCTACCGGAAGGGCCTTCCAAGCGGATACTTGGGCCGGATACCACGCCCCTTACGCTGACACCGTCCGCGGACACACTGGTAAGAGTTTCGCAAGAAGCTATGGAGACGGCACGACCACTTCCTGCCTTTGGTCCTAATAGTCAAATTCGCTTACCTCTTTCCTCTGGTCGACCATCGAAAGGCGCGGCCCTTAACGCCTAGTTGTGACCTTCTTAGGTTTTAACTACTAAAAAGGCTTCGTGAGTGGAACCTCCCACTTGAGTTATTTAACCGTCGGTTATAAAGTTAACGCGGATTGTACCGTCCACACTTGATAAAGTGGCTGATAATGCTGAGCTAGGGATACCCGCTTGTCTAACGCTAGCCCTAAGACCTTCTTGTCCGAAATTGGATAGGCTGCCTAGGTAAGCATAACAGCCACGGCTGGAAACTACCTCTACATCAAGCGTAGCCCCCAGCG</t>
+          <t>TACTTCCTTGCGGGAGTTTTTAGCAAGAGGCAGGGACACCTTCGTCGCCTTGACCGGTTTAGTGCGGTCATAGGCAGATTGGTCCGCTTGCCGCTGCTTGTCGCGATGCGGCCCCCGCTAGCGATGAAATACAGCAAGTGTTTTCCAGAGTAATTATTACTGTTTTGGCCTGACGACCTTCTAGGAGGACTGAAGCAGCTTAAAGGAGGACGCTAACTACTACCAAAATAGCTAGGAAAATGCCTATTTCACGCGTTGCCCCGATTTATGGTCCAGCACTTGCCTTTTTAGTTTCTGCTTTTTCTAGGTTTTTTTGAGCCACTAAAAGCGGTCAACCTTCGAGGCTGACGTCCACATCATTTACTTGACCTTCCTGGACTGGGCGTTCGACATTGATACGGGGGCCGAGGGGGTAATGACCTGCGGTGGCCTTTGTGTTTGGGCCTCGACTAGAAACTTTACCGCCTCCAAATGCTCAACCGATAGTAGGCGCTAGACGGCAATTTAAGCAAGCTTTTGTTGCCTTGACGACTGCGATTTGACGTTCCGAGCTAACTTGGAGACTTAGTCGACCTAATATAATTTCTTGTCTTGCCGGGAGGAGGATTTCAATTAGGTTAACCCTTTAACCTACGTGTTTGACATAAAGCGCCTAGAAGAGGTCCCCATCTTCATCCGGGTATGAACAGAGTCAAAGACAACTAGCCATTGTTTAGCTAGTTACCACTTCAATTACAACTTCTACCATTTTAATGTATACCGCACGACCTTTAGTTGGTCTTTCATGGCTAGCGATGGGGTTTTAACCTAATATACTGGTTTGAACTACTAATGCATCTACAGGTCGGACCATAGGTTGTTGGCGCGCTTCGCATACTACGGCCAAACGGAAAATAGATATGTGGCGGACTGAACCGGTGAATACATTTAATACTGCGCGACATAGTCCGTATAGACTTGCGTACAGACTAAGACAACCCATACCCATGTGGTAAACTGGGACCGAAACTATTAGACAGCCCACCGCCACACCGCCGTCCGCTAGGTGTTTGGGCTGGATTGCGGTTGCCCAAACGCGACATACCGCCAGGCTTGTAGGACTTAGACCAGTGTCTTCAACGTTGAGGACGGGACTTCCGGCAAGCGAAGGTCTTTAAATTATTGTTAGACGGAGACGCGGGCCTTCGTAATCGCCGAGGACACCTGGACCAGGGAGCGTTTTTACTAACAGTCTAGGTTCTCCTTTAGGGGTTTCGCAACAGGGTTATGCAAGTTCATAAATAACTATTTGACTGGCGATTAGTCCCTGTCACAGTCGACAGGTGGGAACTACTCTAAACGCGCTAGCGATTATTGAGCATGGACGACGGCTACCGCAAAGGGCTTCCAAGCGGGTACTTAGGGCGTATGCCGCGGCCATTACGGTGGCACCGACCGCGCACGCAATGTTAAGACTTTCGCAAGAAGCTATGGAGCCGCCAAGACCAATTTCTACCCTTAGTCCTGATGGTCAAGTTTGCGTACCTCTTTCCTCTAGTCGACCACCGGAAAGCGCGACCATTGACACCGAGTTGAGACCTTCTCAGATTTTAACTACTAAAAAGGCTCCGCGACTGGGACCTCCCACTCGACTTATTCGACCGACGCTTGTAAAGATAGCGAGGATTGTACCGCCCGCATTTGATGAAGTGTCTGATAATGCTAAGATAGGGATACCCCCTCGTCTAGCGTTAGCCGTAGGACCTTCTTGTCCGGGACTGTATAGGCTGACTAGGCAAGCACGAAAGGCATGGCTGGAAACTACCGCTACACCATGGATAGCCCCCAGGA</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>ATGAAAGAGCCTCCTCAGAAGTCCTTCTCCGTACCTGTTGAAGCGGCGGAACTGGCAAAATCACCTCAATACCCGTCGAACCAAGCAAACGGTGACGAACAACGGTATGCGGGTGGCGACCGCTATTTCATGTCCTTTACCAAGGGTCTGATTAACAACGATAAAACCGGCCTGTTAGAGGATCCCCCTGATTTCGTGGAGTTTCCTCCTGCAATCGATGATGGCTTCATTGACCCGTTTACTGATAAAGTGCCTAACGGTGCGAAATACCAGGTCGTGAACGGCAAAATTAAAGATGAAAAAGACCCCAAGAAACTTGGTGATTTCCGCCAGTTGGAAGCGCCGACCGCGGGTGTGGTAAACGAACTGGAAGGGCCGGATCCGCAGGCTGTGACCATGCCGCCGGCACCGCCCCTCCTGGATGCTACGGGTAACACGAACCCTGAGCTGATTTTTGAGATGGCTGAAGTGTACGAGCTGGCCATCATCCCTGATCTCCCGCTGAATTCATTCGAAAATAACGGTACAGCTGATGCGAAGCTGCAAGGCTCTATCGAGCCTTTAAATCAGTTAGACTACATCAAAGAACAGAACGGTCCTCCGCGCAAAGTGAACCCGATCGGTAAACTGGACGCCCAGACAGTGTTCCGCGGCTCGTCCCCGGGAGTCGAAGTGGGCCCGTACCTGTCCCAGTTCCTGTTAATCGGTAATAAATCGATCAATGGTGAGGTTAACGTGGAAGATGGCAAAATTACCTACGGGGTGCTGGAAATCAACCAGAAAGTGCCAATCGCGACCCCGAAGCTGGATTACATGACCAAACTGGATGATTACGTTGATGTGCAACGGGGCATCCAGCAGCCACCTGAGGCCTACGATGCAGGTTTACGCTTTATTTACACCCCTCCTGACTTGGCCACGTATGTCAACTACGATGCCCTGTACCAAGCCTATCTGAATGCCTGTCTGATCCTGCTGGGAATGGGCACCCCGTTCGACCCGGGGTTTGACAACCTGTCGGGTGGCGGTGTGGCGGCGGGCGATCCGCAGACCCGCCGCAATGCAAACGGGTTCGCACTGTACGGCGGTCCGAACATTCTAAACCTGGTGACGGAAGTCGCGACCCGCGCTTTAAAAGCCGTTCCTTTTCAGAAATTCAACAACAACCTTCGCCTGCCTCCGGAGGCACTGGCCGCTCGCGTAGACCTGGTGCCTCCTAAGAATGATTGCCAGATCCAGGAGGAAATCCCTAAGGCGCTCTCGCAGTACGTTCAGGTTTTTATTGATAAACTGACCGCCAATCAAGGGCAGTGCCAGCTGTCGACGCTGGACGAAATCTGTGCCATTGCGAACAACTCGTATTTGTTACCGATGGCCTTCCCGGAAGGTTCGCCTATGAACCCGGCCTATGGTGCGGGGAATGCGACTGTGGCAGGCGCCTGTGTGACCATTCTCAAAGCGTTCTTCGATACCTCTGCCGTGCTGGTGAAGGACGGAAACCAGGATTATCAGTTTAAGCGAATGGAGAAAGGAGACCAGCTGGTAGCTTTCCGCGCCGGGAATTGCGGATCAACACTGGAAGAATCCAAAATTGATGATTTTTCCGAAGCACTCACCTTGGAGGGTGAACTCAATAAATTGGCAGCCAATATTTCAATTGCGCCTAACATGGCAGGTGTGAACTATTTCACCGACTATTACGACTCGATCCCTATGGGCGAACAGATTGCGATCGGGATTCTGGAAGAACAGGCTTTAACCTATCCGACGGATCCATTCGTATTGTCGGTGCCGACCTTTGATGGAGATGTAGTTCGCATCGGGGGTCGC</t>
+          <t>ATGAAGGAACGCCCTCAAAAATCGTTCTCCGTCCCTGTGGAAGCAGCGGAACTGGCCAAATCACGCCAGTATCCGTCTAACCAGGCGAACGGCGACGAACAGCGCTACGCCGGGGGCGATCGCTACTTTATGTCGTTCACAAAAGGTCTCATTAATAATGACAAAACCGGACTGCTGGAAGATCCTCCTGACTTCGTCGAATTTCCTCCTGCGATTGATGATGGTTTTATCGATCCTTTTACGGATAAAGTGCGCAACGGGGCTAAATACCAGGTCGTGAACGGAAAAATCAAAGACGAAAAAGATCCAAAAAAACTCGGTGATTTTCGCCAGTTGGAAGCTCCGACTGCAGGTGTAGTAAATGAACTGGAAGGACCTGACCCGCAAGCTGTAACTATGCCCCCGGCTCCCCCATTACTGGACGCCACCGGAAACACAAACCCGGAGCTGATCTTTGAAATGGCGGAGGTTTACGAGTTGGCTATCATCCGCGATCTGCCGTTAAATTCGTTCGAAAACAACGGAACTGCTGACGCTAAACTGCAAGGCTCGATTGAACCTCTGAATCAGCTGGATTATATTAAAGAACAGAACGGCCCTCCTCCTAAAGTTAATCCAATTGGGAAATTGGATGCACAAACTGTATTTCGCGGATCTTCTCCAGGGGTAGAAGTAGGCCCATACTTGTCTCAGTTTCTGTTGATCGGTAACAAATCGATCAATGGTGAAGTTAATGTTGAAGATGGTAAAATTACATATGGCGTGCTGGAAATCAACCAGAAAGTACCGATCGCTACCCCAAAATTGGATTATATGACCAAACTTGATGATTACGTAGATGTCCAGCCTGGTATCCAACAACCGCGCGAAGCGTATGATGCCGGTTTGCCTTTTATCTATACACCGCCTGACTTGGCCACTTATGTAAATTATGACGCGCTGTATCAGGCATATCTGAACGCATGTCTGATTCTGTTGGGTATGGGTACACCATTTGACCCTGGCTTTGATAATCTGTCGGGTGGCGGTGTGGCGGCAGGCGATCCACAAACCCGACCTAACGCCAACGGGTTTGCGCTGTATGGCGGTCCGAACATCCTGAATCTGGTCACAGAAGTTGCAACTCCTGCCCTGAAGGCCGTTCGCTTCCAGAAATTTAATAACAATCTGCCTCTGCGCCCGGAAGCATTAGCGGCTCCTGTGGACCTGGTCCCTCGCAAAAATGATTGTCAGATCCAAGAGGAAATCCCCAAAGCGTTGTCCCAATACGTTCAAGTATTTATTGATAAACTGACCGCTAATCAGGGACAGTGTCAGCTGTCCACCCTTGATGAGATTTGCGCGATCGCTAATAACTCGTACCTGCTGCCGATGGCGTTTCCCGAAGGTTCGCCCATGAATCCCGCATACGGCGCCGGTAATGCCACCGTGGCTGGCGCGTGCGTTACAATTCTGAAAGCGTTCTTCGATACCTCGGCGGTTCTGGTTAAAGATGGGAATCAGGACTACCAGTTCAAACGCATGGAGAAAGGAGATCAGCTGGTGGCCTTTCGCGCTGGTAACTGTGGCTCAACTCTGGAAGAGTCTAAAATTGATGATTTTTCCGAGGCGCTGACCCTGGAGGGTGAGCTGAATAAGCTGGCTGCGAACATTTCTATCGCTCCTAACATGGCGGGCGTAAACTACTTCACAGACTATTACGATTCTATCCCTATGGGGGAGCAGATCGCAATCGGCATCCTGGAAGAACAGGCCCTGACATATCCGACTGATCCGTTCGTGCTTTCCGTACCGACCTTTGATGGCGATGTGGTACCTATCGGGGGTCCT</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>ATGAAAGAGCCTCCTC</t>
+          <t>ATGAAGGAACGCCC</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>GCGACCCCCGATG</t>
+          <t>AGGACCCCCGATA</t>
         </is>
       </c>
     </row>
@@ -724,22 +724,22 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>TACTGGCTATGGGTCTTGGGATTGGCGCGTCTCCAACGGAAATTTCAGGCGCACAGGCGGCGGCTCAACCGAGCCCGTGCTCCGAGAGGGCGATTGGACAGGTTGTTGAGACTTAGAGCGAAGGCGTTGGGCCTACCTTGGGCGAGGGAAAACCGTTTGAAATGTTTTCCGGAGGGCTTGTAATTTCTTTGTCGTGACCAACTTAGCCGTTAACTAATGCTGGCGAAACATGCGCGTTAGCTAAGACCTCTAGGCGGACTAAAGCGACTGAACGGAGAACCAGGCGTCCCACAGCTCGGCGCTAAATGGAGTCCTTAACGTAGGCTAGGGCTTCACCCGTGAGGACGGAACCTTAGACCGCCACGCCCCGACCACAAGCTGGACCTTCCCGGACTACGTGTCCGCCAATGATACGGGGGCCGGGGGCTCGACCTAAGACTGCTTGATCAGCGGCTTCACTGTCTTACGATGAACTACAGAAATAACGGACTGCACGGTAAGGGTTGCAAGCTCAGGTTGAGATTGTAAGTCCGCCGTCGTCTTAGATAATTATTGTGCGTCAACTAATTTAAATTCTTATTAGGCGGCCGTTTGAACTGTCGCCGCCTTGCGAGGGCGGACGGACCAGGCCAGTGATGGCGTTTGCACAAAGCCCCTTAGTGTGGTCCACTACTCCAACCGGGAATGGACAGTGTCAAGGACGACCAGCCCTGATGACCTTAACGTTTGCCTTTGCTTCATCCACTGCCGAAATATGTCATACCGCCGTACGCGTACCTAGTCGGACAGGCCCACCGCTTCGGCTTATAACTAATATACTGATGGAAACCACGAATAGACCTACAGGTCTTACGGCGATTGCAGAGGCCCGGACTTAACATATTTCTCCTTCTTGGTGCGAAGGCTAAATAGTTGTGAGGTGGACTAGACCGGTGTATACATTTAAAACTGCGTGACATAGTCCGCATAGACTTGCGGACATAGTAAGACGACCTATAACCACGCGGAAAACTAAGACCATAAGGCAAAGTCGACCTATTGCTGTAGCTGTTCGTCGTCCCAAAGCGTTGAAAGCCGCCAGGCTTGTAAGACAGTGAACACTGACTTCAACGCTGTGCGCGAGAGTTTCGGCAGGGAAAGGTTTTCAAATTACATTTGGCGGCGGACGGAGGCCTCCGCTAACCCCGGGGACAGCTAGGAATGACACGCTGATTTCGCGGTCTTAAACGACCACGGCGGTTTGACAGGCTTCGAGACCTATTCCTTGACGAGGTCTTTCACTTACTATTGTTGTTTTTTGTCTTAGACAACAGGCTAGCCCCGTTGGGCGGACGTTTACTGAAATTAGGCCTACCACTCCAGAGACTCCCCTTGGACGACTACGGATACCGGAAAGGTCTCCCGAGTGGATACTTGGGCCGGATGCCCCGCCCGTTACGTTGGCATCGACCGCGCACGCATTGGCACAATTTTCGTAAAAAGCTACCACCGATGGGAGACGGGAAAACGATATAGTGGCTACTCCTGCCATGCCCGAATGTCCGCCAGCTCTAGCTACTCGGAAACTGGCACCTGCCCCTTGACTTATTTTAAACGAGTTTATAGAGATAGCCCGGATTGAACCGACCACACTTGATGAAGTGACTGATGTAACTTAGCTATGCGTAACCGCTCCTTTAACGCTAACCATAAGACGTCCTTGTCTTTAACTGCAAAAGACTTTTGAAGAGATACTGCGACTTGTTCAAACTACCGAGGTGGTAGGCGTAA</t>
+          <t>TACTGCCTGTGGGTCTTAGGATTAGGACGTCTTCAGCGAAAATTTCAAGCTCAAAGGCGGCGGCTTGAACGGGCGCGTGCGCCGAGCGGTCGGTTAAATAGATTGTTAAGCCTTAGCGCGAAAGCTTTAGGCCTACCCTGCGCGAGGAACGATCGCTTGAAATGTTTCCCGGACGGCTTGTAATTTCTTTGCCGAGAACATCTCAGACGTTAACTGATACTAGCGAAGCAAGCGCGCTAACTAAGGCCCCTGGGCGGACTAAAGCGCCTAGACGGAGAACCAGGTGTCCCTCACCTTGGCGCGAAGTGCAGACCTTAACGTAGGCTAGGGCTTCAGCCGTGAGCGCGTAACCTTAGCCCACCCCGGCCGGACCAAAAGCTAGACCTCCCGGGCCTACGTGTCCGACAATGCTACGGCGGTCGGGGACTCGACCTGAGGCTACTCGACCACCGGCTTCAATGACTTACGATAAACTACAGAGACAATGCGCTGCAAGGGAAAGGCTGGAAGCTTAGTTTAAGCTTGTAGGTCCGCCGGCGTCTTAGGTAGTTGTTGTGCGTTAACTAGTTCAAGTTCTTGTTAGGCGGCCGGTTAGACTGCCGTCGCCTCGCGAGAGGAAACGCGCCGGGTCAATGGTGGCGATTGCAAAAAGCGCCTTAATGAGGACCGCTGCTTCAACCCGGAATAGACAGTGTCAAGGACGACCACCCATGTTGGCCATAGCGGTTACCGTTACTCCAGCCGCTACCTAAATAGGTTATGCCGCCATACGCTTACCTAGTCGCGCATGCCCAGCGCTTTGGCTTGTAGCTGATGTACTGGTGTAAACCGCGCATAGAGCTACAAGTTTTGCGTCGCTTACAAAGACCAGGACTCGATATATTTCTTCTCCTTGGAGCCAAAGCGAAGTAGTTGTGGGGTGCTCTAGACCGTTGAATACAATTGAAGCTACGTGACATGGTTCGCATGGACTTGCGAACGTAGTAAGACGACCTATAACCGCGTGGCAAACTGAGTCCTTAAGGTAAAGTTGACCTGTTGCTGTAGCTATTTGTCGTCCCCAAGCGGTGGAAGCCGCCGGGATTATAGGACAGGGACCACTGCCTCCACCGCTGGGGACGCGACTTTCGGCAAGGAAAGGTCTTCAAGTTACAGTTGGCGGCGGACGGAGGGCTTCGCTAGCCGCGAGGACAACTGGGAATAACGCGCTGGTTCCGAGGACTTAAGCGACCGCGTCGTTTTGATAGCCTTCGGGACCTGTTTCTTGACGACGTCTTTCACTTACTATTGTTGTTTTTTGTCTTGGACGACAGCCTAGGACCCTTGGGCGGACGTTTGCTAAAATTGGGTCTGCCTCTCCAGAGCCTCCCCTTAGAGGACTACGGCTACCGGAAAGGCCTTCCAAGCGGCTACTTAGGTCGGATACCACGGCCGTTACGTTGGCACCGTCCCCGTACGCACTGTCACAATTTTCGTAAGAAACTGCCGCCTATAGCGGACGGCAAAACAATGTAGTGACTACTTCTGCCATGCCCAGATGTCCGTCATCTTTATCTGCTTGGTGACTGCCAGCTGCCACTTAACTTGTTTTAAACGAGATTATAGAGTTAACCGGCTTTGAACCGGCCACAATTGATGAAGTGCCTAATGTAACTTAGGTATGCCTATCCGCTTCTTTAGCGGTAGCCATAGAACGTCCTCGTCTTCGACTGGAAAAGACTTTTGAAGAGATACTGGGACTTGTTTAAACTGCCGAGTTGATAGGCGTAG</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>ATGACCGATACCCAGAACCCTAACCGCGCAGAGGTTGCCTTTAAAGTCCGCGTGTCCGCCGCCGAGTTGGCTCGGGCACGAGGCTCTCCCGCTAACCTGTCCAACAACTCTGAATCTCGCTTCCGCAACCCGGATGGAACCCGCTCCCTTTTGGCAAACTTTACAAAAGGCCTCCCGAACATTAAAGAAACAGCACTGGTTGAATCGGCAATTGATTACGACCGCTTTGTACGCGCAATCGATTCTGGAGATCCGCCTGATTTCGCTGACTTGCCTCTTGGTCCGCAGGGTGTCGAGCCGCGATTTACCTCAGGAATTGCATCCGATCCCGAAGTGGGCACTCCTGCCTTGGAATCTGGCGGTGCGGGGCTGGTGTTCGACCTGGAAGGGCCTGATGCACAGGCGGTTACTATGCCCCCGGCCCCCGAGCTGGATTCTGACGAACTAGTCGCCGAAGTGACAGAATGCTACTTGATGTCTTTATTGCCTGACGTGCCATTCCCAACGTTCGAGTCCAACTCTAACATTCAGGCGGCAGCAGAATCTATTAATAACACGCAGTTGATTAAATTTAAGAATAATCCGCCGGCAAACTTGACAGCGGCGGAACGCTCCCGCCTGCCTGGTCCGGTCACTACCGCAAACGTGTTTCGGGGAATCACACCAGGTGATGAGGTTGGCCCTTACCTGTCACAGTTCCTGCTGGTCGGGACTACTGGAATTGCAAACGGAAACGAAGTAGGTGACGGCTTTATACAGTATGGCGGCATGCGCATGGATCAGCCTGTCCGGGTGGCGAAGCCGAATATTGATTATATGACTACCTTTGGTGCTTATCTGGATGTCCAGAATGCCGCTAACGTCTCCGGGCCTGAATTGTATAAAGAGGAAGAACCACGCTTCCGATTTATCAACACTCCACCTGATCTGGCCACATATGTAAATTTTGACGCACTGTATCAGGCGTATCTGAACGCCTGTATCATTCTGCTGGATATTGGTGCGCCTTTTGATTCTGGTATTCCGTTTCAGCTGGATAACGACATCGACAAGCAGCAGGGTTTCGCAACTTTCGGCGGTCCGAACATTCTGTCACTTGTGACTGAAGTTGCGACACGCGCTCTCAAAGCCGTCCCTTTCCAAAAGTTTAATGTAAACCGCCGCCTGCCTCCGGAGGCGATTGGGGCCCCTGTCGATCCTTACTGTGCGACTAAAGCGCCAGAATTTGCTGGTGCCGCCAAACTGTCCGAAGCTCTGGATAAGGAACTGCTCCAGAAAGTGAATGATAACAACAAAAAACAGAATCTGTTGTCCGATCGGGGCAACCCGCCTGCAAATGACTTTAATCCGGATGGTGAGGTCTCTGAGGGGAACCTGCTGATGCCTATGGCCTTTCCAGAGGGCTCACCTATGAACCCGGCCTACGGGGCGGGCAATGCAACCGTAGCTGGCGCGTGCGTAACCGTGTTAAAAGCATTTTTCGATGGTGGCTACCCTCTGCCCTTTTGCTATATCACCGATGAGGACGGTACGGGCTTACAGGCGGTCGAGATCGATGAGCCTTTGACCGTGGACGGGGAACTGAATAAAATTTGCTCAAATATCTCTATCGGGCCTAACTTGGCTGGTGTGAACTACTTCACTGACTACATTGAATCGATACGCATTGGCGAGGAAATTGCGATTGGTATTCTGCAGGAACAGAAATTGACGTTTTCTGAAAACTTCTCTATGACGCTGAACAAGTTTGATGGCTCCACCATCCGCATT</t>
+          <t>ATGACGGACACCCAGAATCCTAATCCTGCAGAAGTCGCTTTTAAAGTTCGAGTTTCCGCCGCCGAACTTGCCCGCGCACGCGGCTCGCCAGCCAATTTATCTAACAATTCGGAATCGCGCTTTCGAAATCCGGATGGGACGCGCTCCTTGCTAGCGAACTTTACAAAGGGCCTGCCGAACATTAAAGAAACGGCTCTTGTAGAGTCTGCAATTGACTATGATCGCTTCGTTCGCGCGATTGATTCCGGGGACCCGCCTGATTTCGCGGATCTGCCTCTTGGTCCACAGGGAGTGGAACCGCGCTTCACGTCTGGAATTGCATCCGATCCCGAAGTCGGCACTCGCGCATTGGAATCGGGTGGGGCCGGCCTGGTTTTCGATCTGGAGGGCCCGGATGCACAGGCTGTTACGATGCCGCCAGCCCCTGAGCTGGACTCCGATGAGCTGGTGGCCGAAGTTACTGAATGCTATTTGATGTCTCTGTTACGCGACGTTCCCTTTCCGACCTTCGAATCAAATTCGAACATCCAGGCGGCCGCAGAATCCATCAACAACACGCAATTGATCAAGTTCAAGAACAATCCGCCGGCCAATCTGACGGCAGCGGAGCGCTCTCCTTTGCGCGGCCCAGTTACCACCGCTAACGTTTTTCGCGGAATTACTCCTGGCGACGAAGTTGGGCCTTATCTGTCACAGTTCCTGCTGGTGGGTACAACCGGTATCGCCAATGGCAATGAGGTCGGCGATGGATTTATCCAATACGGCGGTATGCGAATGGATCAGCGCGTACGGGTCGCGAAACCGAACATCGACTACATGACCACATTTGGCGCGTATCTCGATGTTCAAAACGCAGCGAATGTTTCTGGTCCTGAGCTATATAAAGAAGAGGAACCTCGGTTTCGCTTCATCAACACCCCACGAGATCTGGCAACTTATGTTAACTTCGATGCACTGTACCAAGCGTACCTGAACGCTTGCATCATTCTGCTGGATATTGGCGCACCGTTTGACTCAGGAATTCCATTTCAACTGGACAACGACATCGATAAACAGCAGGGGTTCGCCACCTTCGGCGGCCCTAATATCCTGTCCCTGGTGACGGAGGTGGCGACCCCTGCGCTGAAAGCCGTTCCTTTCCAGAAGTTCAATGTCAACCGCCGCCTGCCTCCCGAAGCGATCGGCGCTCCTGTTGACCCTTATTGCGCGACCAAGGCTCCTGAATTCGCTGGCGCAGCAAAACTATCGGAAGCCCTGGACAAAGAACTGCTGCAGAAAGTGAATGATAACAACAAAAAACAGAACCTGCTGTCGGATCCTGGGAACCCGCCTGCAAACGATTTTAACCCAGACGGAGAGGTCTCGGAGGGGAATCTCCTGATGCCGATGGCCTTTCCGGAAGGTTCGCCGATGAATCCAGCCTATGGTGCCGGCAATGCAACCGTGGCAGGGGCATGCGTGACAGTGTTAAAAGCATTCTTTGACGGCGGATATCGCCTGCCGTTTTGTTACATCACTGATGAAGACGGTACGGGTCTACAGGCAGTAGAAATAGACGAACCACTGACGGTCGACGGTGAATTGAACAAAATTTGCTCTAATATCTCAATTGGCCGAAACTTGGCCGGTGTTAACTACTTCACGGATTACATTGAATCCATACGGATAGGCGAAGAAATCGCCATCGGTATCTTGCAGGAGCAGAAGCTGACCTTTTCTGAAAACTTCTCTATGACCCTGAACAAATTTGACGGCTCAACTATCCGCATC</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>ATGACCGATACCCAG</t>
+          <t>ATGACGGACACCCA</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>AATGCGGATGGTGG</t>
+          <t>GATGCGGATAGTTGAGC</t>
         </is>
       </c>
     </row>
@@ -766,22 +766,22 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>TACTGCGGGGGCTGGGCTGGAGTTTGACGCGAGCACTTTGGATAACGGCGACGTCTGGACCGACGGTTGGGATTGTTGGGCTTGTTACATGCGTTGCGGCTACTCTGTTGGATGTTTGACGGCTTATTGCACACGAGGATATAGAGTCGGAAATGCTTCCCGGACGGGTTATTAGACCTACCCGGAGACCATAGTGGTTTGTTAAAAGTCGAAAAGTAATTACGTCATGCGTGCCCATTACACTTTCTATAACGACGATATGGCGACCCGGGTGGTTTGAGCAGAAGCAAAGGAAGCCCGTAACGCTTTCTGCGGCGTCACGGACCTAACCTCAGGTACCGTCGCCCATTGTGGAAGCTAGAAGTCCCGGGTCTACGGGTCCGCCAATGGTACGGGGGCACGGGTGCGGACTTAAGATTACTTGAACAGTGGCTTTACTGACTTGACATGATATACCGGGACGACGCGCTGCACGGGAAATGGTTGAAGTTATTCTTGTTGGACCAAGTCAGCCGACAGATACTGTACTTGTTGTGGTTGAACTGGTTTAGGTTGGCGACAACGGACGGCGGAGGCCTTGCGGCGGGATTGGGAAGGTTTAAATGGTGACTGTTGTAGAAAGGACCACAGTGGGGCCCGCTATAGTGCCCAGGTATGTAGAGGGTCAAGAATGACCACCCGTGTTTTCCAAACCGCCTACACTTGCTTCTTTGCCTTCCAATGCAAGTCATGCCGCGGTGGGCGTAACTAGTCGGACATGGATGGCATGTCGGTTTTTAGCTAATATACTGCTGGAACCGCCGGATGGACCTACAAGTCTTACCACGTCTAGACGCGGCTTTGAGTCGTATACGCCTTGGAGGTTTAATAGCGAAATAGACATGGGGCGCGCTGGACCGCTGGATACAATTGATGCTGCGAAACATGGTTCGTATGGACTTACGCACATAGTAGGAAGAGCTGTAATTACGGGGCATACTAAGACCAGACGGCAAGTGGCGGCTACTACGGCACCTGTTCGTCGTCCCTAAGCGGTGCAAGCCGCGAGGATTGCACGACTGAGACCACTGCCTTCAACGCTGTGGACGAGAGTTTCGTCAAGCGAAGGTTTTTATGCGGCAGTTGGGAGGAGACGGAGGCCTTCGCCAGCCGCCAAATGACCTCGTCATGGCGGCGATGCCTCCGCCATTGAGACTAGATCGTATGTATTAAGGAGGTTAAGCGTTGGACCGGCTAAGTAATAGGAGACTGGACTACAGATACCACCGGTTTCTTTTGCCAGCGGTTTTGAGCAACTAAGCTCTGTTACCATTAGGTGGAAGTTTACTACTTCCAAGACTACTATGGTTAGAAAACAGATACCGGATGCGCCTTCCTAGAGGCTACTTGGGCAGAATGCCACGACCGTTGCGGTGGCAACGACCGCGTACGCACTGTTAGGACTTTCGTAAGAAACTGTTGTGCAAGTTTGACGGAAAACGCATGCATAGAAGTAGGCTACCTGGATTTGAGTTCTGTCACTTTGACAGCTTTTTCGACTGGCACCTCCTGCTTGACTTGTTCGAACGTCGGTTGTAAAGTTAGCCAGCCAGTAACCGGCCACATTTAATGATAAGGCTAATGCACCTTAGCTAAGCGGACCCCCTTCTCCACCGTTAGCCATACAATTTTCTCGTCTTTGACTGGATAAGTCTCTTTAAGTGGTACTGGTAGGGGTTTAAACTACCGAGACAATAACTCTAG</t>
+          <t>TACTGGGGCGGATGTGGAGCGGTCTGTCGTGAGCATTTCGCGTAGCGGCGGCGCCTAAATCGACGTTTAGCGTTATTGGGTTTATTACAAGCGTTGCGCCTACTTTGGTGCATATTCGACGGCTTGTTGCAAACGAGTATATAAAGGCGTAAATGGTTTCCCGACGGCTTGTTAGACCTGCCGGGAGAGCAAAGAGGATTGTTGAAGGTCAATAAATAGTTGCGCCACGGATGGCCTTTGCAATTTCTATAACGTCGGTAAGGGAACCCAGGCGGCTTGAGGAGGAGCAAAGCGAGGCCGTAGCGGTTTCTACGGCGCCAAGGACCGAACCTTAGCTACCGACGCCCATTATGGAAGCTAAATGTCCCCGGCCTGCGCGTCCGCCACTGGTACGGCGGCACGGGCGGAGAGTTGAGATTACTTAACCAGTGGCTTTACTGCCTTAATATAATATACCGCAACAATGGACTGCAGGGTAAATGCTTGAAATTATTTTTGTTAGACCAAGTCAGTCGGCAAATACTATACTTGTTGTGGTTGAACTGATTTAGGTTAGGAACGACAGACGGCGCGGGTCTTGGAGCGGCTTTGGCGAGATTCAAATGCTGGCTGTTATAAAAGGCTCCACACTGGGGCCCTCTGTAATGTCCAGGCATGTAGAGAGTTAAAGACGACCATCCATGATTTCCAGACCGCCTGCAATTGCTCCTTTGGCTCCCGATACAGGTTATGCCACGATGGGGATAACTAGTCGGACAAGGATGTCACGTTGGATTTTAACTAATGTACTGATGCAACCGGCGCATAGACCTACACGTCTTACCGCGACTAAACGCGGCGTTAAGACGTATGCGACTCGGCGGCTTAATAGCGAAGTAGACGTGGGGTGCGCTAGAGCGCTGCATACACTTAATACTGCGTGACATGGTCCGTATAGACTTGCGCACGTAGTAGGACGAGCTATATTTACGCGGCATGCTGAGACCGGACGGAAAATGTCGACTACTACGGCATCTGTTTGTCGTTCCAAAGCGCTGGAAACCTCGGGGCTTACACAACTGGGACCACTGCCTCCACCGTTGCGCGCGCGAGTTCCGCCAAGGAAAAGTTTTTATACGCCACTTAGGAGGAGACGGAGGCCTTCGCCAACCCCCAGACAATCTTGTCATGGCGGGAATACCACCACCATTAAGGCTGGACCGAATGTAATAAGGAGGTTAAGCGTTAAATCGTCTAAGGGAAAGTAGCCTGGACTACAGGTACCAACGCTTTCTCTTACCCGGAGTCTTAAGTGATTATGCGCTATTACCGTTAGGCGGAAGATTGCTGCTTCCGAGACTACTATGTTTAGACGAAAGGTACCGAATGCGCCTCCCGAGAGGCTACTTGGGCAGGATACCGCGCCCATTACGGTGCCAACGCCCACGAACGCAGTGATAGGACTTTCGGAAGAAGCTATTGTGCAAGTTTGAAGGAAAACGCATGCAAAGAAGAAGACTACCTGGATTTGACTTTTGGCAATTCAACAGATTTTTTGACTGACACCTTCTACTTGACTTGTTTGATCGTCGCTTGTAAAGTTAGCCCGCTAGGAACCGGCCGCACTTGATGATAAGACTGATACACCTTAGATAAGCGGAGCCACTCCTTCAACGTTAGCCGTACGACTTCCTTGTTTTTGACTGAATAAGCCTTTTCAAGTGATACTGATAAGGTTTTAAACTACCGAGTCAATAGCTTTAG</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>ATGACGCCCCCGACCCGACCTCAAACTGCGCTCGTGAAACCTATTGCCGCTGCAGACCTGGCTGCCAACCCTAACAACCCGAACAATGTACGCAACGCCGATGAGACAACCTACAAACTGCCGAATAACGTGTGCTCCTATATCTCAGCCTTTACGAAGGGCCTGCCCAATAATCTGGATGGGCCTCTGGTATCACCAAACAATTTTCAGCTTTTCATTAATGCAGTACGCACGGGTAATGTGAAAGATATTGCTGCTATACCGCTGGGCCCACCAAACTCGTCTTCGTTTCCTTCGGGCATTGCGAAAGACGCCGCAGTGCCTGGATTGGAGTCCATGGCAGCGGGTAACACCTTCGATCTTCAGGGCCCAGATGCCCAGGCGGTTACCATGCCCCCGTGCCCACGCCTGAATTCTAATGAACTTGTCACCGAAATGACTGAACTGTACTATATGGCCCTGCTGCGCGACGTGCCCTTTACCAACTTCAATAAGAACAACCTGGTTCAGTCGGCTGTCTATGACATGAACAACACCAACTTGACCAAATCCAACCGCTGTTGCCTGCCGCCTCCGGAACGCCGCCCTAACCCTTCCAAATTTACCACTGACAACATCTTTCCTGGTGTCACCCCGGGCGATATCACGGGTCCATACATCTCCCAGTTCTTACTGGTGGGCACAAAAGGTTTGGCGGATGTGAACGAAGAAACGGAAGGTTACGTTCAGTACGGCGCCACCCGCATTGATCAGCCTGTACCTACCGTACAGCCAAAAATCGATTATATGACGACCTTGGCGGCCTACCTGGATGTTCAGAATGGTGCAGATCTGCGCCGAAACTCAGCATATGCGGAACCTCCAAATTATCGCTTTATCTGTACCCCGCGCGACCTGGCGACCTATGTTAACTACGACGCTTTGTACCAAGCATACCTGAATGCGTGTATCATCCTTCTCGACATTAATGCCCCGTATGATTCTGGTCTGCCGTTCACCGCCGATGATGCCGTGGACAAGCAGCAGGGATTCGCCACGTTCGGCGCTCCTAACGTGCTGACTCTGGTGACGGAAGTTGCGACACCTGCTCTCAAAGCAGTTCGCTTCCAAAAATACGCCGTCAACCCTCCTCTGCCTCCGGAAGCGGTCGGCGGTTTACTGGAGCAGTACCGCCGCTACGGAGGCGGTAACTCTGATCTAGCATACATAATTCCTCCAATTCGCAACCTGGCCGATTCATTATCCTCTGACCTGATGTCTATGGTGGCCAAAGAAAACGGTCGCCAAAACTCGTTGATTCGAGACAATGGTAATCCACCTTCAAATGATGAAGGTTCTGATGATACCAATCTTTTGTCTATGGCCTACGCGGAAGGATCTCCGATGAACCCGTCTTACGGTGCTGGCAACGCCACCGTTGCTGGCGCATGCGTGACAATCCTGAAAGCATTCTTTGACAACACGTTCAAACTGCCTTTTGCGTACGTATCTTCATCCGATGGACCTAAACTCAAGACAGTGAAACTGTCGAAAAAGCTGACCGTGGAGGACGAACTGAACAAGCTTGCAGCCAACATTTCAATCGGTCGGTCATTGGCCGGTGTAAATTACTATTCCGATTACGTGGAATCGATTCGCCTGGGGGAAGAGGTGGCAATCGGTATGTTAAAAGAGCAGAAACTGACCTATTCAGAGAAATTCACCATGACCATCCCCAAATTTGATGGCTCTGTTATTGAGATC</t>
+          <t>ATGACCCCGCCTACACCTCGCCAGACAGCACTCGTAAAGCGCATCGCCGCCGCGGATTTAGCTGCAAATCGCAATAACCCAAATAATGTTCGCAACGCGGATGAAACCACGTATAAGCTGCCGAACAACGTTTGCTCATATATTTCCGCATTTACCAAAGGGCTGCCGAACAATCTGGACGGCCCTCTCGTTTCTCCTAACAACTTCCAGTTATTTATCAACGCGGTGCCTACCGGAAACGTTAAAGATATTGCAGCCATTCCCTTGGGTCCGCCGAACTCCTCCTCGTTTCGCTCCGGCATCGCCAAAGATGCCGCGGTTCCTGGCTTGGAATCGATGGCTGCGGGTAATACCTTCGATTTACAGGGGCCGGACGCGCAGGCGGTGACCATGCCGCCGTGCCCGCCTCTCAACTCTAATGAATTGGTCACCGAAATGACGGAATTATATTATATGGCGTTGTTACCTGACGTCCCATTTACGAACTTTAATAAAAACAATCTGGTTCAGTCAGCCGTTTATGATATGAACAACACCAACTTGACTAAATCCAATCCTTGCTGTCTGCCGCGCCCAGAACCTCGCCGAAACCGCTCTAAGTTTACGACCGACAATATTTTCCGAGGTGTGACCCCGGGAGACATTACAGGTCCGTACATCTCTCAATTTCTGCTGGTAGGTACTAAAGGTCTGGCGGACGTTAACGAGGAAACCGAGGGCTATGTCCAATACGGTGCTACCCCTATTGATCAGCCTGTTCCTACAGTGCAACCTAAAATTGATTACATGACTACGTTGGCCGCGTATCTGGATGTGCAGAATGGCGCTGATTTGCGCCGCAATTCTGCATACGCTGAGCCGCCGAATTATCGCTTCATCTGCACCCCACGCGATCTCGCGACGTATGTGAATTATGACGCACTGTACCAGGCATATCTGAACGCGTGCATCATCCTGCTCGATATAAATGCGCCGTACGACTCTGGCCTGCCTTTTACAGCTGATGATGCCGTAGACAAACAGCAAGGTTTCGCGACCTTTGGAGCCCCGAATGTGTTGACCCTGGTGACGGAGGTGGCAACGCGCGCGCTCAAGGCGGTTCCTTTTCAAAAATATGCGGTGAATCCTCCTCTGCCTCCGGAAGCGGTTGGGGGTCTGTTAGAACAGTACCGCCCTTATGGTGGTGGTAATTCCGACCTGGCTTACATTATTCCTCCAATTCGCAATTTAGCAGATTCCCTTTCATCGGACCTGATGTCCATGGTTGCGAAAGAGAATGGGCCTCAGAATTCACTAATACGCGATAATGGCAATCCGCCTTCTAACGACGAAGGCTCTGATGATACAAATCTGCTTTCCATGGCTTACGCGGAGGGCTCTCCGATGAACCCGTCCTATGGCGCGGGTAATGCCACGGTTGCGGGTGCTTGCGTCACTATCCTGAAAGCCTTCTTCGATAACACGTTCAAACTTCCTTTTGCGTACGTTTCTTCTTCTGATGGACCTAAACTGAAAACCGTTAAGTTGTCTAAAAAACTGACTGTGGAAGATGAACTGAACAAACTAGCAGCGAACATTTCAATCGGGCGATCCTTGGCCGGCGTGAACTACTATTCTGACTATGTGGAATCTATTCGCCTCGGTGAGGAAGTTGCAATCGGCATGCTGAAGGAACAAAAACTGACTTATTCGGAAAAGTTCACTATGACTATTCCAAAATTTGATGGCTCAGTTATCGAAATC</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>ATGACGCCCCCGA</t>
+          <t>ATGACCCCGCCTA</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>GATCTCAATAACAGAGCCATCAAATTT</t>
+          <t>GATTTCGATAACTGAGCCAT</t>
         </is>
       </c>
     </row>
@@ -808,22 +808,22 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>TACCGGCTTCTTGCGGCGGTCTTGCGTGACCTGTAAGGATAGGTCCGACGGGCGGACCGCTTTTTTGCGCTGTTGGGTTGATTGCTTCGTTTGCCGCTGCTCCTGGGAATAGGTCTTTGCGAGTAGCCAAGTAAGTGGTTTCCAAACGGCTTACTCTTTCTCTGACCGAATGACAGTTTGGGGCGGCTAAAACGGCTAAAGCATGCGCGATAGTTGTGTCCACGCTAATTTCTGTATGCGGGAGACTTCGACCCGTAACTACTCCTAGGCGGAAAATAAAGGCCGTAGCGGAGTTTCCCTCTATTCTTGGGTAAGCGACTATGGGGACGAAACCTTAGATACCGACGCCCAGACTGGATACTGGAGCTTCCAGGCCTGCGCGTCCGTCAATGCTACGGCGGACGCGGCTTTGAACTAAGACTACTTGACCACTGACTTTAGTGCCTTAGTATAAACTACCGAGACTAAGGACTGCAGGGTAAATGGCTTAAACTTGCGCTGCCATTATGGCGACGACGCCGGCGCAGTTAGAGCGGATGGGCGAACCACGTCAAGTTGCTCGTCGGCAGAGTCGGAGGCAGATGCAATTGGCTGCTTCTTTAACGTGCGGACGGACCCGGCATATGATTCTTTTTGCAGAAGGCGCCACAATGGTAACCCCTTTTGCAGCCAGGCATAAACAGGGTCAAGGACGAACACCCGTGGTTTCCGTAGCCGCTACATGTCGTTTAGAGTCTGCCCATGTAAGTTATGCCGAGGTACGCGTACCTGGTCGGACATGCGCACCGTCGCGGTTTTGCGCTGATATACTGGTGGAACCGCAGAAACGACCTGCATGTTTTGCGACCGCTGAATGCTCCGGCCCTTTAGATACTGCTACTATGCGGCAAGGGAAAGTAATGGTGGGGCGCTCTAGATCGGTGCAACCATTTAAAGCTGCGCGACATGGTCCGGATGGACTTACGTACGTAGTAGGACGACCTATAGTTTCGGGGAAAGCTAGGCTTATAAGGTAAGGTCCGGCTACTACTACAACTGTTTGTCGTCCCAAAGCGCTGGAAACCTCCAGGCTTGTAGGACAGAGACACATGTCTTCAACGATGAGGACGTGACTTTCGGCACGGAAAGGTCTTCATGTTGCACTTAGCGGCGGACGCGGGACTCCGGTAGCCACCAGACCATCTTGGAAAATTTTTCTGCTTGCCGCTGCGATTCAAACGAGGACAATTTTTTGAACAATTGCTAGACCTACCGCTATACGACGCGGCGTAGCTCGTCTTATTAACACTTGTCTTGTTCGAGAGACTACTACCGTTACGTGCGGCGCTGCTGATGAGCGGGCTTCCGCTCAGGTTGGTTTGTATAGAAGACGGCTACCGCAAGGGCCTTCCAAGTGGGTACTTGGGTAGAATACCGCGTCCATTGCGCTGGCAACGCCCGCGCACGCATTGGCAAGACTTCCGCAAGAAACTATTACTTATACTCAACCTGAAAACGATACACGGCTGGTGGCTGCCATTTGGAGACCTTTTTCACTTATAGTTACTTTTCGACTGGCACCTTCCCCTTAATTTGTTTGACACGCGCTTATAGACGTAGCCGGGATTGAACCGACCACAATTGATAATGAGCCTAATAAAGCTTAGATATTTCCACCCACTCCTTTAACGCTAGCCATAAGACGTCCTCGTCTTTGACTGCATGCCGCTTCTGAAAAAGTACTGAGACAGCTTTAAACTGCCGCTTTTTTAGGCGTAA</t>
+          <t>TACCGTCTTCTTGCGGCGGTCTTACGTGACCTATAGGCGTAAGTTCGGCGGGGAGACCGCTTTTTTGGACTGTTGGGTTGCTTGCTTCGCTTGCCACTACTTCTAGCGATGGGCCTTTGGAATTAGCCAAGGAAATGGTTTCCCGACGGGTTGCTTTTTCTTTGGCCCGACGACAGGTTGGGACGGCTAAAGCGTCTAAAGCACGCGCGGTAATTGTGTCCGCGCTAATTTCTATAAGGAGCGAATTTTGACCCATAACTGCTCCTGGGAGCGAAGTAAAGACCATAGCGCAGGTTTCCACTATTTTTAGGCAAGCGCCTATGGGCGCGTAACCTCAGCTACCGTCGGCCGGACTGTATGCTAGACCTTCCAGGCCTGCGCGTCCGGCAATGGTACGGAGGCCGTGGTTTTGACCTAAGGCTACTCAACCAGTGGCTTTAGTGTCTTAGGATAAACTACCGAGACTAGGCGCTACAGGGCAAATGGCTTAAACTTGGACTACCCTTGTGGCGCCGACGGCGTCGCAGGTAAAGGGCGTGGGCGAACCACGTCAAATTGCTCGTTGGGAGTGTTGCCGGGAGCTGAGACTGGCTACTCCTTTAGCGGGGAAATGCGCCAGGCATATGATTTTTTTTGCAAAAGGCGCCACACTGTTAACCCCTCTTACATCCCGGTATAGAGAGAGTTAAGGAAGACCATCCATGATTTCCCTAACCGCTGCAAGTCGTCTATAGCCTACCGATGTAGGTCATGCCTAGTTACGCGTACCTAGTCGGACAAGGACATCGACGCGGGTTTGCGCTGATATACTGATGGAACCGGAGCAACGAGCTGCAGGTCTTACGTCCCCTGGACGCTCCAGCGCTTTAGATACTACTACTGTGCGGTAAGGCGAAATAATGCTGGGGCGGACTGGACCGGTGCAACCACTTGAAGCTACGTGACATGGTCCGCATGGAGTTGCGGACGTAGTAAGACGACCTGTAGTTTCGCGGCAAGCTAGGGTTGTAAGGCAAAGTCCGCCTGCTGCTACAACTATTTGTTGTTCCCAAGCGTTGCAAACCCCCGGGGTTGTATGACAGGAATACGTGGCTTCATCGCTGGGCGCGAGACTTCCGTCACGCGAAGGTTTTCATGTTGCACTTGGCGGGAGAGGGAGGCCTTCGCTAACCGCCAGAACAACTTGGAAAATTTTTTTGCTTGCCGCTACGATTTAAGCGAGGCCATTTTTTTGAGCACTTACTAGAACTACCACTATACGAAGCGGCCTAGCTTGTTTTATTGACGCTTGTCTTGTTTGAGAGCCTACTGCCGTTACGTGCCGCGCTACTGATAAGCGGTCTCCCGCTCAGCTTGGTCTGGATAAATGAAGGTTACCGAAAGGGGCTTCCAAGAGGCTACTTGGGCAGAATGCCGCGCCCGTTGCGATGGCAGCGCCCGCGGACACAGTGACAAGAATTTCGCAAAAAGCTGTTACTCATGCTTAATCTAAAGACGATGCAAGGATGGTGGCTGCCGTTTGGAGAACTTTTTCAATTATAATTGCTTTTTGACTGGCAGCTTCCGCTTGACTTATTCAACACACGTTTGTAAACATAGCCAGCGTTAAACCGCCCCCAATTAATAATAAGACTGATAAAGCTTAGATATTTTCACCCGCTTCTTTAACGGTAACCTTAAGAAGTCCTTGTCTTCGACTGGATACCACTTCTAAAGAAGTACTGCGACAGGTTCAAGCTGCCTCTCTTTTAGGCCTAA</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>ATGGCCGAAGAACGCCGCCAGAACGCACTGGACATTCCTATCCAGGCTGCCCGCCTGGCGAAAAAACGCGACAACCCAACTAACGAAGCAAACGGCGACGAGGACCCTTATCCAGAAACGCTCATCGGTTCATTCACCAAAGGTTTGCCGAATGAGAAAGAGACTGGCTTACTGTCAAACCCCGCCGATTTTGCCGATTTCGTACGCGCTATCAACACAGGTGCGATTAAAGACATACGCCCTCTGAAGCTGGGCATTGATGAGGATCCGCCTTTTATTTCCGGCATCGCCTCAAAGGGAGATAAGAACCCATTCGCTGATACCCCTGCTTTGGAATCTATGGCTGCGGGTCTGACCTATGACCTCGAAGGTCCGGACGCGCAGGCAGTTACGATGCCGCCTGCGCCGAAACTTGATTCTGATGAACTGGTGACTGAAATCACGGAATCATATTTGATGGCTCTGATTCCTGACGTCCCATTTACCGAATTTGAACGCGACGGTAATACCGCTGCTGCGGCCGCGTCAATCTCGCCTACCCGCTTGGTGCAGTTCAACGAGCAGCCGTCTCAGCCTCCGTCTACGTTAACCGACGAAGAAATTGCACGCCTGCCTGGGCCGTATACTAAGAAAAACGTCTTCCGCGGTGTTACCATTGGGGAAAACGTCGGTCCGTATTTGTCCCAGTTCCTGCTTGTGGGCACCAAAGGCATCGGCGATGTACAGCAAATCTCAGACGGGTACATTCAATACGGCTCCATGCGCATGGACCAGCCTGTACGCGTGGCAGCGCCAAAACGCGACTATATGACCACCTTGGCGTCTTTGCTGGACGTACAAAACGCTGGCGACTTACGAGGCCGGGAAATCTATGACGATGATACGCCGTTCCCTTTCATTACCACCCCGCGAGATCTAGCCACGTTGGTAAATTTCGACGCGCTGTACCAGGCCTACCTGAATGCATGCATCATCCTGCTGGATATCAAAGCCCCTTTCGATCCGAATATTCCATTCCAGGCCGATGATGATGTTGACAAACAGCAGGGTTTCGCGACCTTTGGAGGTCCGAACATCCTGTCTCTGTGTACAGAAGTTGCTACTCCTGCACTGAAAGCCGTGCCTTTCCAGAAGTACAACGTGAATCGCCGCCTGCGCCCTGAGGCCATCGGTGGTCTGGTAGAACCTTTTAAAAAGACGAACGGCGACGCTAAGTTTGCTCCTGTTAAAAAACTTGTTAACGATCTGGATGGCGATATGCTGCGCCGCATCGAGCAGAATAATTGTGAACAGAACAAGCTCTCTGATGATGGCAATGCACGCCGCGACGACTACTCGCCCGAAGGCGAGTCCAACCAAACATATCTTCTGCCGATGGCGTTCCCGGAAGGTTCACCCATGAACCCATCTTATGGCGCAGGTAACGCGACCGTTGCGGGCGCGTGCGTAACCGTTCTGAAGGCGTTCTTTGATAATGAATATGAGTTGGACTTTTGCTATGTGCCGACCACCGACGGTAAACCTCTGGAAAAAGTGAATATCAATGAAAAGCTGACCGTGGAAGGGGAATTAAACAAACTGTGCGCGAATATCTGCATCGGCCCTAACTTGGCTGGTGTTAACTATTACTCGGATTATTTCGAATCTATAAAGGTGGGTGAGGAAATTGCGATCGGTATTCTGCAGGAGCAGAAACTGACGTACGGCGAAGACTTTTTCATGACTCTGTCGAAATTTGACGGCGAAAAAATCCGCATT</t>
+          <t>ATGGCAGAAGAACGCCGCCAGAATGCACTGGATATCCGCATTCAAGCCGCCCCTCTGGCGAAAAAACCTGACAACCCAACGAACGAAGCGAACGGTGATGAAGATCGCTACCCGGAAACCTTAATCGGTTCCTTTACCAAAGGGCTGCCCAACGAAAAAGAAACCGGGCTGCTGTCCAACCCTGCCGATTTCGCAGATTTCGTGCGCGCCATTAACACAGGCGCGATTAAAGATATTCCTCGCTTAAAACTGGGTATTGACGAGGACCCTCGCTTCATTTCTGGTATCGCGTCCAAAGGTGATAAAAATCCGTTCGCGGATACCCGCGCATTGGAGTCGATGGCAGCCGGCCTGACATACGATCTGGAAGGTCCGGACGCGCAGGCCGTTACCATGCCTCCGGCACCAAAACTGGATTCCGATGAGTTGGTCACCGAAATCACAGAATCCTATTTGATGGCTCTGATCCGCGATGTCCCGTTTACCGAATTTGAACCTGATGGGAACACCGCGGCTGCCGCAGCGTCCATTTCCCGCACCCGCTTGGTGCAGTTTAACGAGCAACCCTCACAACGGCCCTCGACTCTGACCGATGAGGAAATCGCCCCTTTACGCGGTCCGTATACTAAAAAAAACGTTTTCCGCGGTGTGACAATTGGGGAGAATGTAGGGCCATATCTCTCTCAATTCCTTCTGGTAGGTACTAAAGGGATTGGCGACGTTCAGCAGATATCGGATGGCTACATCCAGTACGGATCAATGCGCATGGATCAGCCTGTTCCTGTAGCTGCGCCCAAACGCGACTATATGACTACCTTGGCCTCGTTGCTCGACGTCCAGAATGCAGGGGACCTGCGAGGTCGCGAAATCTATGATGATGACACGCCATTCCGCTTTATTACGACCCCGCCTGACCTGGCCACGTTGGTGAACTTCGATGCACTGTACCAGGCGTACCTCAACGCCTGCATCATTCTGCTGGACATCAAAGCGCCGTTCGATCCCAACATTCCGTTTCAGGCGGACGACGATGTTGATAAACAACAAGGGTTCGCAACGTTTGGGGGCCCCAACATACTGTCCTTATGCACCGAAGTAGCGACCCGCGCTCTGAAGGCAGTGCGCTTCCAAAAGTACAACGTGAACCGCCCTCTCCCTCCGGAAGCGATTGGCGGTCTTGTTGAACCTTTTAAAAAAACGAACGGCGATGCTAAATTCGCTCCGGTAAAAAAACTCGTGAATGATCTTGATGGTGATATGCTTCGCCGGATCGAACAAAATAACTGCGAACAGAACAAACTCTCGGATGACGGCAATGCACGGCGCGATGACTATTCGCCAGAGGGCGAGTCGAACCAGACCTATTTACTTCCAATGGCTTTCCCCGAAGGTTCTCCGATGAACCCGTCTTACGGCGCGGGCAACGCTACCGTCGCGGGCGCCTGTGTCACTGTTCTTAAAGCGTTTTTCGACAATGAGTACGAATTAGATTTCTGCTACGTTCCTACCACCGACGGCAAACCTCTTGAAAAAGTTAATATTAACGAAAAACTGACCGTCGAAGGCGAACTGAATAAGTTGTGTGCAAACATTTGTATCGGTCGCAATTTGGCGGGGGTTAATTATTATTCTGACTATTTCGAATCTATAAAAGTGGGCGAAGAAATTGCCATTGGAATTCTTCAGGAACAGAAGCTGACCTATGGTGAAGATTTCTTCATGACGCTGTCCAAGTTCGACGGAGAGAAAATCCGGATT</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>ATGGCCGAAGAACG</t>
+          <t>ATGGCAGAAGAACGC</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>AATGCGGATTTTTTCGC</t>
+          <t>AATCCGGATTTTCTCTCC</t>
         </is>
       </c>
     </row>
@@ -850,22 +850,22 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>TACAGTCGACGCGCGGCGGTTCTTCGGAAGGTCTGGGGACAGGCGCGGCGTGCTGAACGAGCGCTAGCCCTATTGGTCCAGAAGCTCGGCTTACCACTTCTTCTAGCGATAAAGGGAGGCTTGAGTGTTTAGAAGAGCATAGAACCGAGGATGTGCTTTCCGAACGGATTATTGGCGGCGTGCCGAAATTAATGGAGCGGTTTGTTGAAACAAGCTAAGCAGGCGCGTTAACTGAGTCCGCTCGGTCGCCTAAAGTAGTTCCAAGGTGACCCAGGAGCGGGGCGCGAAGTCAAACTTAGCCTCCTTCTTACAGCGCGGCGTTTGGACAAATTTAGTCCATAGCGCCCGGCTTTATTGTGCAAGGGCAGGAGGACGAACGCGCGAAACCTCAGATACCCACGACCGGACCACAAGCTAGACCTCCCGGGACTGCGCGTCCGGCACCCGTACGGCGGTCGCGGGTGCAACCTAAGGCTGCTCGACCAGCGCCTCTAAAGGCTCCATATAAACTACCGCAATGACGGACTGCAAGGAAAGTGGCTAAAATGATTAGGCCCGGGCTAGCCCGGACGCTATTTGTGTGAATTATTTTGGCGCAACTAGGCGCGCCGCGGACTGGGCGGTCTAAGGGACTGGGGCGTTCTCGGACGCGGAGACGGACCAGGCAAATTGGGCAGATTATAAAAGGCTCCGTGCAACGGTCCGCTACTACACCCAGGCATAGAGAGCGTCAAGGAGGAACATCCGTGGTTTCCGTAACCACCGCGGGTTCTGTACCGCCTACCGAAGTAAAGGATGCCGCGCTTAGGATAACTAGTCGGACAAGCGTTACGAGGATTCCTTGACCTGATATACTGGAGGAACCTTCGTAAGAATCTACAAGTCTTGCCCCGGCTACAATGGCCCGCGCTGTGAAAGCTTAGACCGAGCCTACGGAAAGGAAAGTAGTGGTGGGGCGCGCTAGAACGTTGGATACAGTTGAAACTACGAGAGATAGTCCGCATAGAGTTGCGGACAGAGTAATACGAACTGAGGCCACAAGGAAAGCTATTTCCCTAAGGCAAGCCTCTTGGACTGAAATTTCTATTAGTCGGACCAAAACGTTTGAAGCCACCGGGCTTATAGGAAAGAGAACACTGCCTTCATCGCTGGGCGCGTGACTTTCGCCATGGAAAGGTCTTTAAATTGTGGTTGGCGGCGGACGGAGGCCTTCGTCAGCCGCCAGACTAACTTGGAAAATTGAGATTGGGACTACTAGGCGTCAAGGTCCTGCAGTTTGGCGACAAGCTCCGAGACCTACTTCTGTACTACGCGGGACAACGTGGATTGTTAGCGCTTGTTTTGGTCCCAAGACTGAAGCCATACGGCGCGCGTCTACTGAAGTTAGGCCGCCCCCTGTGGGACCTTTGATACGACAACGGATACCGCAAGGGGCTCCCAAGGGGGTACTTGGGGAGCATGCCTCGGCCTTTGCGCTGACATCGACCGCGTACACACTGCCACGAGTTTCGGAAGAAGGTTTTACTATGGCTCGACCTAAAAACGAAACACGGCAGGCTACTACCAAGTGCGGACCACCTGCGGAGGTTGTTGTACTTGTTCTTCGACTGGCAGCTCCCCCTCAACTTGTTTCAGACGAGATTGTAAAGATAACCAGCCTTAAACCGTCCGCACTTAATGAAATGCCTGATATAGCTTAGGTAGAACGACCCGCTCGTCTAGCGAGAGCCATAAGACCTCCTTGTTTACGAGTGGAAAGGCCTTTGGAAGTGCTACTGGCACGGTAACAAGAGGCCCCTCAATTTTCATGACGGAAGATGG</t>
+          <t>TACAGCCGGCGCGCGGCCGTTCTTCGCAAAGTTTGAGCGCATGGACGCCGGGCTAATCGGGGACTGGCGCTGTTGGTTCACAAGCTTGGGTTACCGCTTCTTCTAGGAATAAAAGGAGGTTTGAGCGTCTAAAAGAGTATAGAGCCAAGGATATGATTTCCTGACGGCTTGTTAGCGGCGTGACGGAACTAATGGAGGGGTTTGTTGAAACAAGCGAAACAGGGACGATAGCTGAGGCCCCTTGGCCGTCTAAAATAGTTTCACGGGAATCCGGGCGGAGGCCGAGACGTCAAACTTAGACTCCTTCTTACGGCGCGTCGCTTGGAGAAGTTTAGGCCATAGCGACCGGCGTTGTTGTGGAAAGGCAGTAGTACGGACGCCCGAAACCTTAGATACCCACGCCCTGACCATAAACTGGAGCTTCCGGGACTGCGAGTCCGTCACCCATACGGCGGTCGGGGCTGGGACCTAAGACTGCTTGAGCACCGACTTTATAGACTTCATATGAACTACCGCGACGACGCGCTACAGGCGAAATGCCTAAAATGATTGGGCCCCGGTTAACCAGGACGTTAATTGTGCGACTTGTTTTGGCGCAACTATGCTCGACGCGGACTAGGAGGCCTGAGAGACTGGGGCGTCCTTGCCCGCGCGGACGCGCCGGGTAAGTTGGGAAGGTTGTAAAAGGCGCCATGGGACGGTCCACTACTGCATCCTGGCATGGACAGTGTCAAGGAAAACCAACCGTGGTTTCCTTAACCACCACGCGTTCTGTACCGCCTGCCAAAATAAAGAATGCCACGCTTGGCCTAGCTAGTTGGACAAGCGTTACGCGGATTTCTCAACCTAATGTACTGGAGGAACCTTCGCAAGGACCTGCACGTCTTGCCACGCCTACACTGCCCGGGACTATGGAAACTCAGCCCGAGACTGCGGAAGGCCAAATAATGTTGTGGTGCCCTAAATCGATGAATACACTTGAAACTGCGTGACATGGTTCGCATAGATTTGCGTACAGACTAATACGACCTAAGACCACATGGAAAGCTATTCCCATAAGGGAAACCGCTCGGCCTGAAATTTCTATTGGTCGCGCCAAAGCGATTGAAGCCGCCAGGCTTGTAAGAAAGTGACCACTGGCTTCAACGTTGGGCCCGCGACTTCCGACAAGGAAAGGTCTTCAAATTATGATTAGGAGCGGAAGGAGGACTTCGACACCCGCCAGATTAACTTGGAAAATTGAGTTTAGGCCTGCTGGGAGTCAAAGTCCTGCACTTTGGCAACAAACTTCGAGACCTACTCCTGTACTACGCCGCGCAACGCGCTTTGTTGGGACTTGTTTTAGTTCCGAGACTAAAACCTTACGGAGCTCGCCTGCTGAAGTTGGGCCGCCCGCTGTGCAATCTTTGTTACGACGACGGTTACCGTAAAGGTCTTCCAAGTGGCTACTTAGGTAGAATACCACGACCGTTACGGTGCCAGCGTCCGCGCACACAATGCCAGGACTTTCGGAAGAAAGTCTTACTATGACTCGACCTAAAAACGAAGCAGGGTAGGCTGCTACCAAGAGGAGACCAACTGCGCAGTTTATTGTACTTGTTCTTTGACTGACACCTTCCGCTTAACTTGTTTCATACGAGCTTGTAAAGCTAGCCAGGATTGAACCGACCGCATTTAATGAAGTGCCTGATGTAGCTTAGTTATGACAACCCCCTTGTCTAGCGAAACCCATAAGACCTTCTCGTCTACGACTGGAAGGGCCTTTGGAAATGGTACTGGCACGGGGAGAAAAGGCCACTTGACTTTCACGAAGCGAGGTGC</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>ATGTCAGCTGCGCGCCGCCAAGAAGCCTTCCAGACCCCTGTCCGCGCCGCACGACTTGCTCGCGATCGGGATAACCAGGTCTTCGAGCCGAATGGTGAAGAAGATCGCTATTTCCCTCCGAACTCACAAATCTTCTCGTATCTTGGCTCCTACACGAAAGGCTTGCCTAATAACCGCCGCACGGCTTTAATTACCTCGCCAAACAACTTTGTTCGATTCGTCCGCGCAATTGACTCAGGCGAGCCAGCGGATTTCATCAAGGTTCCACTGGGTCCTCGCCCCGCGCTTCAGTTTGAATCGGAGGAAGAATGTCGCGCCGCAAACCTGTTTAAATCAGGTATCGCGGGCCGAAATAACACGTTCCCGTCCTCCTGCTTGCGCGCTTTGGAGTCTATGGGTGCTGGCCTGGTGTTCGATCTGGAGGGCCCTGACGCGCAGGCCGTGGGCATGCCGCCAGCGCCCACGTTGGATTCCGACGAGCTGGTCGCGGAGATTTCCGAGGTATATTTGATGGCGTTACTGCCTGACGTTCCTTTCACCGATTTTACTAATCCGGGCCCGATCGGGCCTGCGATAAACACACTTAATAAAACCGCGTTGATCCGCGCGGCGCCTGACCCGCCAGATTCCCTGACCCCGCAAGAGCCTGCGCCTCTGCCTGGTCCGTTTAACCCGTCTAATATTTTCCGAGGCACGTTGCCAGGCGATGATGTGGGTCCGTATCTCTCGCAGTTCCTCCTTGTAGGCACCAAAGGCATTGGTGGCGCCCAAGACATGGCGGATGGCTTCATTTCCTACGGCGCGAATCCTATTGATCAGCCTGTTCGCAATGCTCCTAAGGAACTGGACTATATGACCTCCTTGGAAGCATTCTTAGATGTTCAGAACGGGGCCGATGTTACCGGGCGCGACACTTTCGAATCTGGCTCGGATGCCTTTCCTTTCATCACCACCCCGCGCGATCTTGCAACCTATGTCAACTTTGATGCTCTCTATCAGGCGTATCTCAACGCCTGTCTCATTATGCTTGACTCCGGTGTTCCTTTCGATAAAGGGATTCCGTTCGGAGAACCTGACTTTAAAGATAATCAGCCTGGTTTTGCAAACTTCGGTGGCCCGAATATCCTTTCTCTTGTGACGGAAGTAGCGACCCGCGCACTGAAAGCGGTACCTTTCCAGAAATTTAACACCAACCGCCGCCTGCCTCCGGAAGCAGTCGGCGGTCTGATTGAACCTTTTAACTCTAACCCTGATGATCCGCAGTTCCAGGACGTCAAACCGCTGTTCGAGGCTCTGGATGAAGACATGATGCGCCCTGTTGCACCTAACAATCGCGAACAAAACCAGGGTTCTGACTTCGGTATGCCGCGCGCAGATGACTTCAATCCGGCGGGGGACACCCTGGAAACTATGCTGTTGCCTATGGCGTTCCCCGAGGGTTCCCCCATGAACCCCTCGTACGGAGCCGGAAACGCGACTGTAGCTGGCGCATGTGTGACGGTGCTCAAAGCCTTCTTCCAAAATGATACCGAGCTGGATTTTTGCTTTGTGCCGTCCGATGATGGTTCACGCCTGGTGGACGCCTCCAACAACATGAACAAGAAGCTGACCGTCGAGGGGGAGTTGAACAAAGTCTGCTCTAACATTTCTATTGGTCGGAATTTGGCAGGCGTGAATTACTTTACGGACTATATCGAATCCATCTTGCTGGGCGAGCAGATCGCTCTCGGTATTCTGGAGGAACAAATGCTCACCTTTCCGGAAACCTTCACGATGACCGTGCCATTGTTCTCCGGGGAGTTAAAAGTACTGCCTTCTACC</t>
+          <t>ATGTCGGCCGCGCGCCGGCAAGAAGCGTTTCAAACTCGCGTACCTGCGGCCCGATTAGCCCCTGACCGCGACAACCAAGTGTTCGAACCCAATGGCGAAGAAGATCCTTATTTTCCTCCAAACTCGCAGATTTTCTCATATCTCGGTTCCTATACTAAAGGACTGCCGAACAATCGCCGCACTGCCTTGATTACCTCCCCAAACAACTTTGTTCGCTTTGTCCCTGCTATCGACTCCGGGGAACCGGCAGATTTTATCAAAGTGCCCTTAGGCCCGCCTCCGGCTCTGCAGTTTGAATCTGAGGAAGAATGCCGCGCAGCGAACCTCTTCAAATCCGGTATCGCTGGCCGCAACAACACCTTTCCGTCATCATGCCTGCGGGCTTTGGAATCTATGGGTGCGGGACTGGTATTTGACCTCGAAGGCCCTGACGCTCAGGCAGTGGGTATGCCGCCAGCCCCGACCCTGGATTCTGACGAACTCGTGGCTGAAATATCTGAAGTATACTTGATGGCGCTGCTGCGCGATGTCCGCTTTACGGATTTTACTAACCCGGGGCCAATTGGTCCTGCAATTAACACGCTGAACAAAACCGCGTTGATACGAGCTGCGCCTGATCCTCCGGACTCTCTGACCCCGCAGGAACGGGCGCGCCTGCGCGGCCCATTCAACCCTTCCAACATTTTCCGCGGTACCCTGCCAGGTGATGACGTAGGACCGTACCTGTCACAGTTCCTTTTGGTTGGCACCAAAGGAATTGGTGGTGCGCAAGACATGGCGGACGGTTTTATTTCTTACGGTGCGAACCGGATCGATCAACCTGTTCGCAATGCGCCTAAAGAGTTGGATTACATGACCTCCTTGGAAGCGTTCCTGGACGTGCAGAACGGTGCGGATGTGACGGGCCCTGATACCTTTGAGTCGGGCTCTGACGCCTTCCGGTTTATTACAACACCACGGGATTTAGCTACTTATGTGAACTTTGACGCACTGTACCAAGCGTATCTAAACGCATGTCTGATTATGCTGGATTCTGGTGTACCTTTCGATAAGGGTATTCCCTTTGGCGAGCCGGACTTTAAAGATAACCAGCGCGGTTTCGCTAACTTCGGCGGTCCGAACATTCTTTCACTGGTGACCGAAGTTGCAACCCGGGCGCTGAAGGCTGTTCCTTTCCAGAAGTTTAATACTAATCCTCGCCTTCCTCCTGAAGCTGTGGGCGGTCTAATTGAACCTTTTAACTCAAATCCGGACGACCCTCAGTTTCAGGACGTGAAACCGTTGTTTGAAGCTCTGGATGAGGACATGATGCGGCGCGTTGCGCGAAACAACCCTGAACAAAATCAAGGCTCTGATTTTGGAATGCCTCGAGCGGACGACTTCAACCCGGCGGGCGACACGTTAGAAACAATGCTGCTGCCAATGGCATTTCCAGAAGGTTCACCGATGAATCCATCTTATGGTGCTGGCAATGCCACGGTCGCAGGCGCGTGTGTTACGGTCCTGAAAGCCTTCTTTCAGAATGATACTGAGCTGGATTTTTGCTTCGTCCCATCCGACGATGGTTCTCCTCTGGTTGACGCGTCAAATAACATGAACAAGAAACTGACTGTGGAAGGCGAATTGAACAAAGTATGCTCGAACATTTCGATCGGTCCTAACTTGGCTGGCGTAAATTACTTCACGGACTACATCGAATCAATACTGTTGGGGGAACAGATCGCTTTGGGTATTCTGGAAGAGCAGATGCTGACCTTCCCGGAAACCTTTACCATGACCGTGCCCCTCTTTTCCGGTGAACTGAAAGTGCTTCGCTCCACG</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>ATGTCAGCTGCGC</t>
+          <t>ATGTCGGCCGCGC</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>GGTAGAAGGCAGTAC</t>
+          <t>CGTGGAGCGAAGCACTTTC</t>
         </is>
       </c>
     </row>
@@ -892,22 +892,22 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>TACCGTTGGGGCACAAAGCGGGTCCGAGGTCGCGGCTGCAACGCGGGAAGAGGTGCTGCGAATGGAGACTGCGGTTGAAGAAAAGACGGCGGAGGCAAAGATGGGTTTGGTAAAGGCGCGAGAGGCGCGTTAGGCTTGGGGGCGGACTTACGGCGTAGTCGCGCGTGAAGGCGCCGGGTCGGAGGCCTGGCGCGCCGATGCGGCACACGCTGAGCGGTCGTCGTCCGCGACCTCAACGCGGGACGCCGTCGCGTTGATCGGTTACTGGGACGCTTAGGCCGATTGCAAAGATTGCCGAGGCTTCTTAATTTGGACTTAGGCTTTTGGCCACGCGGAGACAACGACCGATTGAAGTGATTTCCGGAGGGCTTACTCGCGCTGTGGCCAAACCGTCGTCTACGTCGCTTAATACTGGACAAGCAGCGCCGTCACTTGAGCCCAAATGGCCTGCTGTAGGGACGCTAAGGCAATCCAGGCGTTCGTCGTGGTCCACACGGAAACGGTGGAAGAGACGGAAAAGCGAGACCTTAGCGAGGAAGCAGGTTGGACAAAGGTTTGTGGCTACAGGCGCGAAACCTTAGCTACCGCCGCCCCTTACGCAAGCTAGAGGTTCCGGGGCTACGTGTCCGTCACTGTTACGGGGGCCGCGGTCGAGAACGTAGTGGCCTTGACCGCGACCTCTACTGCCTTTTGATGAACTACCGCGACGACGGACTACAAGGAAAAAGCGTCAAGCGGCGCCTGGGCTGACAACGCCGGCGGTACCTTAGGTACTTACGGTGGCTTAACCAGCGCGACCGTACGCCACTGCGCAGACGTCACCGCCTCCTTCTTGGATTTGGAGACGGACCCGGCAAGTGGCGAGTCTTGCAAAAGGGACCGTTGTGGGTCCCCCTGACATTTCCAGGTATATAGAGGGTTAAAAATGACAGGCCAAGTCGTCCTGACCCAGTTCAGTTGAGACCACGACTGCCTATGTAAGTCATGCCACGTTACGGATACCTGGTCGGACAAGGACAGCGTAATCTCCCGGACCTAATGTACTGATGGAACCTTAGAAACGACCTACAGGTCTTACCGCGCCTGGACGCGCCGGCCCTTAACATACTCCTACCCCTCGCGAAGGGAAAGTAAACATGTGGTGCTCTGGACCGCTGTATACAGTTGATACTACGAGACATGGTCCGCATAGACTTACGCACATAGTAATACGATTTGTTTTTTTAGGGCAAACTGTTCCCGAATGGCAAGGTTTTCCTGCTACTGTAACTGTTCGTTGTTCCAAAGCGGGAGAAACCAGGCGGGTTGTAGGACTGAGACACATGACTCCACCGTTGGGCGCGGGAATTTCCGTAGGCGAAGGTCTTTATGTTACACTTGGCGGGAGACGCGGGCCTTCGACAGCCTCCAGGACAGCTCGCGATGTTGTTGTTGACGCTCCTAGGCGACAAACGTCTGCAGTTTGGCAACATACTGCGGGACCTATTTCTGTACGACCTTGCGCAGCGCCGGTTGTTGCGTCTCGTCTTGCGCTTTCTACTAAAGCCTTTAAGTGGAAAACTTCTAATGAGAGGGTGGCCAAGGAGCCCAGCGTGGATGGACGAAGGCTACCGCAAAGGCCTCCCGAGAGGATACTTGGGCCGCATACCGCGACCATTGCGTCGTCATCGCCCACGCACGTGGTGATAAGACTTTCGAAAGAAGCTGTTACTTTTGCTTGACCTAAAACGGATACAAGGGTGGCGTCTACCGAGGTTTAATCTTCTGCAACAACTAAGTAACCCGCTTTTTGACTGGCAACTCCCTCTCAACTTGTTTCACACAAGATTGTAAAGACAGCCGGCGTTAAACCGCCCACAGTTAATGAAATGGCTAATAGGACTTAGATAATAGGAGCCGCTTTTTTAACGGGACCCGGACGAGCTTCTTGTCTTTGATTGGATACGTCTCCTTAAAAGATACTGCTAGGGAGACAAGCTACCAAGGTGGCATTGGTAA</t>
+          <t>TACCGCTGGGGTACGAAGCGGGTCCGGGGACGAGGATGGGACGCGGGAAGGGGTGGAGGAAACGGCAATTGCGGCTGCAGGAAAGAAGGAGCGGGCAAAGACGGCTTTGGCAAGGGTGGAAGTGGAGCCTTAGGATTGGGAGGAGACTTGCGCCGCAGACGTGCGTGGAGCCGCCGAGTCGGCGGCCTGGGACGCCGTTGAGGCACACGTTGGGGAGTCGTCGTTCGCAATCTCGACGGAGGACGCCGTCGCGTCGACCGCTTACTGGGACGATTAGGACGCTTACATAGATTGCCGAGGCTCCTTGACTTAAATTTAGGTTTTTGCCCGCGTGGTGAAGACGACCGGTTGAAGTGGTTTCCAGACGGGTTGCTTGGACTATGGCCTGACCGCCGGCTGCGTCGATTGATACTGGACAAACACCGCCGTCAATTAAGGCCCGACGGTCTACTATAAGCCCGCTAAGGCGACCCAGGGGTCCGGCGAGGCCCACACGCGGAGGGCGGAAGCGACGGAAAGGCCAGCCCGTAGCGTGCGAGTAGATTGGACAAAGGTTTGTGGCTACACGCCCGGAACCTCAGATACCGCCGTCCCTTACGCAAGCTAGACGTTCCGGGCCTGCGGGTCCGCCACTGGTACGGCGGTCGCGGACGCGACCGGAGAGGACTTGACCGAGACCTTTACTGGCTTTTGATAAACTACCGGGACAATGCTCTACACGCGAAAAGTGTCAAACGACGCCTGGGCTGGCAACGGCGCCGGTACCTTAGCTACTTGCGCTGGCTCAACCAGCGCGAACGCACACCGCTACGCAGCCGGCACCGCCTCCTCCTTGCGTTTGCGAATGCGCCGGGCAAATGGCGTGTTTTACACAAGGGACCATTGTGGGTCCCACTGACGTTTCCAGGCATGTAAAGAGTCAAGGACGAGAGACCAAGTCGGCCAGAACCAGTCCACTTGAGCCCGCGCCTACCAATATAAGTTATACCACGCTACGCGTACCTAGTTGGACATGCGCAGCGCGACCTTCCGGACCTGATATACTGATGCAACCTTAGCAACGACCTGCATGTCTTACCACGGCTAGACGCCCCAGCGCTTGACATACTTCTGCCCCTCGCTAAAGGAAAGTAGACGTGGGGCGCTCTAGACCGGTGAATACACTTGATACTACGCGAGATAGTCCGCATGAATTTGCGCACATATTAATACAACTTGTTTTTTTAAGGTAAGCTATTTCCGGACGGCAAGGTCTTTCTGCTACTATAACTGTTTGTCGTCCCGAAACGCGACAAGCCAGGCGGATTGTAGGACTGTGAGACGTGGCTTCAGCGTTGTGCGCGGGACTTTCCATAGGGAAAGGTTTTTATATTACACTTGGGAGCGGACGGAGGCCTTCGCCACCCGCCGGCTCAACTCGCGATGTTGTTGTTGACGCTTCTAGGCGACAAGCGACTACACTTTGGAGACATGCTACGGAATCTGTTTCTATACAATCTTGCGCACCGCCGGTTGTTGCGCCTCGTCTTGCGGTTTCTGCTAAAGCCATTAAGAGGAAAGCTTCTAATGAGGGGATGGCCCAGTAGACCAGGATGAATGGAAGAAGGGTACCGTAAAGGCCTCCCTAGGGGTTACTTGGGCCGTATACCGCGTCCTTTGCGGCGTCAACGGCCTCGCACGTGGTGATATGACTTTCGTAAGAAGCTGTTGCTTTTGCTCGAACTGAAGCGCATACACGGCTGCCGCCTACCAAGCTTTGACCTTCTGCACCACCTGAGGGACCCACTCTTTGACTGGCATCTTCCCCTTGACTTGTTTCAAACGAGATTATAAAGCCATCCCGCGTTGAACCGGCCACAGTTAATAAAATGGCTAATAGGACTCAGATAGTAGGACCCGCTCTTTTATCGGAATCCCGAGGACCTTCTTGTCTTCGACTGCATACGCCTCCTTAAAAGCTACTGCTAGGGCAACAAACTACCGAGATGTCAATGTTAA</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>ATGGCAACCCCGTGTTTCGCCCAGGCTCCAGCGCCGACGTTGCGCCCTTCTCCACGACGCTTACCTCTGACGCCAACTTCTTTTCTGCCGCCTCCGTTTCTACCCAAACCATTTCCGCGCTCTCCGCGCAATCCGAACCCCCGCCTGAATGCCGCATCAGCGCGCACTTCCGCGGCCCAGCCTCCGGACCGCGCGGCTACGCCGTGTGCGACTCGCCAGCAGCAGGCGCTGGAGTTGCGCCCTGCGGCAGCGCAACTAGCCAATGACCCTGCGAATCCGGCTAACGTTTCTAACGGCTCCGAAGAATTAAACCTGAATCCGAAAACCGGTGCGCCTCTGTTGCTGGCTAACTTCACTAAAGGCCTCCCGAATGAGCGCGACACCGGTTTGGCAGCAGATGCAGCGAATTATGACCTGTTCGTCGCGGCAGTGAACTCGGGTTTACCGGACGACATCCCTGCGATTCCGTTAGGTCCGCAAGCAGCACCAGGTGTGCCTTTGCCACCTTCTCTGCCTTTTCGCTCTGGAATCGCTCCTTCGTCCAACCTGTTTCCAAACACCGATGTCCGCGCTTTGGAATCGATGGCGGCGGGGAATGCGTTCGATCTCCAAGGCCCCGATGCACAGGCAGTGACAATGCCCCCGGCGCCAGCTCTTGCATCACCGGAACTGGCGCTGGAGATGACGGAAAACTACTTGATGGCGCTGCTGCCTGATGTTCCTTTTTCGCAGTTCGCCGCGGACCCGACTGTTGCGGCCGCCATGGAATCCATGAATGCCACCGAATTGGTCGCGCTGGCATGCGGTGACGCGTCTGCAGTGGCGGAGGAAGAACCTAAACCTCTGCCTGGGCCGTTCACCGCTCAGAACGTTTTCCCTGGCAACACCCAGGGGGACTGTAAAGGTCCATATATCTCCCAATTTTTACTGTCCGGTTCAGCAGGACTGGGTCAAGTCAACTCTGGTGCTGACGGATACATTCAGTACGGTGCAATGCCTATGGACCAGCCTGTTCCTGTCGCATTAGAGGGCCTGGATTACATGACTACCTTGGAATCTTTGCTGGATGTCCAGAATGGCGCGGACCTGCGCGGCCGGGAATTGTATGAGGATGGGGAGCGCTTCCCTTTCATTTGTACACCACGAGACCTGGCGACATATGTCAACTATGATGCTCTGTACCAGGCGTATCTGAATGCGTGTATCATTATGCTAAACAAAAAAATCCCGTTTGACAAGGGCTTACCGTTCCAAAAGGACGATGACATTGACAAGCAACAAGGTTTCGCCCTCTTTGGTCCGCCCAACATCCTGACTCTGTGTACTGAGGTGGCAACCCGCGCCCTTAAAGGCATCCGCTTCCAGAAATACAATGTGAACCGCCCTCTGCGCCCGGAAGCTGTCGGAGGTCCTGTCGAGCGCTACAACAACAACTGCGAGGATCCGCTGTTTGCAGACGTCAAACCGTTGTATGACGCCCTGGATAAAGACATGCTGGAACGCGTCGCGGCCAACAACGCAGAGCAGAACGCGAAAGATGATTTCGGAAATTCACCTTTTGAAGATTACTCTCCCACCGGTTCCTCGGGTCGCACCTACCTGCTTCCGATGGCGTTTCCGGAGGGCTCTCCTATGAACCCGGCGTATGGCGCTGGTAACGCAGCAGTAGCGGGTGCGTGCACCACTATTCTGAAAGCTTTCTTCGACAATGAAAACGAACTGGATTTTGCCTATGTTCCCACCGCAGATGGCTCCAAATTAGAAGACGTTGTTGATTCATTGGGCGAAAAACTGACCGTTGAGGGAGAGTTGAACAAAGTGTGTTCTAACATTTCTGTCGGCCGCAATTTGGCGGGTGTCAATTACTTTACCGATTATCCTGAATCTATTATCCTCGGCGAAAAAATTGCCCTGGGCCTGCTCGAAGAACAGAAACTAACCTATGCAGAGGAATTTTCTATGACGATCCCTCTGTTCGATGGTTCCACCGTAACCATT</t>
+          <t>ATGGCGACCCCATGCTTCGCCCAGGCCCCTGCTCCTACCCTGCGCCCTTCCCCACCTCCTTTGCCGTTAACGCCGACGTCCTTTCTTCCTCGCCCGTTTCTGCCGAAACCGTTCCCACCTTCACCTCGGAATCCTAACCCTCCTCTGAACGCGGCGTCTGCACGCACCTCGGCGGCTCAGCCGCCGGACCCTGCGGCAACTCCGTGTGCAACCCCTCAGCAGCAAGCGTTAGAGCTGCCTCCTGCGGCAGCGCAGCTGGCGAATGACCCTGCTAATCCTGCGAATGTATCTAACGGCTCCGAGGAACTGAATTTAAATCCAAAAACGGGCGCACCACTTCTGCTGGCCAACTTCACCAAAGGTCTGCCCAACGAACCTGATACCGGACTGGCGGCCGACGCAGCTAACTATGACCTGTTTGTGGCGGCAGTTAATTCCGGGCTGCCAGATGATATTCGGGCGATTCCGCTGGGTCCCCAGGCCGCTCCGGGTGTGCGCCTCCCGCCTTCGCTGCCTTTCCGGTCGGGCATCGCACGCTCATCTAACCTGTTTCCAAACACCGATGTGCGGGCCTTGGAGTCTATGGCGGCAGGGAATGCGTTCGATCTGCAAGGCCCGGACGCCCAGGCGGTGACCATGCCGCCAGCGCCTGCGCTGGCCTCTCCTGAACTGGCTCTGGAAATGACCGAAAACTATTTGATGGCCCTGTTACGAGATGTGCGCTTTTCACAGTTTGCTGCGGACCCGACCGTTGCCGCGGCCATGGAATCGATGAACGCGACCGAGTTGGTCGCGCTTGCGTGTGGCGATGCGTCGGCCGTGGCGGAGGAGGAACGCAAACGCTTACGCGGCCCGTTTACCGCACAAAATGTGTTCCCTGGTAACACCCAGGGTGACTGCAAAGGTCCGTACATTTCTCAGTTCCTGCTCTCTGGTTCAGCCGGTCTTGGTCAGGTGAACTCGGGCGCGGATGGTTATATTCAATATGGTGCGATGCGCATGGATCAACCTGTACGCGTCGCGCTGGAAGGCCTGGACTATATGACTACGTTGGAATCGTTGCTGGACGTACAGAATGGTGCCGATCTGCGGGGTCGCGAACTGTATGAAGACGGGGAGCGATTTCCTTTCATCTGCACCCCGCGAGATCTGGCCACTTATGTGAACTATGATGCGCTCTATCAGGCGTACTTAAACGCGTGTATAATTATGTTGAACAAAAAAATTCCATTCGATAAAGGCCTGCCGTTCCAGAAAGACGATGATATTGACAAACAGCAGGGCTTTGCGCTGTTCGGTCCGCCTAACATCCTGACACTCTGCACCGAAGTCGCAACACGCGCCCTGAAAGGTATCCCTTTCCAAAAATATAATGTGAACCCTCGCCTGCCTCCGGAAGCGGTGGGCGGCCGAGTTGAGCGCTACAACAACAACTGCGAAGATCCGCTGTTCGCTGATGTGAAACCTCTGTACGATGCCTTAGACAAAGATATGTTAGAACGCGTGGCGGCCAACAACGCGGAGCAGAACGCCAAAGACGATTTCGGTAATTCTCCTTTCGAAGATTACTCCCCTACCGGGTCATCTGGTCCTACTTACCTTCTTCCCATGGCATTTCCGGAGGGATCCCCAATGAACCCGGCATATGGCGCAGGAAACGCCGCAGTTGCCGGAGCGTGCACCACTATACTGAAAGCATTCTTCGACAACGAAAACGAGCTTGACTTCGCGTATGTGCCGACGGCGGATGGTTCGAAACTGGAAGACGTGGTGGACTCCCTGGGTGAGAAACTGACCGTAGAAGGGGAACTGAACAAAGTTTGCTCTAATATTTCGGTAGGGCGCAACTTGGCCGGTGTCAATTATTTTACCGATTATCCTGAGTCTATCATCCTGGGCGAGAAAATAGCCTTAGGGCTCCTGGAAGAACAGAAGCTGACGTATGCGGAGGAATTTTCGATGACGATCCCGTTGTTTGATGGCTCTACAGTTACAATT</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>ATGGCAACCCCGT</t>
+          <t>ATGGCGACCCCAT</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>AATGGTTACGGTGGAAC</t>
+          <t>AATTGTAACTGTAGAGCCATC</t>
         </is>
       </c>
     </row>
@@ -934,22 +934,22 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>TACAGACTGTACAGGTGACTTTAGAGTGGAGGAGTCGTTCTTCGCATACTATAGGCGCAACGACGCCGTTGGGACCGGAACCGCGGACTAGGATTTGCGTTTCACAAACTTGGATTGCCCCTTCTTCTAGCGATAAAGGGAGGGTTGAGGGTCTAAAATAGGATGGACCCCAGGATGTGGTTTCCAGACGGCTTGTTGGCTAGATGCCGGGAACACTGGAGAGGATTGTTGAAGCATGGAAAGCAGGTCCGGTAGCTGAGCCCACTTGGCCGCCTGAAGTAGTTTCAAGGCGACCCCGGCGCGGGACGTGAACTTAAATGCTGGCTTCTCCTTACGTAGCGCCGATTGGACAAGTTTAGGCCATAGCGATGGGGATTACTAAGGAAACTAGGACGAACGAATGGACGTAACCTTAGCTACCCGCGTCCAAATCACAAGCTAGACCTTCCTGGACTGCGCGTCCGTCAACCGTACGGGGGCCGCGGCTGGGACCTGAGGCTACTTGACCACCGGCTTTAAAGTCTTGACATGAACTACCGCGAGGAAGCGCTACACGGAAAGTGCCTAAAATGGTTGGGACCTGGCTAAGGAGCGCGGTAGTTGTGCAACTTGGCGTGGTGCAACTATGGACGTCGGGGACTGGGCGGCCTAAGCGAGTGTGGCGTCCTTGCTCGGGGAGACGCGCCCGGCAAGTTGGGTAGCAGATAAAAAGCGCCATGTGACGGCCCGCTGCTGCAACCAGGAATGGAAAGCGTCAAGAACGACCATCCTTGCCTTCCGTAACCGCCACGGGTCCTAGGACGCCTACCGAAGTAAAGTATACCACGTTTAGGATAGCTAGTTGGACAGGCGTTGCGATGGTTTCTCGACCTAATGTACTGCAGCAACCTCCGTAAAGACCTGCACGTCTTGCCGCGTCTACAACGCCCGGCGCTGTGGAAGCTTAGGCCGAGCCTGCGCAAGGGAAAGTAGTGGTGGGGGGCGCTGGACCGATGGATACACTTGAAGCTGCGAGACATAGTTCGGATAGAATTGCGGACAGACTAAGACGAGCTATTGTTTCACTTCAAGCTGGTTCCATAGGGATACCCGCTTGGACTAAAGTTACCCTTAGTCCCGTAGGGCAAGGTCCTGGGCCTAAAGTTTCTATTGGTCGGACCAAAGCGCTTGAAGCCACCTGGCTTGTAGGAGAGCGAGCAGTGTCTTCAGCGATGTGCGCGAGAATTTCGGCAGGCGAAGGTCTTTAAGTTGTGGTTAGGAGCGGAAGCTGGCCTTCGGCATCCACCGGAGTAGCTTGGAAAATTAAGGTTGGGACTACTAGGCGTTAAGGTCCTACACTTTGGGAACAAACTTCGCGACCTACTCCTGTACGACGCGGGACAACGCAGCTTGTTGGCGCTTGTTTTACTTGGAAGGCTAAAGCCGTACGGCGCGCGACTGCTGAAGTTGGGCCGTCCGCTGTGGGACCTCTGTTACAACGACGGTTACCGGAAAGGCCTTCCGAGAGGCTACTTGGGCAGCATGCCACGCCCATTACGCTGCCACCGTCCGCGCACGCAATGCCAAGACTTCCGAAAGAAAGTTTTACTACGTTGCAACCTAAAGACGATGCACGGCAGGCTACTACCGAGGGCGGAACTGCTACGGAGGTTATGGGACTTGTTCTTTAACTGGCAACTCCCTCTCGAATTATTCCACACAAGATTATATAGATAGCCAGGATTAAACCGCCCGCATTTAATAAAATGCCTAATGTAGCTTAGTTAAGACGACCCGCTCGTTTAACGCAACCCATAGGACCTTCTTGTCTACAACTGCAAGGGGCTCTGGAAGTGATACTGGCAGGGTAATAAAAGCCCGCCAAAAGCGTGCGAGTAAAGTTGTAGTCTAGGC</t>
+          <t>TACAGACTATACAGCTGGCTTTAGAGAGGAGGAGTTGTCCTTCGTATGCTATAAGGACAGCGTCGTCGTTGAGACCGCGACCGTGGACTGGCGTTCGGATTTCATAAACTTGGCTTGCCCCTTCTTCTGGGAATAAAGGCTGGATTGAGAGTCTAGGAGAGAATAGAACCAAGCATATGGTTTCCCGACGGGTTATTGGCGAGTTGGCGGGACCACTGGAGGGGCTTGTTGAAGCACGGAAAACACGTCCGATAGCTGAGCCCGCTCGGTCGGCTGAAGTATTTCCACGGTGACCCGGGTGCGGGACGAGACCTTAAATGGTGTCTTCTTCTTACGTAGCGCCGTTTGGACAAATTTAGCCCATAACGCTGCGCGTTGCTGAGTAAACTAGGCCGGACAGACGCCCGTAACCTCAGATACCCGCGCCCCAATCAGAAGCTAAACCTCCCGGGTCTACGTGTCCGACACCCTTACGGCGGACGTGGTTGAAATCTAAGACTACTTGACCACCGCCTCTAAAGCCTTGAAATAAACTACCGGAACAATGGACTACAGGCGAAATGGCTGAAGTGATTGGGCCCAGGCTATGGAGCGCGATAATTGTGCAACTTGGCGTGATGGAACTAAGCGCGGCGCGCGCTAGGCGGCCTGAGAGACTGTGGCGTTCTCGGACGTGGAGACGCTCCAGGCAAATTGGGCAGGAGCTAAAAGGGACCTTGAAACGGCCCACTACTGCATCCAGGAATGGACAGCGTTAAGGACGACCACCCGTGGCTTCCATAACCGCCGCGAGTCCTGGCGCGCCTGCCAAAGTAAAGTATACCACGGTTAGCGTAACTAGTTGCGCACGCGTTGCGGTGGTTTCTTAACCTAATATACTGGAGGAACCTTCGAAAAGACCTACAAGTCTTACCGCGACTACATCGCCCGGGACTGTGGAAGCTCAGACCAAGCCTACGTAAAGCCAAGTAGTGCTGCGGCGGACTAGACCGATGGATACAATTAAAGCTACGAGAAATAGTCCGCATGGACTTGCGGACAGACTAGGAAGAGCTGTTGTTTCATTTTAAACTGGTCCCGTAAGGCTACCCGCTTGGCCTGAAGTTGCCTTTGGTTCCGTAGGGCAAGGTCCTAGGCCTAAAATTTCTGTTAGTCGGACCAAAGCGCTTAAAACCACCGGGGTTGTAAGACAGTGACCAATGTCTTCACCGGTGCGGACGCGACTTCCGCCATGGAAAAGTCTTTAAATTGTGGTTGGCGGGAGAGGCGGGGCTTCGTCAGCCACCAGACTAACTTGGAAAATTAAGCTTAGGCCTGCTGGGAGTCAAGGTCCTACAATTCGGCGACAAACTCCGGAACCTGCTTCTGTACGACGGAGGACAACGCAGCTTATTGGGACTTGTCTTACTTGGAAGTCTAAAACCCTACGGGGCTCGCCTACTAAAGTTGGGCCGCCCGCTATGAAATCTTTGGTACGACGAGGGTTACCGTAAAGGCCTTCCGAGAGGTTACTTGGGTAGAATACCGCGTCCGTTGCGTTGGCATCGTCCGCGCACGCACTGGCACGACTTTCGCAAAAAGGTCTTACTACGATGCGACCTAAAAACGATACACGGCAGCCTACTGCCTAGGGCGGACCTGCTGCGAAGGTTATGGGACTTGTTCTTCGACTGGCATCTCCCTCTCGAATTATTCCATACGAGATTGTAAAGATAACCGGCGTTAAACCGACCTCACTTGATGAAGTGACTAATGTAACTCAGATAAGACAATCCGCTCGTTTAGCGTGAACCATAGGACCTTCTCGTCTACGAGTGCAAAGGACTTTGTAAATGCTACTGACATGGCGACAAGAGACCGCCCAAAGGATGCGAGTAAAGCTGAAGACTAGGC</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>ATGTCTGACATGTCCACTGAAATCTCACCTCCTCAGCAAGAAGCGTATGATATCCGCGTTGCTGCGGCAACCCTGGCCTTGGCGCCTGATCCTAAACGCAAAGTGTTTGAACCTAACGGGGAAGAAGATCGCTATTTCCCTCCCAACTCCCAGATTTTATCCTACCTGGGGTCCTACACCAAAGGTCTGCCGAACAACCGATCTACGGCCCTTGTGACCTCTCCTAACAACTTCGTACCTTTCGTCCAGGCCATCGACTCGGGTGAACCGGCGGACTTCATCAAAGTTCCGCTGGGGCCGCGCCCTGCACTTGAATTTACGACCGAAGAGGAATGCATCGCGGCTAACCTGTTCAAATCCGGTATCGCTACCCCTAATGATTCCTTTGATCCTGCTTGCTTACCTGCATTGGAATCGATGGGCGCAGGTTTAGTGTTCGATCTGGAAGGACCTGACGCGCAGGCAGTTGGCATGCCCCCGGCGCCGACCCTGGACTCCGATGAACTGGTGGCCGAAATTTCAGAACTGTACTTGATGGCGCTCCTTCGCGATGTGCCTTTCACGGATTTTACCAACCCTGGACCGATTCCTCGCGCCATCAACACGTTGAACCGCACCACGTTGATACCTGCAGCCCCTGACCCGCCGGATTCGCTCACACCGCAGGAACGAGCCCCTCTGCGCGGGCCGTTCAACCCATCGTCTATTTTTCGCGGTACACTGCCGGGCGACGACGTTGGTCCTTACCTTTCGCAGTTCTTGCTGGTAGGAACGGAAGGCATTGGCGGTGCCCAGGATCCTGCGGATGGCTTCATTTCATATGGTGCAAATCCTATCGATCAACCTGTCCGCAACGCTACCAAAGAGCTGGATTACATGACGTCGTTGGAGGCATTTCTGGACGTGCAGAACGGCGCAGATGTTGCGGGCCGCGACACCTTCGAATCCGGCTCGGACGCGTTCCCTTTCATCACCACCCCCCGCGACCTGGCTACCTATGTGAACTTCGACGCTCTGTATCAAGCCTATCTTAACGCCTGTCTGATTCTGCTCGATAACAAAGTGAAGTTCGACCAAGGTATCCCTATGGGCGAACCTGATTTCAATGGGAATCAGGGCATCCCGTTCCAGGACCCGGATTTCAAAGATAACCAGCCTGGTTTCGCGAACTTCGGTGGACCGAACATCCTCTCGCTCGTCACAGAAGTCGCTACACGCGCTCTTAAAGCCGTCCGCTTCCAGAAATTCAACACCAATCCTCGCCTTCGACCGGAAGCCGTAGGTGGCCTCATCGAACCTTTTAATTCCAACCCTGATGATCCGCAATTCCAGGATGTGAAACCCTTGTTTGAAGCGCTGGATGAGGACATGCTGCGCCCTGTTGCGTCGAACAACCGCGAACAAAATGAACCTTCCGATTTCGGCATGCCGCGCGCTGACGACTTCAACCCGGCAGGCGACACCCTGGAGACAATGTTGCTGCCAATGGCCTTTCCGGAAGGCTCTCCGATGAACCCGTCGTACGGTGCGGGTAATGCGACGGTGGCAGGCGCGTGCGTTACGGTTCTGAAGGCTTTCTTTCAAAATGATGCAACGTTGGATTTCTGCTACGTGCCGTCCGATGATGGCTCCCGCCTTGACGATGCCTCCAATACCCTGAACAAGAAATTGACCGTTGAGGGAGAGCTTAATAAGGTGTGTTCTAATATATCTATCGGTCCTAATTTGGCGGGCGTAAATTATTTTACGGATTACATCGAATCAATTCTGCTGGGCGAGCAAATTGCGTTGGGTATCCTGGAAGAACAGATGTTGACGTTCCCCGAGACCTTCACTATGACCGTCCCATTATTTTCGGGCGGTTTTCGCACGCTCATTTCAACATCAGATCCG</t>
+          <t>ATGTCTGATATGTCGACCGAAATCTCTCCTCCTCAACAGGAAGCATACGATATTCCTGTCGCAGCAGCAACTCTGGCGCTGGCACCTGACCGCAAGCCTAAAGTATTTGAACCGAACGGGGAAGAAGACCCTTATTTCCGACCTAACTCTCAGATCCTCTCTTATCTTGGTTCGTATACCAAAGGGCTGCCCAATAACCGCTCAACCGCCCTGGTGACCTCCCCGAACAACTTCGTGCCTTTTGTGCAGGCTATCGACTCGGGCGAGCCAGCCGACTTCATAAAGGTGCCACTGGGCCCACGCCCTGCTCTGGAATTTACCACAGAAGAAGAATGCATCGCGGCAAACCTGTTTAAATCGGGTATTGCGACGCGCAACGACTCATTTGATCCGGCCTGTCTGCGGGCATTGGAGTCTATGGGCGCGGGGTTAGTCTTCGATTTGGAGGGCCCAGATGCACAGGCTGTGGGAATGCCGCCTGCACCAACTTTAGATTCTGATGAACTGGTGGCGGAGATTTCGGAACTTTATTTGATGGCCTTGTTACCTGATGTCCGCTTTACCGACTTCACTAACCCGGGTCCGATACCTCGCGCTATTAACACGTTGAACCGCACTACCTTGATTCGCGCCGCGCGCGATCCGCCGGACTCTCTGACACCGCAAGAGCCTGCACCTCTGCGAGGTCCGTTTAACCCGTCCTCGATTTTCCCTGGAACTTTGCCGGGTGATGACGTAGGTCCTTACCTGTCGCAATTCCTGCTGGTGGGCACCGAAGGTATTGGCGGCGCTCAGGACCGCGCGGACGGTTTCATTTCATATGGTGCCAATCGCATTGATCAACGCGTGCGCAACGCCACCAAAGAATTGGATTATATGACCTCCTTGGAAGCTTTTCTGGATGTTCAGAATGGCGCTGATGTAGCGGGCCCTGACACCTTCGAGTCTGGTTCGGATGCATTTCGGTTCATCACGACGCCGCCTGATCTGGCTACCTATGTTAATTTCGATGCTCTTTATCAGGCGTACCTGAACGCCTGTCTGATCCTTCTCGACAACAAAGTAAAATTTGACCAGGGCATTCCGATGGGCGAACCGGACTTCAACGGAAACCAAGGCATCCCGTTCCAGGATCCGGATTTTAAAGACAATCAGCCTGGTTTCGCGAATTTTGGTGGCCCCAACATTCTGTCACTGGTTACAGAAGTGGCCACGCCTGCGCTGAAGGCGGTACCTTTTCAGAAATTTAACACCAACCGCCCTCTCCGCCCCGAAGCAGTCGGTGGTCTGATTGAACCTTTTAATTCGAATCCGGACGACCCTCAGTTCCAGGATGTTAAGCCGCTGTTTGAGGCCTTGGACGAAGACATGCTGCCTCCTGTTGCGTCGAATAACCCTGAACAGAATGAACCTTCAGATTTTGGGATGCCCCGAGCGGATGATTTCAACCCGGCGGGCGATACTTTAGAAACCATGCTGCTCCCAATGGCATTTCCGGAAGGCTCTCCAATGAACCCATCTTATGGCGCAGGCAACGCAACCGTAGCAGGCGCGTGCGTGACCGTGCTGAAAGCGTTTTTCCAGAATGATGCTACGCTGGATTTTTGCTATGTGCCGTCGGATGACGGATCCCGCCTGGACGACGCTTCCAATACCCTGAACAAGAAGCTGACCGTAGAGGGAGAGCTTAATAAGGTATGCTCTAACATTTCTATTGGCCGCAATTTGGCTGGAGTGAACTACTTCACTGATTACATTGAGTCTATTCTGTTAGGCGAGCAAATCGCACTTGGTATCCTGGAAGAGCAGATGCTCACGTTTCCTGAAACATTTACGATGACTGTACCGCTGTTCTCTGGCGGGTTTCCTACGCTCATTTCGACTTCTGATCCG</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>ATGTCTGACATGTCCAC</t>
+          <t>ATGTCTGATATGTCGACC</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>CGGATCTGATGTTGAAATG</t>
+          <t>CGGATCAGAAGTCGAAAT</t>
         </is>
       </c>
     </row>
@@ -976,22 +976,22 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>TACCCTTAAGGGCGTCTGTTGGACGTCAGAGGACGATTTCGTAGGAAGCTATGGGGACATAGACGTCGCCTTAACCGTGAGCGCGCGCCCCAGCAAGGCAGAGACCGCTTGCCACTTCTTGAGGAAATAGCGTTAGGTCTGGGTCTTTTGCCACTAGGGAGGAAGTAGCAAAGTAAATGCTTCCCGGAAGGCTTGCTGCTATTGCCACGCTAGTAACTAGGCCTACTGAAAGACCGAAAACAGGGACGGTATTTAAGGCCACTGCTTTTTCTTTAACGGCTAGACTGGGATCCGGGTCGGGGACTAGGCCTGTGTCCAGATGGCTAAAACGCGAGACTAGAGCGATTGAGCGACCTTGACCTCCACGGACCTAACCTTTTAAGAAGACGCCCGGAGTGGAAACTAAACCTTCCAGGACTACGCGTCAGGTAGCGTTACGGTGGCCGCGGCCACGACTGCAGCGGACTTGACTAACGACTCTAGCGTCTTGACATGGACTACCGCGACCCAGCGCTCTAGCTTAAAAGTCTCAAACTGAGGGGTTTTTTACGACTTATATAGGTCAAGCGCTAACTGGTTGACTTACCGGACCTTAACAAGTTATGAGGCCGTTACGACCCGCTGGGAGGCCGTCTTTAGGCGGCTGGAGGACCACTCCACTGCCACCCGTTGGACAAGGGACCCTAAGACGGCCCGAGGCTTCATCCAGGAATGAATAGAGTCATATAATAACACCCAAGCTTTGTTTAGCCGAGTCGCTGTCCGCCGTTATTTTGGAACCATAGAGGCTTGCGCCGTCTACTTAAACTACCACTTTAACGCATACCCAGTTAGTGGTATAGTGTTGCGCACGCGTAACGGTGAGGCCCAGGACTGAAATACTGGCTAAACTTTCACAAGGACCTGCAAGTCCTACGCCGACTAAAAGCCCCAAAGCTTAGTATGCTTGGCCCGCGTGCGAATTAAGGATGGTAGGCCCTAGACCGGTGGAACCACTTAAAGCTACGTGAAATACTTCGAATGGACTTACGGACAGACTAGAATGACCGCTTGGCGCACGGTAAGCTAGGCTTGTAGGGCAAGGTCGTCCTCCTGTTTGATCTATTAGTTCTACACAAACAGTTGAAGCCGCTACGGTTGCACAACAGAAACCATTGGCTTCAGCGCTGGGGACGTGAGTTTCGTCACGCCATGGTCTTTAAATTGTAGTTAGCGGCGGACGGAGGACTTCGTTGGCCGCCTAACTAGAGCCAGTTGTTTTAACGCCGGCTTTTCCCACTTAGACATAAAGGGCTTCAGCTAGAGCGCCAACTTCTCGACCTTCTATAAAACCTTTTTCGGCTTTAAAGATTAGCGTTTGTCTTATAACGTCTACCACTAGGTCTAGGGCTGGGGAGAAAAGACGACGGCGTTCGCAAGCGTCTTCCAAGCGGGAAATTGGGAAGAATACCGAGGCCTTTGCGGCAGCAGCGCCCGCGCACGCACTGGTAGGACTTTCGCAAGAAACTGAGCTTGAAAGTCTAACTAGTCCACAAACTTCATCTATTTCTACTTCTGTTTGACCAATTTAGAAGTAAGTTTCCGTGTGACTGACAGCGCCCGCTTGAGTTGTTTGACCGTCTATTGTAACGCTAACCTGGATTATACCGGCCGCAATTAATAAAAAGGCTAGTCAAACTTAGATAAGACAACCCGCTTGTTCATCGGTAGCCATAAGACCTTCTTGTCAGGGACTGGATGCCACTCTTGAAAAAGAAATTAGACGGTTTTAAGCTACCATGGTGCTAGGTCTAA</t>
+          <t>TACCCATAAGGCCGTCTGTTGGACGTCAGTGCGCGCTTTCGGAGAAAACTGTGAGCTCACAGCCGTCGACTCGACCGGGACCGTGCGCCGCAACACGGCAGCGACCGATTGCCACTCCTTGATGATATGGGATTGGGCCTAGGCCTTTTACCACTAGGCAGGAAATAACACAGAAAGTGATTTCCGGACGGATTGCTGCTATTACCACGTTAATAACTAGGCCTACTAAAGGACCGCAAACACGGACGGTAATTGAGGCCACTACTTTTCCTTTAGCGCCTAGACTGGGACCCGGGCCGTGGACTGGGCCTATGCCCAAATGGATATAACGCGAGGCTGGATCGCTTGAGCGACCTTGAGCTTCACGCCCCTAACCTCTTAAGCAGACGTCCGGAGTGTAAACTAGACCTTCCGGGCCTACGGGTCAGATAGCGCTACGGCGGACGTGGCCATGACTGCAGCGGGCTCGACTAACGGCTCTAGCGACTCAACATAGAGTACCGCGAGCCAGCTCTTTAACTTAAAAGTCTTAAGCTAAGGGGCTTCTTACGTCTTATGTAAGTCAAGCGGTATCTAGTCGAGTTACCTGAACTTAACAAATTGTGAGGACGCTACGACCCGCTGGGCGGACGTCTCTAAGGAGGAGGAGGACCACTTCACTGGCATCCCTTGGACAAGGCGCCATAGGACGGCCCAAGACTTCAGCCGGGCATAGACAGAGTCATGTAATAACAACCAAGGTTTGTCTAGCCGAGTCGTTGTCCCCCCTTGTTTTGCGACCACAGTGGCTTACGCCGACTACTTAAGCTGCCGCTTTAACGCATACCGAGCTAGTGGTAAAGGGTCGGACACGCCTAACGGTGTGGCCCAGGACTGAAATACTGGCTGGACTTTCAAAAAAATCTACAAGTCCTGCGTCGCCTGAAGGCGCCCAAGCTTAGAATACTCGGTCCACGCGCGGACTAGGGATGGTAGGGACTAGATCGATGTAACCACTTGAAACTACGCAATATACTTCGGATGGACTTACGCACGGACTAGGACGACCGATTGGGACACGGCAAACTAGGCTTGTAAGGCAAGGTTGTCCTCCTATTTGAACTGTTAGTCCTGCAGAAGCATTTGAAGCCCCTGCGTTTGCAGGACAGGGAGCACTGCCTTCACCGTTGTGCCCGCGACTTTCGGCACGGAATAGTTTTTAAGTTATATTTAGCTGCGGAGGGAGGTCTTCGATGTCCGCCGGAATAGAGACACTTGTTTTAACGCCGGCTCTTTCCTCTCAGGCACAAAGGGCTCCAACTAGAACGCCAACTTCTCGACCTCCTGTAGGACCTCTTTCGCCTTTAAAGCTTGGCCTTTGTTTTATAGCGACTACCACTAGGCCTAGGTCTGGGCAGCAAAGAGGACGGCGTTCGCAAGCGCCTCCCCAGGGGCAAATTAGGGAGAATGCCAAGGCCCTTACGCCATCAACGACCACGCACGCACTGCTAAAACTTTCGCAAAAAACTGAGATTAAAAGTCTAGCTAGTCCACAAGCTCCAACTGTTTCTGCTTCTATTTAATCACTTCAGAAGCAAGTTTCCCTGTGAATGGCAACGCCCACTTAATTTATTCGACCGGCTGTTGTAGCGATAGCCGGGATTATACCGCCCCCAATTAATAAAAAGGCTAGTTAAACTCAGTTAAAATGAGCCACTTGTCCAACGTTAACCATAAGAACTTCTCGTTAGTGACTGGATACCGCTCTTGAAAAAGAAATTGGACGGCTTCAAGCTGCCATGATGGTATGTCTAG</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>ATGGGAATTCCCGCAGACAACCTGCAGTCTCCTGCTAAAGCATCCTTCGATACCCCTGTATCTGCAGCGGAATTGGCACTCGCGCGCGGGGTCGTTCCGTCTCTGGCGAACGGTGAAGAACTCCTTTATCGCAATCCAGACCCAGAAAACGGTGATCCCTCCTTCATCGTTTCATTTACGAAGGGCCTTCCGAACGACGATAACGGTGCGATCATTGATCCGGATGACTTTCTGGCTTTTGTCCCTGCCATAAATTCCGGTGACGAAAAAGAAATTGCCGATCTGACCCTAGGCCCAGCCCCTGATCCGGACACAGGTCTACCGATTTTGCGCTCTGATCTCGCTAACTCGCTGGAACTGGAGGTGCCTGGATTGGAAAATTCTTCTGCGGGCCTCACCTTTGATTTGGAAGGTCCTGATGCGCAGTCCATCGCAATGCCACCGGCGCCGGTGCTGACGTCGCCTGAACTGATTGCTGAGATCGCAGAACTGTACCTGATGGCGCTGGGTCGCGAGATCGAATTTTCAGAGTTTGACTCCCCAAAAAATGCTGAATATATCCAGTTCGCGATTGACCAACTGAATGGCCTGGAATTGTTCAATACTCCGGCAATGCTGGGCGACCCTCCGGCAGAAATCCGCCGACCTCCTGGTGAGGTGACGGTGGGCAACCTGTTCCCTGGGATTCTGCCGGGCTCCGAAGTAGGTCCTTACTTATCTCAGTATATTATTGTGGGTTCGAAACAAATCGGCTCAGCGACAGGCGGCAATAAAACCTTGGTATCTCCGAACGCGGCAGATGAATTTGATGGTGAAATTGCGTATGGGTCAATCACCATATCACAACGCGTGCGCATTGCCACTCCGGGTCCTGACTTTATGACCGATTTGAAAGTGTTCCTGGACGTTCAGGATGCGGCTGATTTTCGGGGTTTCGAATCATACGAACCGGGCGCACGCTTAATTCCTACCATCCGGGATCTGGCCACCTTGGTGAATTTCGATGCACTTTATGAAGCTTACCTGAATGCCTGTCTGATCTTACTGGCGAACCGCGTGCCATTCGATCCGAACATCCCGTTCCAGCAGGAGGACAAACTAGATAATCAAGATGTGTTTGTCAACTTCGGCGATGCCAACGTGTTGTCTTTGGTAACCGAAGTCGCGACCCCTGCACTCAAAGCAGTGCGGTACCAGAAATTTAACATCAATCGCCGCCTGCCTCCTGAAGCAACCGGCGGATTGATCTCGGTCAACAAAATTGCGGCCGAAAAGGGTGAATCTGTATTTCCCGAAGTCGATCTCGCGGTTGAAGAGCTGGAAGATATTTTGGAAAAAGCCGAAATTTCTAATCGCAAACAGAATATTGCAGATGGTGATCCAGATCCCGACCCCTCTTTTCTGCTGCCGCAAGCGTTCGCAGAAGGTTCGCCCTTTAACCCTTCTTATGGCTCCGGAAACGCCGTCGTCGCGGGCGCGTGCGTGACCATCCTGAAAGCGTTCTTTGACTCGAACTTTCAGATTGATCAGGTGTTTGAAGTAGATAAAGATGAAGACAAACTGGTTAAATCTTCATTCAAAGGCACACTGACTGTCGCGGGCGAACTCAACAAACTGGCAGATAACATTGCGATTGGACCTAATATGGCCGGCGTTAATTATTTTTCCGATCAGTTTGAATCTATTCTGTTGGGCGAACAAGTAGCCATCGGTATTCTGGAAGAACAGTCCCTGACCTACGGTGAGAACTTTTTCTTTAATCTGCCAAAATTCGATGGTACCACGATCCAGATT</t>
+          <t>ATGGGTATTCCGGCAGACAACCTGCAGTCACGCGCGAAAGCCTCTTTTGACACTCGAGTGTCGGCAGCTGAGCTGGCCCTGGCACGCGGCGTTGTGCCGTCGCTGGCTAACGGTGAGGAACTACTATACCCTAACCCGGATCCGGAAAATGGTGATCCGTCCTTTATTGTGTCTTTCACTAAAGGCCTGCCTAACGACGATAATGGTGCAATTATTGATCCGGATGATTTCCTGGCGTTTGTGCCTGCCATTAACTCCGGTGATGAAAAGGAAATCGCGGATCTGACCCTGGGCCCGGCACCTGACCCGGATACGGGTTTACCTATATTGCGCTCCGACCTAGCGAACTCGCTGGAACTCGAAGTGCGGGGATTGGAGAATTCGTCTGCAGGCCTCACATTTGATCTGGAAGGCCCGGATGCCCAGTCTATCGCGATGCCGCCTGCACCGGTACTGACGTCGCCCGAGCTGATTGCCGAGATCGCTGAGTTGTATCTCATGGCGCTCGGTCGAGAAATTGAATTTTCAGAATTCGATTCCCCGAAGAATGCAGAATACATTCAGTTCGCCATAGATCAGCTCAATGGACTTGAATTGTTTAACACTCCTGCGATGCTGGGCGACCCGCCTGCAGAGATTCCTCCTCCTCCTGGTGAAGTGACCGTAGGGAACCTGTTCCGCGGTATCCTGCCGGGTTCTGAAGTCGGCCCGTATCTGTCTCAGTACATTATTGTTGGTTCCAAACAGATCGGCTCAGCAACAGGGGGGAACAAAACGCTGGTGTCACCGAATGCGGCTGATGAATTCGACGGCGAAATTGCGTATGGCTCGATCACCATTTCCCAGCCTGTGCGGATTGCCACACCGGGTCCTGACTTTATGACCGACCTGAAAGTTTTTTTAGATGTTCAGGACGCAGCGGACTTCCGCGGGTTCGAATCTTATGAGCCAGGTGCGCGCCTGATCCCTACCATCCCTGATCTAGCTACATTGGTGAACTTTGATGCGTTATATGAAGCCTACCTGAATGCGTGCCTGATCCTGCTGGCTAACCCTGTGCCGTTTGATCCGAACATTCCGTTCCAACAGGAGGATAAACTTGACAATCAGGACGTCTTCGTAAACTTCGGGGACGCAAACGTCCTGTCCCTCGTGACGGAAGTGGCAACACGGGCGCTGAAAGCCGTGCCTTATCAAAAATTCAATATAAATCGACGCCTCCCTCCAGAAGCTACAGGCGGCCTTATCTCTGTGAACAAAATTGCGGCCGAGAAAGGAGAGTCCGTGTTTCCCGAGGTTGATCTTGCGGTTGAAGAGCTGGAGGACATCCTGGAGAAAGCGGAAATTTCGAACCGGAAACAAAATATCGCTGATGGTGATCCGGATCCAGACCCGTCGTTTCTCCTGCCGCAAGCGTTCGCGGAGGGGTCCCCGTTTAATCCCTCTTACGGTTCCGGGAATGCGGTAGTTGCTGGTGCGTGCGTGACGATTTTGAAAGCGTTTTTTGACTCTAATTTTCAGATCGATCAGGTGTTCGAGGTTGACAAAGACGAAGATAAATTAGTGAAGTCTTCGTTCAAAGGGACACTTACCGTTGCGGGTGAATTAAATAAGCTGGCCGACAACATCGCTATCGGCCCTAATATGGCGGGGGTTAATTATTTTTCCGATCAATTTGAGTCAATTTTACTCGGTGAACAGGTTGCAATTGGTATTCTTGAAGAGCAATCACTGACCTATGGCGAGAACTTTTTCTTTAACCTGCCGAAGTTCGACGGTACTACCATACAGATC</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>ATGGGAATTCCCGC</t>
+          <t>ATGGGTATTCCGGC</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>AATCTGGATCGTGGTAC</t>
+          <t>GATCTGTATGGTAGTACCG</t>
         </is>
       </c>
     </row>
@@ -1144,12 +1144,12 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>TACCGCAGGGTCATATTAGGAAAGTGCCTTCGCATGTTGCACGCGGACCTTCGACGATGGGACCGGTTTTTGGGAGGCTTGGGCTATTTGAATCGCTTGTGGCTCCTTGACGCGATAGGAGCCGGCAAGCTGACACTTAAGGGACCGGTCGGAAGCTTATAGCGGAGGATATGTTTCCCGGACGGATTGCTAGGGTTTTGGCCGGAGGACTAATTTGGCTTACTAAAAGTCTGGAAATAGGGACGTGACCTACGCCCCCTGCTTAAAAGTTAGGGACTTCAGGGAGACCCAGGCGTCTAGGGCCTCGGCGCCAAATAGAGCCCATAACGCAGCTGTGGCTTCCGACTACCTAGGGGGTGGCTGCAAGGACGCAACCTCAGATACCGCCGACCCTTGTGAATACCAGACCTTCCGGGGCTGCGCGTCCGTCACTGGTACGGTGGGCGTGGTCGGGACCTGAGATTCCTTGACCAGATACTTTAAAGACTTAGAATGAACTACCGAGACCATGCCCTGCACGGGAAGTGGGGAAAGCTGCTACTACAACACGGACTGCGTCACGGAAGCGACTTGGTCTGGCTTAACTAAGGAAAGGACCGCTTCCCGCCTGGCGACGGAGGGAGGGAGAGCCTGCGTGTTGGATTTGCGGACGGATTTGGTAAGTGCTAACTATGTCATAAAGCGCCGCACTGCTTTCCACTGGACCTTCCAGGTATAGACAGGGTCAAGTACGAATAGCCCTTGAGTCCGTAGCGGTTGCCCTTATTTTAGCTTCTACCCAAACACGTTATGCCGCGATTGGGACACCTAGTCTTTCACGGACGACAGCTTCTACCCGCGCTAATGTACTGGTGCAAGTTTAGTAAGCAGCTACATGTCTTACCGCGCCTGCAAGCGCCGGGACTTCAAATAAGACTGCCTAAGGGAAAGTAGTGCTGGGGAGGACTAAACTGATGCATACACTTGAAGCTACGTGACATGGTCCGGATGGACTTGCGTACAGACTAAGATGACCCATACTTTCACGGCAAACTATTTCCGAACGGCAAAGTCGACCTACTGCTGCAACTATTTGTTGTCTGGAAACGCTGTAAACCGCCGGGTTTGTAGGACAGAAATCACTGGCTTCAGCGTTGAGCGCGAGACTTTCGCCACGCGAAAGTCTTCATGTTGCAATTGGCGGGAGAGGCGGGCCTTCGCCAACCGCCAGACTAACTCATAATGTTATTATTGGGGCTAAGGCTTTAACAGCGTCCACAGTTCGGTAATATGCTTCGAGACCTATTTCTGTACGACTTGGCGCATAGTTACTTATTGCTTAGTGTCTTGTTTGACACGCTACCACTGCAGGGAGGATACAGTCTGAAGCTTCTGCCACTTAGAAGCCGATGTGCTGACGACGGCTACCGTAAGGGTCTCCCGAGAGGCTACTTAGGGAGAATACCACGTCCATTGCGCCGCCAGCGACCCCGCACGCAATGACAGGACTTTCGCAAGAAACTATTACCGATACTTGACGGATACGACCTACTTTTGCCGTTATACCAGGGGAAACGGAAGCAGGGCTGCGCGCTACCGGTCAGAAATTTTTTGCACTAGAGTCTCATACCTTTGTTTGGTAATTGGCACCTTCCCCTTGACTTGTTTCAGACGAGGTTGTAAAGTTAGCCCGCCTTAAACCGCCCGCACTTGATAAAGTGGCTAATAGCGCTTAGGTAATGGAATCCGCTCTTTTAACGATAGCCGTAAGAGCTTCTCGTTTTTGAATGAATGCCGCTTTTGAAAAGTTACTGGCACGGCGAGAAACTACCATGACAAATAGCCTAT</t>
+          <t>TACCGCAGGGTCATATTAGCTAAATGACTTCGTATGTTGCAAGGAGACCTCCGCCGCTGTGAACGCTTTTTAGCGGGCTTGGGTTAGTTGGACCGCTTGTGGCTCCTTGACGCCATGGCGGCGGGGAAGCTAACACTTAAGGGACCAGTCGGAAGCTTGTAACGGAGGATGTGCTTTCCAAACGGCTTGCTAGGCTTTTGCCCGAATAACTAATTTGGGTTACTGAAGGTCTGGAAGTAAGCTCGTGACCTGCGCCCGCTGCTCAAGAGTTAAGGACTTCATGGCGACCCAGGGGTTTAAGGTCTCGGCGCGAAGTAAAGGCCGTAGCGCAGCTGGGGGTTTCGACTACCGAGCGGATGGCTACACGGACGAAACCTTAGATACCGTCGACCTTTATGCATGCCCGAACTTCCGGGCCTGCGCGTCCGCCAATGTTACGGAGGCCGAGGCCGGGAACTAAGATTCCTTGACCAAATACTTTAGAGACTTAGGATAAACTACCGAGAGCAAGGACTGCAAGGCAAATGGGGAAAGCTACTACTACACCACGCCCTACGCCATGGAAGCGACTTAGTCTGCCTCAACTAGGCGAAGGACCGGTTCCCGCCAGGTAATGGTGGTAGAAACAGGCTGCGCGTTGCGTTTGGAGACGCTTTTGGCAAATGATAGCTATGGCACAAAGGACCACAATGATTTCCACTGGACCTTCCGGGCATGGACAGAGTCAAATACGACTAACCATTAAGGCCATAACGTTTACCATTGTTTTAGCTCCTACCGAAACAAGTTATGCCGCGGTTAGCGCATCTGGTTTTTCAAGCGCGACAACTTCTACCAGGACTGATGTACTGCTGGAAATTTAGTAAACAGCTGCAAGTCTTACCGCGCCTACAAGGACCGGCGCTTCAAATGAGGCTACCAAAAGCGAAGTAGTGCTGTGGCGCCCTGGATTGCTGGATGCATTTGAAACTACGCGAAATGGTTCGTATGAATTTGCGGACGGAATAGGAAGACCCATACTTTCAGGGAAAGCTGTTTCCGGACGGTAAGGTCAACCTACTGCTGCACCTATTTGTCGTCTGTAAACGCTGCAAACCGCCTGGATTGTAAGACAGGAACCAATGGCTTCAACGATGGGCTCGGGACTTCCGGCACGCGAAGGTCTTTATATTGCAATTGGCTGCGGACGGAGGCCTTCGCCACCCACCGAACTAACTCATAATATTATTGTTGGGTCTGAGCCTCTAGCAGCGGCCGCAGTTTGGCGACATACTCCGAGAGCTATTCCTATACGACTTAGGACAAAGATACTTGTTACTTAGTGTTTTATTTGACACACTGCCGCTACAAGGGGCGTACAGACTGAAGCTCCTACCCCTCAGCAGGCGCTGTGGAGACGACGGCTACCGCAAAGGACTCCCGAGCGGTTACTTGGGAAGTATGCCACGACCGTTGCGCCGTCACCGGCCGCGCACGCATTGACAAGAATTTCGCAAAAAGCTGTTACCGATACTTGAGGCGTACGACCTACTCTTGCCGTTATACCACGGTAAACGCAAGCATGGATGGGGACTGCCGGTTAGAGACTTTTTGCAGTAAAGTCTCATACCGTTGTTTGGCGACTGGCACCTTCCTCTTGACTTGTTTCAGACGAGATTGTAAAGGTAGCCGGGATTGAACCGCCCGCACTTAATGAAGTGGCTGATAGCGCTCAGATATTGTGACCCGCTTTTTTAACGTTAGCCGTAAGACCTTCTTGTCTTCGACTGAATACCACTTTTGAAAAGTTACTGGCAAGGTAATAAGCTACCTTGGCACATAGGATAA</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>ATGGCGTCCCAGTATAATCCTTTCACGGAAGCGTACAACGTGCGCCTGGAAGCTGCTACCCTGGCCAAAAACCCTCCGAACCCGATAAACTTAGCGAACACCGAGGAACTGCGCTATCCTCGGCCGTTCGACTGTGAATTCCCTGGCCAGCCTTCGAATATCGCCTCCTATACAAAGGGCCTGCCTAACGATCCCAAAACCGGCCTCCTGATTAAACCGAATGATTTTCAGACCTTTATCCCTGCACTGGATGCGGGGGACGAATTTTCAATCCCTGAAGTCCCTCTGGGTCCGCAGATCCCGGAGCCGCGGTTTATCTCGGGTATTGCGTCGACACCGAAGGCTGATGGATCCCCCACCGACGTTCCTGCGTTGGAGTCTATGGCGGCTGGGAACACTTATGGTCTGGAAGGCCCCGACGCGCAGGCAGTGACCATGCCACCCGCACCAGCCCTGGACTCTAAGGAACTGGTCTATGAAATTTCTGAATCTTACTTGATGGCTCTGGTACGGGACGTGCCCTTCACCCCTTTCGACGATGATGTTGTGCCTGACGCAGTGCCTTCGCTGAACCAGACCGAATTGATTCCTTTCCTGGCGAAGGGCGGACCGCTGCCTCCCTCCCTCTCGGACGCACAACCTAAACGCCTGCCTAAACCATTCACGATTGATACAGTATTTCGCGGCGTGACGAAAGGTGACCTGGAAGGTCCATATCTGTCCCAGTTCATGCTTATCGGGAACTCAGGCATCGCCAACGGGAATAAAATCGAAGATGGGTTTGTGCAATACGGCGCTAACCCTGTGGATCAGAAAGTGCCTGCTGTCGAAGATGGGCGCGATTACATGACCACGTTCAAATCATTCGTCGATGTACAGAATGGCGCGGACGTTCGCGGCCCTGAAGTTTATTCTGACGGATTCCCTTTCATCACGACCCCTCCTGATTTGACTACGTATGTGAACTTCGATGCACTGTACCAGGCCTACCTGAACGCATGTCTGATTCTACTGGGTATGAAAGTGCCGTTTGATAAAGGCTTGCCGTTTCAGCTGGATGACGACGTTGATAAACAACAGACCTTTGCGACATTTGGCGGCCCAAACATCCTGTCTTTAGTGACCGAAGTCGCAACTCGCGCTCTGAAAGCGGTGCGCTTTCAGAAGTACAACGTTAACCGCCCTCTCCGCCCGGAAGCGGTTGGCGGTCTGATTGAGTATTACAATAATAACCCCGATTCCGAAATTGTCGCAGGTGTCAAGCCATTATACGAAGCTCTGGATAAAGACATGCTGAACCGCGTATCAATGAATAACGAATCACAGAACAAACTGTGCGATGGTGACGTCCCTCCTATGTCAGACTTCGAAGACGGTGAATCTTCGGCTACACGACTGCTGCCGATGGCATTCCCAGAGGGCTCTCCGATGAATCCCTCTTATGGTGCAGGTAACGCGGCGGTCGCTGGGGCGTGCGTTACTGTCCTGAAAGCGTTCTTTGATAATGGCTATGAACTGCCTATGCTGGATGAAAACGGCAATATGGTCCCCTTTGCCTTCGTCCCGACGCGCGATGGCCAGTCTTTAAAAAACGTGATCTCAGAGTATGGAAACAAACCATTAACCGTGGAAGGGGAACTGAACAAAGTCTGCTCCAACATTTCAATCGGGCGGAATTTGGCGGGCGTGAACTATTTCACCGATTATCGCGAATCCATTACCTTAGGCGAGAAAATTGCTATCGGCATTCTCGAAGAGCAAAAACTTACTTACGGCGAAAACTTTTCAATGACCGTGCCGCTCTTTGATGGTACTGTTTATCGGATA</t>
+          <t>ATGGCGTCCCAGTATAATCGATTTACTGAAGCATACAACGTTCCTCTGGAGGCGGCGACACTTGCGAAAAATCGCCCGAACCCAATCAACCTGGCGAACACCGAGGAACTGCGGTACCGCCGCCCCTTCGATTGTGAATTCCCTGGTCAGCCTTCGAACATTGCCTCCTACACGAAAGGTTTGCCGAACGATCCGAAAACGGGCTTATTGATTAAACCCAATGACTTCCAGACCTTCATTCGAGCACTGGACGCGGGCGACGAGTTCTCAATTCCTGAAGTACCGCTGGGTCCCCAAATTCCAGAGCCGCGCTTCATTTCCGGCATCGCGTCGACCCCCAAAGCTGATGGCTCGCCTACCGATGTGCCTGCTTTGGAATCTATGGCAGCTGGAAATACGTACGGGCTTGAAGGCCCGGACGCGCAGGCGGTTACAATGCCTCCGGCTCCGGCCCTTGATTCTAAGGAACTGGTTTATGAAATCTCTGAATCCTATTTGATGGCTCTCGTTCCTGACGTTCCGTTTACCCCTTTCGATGATGATGTGGTGCGGGATGCGGTACCTTCGCTGAATCAGACGGAGTTGATCCGCTTCCTGGCCAAGGGCGGTCCATTACCACCATCTTTGTCCGACGCGCAACGCAAACCTCTGCGAAAACCGTTTACTATCGATACCGTGTTTCCTGGTGTTACTAAAGGTGACCTGGAAGGCCCGTACCTGTCTCAGTTTATGCTGATTGGTAATTCCGGTATTGCAAATGGTAACAAAATCGAGGATGGCTTTGTTCAATACGGCGCCAATCGCGTAGACCAAAAAGTTCGCGCTGTTGAAGATGGTCCTGACTACATGACGACCTTTAAATCATTTGTCGACGTTCAGAATGGCGCGGATGTTCCTGGCCGCGAAGTTTACTCCGATGGTTTTCGCTTCATCACGACACCGCGGGACCTAACGACCTACGTAAACTTTGATGCGCTTTACCAAGCATACTTAAACGCCTGCCTTATCCTTCTGGGTATGAAAGTCCCTTTCGACAAAGGCCTGCCATTCCAGTTGGATGACGACGTGGATAAACAGCAGACATTTGCGACGTTTGGCGGACCTAACATTCTGTCCTTGGTTACCGAAGTTGCTACCCGAGCCCTGAAGGCCGTGCGCTTCCAGAAATATAACGTTAACCGACGCCTGCCTCCGGAAGCGGTGGGTGGCTTGATTGAGTATTATAATAACAACCCAGACTCGGAGATCGTCGCCGGCGTCAAACCGCTGTATGAGGCTCTCGATAAGGATATGCTGAATCCTGTTTCTATGAACAATGAATCACAAAATAAACTGTGTGACGGCGATGTTCCCCGCATGTCTGACTTCGAGGATGGGGAGTCGTCCGCGACACCTCTGCTGCCGATGGCGTTTCCTGAGGGCTCGCCAATGAACCCTTCATACGGTGCTGGCAACGCGGCAGTGGCCGGCGCGTGCGTAACTGTTCTTAAAGCGTTTTTCGACAATGGCTATGAACTCCGCATGCTGGATGAGAACGGCAATATGGTGCCATTTGCGTTCGTACCTACCCCTGACGGCCAATCTCTGAAAAACGTCATTTCAGAGTATGGCAACAAACCGCTGACCGTGGAAGGAGAACTGAACAAAGTCTGCTCTAACATTTCCATCGGCCCTAACTTGGCGGGCGTGAATTACTTCACCGACTATCGCGAGTCTATAACACTGGGCGAAAAAATTGCAATCGGCATTCTGGAAGAACAGAAGCTGACTTATGGTGAAAACTTTTCAATGACCGTTCCATTATTCGATGGAACCGTGTATCCTATT</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1159,7 +1159,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>TATCCGATAAACAGTACCAT</t>
+          <t>AATAGGATACACGGTTCC</t>
         </is>
       </c>
     </row>
@@ -1186,22 +1186,22 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>TACCGCAGAGTCATGTTAGCGAAATGGCTTCGAATATTACACGCGGACCTTCGTCGGTGCGACCGATTTTTAGCGGGGTTAGGATAGTTAGAACGGTTATGACTTCTCGACGGAATGGCCGCGGGGAAGCTAACGCTCAAGGGCCCCGTTGGCAGATTGTAGCGCAGCATGTGCTTTCCCAACGGCTTGCTGGGCTTCTGGCCCGACGACTAATTTGGTTTACTAAAAGTTTGAAAATAAGCGCGTGACCTACGACCACTACTTAAAAGCTAAGCGCTCCATGGCGACCCGGGCGTCTAGGGCCTTGGTGCGAAGTAGAGTCCTTAACGTAGGTGTGGCTTCCGCCTACCGAGAGGGTGCCTACATGCGCGTAACCTCAGGTACCGACGACCGTTGTGGATACTGAACCTTCCAGGACTGCGGTTACGCCACTGGTACGGAGGCCGGGGGCGCGATCTGAGTTTTCTCGACCAAATACTTTAAAGACTCAGGATGAACTACCGTGACCACGGACTACAGGGCAAGTGGGGAAAACTACTGCTGCACCACGCTCTACGGCACGGAAGAGAGTTGGTTTGGCTTAACTAGGCGAAAGAGCGCTTCCCACCAGGCAACGGCGGCAGAGACAGACTACGGGTCGGATTTGGAGAAGGATTTGGAAAATGCTAACTATGGCATAAAGGACCACAATGTTTCCCGCTAAATCTTCCGGGCATAGATAGGGTTAAATACGACTATCCGTTGAGGCCATAGCGGTTGCCGTTATTTTAGCTTCTACCAAAGCATGTTATGCCGCGCTTGGCGCAACTAGTCTTCCATGCGCGTCACCTTCTACCCGGACTGATGTACTGTTGGAAGTTTAGTAAGCAGCTGCACGTCTTGCCACGGCTACAAGCGCCGGCCCTCCACATGAGTCTACCAAAGGCGAAGTAGTGCTGAGGCGGACTAAACTGGTGGATACAATTAAAGCTACGGGACATAGTCCGGATAGACTTGCGCACGAACTATAACGAGCCCTACTTCCAAGGCAAGCTGTTCCCCGAGGGCAAAGTCGAGCTACTGCTGCACCTATTTGTCGTCTGAAAGCGCTGAAAGCCGCCAGGCTTGTAAAACAGAAACCAATGGCTTCAGCGCTGAGGACGAGAGTTTCGGCAAGGAAAAGTTTTTATGTTGCAATTGGCGGGAAACGCGGGTCTCCGCCAACCACCCGACTAACTTATGATATTATTATTGGGCCTAAGCCTCTAACAGCGCCCACACTTTGGTAACATACTTCGGGAACTATTTCTATACGACTTGGCGCACAGATACTTGTTACTCAGCGTCTTGTTTAATACGCTACCTCTACAGGGCGCCTACAGGCTAAAGCTTCTGCCACTCAGAAGCCGCTGTGCGAACGACGGTTACCGCAAAGGCCTCCCAAGAGGCTACTTGGGCAGAATACCGCGCCCTTTACGACGGCACCGGCCGCGTACACACTGTCACGACTTTCGCAAGAAACTGTTACCGATACTTGACGCGTACGGCCTGCTTTTGCCGTTGTACCATGGTAAACGGAAACAAGGCTGCGCTCTGCCAGTCAGAAATTTTTTGCACTAAAGACTCATGCCGTTGTTTGGTGAATGGCAACTTCCGCTTGACTTGTTTCAAACAAGGTTGTATAGATAACCCGCGTTGAACCGCCCACAGTTGATGAAATGGCTGATGGCGCTCAGATAATGGGATCCGCTTTTTTAGCGGTAACCGTAAGACCTTCTCGTCTTTGACTGTATACCACTTTTAAAAAGGTACTGGCACGGCGACAAACTACCGTGTCAAATAGCCTAA</t>
+          <t>TACCGAAGCGTTATGTTGGGAAAGTGGCTCCGCATATTGCAGGCTGACCTTCGGCGTTGCGACCGCTTTTTAGGAGGATTGGGGTAGTTGGACCGGTTGTGGCTTCTTAACGCGATGGGAGCGGGCAAACTAACACTTAAGGGCCCGGTCGGTAGATTGTAGCGTAGAATGTGTTTTCCAGACGGTTTGCTGGGCTTTTGCCCGGACGAGTAATTTGGCTTGCTGAAGGTCTGGAAATAGGGACGCGAACTACGTCCCCTGCTTAAGAGCTAAGCGCTCCAAGGCAATCCAGGCGTCTAAGGCCTTGGCGCCAAATAGAGCCCATATCGTAGATGGGGTTTTCGTCTACCAAGAGGCTGTCTACACGCGCGTAACCTCAGATACCGTCGCCCGTTGTGTATACTGGACCTTCCGGGTCTGCGCTTGCGCCAATGATACGGCGGCCGGGGCCGCGACCTAAGCTTTCTTGACCAGATACTTTAGAGGCTTAGCATGAACTACCGGGACCAGGGACTGCATGGAAAGTGCGCGAAACTGCTACTACAACAGGCGCTACGCCACGGAAGGGAGTTAGTCTGACTTAACTAAGCGAAGGACCGCTTTCCACCAGGCGACGGCGGGAGCAACAGGCTACGGGTCGCGTTTGCGAACGCGTTCGGTAAGTGCTAGCTGTGGCACAAGGCGCCCCATTGGTTCCCACTAGAGCTTCCAGGCATAAACAGAGTCAAGTACGAATAGCCCTTAAGGCCGTAACGTTTGCCATTATTCTAGCTTCTGCCAAAGCAGGTCATGCCACGCTTGGGACAGCTAGTTTTCCACGGACGCCAGCTCCTACCGGGACTAATATACTGGTGCAAATTTAGAAAGCAACTGCACGTCTTGCCACGCCTGCACGGACCGGCGCTTCACATGAGCCTGCCAAAGGGAAAATAGTGTTGCGGTGCCCTAGACTGGTGAATACATTTAAAACTGCGCGACATAGTCCGGATGAATTTGCGGACAGACTAAGACGAACCATACTTTCAGGGCAAACTGTTTCCGGACGGTAAGGTTGACCTACTGCTACATCTGTTTGTCGTCTGGAAGCGTTGCAAACCTCCTGGCTTGTAGGACAGCAATCAATGGCTTCAACGCTGGGCGCGAGACTTTCGGCATGGAAAAGTTTTTATGTTGCAGTTGGCGGCGGATGGAGGCCTCCGACACCCGCCGAATTAACTCATGATATTGTTGTTAGGCCTAAGTCTTTAGCAACGGCCACATTTTGGGAATATACTCCGAGACCTATTCCTATACAACTTGGCGCATAGGTACTTGTTGCTTAGAGTCTTGTTTGACACACTACCACTACACGGCGCCTACAGCCTAAAACTTCTGCCGCTTAGAAGACGCTGAGGAGACGACGGCTACCGAAAAGGCCTTCCGAGAGGCTACTTGGGCAGGATACCGCGGCCGTTGCGCCGCCATCGGCCGCGCACGCAATGGCAAGAGTTTCGTAAGAAGCTGTTACCAATACTTGACGCCTACGGCCTGCTTTTACCGTTATACCAAGGTAAGCGGAAACAAGGCTGGGCTCTACCAGTCAGCGACTTTTTACAGTAGAGACTTATGCCGTTGTTCGGCGAGTGCCAGCTTCCGCTTGACTTGTTTCAAACGAGATTGTAAAGGTAACCAGGATTAAACCGTCCGCACTTAATAAAATGGCTGATGGCGCTCAGTTAGTGCGAACCGCTCTTTTAACGGTAACCGTAAGACCTTCTTGTTTTTGAGTGCATGCCACTTTTAAAAAGCTACTGCCAAGGCGACAAGCTACCATGTCACATAGGATAA</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>ATGGCGTCTCAGTACAATCGCTTTACCGAAGCTTATAATGTGCGCCTGGAAGCAGCCACGCTGGCTAAAAATCGCCCCAATCCTATCAATCTTGCCAATACTGAAGAGCTGCCTTACCGGCGCCCCTTCGATTGCGAGTTCCCGGGGCAACCGTCTAACATCGCGTCGTACACGAAAGGGTTGCCGAACGACCCGAAGACCGGGCTGCTGATTAAACCAAATGATTTTCAAACTTTTATTCGCGCACTGGATGCTGGTGATGAATTTTCGATTCGCGAGGTACCGCTGGGCCCGCAGATCCCGGAACCACGCTTCATCTCAGGAATTGCATCCACACCGAAGGCGGATGGCTCTCCCACGGATGTACGCGCATTGGAGTCCATGGCTGCTGGCAACACCTATGACTTGGAAGGTCCTGACGCCAATGCGGTGACCATGCCTCCGGCCCCCGCGCTAGACTCAAAAGAGCTGGTTTATGAAATTTCTGAGTCCTACTTGATGGCACTGGTGCCTGATGTCCCGTTCACCCCTTTTGATGACGACGTGGTGCGAGATGCCGTGCCTTCTCTCAACCAAACCGAATTGATCCGCTTTCTCGCGAAGGGTGGTCCGTTGCCGCCGTCTCTGTCTGATGCCCAGCCTAAACCTCTTCCTAAACCTTTTACGATTGATACCGTATTTCCTGGTGTTACAAAGGGCGATTTAGAAGGCCCGTATCTATCCCAATTTATGCTGATAGGCAACTCCGGTATCGCCAACGGCAATAAAATCGAAGATGGTTTCGTACAATACGGCGCGAACCGCGTTGATCAGAAGGTACGCGCAGTGGAAGATGGGCCTGACTACATGACAACCTTCAAATCATTCGTCGACGTGCAGAACGGTGCCGATGTTCGCGGCCGGGAGGTGTACTCAGATGGTTTCCGCTTCATCACGACTCCGCCTGATTTGACCACCTATGTTAATTTCGATGCCCTGTATCAGGCCTATCTGAACGCGTGCTTGATATTGCTCGGGATGAAGGTTCCGTTCGACAAGGGGCTCCCGTTTCAGCTCGATGACGACGTGGATAAACAGCAGACTTTCGCGACTTTCGGCGGTCCGAACATTTTGTCTTTGGTTACCGAAGTCGCGACTCCTGCTCTCAAAGCCGTTCCTTTTCAAAAATACAACGTTAACCGCCCTTTGCGCCCAGAGGCGGTTGGTGGGCTGATTGAATACTATAATAATAACCCGGATTCGGAGATTGTCGCGGGTGTGAAACCATTGTATGAAGCCCTTGATAAAGATATGCTGAACCGCGTGTCTATGAACAATGAGTCGCAGAACAAATTATGCGATGGAGATGTCCCGCGGATGTCCGATTTCGAAGACGGTGAGTCTTCGGCGACACGCTTGCTGCCAATGGCGTTTCCGGAGGGTTCTCCGATGAACCCGTCTTATGGCGCGGGAAATGCTGCCGTGGCCGGCGCATGTGTGACAGTGCTGAAAGCGTTCTTTGACAATGGCTATGAACTGCGCATGCCGGACGAAAACGGCAACATGGTACCATTTGCCTTTGTTCCGACGCGAGACGGTCAGTCTTTAAAAAACGTGATTTCTGAGTACGGCAACAAACCACTTACCGTTGAAGGCGAACTGAACAAAGTTTGTTCCAACATATCTATTGGGCGCAACTTGGCGGGTGTCAACTACTTTACCGACTACCGCGAGTCTATTACCCTAGGCGAAAAAATCGCCATTGGCATTCTGGAAGAGCAGAAACTGACATATGGTGAAAATTTTTCCATGACCGTGCCGCTGTTTGATGGCACAGTTTATCGGATT</t>
+          <t>ATGGCTTCGCAATACAACCCTTTCACCGAGGCGTATAACGTCCGACTGGAAGCCGCAACGCTGGCGAAAAATCCTCCTAACCCCATCAACCTGGCCAACACCGAAGAATTGCGCTACCCTCGCCCGTTTGATTGTGAATTCCCGGGCCAGCCATCTAACATCGCATCTTACACAAAAGGTCTGCCAAACGACCCGAAAACGGGCCTGCTCATTAAACCGAACGACTTCCAGACCTTTATCCCTGCGCTTGATGCAGGGGACGAATTCTCGATTCGCGAGGTTCCGTTAGGTCCGCAGATTCCGGAACCGCGGTTTATCTCGGGTATAGCATCTACCCCAAAAGCAGATGGTTCTCCGACAGATGTGCGCGCATTGGAGTCTATGGCAGCGGGCAACACATATGACCTGGAAGGCCCAGACGCGAACGCGGTTACTATGCCGCCGGCCCCGGCGCTGGATTCGAAAGAACTGGTCTATGAAATCTCCGAATCGTACTTGATGGCCCTGGTCCCTGACGTACCTTTCACGCGCTTTGACGATGATGTTGTCCGCGATGCGGTGCCTTCCCTCAATCAGACTGAATTGATTCGCTTCCTGGCGAAAGGTGGTCCGCTGCCGCCCTCGTTGTCCGATGCCCAGCGCAAACGCTTGCGCAAGCCATTCACGATCGACACCGTGTTCCGCGGGGTAACCAAGGGTGATCTCGAAGGTCCGTATTTGTCTCAGTTCATGCTTATCGGGAATTCCGGCATTGCAAACGGTAATAAGATCGAAGACGGTTTCGTCCAGTACGGTGCGAACCCTGTCGATCAAAAGGTGCCTGCGGTCGAGGATGGCCCTGATTATATGACCACGTTTAAATCTTTCGTTGACGTGCAGAACGGTGCGGACGTGCCTGGCCGCGAAGTGTACTCGGACGGTTTCCCTTTTATCACAACGCCACGGGATCTGACCACTTATGTAAATTTTGACGCGCTGTATCAGGCCTACTTAAACGCCTGTCTGATTCTGCTTGGTATGAAAGTCCCGTTTGACAAAGGCCTGCCATTCCAACTGGATGACGATGTAGACAAACAGCAGACCTTCGCAACGTTTGGAGGACCGAACATCCTGTCGTTAGTTACCGAAGTTGCGACCCGCGCTCTGAAAGCCGTACCTTTTCAAAAATACAACGTCAACCGCCGCCTACCTCCGGAGGCTGTGGGCGGCTTAATTGAGTACTATAACAACAATCCGGATTCAGAAATCGTTGCCGGTGTAAAACCCTTATATGAGGCTCTGGATAAGGATATGTTGAACCGCGTATCCATGAACAACGAATCTCAGAACAAACTGTGTGATGGTGATGTGCCGCGGATGTCGGATTTTGAAGACGGCGAATCTTCTGCGACTCCTCTGCTGCCGATGGCTTTTCCGGAAGGCTCTCCGATGAACCCGTCCTATGGCGCCGGCAACGCGGCGGTAGCCGGCGCGTGCGTTACCGTTCTCAAAGCATTCTTCGACAATGGTTATGAACTGCGGATGCCGGACGAAAATGGCAATATGGTTCCATTCGCCTTTGTTCCGACCCGAGATGGTCAGTCGCTGAAAAATGTCATCTCTGAATACGGCAACAAGCCGCTCACGGTCGAAGGCGAACTGAACAAAGTTTGCTCTAACATTTCCATTGGTCCTAATTTGGCAGGCGTGAATTATTTTACCGACTACCGCGAGTCAATCACGCTTGGCGAGAAAATTGCCATTGGCATTCTGGAAGAACAAAAACTCACGTACGGTGAAAATTTTTCGATGACGGTTCCGCTGTTCGATGGTACAGTGTATCCTATT</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>ATGGCGTCTCAGTACA</t>
+          <t>ATGGCTTCGCAATACA</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>AATCCGATAAACTGTGCC</t>
+          <t>AATAGGATACACTGTACCA</t>
         </is>
       </c>
     </row>
@@ -1228,22 +1228,22 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>TACCGGAGGGTCATATTGGCGAAGTGGCTCCGGATGTTACAAGCGAATCTTCGGCGTTGGGACCGGTTTTTGGCGGGCTTGGGTTAGTTGAACCGCTTGTGGCTCCTTGAAGCGATGGCTGGAGGCAAACTAACGCTTAAGGGGCCGGTCGGCAGCTTGTAACGCAGGATGTGGTTCCCGAATGGATTACTGGGCTTTTGACCGGACGACTAATTTGGGTTGCTAAAAGTCTGCAAGTAAGGACGAGACCTACGCCCGCTGCTTAAAAGATATGGACTTCACGGTGACCCGGGCGTCTAAGGCCTTGGCGCGAAATAGAGGCCATATCGCAGGTGCGGTTTCCGGCTACCAAGAGGTTGGCTACAAGCGCGCAACCTCAGTTACCGGCGCCCGTTGTGGATGCTAAACCTTCCAGGACTACGCTTGCGGCAATGATACGGCGGGCGGGGTCGCGAACTGAGATTTCTTGACCAAATGCTTTAGAGTCTTAGGATGAACTACCGCGACCATGCTCTACACGGCAAGTGGGGAAAGCTACTGCTACAGCAAGCTCTACGGCACGCCAGGGACTTGGTCTGACTTAACTAGGGAAAAGACCGTTTCCCGCCGGGCGAAGGCGGCAGCAATAGTCTACGCGTCGCGTTTGGAGAGGGATTCGGAAAGTGATAACTGTGCCAAAAGGGACCGCATTGGTTCCCGCTGAATCTTCCGGGCATAGACAGTGTCAAATACAACTAACCATTGAGACCATAACGTTTGCCGTTGTTTTAGCTTCTACCAAAGCAAGTCATGCCCCGCTTGGGACATCTGGTCTTCCAGGCGCGGCAACTTCTACCGGGACTAATATACTGCTGGAAATTTAGTAAACAGCTACACGTCTTGCCACGGCTGCAAGCGCCTGCCCTTCAGATGAGACTACCAAAGGGAAAATAATGGTGGGGAGCTCTAGAACGGTGTATACATTTGAAACTGCGTGACATAGTCCGAATAGACTTGCGTACGGACTAGGACGACCCGTACTTTCATGGAAAACTGTTTCCGGACGGCAAGGTCGACCTACTGCTACAACTGTTTGTCGTCTGGAAACGATGAAAGCCACCAGGTTTATAGGACAGAGACCAATGGCTTCATCGTTGAGGACGTGACTTTCGGCAAGGAAAAGTCTTCATGTTGCATTTGGCGGGAGACGCGGGCCTCCGACATCCGCCGGACTAACTTATGATATTGTTATTGGGCCTAAGGCTTTAGCAACGTCCACAATTTGGGGAGATGCTCCGGGACCTATTTCTATACGACTTGGGACACAGATACTTGTTACTCAGAGTTTTGTTCAACACACTGCCACTGCATGGCGCTTACAGGCTGAAGCTTCTGCCGCTCAGTAGACGCTGGGGAGACGACGGCTACCGCAAAGGCCTTCCGAGAGGTTACTTAGGCAGGATACCGCGACCTTTGCGTCGACATCGGCCGCGCACGCATTGACAAGACTTCCGCAAAAAGCTATTACCATTGCTCGACGGATACGGTCTGCTCTTGCCTTTGTACCACGGTAAGCGCAAACATGGGTGCGGACTACCGGTTAGGGACTTTTTGCACTAAAGACTTATGCCGTTATTCGGCGACTGTCATCTTCCGCTCGAATTGTTTCAGACGAGGTTATAAAGCTATCCGGCGTTGAACCGACCGCAGTTGATGAAGTGTCTAATAGCGCTTAGCTAGTGCAACCCGCTCTTTTAGCGCTAACCATATGAACTTCTCGTCTTTGAATGTATGCCGCTTTTGAAAAGATACTGCCACGGTGACAAACTGCCATGGCACATGGCTTAA</t>
+          <t>TACCGCAGAGTTATATTAGGAAAATGCCTTCGCATGTTGCAGGGAGAGCTTCGCCGGTGTGACCGCTTCTTAGGAGGATTGGGCTAATTGAATCGTTTGTGGCTTCTTGAGGCGATGGCGGCGGGCAAGCTAACGCTCAAGGGACCTGTTGGCAGATTGTAGCGCAGGATGTGTTTTCCTGACGGATTGCTAGGCTTTTGGCCTGACGACTAATTTGGATTACTAAAGGTCTGAAAATAGGGACGAGAACTGCGACCGCTGCTTAAGAGATAGGCGCTTCAAGGCAATCCCGGCGTCTAAGGCCTCGGCGGAAAATAAAGGCCGTAGCGGAGATGGGGCTTTCGTCTGCCGAGTGGATGCCTACAGGGACGAAACCTTAGCTACCGACGCCCGTTGTGGATACTAGACCTCCCAGGCCTGCGTTTGCGCCACTGGTACGGCGGCCGTGGGCGCGACCTAAGTTTCCTTAACCATATGCTTTAAAGCCTTAGTATAAACTACCGCAACCACGGACTGCAAGGCAAATGGGCCAAGCTGCTACTACAGCAAGGACTGCGACAGGGAAGAGACTTAGTCTGGCTTAACTAAGCGAAAGACCGCTTTCCTCCGGGTAATGGAGGCAGTGACAGCCTACGAGTCGGATTTGGAGACGCGTTTGGAAAATGCTAGCTATGTCACAAAGGACCACAGTGGTTTCCACTAGACCTTCCGGGCATGGACAGTGTCAAGTACGACTATCCGTTGAGACCCTAGCGATTGCCATTGTTTTAGCTTCTACCGAAGCACGTTATGCCACGATTGGCCCAGCTGGTCTTTCAAGCGCGACAACTCCTACCGGGACTGATATACTGGTGAAAATTTAGCAAACAACTACAGGTCTTGCCGCGCCTACAAGCGCCGGCGCTCCATATGAGGCTACCGAAGGGAAAATAGTGGTGTGGCGCGCTAGACCGTTGGATACATTTAAAACTGCGTAATATGGTCCGAATGAATTTGCGGACGGAATATGACGAACCATACTTTCATGGCAAGCTATTTCCGGACGGAAAAGTTGACCTACTACTGCACCTATTCGTCGTCTGGAAGCGGTGGAAGCCACCAGGGTTGTAGGACAGCAATCAATGGCTCCAGCGTTGGGGACGCGACTTTCGGCACGGAAAAGTCTTTATATTACACTTGGCGGCCGACGGAGGACTTCGCCAACCGCCGAATTAGCTTATAATATTGTTGTTGGGCCTAAGCCTTTATCACCGCCCTCAATTTGGCGACATGCTTCGAGACCTGTTTCTGTACAATTTAGCGCACAGTTACTTATTGCTTAGAGTTTTATTTGAGACGCTACCCCTGCACGGCGGATACAGACTGAAGCTCCTACCGCTTAGGAGGCGATGCGCGAACGACGGCTACCGCAAGGGCCTCCCCAGAGGCTACTTGGGCAGGATGCCACGCCCGTTGCGGCGGCACCGACCGCGGACGCATTGACAAGACTTTCGAAAGAAGCTGTTGCCGTTACTTGAGGGATACGGCCTACTTTTGCCATTGTACCAAGGTAAACGCAAGCACGGCTGTGCGCTGCCAGTCAGGAACTTCTTGCACTAGAGGCTTATACCGTTGTTTGGCGACTGGCAGCTTCCACTTAATTTATTTCAAACGAGATTGTAAAGGTAGCCAGCGTTGAACCGCCCACACTTGATGAAATGGCTGATAGCCCTCAGGTAGTGCGACCCACTCTTTTAACGTTAGCCGTAAGAGCTTCTTGTCTTTGACTGAATACCCCTTTTAAAGAGTTACTGGCAAGGAAATAAACTGCCATGCCAGATGGCGTAA</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>ATGGCCTCCCAGTATAACCGCTTCACCGAGGCCTACAATGTTCGCTTAGAAGCCGCAACCCTGGCCAAAAACCGCCCGAACCCAATCAACTTGGCGAACACCGAGGAACTTCGCTACCGACCTCCGTTTGATTGCGAATTCCCCGGCCAGCCGTCGAACATTGCGTCCTACACCAAGGGCTTACCTAATGACCCGAAAACTGGCCTGCTGATTAAACCCAACGATTTTCAGACGTTCATTCCTGCTCTGGATGCGGGCGACGAATTTTCTATACCTGAAGTGCCACTGGGCCCGCAGATTCCGGAACCGCGCTTTATCTCCGGTATAGCGTCCACGCCAAAGGCCGATGGTTCTCCAACCGATGTTCGCGCGTTGGAGTCAATGGCCGCGGGCAACACCTACGATTTGGAAGGTCCTGATGCGAACGCCGTTACTATGCCGCCCGCCCCAGCGCTTGACTCTAAAGAACTGGTTTACGAAATCTCAGAATCCTACTTGATGGCGCTGGTACGAGATGTGCCGTTCACCCCTTTCGATGACGATGTCGTTCGAGATGCCGTGCGGTCCCTGAACCAGACTGAATTGATCCCTTTTCTGGCAAAGGGCGGCCCGCTTCCGCCGTCGTTATCAGATGCGCAGCGCAAACCTCTCCCTAAGCCTTTCACTATTGACACGGTTTTCCCTGGCGTAACCAAGGGCGACTTAGAAGGCCCGTATCTGTCACAGTTTATGTTGATTGGTAACTCTGGTATTGCAAACGGCAACAAAATCGAAGATGGTTTCGTTCAGTACGGGGCGAACCCTGTAGACCAGAAGGTCCGCGCCGTTGAAGATGGCCCTGATTATATGACGACCTTTAAATCATTTGTCGATGTGCAGAACGGTGCCGACGTTCGCGGACGGGAAGTCTACTCTGATGGTTTCCCTTTTATTACCACCCCTCGAGATCTTGCCACATATGTAAACTTTGACGCACTGTATCAGGCTTATCTGAACGCATGCCTGATCCTGCTGGGCATGAAAGTACCTTTTGACAAAGGCCTGCCGTTCCAGCTGGATGACGATGTTGACAAACAGCAGACCTTTGCTACTTTCGGTGGTCCAAATATCCTGTCTCTGGTTACCGAAGTAGCAACTCCTGCACTGAAAGCCGTTCCTTTTCAGAAGTACAACGTAAACCGCCCTCTGCGCCCGGAGGCTGTAGGCGGCCTGATTGAATACTATAACAATAACCCGGATTCCGAAATCGTTGCAGGTGTTAAACCCCTCTACGAGGCCCTGGATAAAGATATGCTGAACCCTGTGTCTATGAACAATGAGTCTCAAAACAAGTTGTGTGACGGTGACGTACCGCGAATGTCCGACTTCGAAGACGGCGAGTCATCTGCGACCCCTCTGCTGCCGATGGCGTTTCCGGAAGGCTCTCCAATGAATCCGTCCTATGGCGCTGGAAACGCAGCTGTAGCCGGCGCGTGCGTAACTGTTCTGAAGGCGTTTTTCGATAATGGTAACGAGCTGCCTATGCCAGACGAGAACGGAAACATGGTGCCATTCGCGTTTGTACCCACGCCTGATGGCCAATCCCTGAAAAACGTGATTTCTGAATACGGCAATAAGCCGCTGACAGTAGAAGGCGAGCTTAACAAAGTCTGCTCCAATATTTCGATAGGCCGCAACTTGGCTGGCGTCAACTACTTCACAGATTATCGCGAATCGATCACGTTGGGCGAGAAAATCGCGATTGGTATACTTGAAGAGCAGAAACTTACATACGGCGAAAACTTTTCTATGACGGTGCCACTGTTTGACGGTACCGTGTACCGAATT</t>
+          <t>ATGGCGTCTCAATATAATCCTTTTACGGAAGCGTACAACGTCCCTCTCGAAGCGGCCACACTGGCGAAGAATCCTCCTAACCCGATTAACTTAGCAAACACCGAAGAACTCCGCTACCGCCGCCCGTTCGATTGCGAGTTCCCTGGACAACCGTCTAACATCGCGTCCTACACAAAAGGACTGCCTAACGATCCGAAAACCGGACTGCTGATTAAACCTAATGATTTCCAGACTTTTATCCCTGCTCTTGACGCTGGCGACGAATTCTCTATCCGCGAAGTTCCGTTAGGGCCGCAGATTCCGGAGCCGCCTTTTATTTCCGGCATCGCCTCTACCCCGAAAGCAGACGGCTCACCTACGGATGTCCCTGCTTTGGAATCGATGGCTGCGGGCAACACCTATGATCTGGAGGGTCCGGACGCAAACGCGGTGACCATGCCGCCGGCACCCGCGCTGGATTCAAAGGAATTGGTATACGAAATTTCGGAATCATATTTGATGGCGTTGGTGCCTGACGTTCCGTTTACCCGGTTCGACGATGATGTCGTTCCTGACGCTGTCCCTTCTCTGAATCAGACCGAATTGATTCGCTTTCTGGCGAAAGGAGGCCCATTACCTCCGTCACTGTCGGATGCTCAGCCTAAACCTCTGCGCAAACCTTTTACGATCGATACAGTGTTTCCTGGTGTCACCAAAGGTGATCTGGAAGGCCCGTACCTGTCACAGTTCATGCTGATAGGCAACTCTGGGATCGCTAACGGTAACAAAATCGAAGATGGCTTCGTGCAATACGGTGCTAACCGGGTCGACCAGAAAGTTCGCGCTGTTGAGGATGGCCCTGACTATATGACCACTTTTAAATCGTTTGTTGATGTCCAGAACGGCGCGGATGTTCGCGGCCGCGAGGTATACTCCGATGGCTTCCCTTTTATCACCACACCGCGCGATCTGGCAACCTATGTAAATTTTGACGCATTATACCAGGCTTACTTAAACGCCTGCCTTATACTGCTTGGTATGAAAGTACCGTTCGATAAAGGCCTGCCTTTTCAACTGGATGATGACGTGGATAAGCAGCAGACCTTCGCCACCTTCGGTGGTCCCAACATCCTGTCGTTAGTTACCGAGGTCGCAACCCCTGCGCTGAAAGCCGTGCCTTTTCAGAAATATAATGTGAACCGCCGGCTGCCTCCTGAAGCGGTTGGCGGCTTAATCGAATATTATAACAACAACCCGGATTCGGAAATAGTGGCGGGAGTTAAACCGCTGTACGAAGCTCTGGACAAAGACATGTTAAATCGCGTGTCAATGAATAACGAATCTCAAAATAAACTCTGCGATGGGGACGTGCCGCCTATGTCTGACTTCGAGGATGGCGAATCCTCCGCTACGCGCTTGCTGCCGATGGCGTTCCCGGAGGGGTCTCCGATGAACCCGTCCTACGGTGCGGGCAACGCCGCCGTGGCTGGCGCCTGCGTAACTGTTCTGAAAGCTTTCTTCGACAACGGCAATGAACTCCCTATGCCGGATGAAAACGGTAACATGGTTCCATTTGCGTTCGTGCCGACACGCGACGGTCAGTCCTTGAAGAACGTGATCTCCGAATATGGCAACAAACCGCTGACCGTCGAAGGTGAATTAAATAAAGTTTGCTCTAACATTTCCATCGGTCGCAACTTGGCGGGTGTGAACTACTTTACCGACTATCGGGAGTCCATCACGCTGGGTGAGAAAATTGCAATCGGCATTCTCGAAGAACAGAAACTGACTTATGGGGAAAATTTCTCAATGACCGTTCCTTTATTTGACGGTACGGTCTACCGCATT</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>ATGGCCTCCCAGT</t>
+          <t>ATGGCGTCTCAATATAATC</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>AATTCGGTACACGGTAC</t>
+          <t>AATGCGGTAGACCG</t>
         </is>
       </c>
     </row>
@@ -1270,22 +1270,22 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>TACCGGCGACCGTTGTGGATACTAAACCTCCCGGGCCTACGCTTACGGCATTGGTACGGAGGCGGCGGGCGGAATCTAAGTTTTCTCAATCAGATGCTTTAGAGACTCAGGATGAACTACCGGAATCAAGGACTGCACGGCAAGTGGGCGAAGCTGCTGCTACACCATGGACTACGCCAAGGAAGCGACTTAGTCTGTCTTAACTAAGGAAAAGACCGCTTTCCGCCTGGGGACGGCGGCAGAGAAAGGCTGCGCGTCGCCTTTGCGGAAGCGTTTGGCAAGTGGTAACTGTGGCAAAAGGGACCACATTGGTTTCCGCTGGACCTCCCAGGTATGGAAAGAGTTAAATACGACTAGCCATTGAGGCCCTAACGGTTGCCATTATTTTAACTCCTGCCCAAACATGTTATGCCCCGCTTGGCTCAACTAGTCTTTCGAATAGACTTGCGTACGGACTAAGACGACCCATACTTTCAAGGCAAGCTATTTCCGGACGGCAAGGTCGAGCTACTACTGCATCTGTTTGTCGTCTGGAAACGATGGAAGCCACCAGGCTTGTAAGACAGGGACCAGTGCCTTCACCGATGCGGACGCGACTTTCGCCACGGAAAGGTTTTTATATTGCATTTAGGAGGAGAAGCGGGACTTCGACAGCCTCCAGACTAACTTATGATGTTGTTGTTAGGTCTAAGCCTTTAACATCGCCCCCACTTTGGCGACATACTTCGCGACCTATTCCTATACGATTTGGCCCACAGCTACTTGTTGCTTAGCGTCTTGTTTGACACACTACCTCTACACGGCGCGTACAGACTAAAACTCCTGCCGCTTAGGAGCCGGTGCGGAGACGACGGTTACCGGAAGGGCCTTCCCAGAGGCTACTTGGGCAGTATGCCGCGACCGTTGCGCCGTCAACGTCCACGGACACAATGTCACGACTTTCGTAAGAAGCTATTACCAATGCTTAACGCGTACGGTCTACTTTTACCGTTATACCAAGGTAAACGTAAGCACGGCTGGGGACTACCGGTCAGTAATTTCTTGCAATAGAGGCTTATGCCGTTGTTTGGCAATTGCCAACTTCCGCTTAACTTGTTTCAAACAAGATTGTAGAGTTAGCCGGGATTAAACCGCCCCCATTTGATAAAATGGCTAATAGGACTCAGATAGTGGGGAGCGTTTCTGACGCTAAACTTGGACCCGCCATGTCTTTGACTATAGAAC</t>
+          <t>TACCGTCGTCCATTGTGCATGCTAAATCTCCCGGGTCTGCGCTTGCGTCAGTGCTACGGCGGTGGCGGTCGCGACCTAAGGTTTCTTGACCACATGCTTTAAAGGCTCAGTATAAACTACCGCAATCAGGGACTACATGGCAAATGGGCTAAGCTACTACTGCATCATGCCCTGCGCCAGGCGAGAGACTTAGTTTGGCTTAACTAAGCTAAGAATCGGTTCCCACCAGGCGACGGTGGCAGAGACAGACTGCGTGTTGGATTTGCGGAAGCGTTTGGCAAGTGGTAGCTATGTCAAAAAGCGCCGCACTGATTTCCGCTAGACCTTCCGGGCATGGAGAGTGTCAAATACGACTAACCGTTAAGACCGTAGCGATTGCCCTTGTTCTAACTTCTACCAAAACAGGTCATGCCGCGATTGGGACAACTAGTCTTTCGCATAGACTTGCGTACGGACTAAAATGACCCCTACTTCCAGGGAAAACTGTTTCCAAACGGCAAAGTTAATCTGCTACTACATCTATTTGTTGTCTGTAAGCGATGAAAACCGCCGGGCTTGTAAGACAGCGACCAATGTCTCCATCGCTGGGCGCGAGACTTTCGGCACGCCAAGGTCTTTATATTACAATTGGCCGGAGACGCGGGGCTTCGACAACCGCCAGACTAGCTTATGATATTATTATTGGGCCTGAGGCTCTAGCACCGGCCGCAATTCGGCGACATACTCCGAGACCTATTTCTATACAATTTGGGACAAAGATACTTATTACTCAGGGTTTTATTTGACACGCTGCCGCTGCACGGCGCGTACAGCCTGAAGCTCCTGCCGCTTAGGAGACGCTGCGGAGACGAGGGTTACCGCAAGGGTCTTCCCAGCGGCTACTTAGGCAGCATACCACGACCATTACGGCGTCACCGGCCGCGGACGCAATGGCAGGACTTTCGAAAGAAACTATTGCCCATACTTGATGGATACGGTCTGCTTTTGCCGTTGTACCAGGGGAAGCGCAAGCAAGGCTGGGCGCTGCCCGTCAGTGACTTTTTACACTAAAGACTTATGCCGTTGTTTGGAAACTGGCACCTTCCCCTTGACTTGTTCCACACGAGTTTGTAGAGTTAGCCGGCGTTGAACCGCCCGCACTTGATAAAATGGCTGATGGCGCTTAGATAGTGCGCGGGATTTCTAACGCTAAACTTGAATCCACCATGGCTCTGCCTATAAAAC</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>ATGGCCGCTGGCAACACCTATGATTTGGAGGGCCCGGATGCGAATGCCGTAACCATGCCTCCGCCGCCCGCCTTAGATTCAAAAGAGTTAGTCTACGAAATCTCTGAGTCCTACTTGATGGCCTTAGTTCCTGACGTGCCGTTCACCCGCTTCGACGACGATGTGGTACCTGATGCGGTTCCTTCGCTGAATCAGACAGAATTGATTCCTTTTCTGGCGAAAGGCGGACCCCTGCCGCCGTCTCTTTCCGACGCGCAGCGGAAACGCCTTCGCAAACCGTTCACCATTGACACCGTTTTCCCTGGTGTAACCAAAGGCGACCTGGAGGGTCCATACCTTTCTCAATTTATGCTGATCGGTAACTCCGGGATTGCCAACGGTAATAAAATTGAGGACGGGTTTGTACAATACGGGGCGAACCGAGTTGATCAGAAAGCTTATCTGAACGCATGCCTGATTCTGCTGGGTATGAAAGTTCCGTTCGATAAAGGCCTGCCGTTCCAGCTCGATGATGACGTAGACAAACAGCAGACCTTTGCTACCTTCGGTGGTCCGAACATTCTGTCCCTGGTCACGGAAGTGGCTACGCCTGCGCTGAAAGCGGTGCCTTTCCAAAAATATAACGTAAATCCTCCTCTTCGCCCTGAAGCTGTCGGAGGTCTGATTGAATACTACAACAACAATCCAGATTCGGAAATTGTAGCGGGGGTGAAACCGCTGTATGAAGCGCTGGATAAGGATATGCTAAACCGGGTGTCGATGAACAACGAATCGCAGAACAAACTGTGTGATGGAGATGTGCCGCGCATGTCTGATTTTGAGGACGGCGAATCCTCGGCCACGCCTCTGCTGCCAATGGCCTTCCCGGAAGGGTCTCCGATGAACCCGTCATACGGCGCTGGCAACGCGGCAGTTGCAGGTGCCTGTGTTACAGTGCTGAAAGCATTCTTCGATAATGGTTACGAATTGCGCATGCCAGATGAAAATGGCAATATGGTTCCATTTGCATTCGTGCCGACCCCTGATGGCCAGTCATTAAAGAACGTTATCTCCGAATACGGCAACAAACCGTTAACGGTTGAAGGCGAATTGAACAAAGTTTGTTCTAACATCTCAATCGGCCCTAATTTGGCGGGGGTAAACTATTTTACCGATTATCCTGAGTCTATCACCCCTCGCAAAGACTGCGATTTGAACCTGGGCGGTACAGAAACTGATATCTTG</t>
+          <t>ATGGCAGCAGGTAACACGTACGATTTAGAGGGCCCAGACGCGAACGCAGTCACGATGCCGCCACCGCCAGCGCTGGATTCCAAAGAACTGGTGTACGAAATTTCCGAGTCATATTTGATGGCGTTAGTCCCTGATGTACCGTTTACCCGATTCGATGATGACGTAGTACGGGACGCGGTCCGCTCTCTGAATCAAACCGAATTGATTCGATTCTTAGCCAAGGGTGGTCCGCTGCCACCGTCTCTGTCTGACGCACAACCTAAACGCCTTCGCAAACCGTTCACCATCGATACAGTTTTTCGCGGCGTGACTAAAGGCGATCTGGAAGGCCCGTACCTCTCACAGTTTATGCTGATTGGCAATTCTGGCATCGCTAACGGGAACAAGATTGAAGATGGTTTTGTCCAGTACGGCGCTAACCCTGTTGATCAGAAAGCGTATCTGAACGCATGCCTGATTTTACTGGGGATGAAGGTCCCTTTTGACAAAGGTTTGCCGTTTCAATTAGACGATGATGTAGATAAACAACAGACATTCGCTACTTTTGGCGGCCCGAACATTCTGTCGCTGGTTACAGAGGTAGCGACCCGCGCTCTGAAAGCCGTGCGGTTCCAGAAATATAATGTTAACCGGCCTCTGCGCCCCGAAGCTGTTGGCGGTCTGATCGAATACTATAATAATAACCCGGACTCCGAGATCGTGGCCGGCGTTAAGCCGCTGTATGAGGCTCTGGATAAAGATATGTTAAACCCTGTTTCTATGAATAATGAGTCCCAAAATAAACTGTGCGACGGCGACGTGCCGCGCATGTCGGACTTCGAGGACGGCGAATCCTCTGCGACGCCTCTGCTCCCAATGGCGTTCCCAGAAGGGTCGCCGATGAATCCGTCGTATGGTGCTGGTAATGCCGCAGTGGCCGGCGCCTGCGTTACCGTCCTGAAAGCTTTCTTTGATAACGGGTATGAACTACCTATGCCAGACGAAAACGGCAACATGGTCCCCTTCGCGTTCGTTCCGACCCGCGACGGGCAGTCACTGAAAAATGTGATTTCTGAATACGGCAACAAACCTTTGACCGTGGAAGGGGAACTGAACAAGGTGTGCTCAAACATCTCAATCGGCCGCAACTTGGCGGGCGTGAACTATTTTACCGACTACCGCGAATCTATCACGCGCCCTAAAGATTGCGATTTGAACTTAGGTGGTACCGAGACGGATATTTTG</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>ATGGCCGCTGGCA</t>
+          <t>ATGGCAGCAGGTAAC</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>CAAGATATCAGTTTCTGTACCGC</t>
+          <t>CAAAATATCCGTCTCGGT</t>
         </is>
       </c>
     </row>
@@ -1312,22 +1312,22 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>TACCTATTAATATGGTTGCAAGTCAAGCTAAACCGAGCGGGATTACGTCGTAAGCTGCAAGCGGAAGGACGCCGCCAGGTCAGTGCGCTACGGAGCATAAGTCCGCTACTGCCATTGCAATGATTGCCGCTACTCCGGGGAAAAGGTTGGTGGGACGACCCGTGGAAGTGCTTTCCTGAGGGTTTAAGCGACGGTAACCGCGAGGGCTGGCTAGGAAGGCGCAAGCTACGCAAACATAGTCCCCAATTGTGGCCACTGGACCTGTGATAATTTAGATAGGGTGAGCCTGGCCTAGGTCTCCCGCTATTGAGTAAAAGTAGTAGCCGCTACTGGTGCCCACGTTTTCACGGACCGAACCTTAGCTACCGACGACCAGACCGGAAGTGGGAGCTCCGCGGGCTAGGCGTTGGACAGTGGTACGGAGGCCGGGGGGTCTAGCTAAGTCAGCTTGACCCTATACTTGACAGCCTTAGGATAAACTACCGCGACACAGCCCTATAGCGTAAATGGCTTAAGCTGTTGAGGCTATGGCAACGGCTCCGGCGACGCAGATACCGTCGATTGCGCAACCATCGCCTCCTACCCACGCTGGTCGACCCCCTTGACTGTGGCTGGGTCTGCCGTTTAGCCCTTAATCTCTACTTTTTACCGCTTCCTTAATGTGTTCCGTGCTAAAAGGGACCAAGAGACTTGCCGCTGTTGTAACCGGGCATGAACAGTGTCAAAGAGGATTAGCCGACGCTATGGGACCCAAGGGCGAAGAGGTTTCTACTAGGACTTAGGATAAACTGCCCATTGTAGGCGAAACCTCGATTGGCCTAGCTAGTTGCGCATGCGTTTCGCCACGGTCTGGCTCTAATATACTGCTGGAACCCGCGCATGTAGCTACACCGATTACCGCGTCTGCAAGCGCCTGGACTTAGTATACAATGGCGACTTCCACTATTGAAGTTACTACTCCTTTGATTAGCGAAGTAGTTGTGGGGAGGACTGAATCGTTGGATGCAATTGATGCTACGCAACATAGTCGGAATGTAATTGCGCACGGAGGACTACGATCGTTACCCTTAGCTCATACTACGCCCAGACGGCAAACCACTACTTCTGCTTCAGCTATTTGTTTGACCAAAACGGGACAAACCGCCGGGCTTATAGGACAGCGACAACCGCCTTCAACATGACTTTCGGAATTTTCGGCACGCGAAAGTCTTTAAACGCTACTTGGCGGCGCGAGGAGGTCTCTGACAGCGCCCAAACTAGCTAACACATGTTGCGGGTGGATGCAGCCTACTCGTCCTCCCGTTGCTCCCAGTCTGTCAAAAGTTTGGCTAGCTTTTTAATACGGTCATGCACCTAAGGCTAAACGATGTCTTTCAAGGACTTTTATTGCAATGTGTTTTATTGTGGGTCTACCTGGCCCTATAACGAGCGGACATACTAATACTGGGCCAGCTATGTCAACGTCTAACGAGACGTCTCGTCGTTCTTCTTGTCTGGCTTCTACTCCCAGTCGTTGTCGTTGTCCCGCCCTGCATAAACGACGGCTACCGTATGCGACTCCCCAGCGGCTACTTGGGGCGAATACCACGCCCGTTACGCTGGCATCGGCCGCGGACATGGTGCTAGGACTTTCGCAAGAAACTATGTTGAGTTTGAGACGGCATACGCAAATGGAGGTGGCTCCTGCCCTGGTTCAACTGGGTCTAGCTTCACCTACTCGGCAACTGCCAACTTCCACTTAACTTGTTCGAGACGAGCTTGTAAAGATAGCCGGCGTTGAACCGACCACAGTTAAACTTCAGGCTGATATGGCTTAGCTAGTTTGAACCACTTCTTTAACGATAGCCAGAGGACGGACTTGTCTTTTTGCAGATAAGACTCCTAAAAAGATACTGCTAGGGTGACAAGCTACCCAGGACACAATGGCAT</t>
+          <t>TACCTATTGATGTGATTACAAGTCAAACTAAACCGCGCGGGATTGCGACGGAAACTACAAGGAGACGGACGGCGTCACGTTAGCGCGCTGCGGAGAATAAGGCCGCTACTACCCTTACAATGTTTGCCACTGCTCCGTGCGAAGGGATGGTGGGACAATCCATGGAAATGGTTTCCAAACGGCTTGAGCGAGGGCAACCGGGAGGGCTGACTAGCTAGTCGGAAGCTACGGAAGCACAGCCCGCAATTATGGCCGCTAAATCTGTGGTAATTTAGGTAGGGCGAACCGGGACTGGGCCTTCCACTATTAAGTAAAAGTAGCAGCCGCTACTGGTGCCCCCGCTTTCACGCGCCGAACCTCAGCTACCGGCGTCCAGACCGGAAGTGCGAGCTCCGTGGACTGGGCGTTGCGCATTGGTACGGTGGCCGCGGCGTTTAGCTAAGTCAGCTTGACCCTATACTCAACAGTCTTAGCATGAACTACCGCGACACGGCCCTATAACGAAAATGCCTCAAACTGTTGAGGCTGTGGCATCGACTTCGCCGCCGCAGATACCGTCGTTTACGTAACCACCGTCTTCTACCGACACTAGTTGACCCCCTTGACTGGGGCTGTGTCTGACGTTTGGGACTTGAGCTTTACTTCTTGCCGCTTCCGTAGTGAGTTCCGTGGTAGAAGGCGCCAAGTAACTTGCCACTGTTGTAACCAGGCATGGACAGAGTCAAGAATGAATAGCCGACGCTGTGTAACCCGAGAGCGAAAAGCTTTCTGCTAGGTCTTAGGATAGAGTGGCCGTTATAGGCGAAGCCACGTTTGGGATAACTAGTCGGACATGCGTTTCGTCAGGGCCTGGCGCTGATGTACTGATGTAACCCGCGAATATAGCTACAACGATTGCCACGCCTACACGGACCTGCGCTTAGTATACAGTGGCGTCTCCCCCTGTTAAAATTGCTACTTCTTTGATTGGCTAAATAGTTGTGTGGCGGACTGAATCGCTGTATACAATTAATGCTGCGTGACATGGTCGGTATATAATTACGCACGAATGACTACGAACGCTACCCCTAGCTCATGCTACGCCCTGACGGAAAACCCCTGCTTCTACTTCACCTGTTTGTCTGGCCGAAGCGGGATAAGCCGCCAGGTTTATAAGACAGGGATGAGCGGCTTCACCAAGACTTTCGAAATTTTCGACACGCGAAGGTCTTCAAACGCTACTTGGCGGGACGTGCTGGTCTCTGGCAGCGGCCGAACTAGCTAACACACGTCGCGGGCGCGTGCAGACTACTTGTCCTCCCCTTGCTTCCAGTTTGCCATAAATTTGGATAACTTTTTGAAACGGTCATACAACTAAGGCTAGACGACGTCTTTCAAGCGCTTTTGTTACACTGGGTCTTATTATGGGTCTACCTAGCGCTATAGCGGGGAGACATGCTGATACTAGGCCAACTATGCCAGCGTCTAACAAGACGCCTTGTCGTTCTTCTCGTCTGTCTTCTGCTTCCTGTCGTTGTCGTTGTCCCCCCCTGGATAAACGACGGCTACCGCATACGGCTCCCTAGCGGATACTTAGGCCGAATACCGCGCCCGTTACGCTGGCACCGGCCACGAACGTGGTGGTAGGACTTTCGCAAGAAGCTATGCTGCGTTTGGGAGGGAATGCGCAAGTGGAGTTGTCTCCTACCGTGGTTTGACTGTGTCTATCTCCACCTACTCGGTGAGTGGCAACTTCCACTCGAGTTATTTGACACGAGATTATATAGGTAACCAGGATTGAACCGCCCACACTTGAACTTTAGCCTAATATGGCTCAGATAATTTGACCCACTTCTTTAACGATAACCGGACGAAGGACTTGTTTTTTTGCACATGAGGCTCCTAAAAAGGTACTGATAAGGAAATAAACTGCCAAGCACACAGTGGCAT</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>ATGGATAATTATACCAACGTTCAGTTCGATTTGGCTCGCCCTAATGCAGCATTCGACGTTCGCCTTCCTGCGGCGGTCCAGTCACGCGATGCCTCGTATTCAGGCGATGACGGTAACGTTACTAACGGCGATGAGGCCCCTTTTCCAACCACCCTGCTGGGCACCTTCACGAAAGGACTCCCAAATTCGCTGCCATTGGCGCTCCCGACCGATCCTTCCGCGTTCGATGCGTTTGTATCAGGGGTTAACACCGGTGACCTGGACACTATTAAATCTATCCCACTCGGACCGGATCCAGAGGGCGATAACTCATTTTCATCATCGGCGATGACCACGGGTGCAAAAGTGCCTGGCTTGGAATCGATGGCTGCTGGTCTGGCCTTCACCCTCGAGGCGCCCGATCCGCAACCTGTCACCATGCCTCCGGCCCCCCAGATCGATTCAGTCGAACTGGGATATGAACTGTCGGAATCCTATTTGATGGCGCTGTGTCGGGATATCGCATTTACCGAATTCGACAACTCCGATACCGTTGCCGAGGCCGCTGCGTCTATGGCAGCTAACGCGTTGGTAGCGGAGGATGGGTGCGACCAGCTGGGGGAACTGACACCGACCCAGACGGCAAATCGGGAATTAGAGATGAAAAATGGCGAAGGAATTACACAAGGCACGATTTTCCCTGGTTCTCTGAACGGCGACAACATTGGCCCGTACTTGTCACAGTTTCTCCTAATCGGCTGCGATACCCTGGGTTCCCGCTTCTCCAAAGATGATCCTGAATCCTATTTGACGGGTAACATCCGCTTTGGAGCTAACCGGATCGATCAACGCGTACGCAAAGCGGTGCCAGACCGAGATTATATGACGACCTTGGGCGCGTACATCGATGTGGCTAATGGCGCAGACGTTCGCGGACCTGAATCATATGTTACCGCTGAAGGTGATAACTTCAATGATGAGGAAACTAATCGCTTCATCAACACCCCTCCTGACTTAGCAACCTACGTTAACTACGATGCGTTGTATCAGCCTTACATTAACGCGTGCCTCCTGATGCTAGCAATGGGAATCGAGTATGATGCGGGTCTGCCGTTTGGTGATGAAGACGAAGTCGATAAACAAACTGGTTTTGCCCTGTTTGGCGGCCCGAATATCCTGTCGCTGTTGGCGGAAGTTGTACTGAAAGCCTTAAAAGCCGTGCGCTTTCAGAAATTTGCGATGAACCGCCGCGCTCCTCCAGAGACTGTCGCGGGTTTGATCGATTGTGTACAACGCCCACCTACGTCGGATGAGCAGGAGGGCAACGAGGGTCAGACAGTTTTCAAACCGATCGAAAAATTATGCCAGTACGTGGATTCCGATTTGCTACAGAAAGTTCCTGAAAATAACGTTACACAAAATAACACCCAGATGGACCGGGATATTGCTCGCCTGTATGATTATGACCCGGTCGATACAGTTGCAGATTGCTCTGCAGAGCAGCAAGAAGAACAGACCGAAGATGAGGGTCAGCAACAGCAACAGGGCGGGACGTATTTGCTGCCGATGGCATACGCTGAGGGGTCGCCGATGAACCCCGCTTATGGTGCGGGCAATGCGACCGTAGCCGGCGCCTGTACCACGATCCTGAAAGCGTTCTTTGATACAACTCAAACTCTGCCGTATGCGTTTACCTCCACCGAGGACGGGACCAAGTTGACCCAGATCGAAGTGGATGAGCCGTTGACGGTTGAAGGTGAATTGAACAAGCTCTGCTCGAACATTTCTATCGGCCGCAACTTGGCTGGTGTCAATTTGAAGTCCGACTATACCGAATCGATCAAACTTGGTGAAGAAATTGCTATCGGTCTCCTGCCTGAACAGAAAAACGTCTATTCTGAGGATTTTTCTATGACGATCCCACTGTTCGATGGGTCCTGTGTTACCGTA</t>
+          <t>ATGGATAACTACACTAATGTTCAGTTTGATTTGGCGCGCCCTAACGCTGCCTTTGATGTTCCTCTGCCTGCCGCAGTGCAATCGCGCGACGCCTCTTATTCCGGCGATGATGGGAATGTTACAAACGGTGACGAGGCACGCTTCCCTACCACCCTGTTAGGTACCTTTACCAAAGGTTTGCCGAACTCGCTCCCGTTGGCCCTCCCGACTGATCGATCAGCCTTCGATGCCTTCGTGTCGGGCGTTAATACCGGCGATTTAGACACCATTAAATCCATCCCGCTTGGCCCTGACCCGGAAGGTGATAATTCATTTTCATCGTCGGCGATGACCACGGGGGCGAAAGTGCGCGGCTTGGAGTCGATGGCCGCAGGTCTGGCCTTCACGCTCGAGGCACCTGACCCGCAACGCGTAACCATGCCACCGGCGCCGCAAATCGATTCAGTCGAACTGGGATATGAGTTGTCAGAATCGTACTTGATGGCGCTGTGCCGGGATATTGCTTTTACGGAGTTTGACAACTCCGACACCGTAGCTGAAGCGGCGGCGTCTATGGCAGCAAATGCATTGGTGGCAGAAGATGGCTGTGATCAACTGGGGGAACTGACCCCGACACAGACTGCAAACCCTGAACTCGAAATGAAGAACGGCGAAGGCATCACTCAAGGCACCATCTTCCGCGGTTCATTGAACGGTGACAACATTGGTCCGTACCTGTCTCAGTTCTTACTTATCGGCTGCGACACATTGGGCTCTCGCTTTTCGAAAGACGATCCAGAATCCTATCTCACCGGCAATATCCGCTTCGGTGCAAACCCTATTGATCAGCCTGTACGCAAAGCAGTCCCGGACCGCGACTACATGACTACATTGGGCGCTTATATCGATGTTGCTAACGGTGCGGATGTGCCTGGACGCGAATCATATGTCACCGCAGAGGGGGACAATTTTAACGATGAAGAAACTAACCGATTTATCAACACACCGCCTGACTTAGCGACATATGTTAATTACGACGCACTGTACCAGCCATATATTAATGCGTGCTTACTGATGCTTGCGATGGGGATCGAGTACGATGCGGGACTGCCTTTTGGGGACGAAGATGAAGTGGACAAACAGACCGGCTTCGCCCTATTCGGCGGTCCAAATATTCTGTCCCTACTCGCCGAAGTGGTTCTGAAAGCTTTAAAAGCTGTGCGCTTCCAGAAGTTTGCGATGAACCGCCCTGCACGACCAGAGACCGTCGCCGGCTTGATCGATTGTGTGCAGCGCCCGCGCACGTCTGATGAACAGGAGGGGAACGAAGGTCAAACGGTATTTAAACCTATTGAAAAACTTTGCCAGTATGTTGATTCCGATCTGCTGCAGAAAGTTCGCGAAAACAATGTGACCCAGAATAATACCCAGATGGATCGCGATATCGCCCCTCTGTACGACTATGATCCGGTTGATACGGTCGCAGATTGTTCTGCGGAACAGCAAGAAGAGCAGACAGAAGACGAAGGACAGCAACAGCAACAGGGGGGGACCTATTTGCTGCCGATGGCGTATGCCGAGGGATCGCCTATGAATCCGGCTTATGGCGCGGGCAATGCGACCGTGGCCGGTGCTTGCACCACCATCCTGAAAGCGTTCTTCGATACGACGCAAACCCTCCCTTACGCGTTCACCTCAACAGAGGATGGCACCAAACTGACACAGATAGAGGTGGATGAGCCACTCACCGTTGAAGGTGAGCTCAATAAACTGTGCTCTAATATATCCATTGGTCCTAACTTGGCGGGTGTGAACTTGAAATCGGATTATACCGAGTCTATTAAACTGGGTGAAGAAATTGCTATTGGCCTGCTTCCTGAACAAAAAAACGTGTACTCCGAGGATTTTTCCATGACTATTCCTTTATTTGACGGTTCGTGTGTCACCGTA</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>ATGGATAATTATACCAACGTT</t>
+          <t>ATGGATAACTACACTAATGTTC</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>TACGGTAACACAGGAC</t>
+          <t>TACGGTGACACACGA</t>
         </is>
       </c>
     </row>
@@ -1354,22 +1354,22 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>TACCTTTTAATGTGGTTATAGGGCAAGCTGAACCGCGGAGGATTGCGTCGAAAGCTACAGGGAAATGCGTGACGACAAGTCAGGGGACTCCGTAGTATAAGCCCACTGCTACCATTGCACTGATTGCCACTACTTCGTGCGAAAGGGTGATGGGACGAACCGTGGAAATGCTTTCCAGACGGATTGAGTGACGGAGACCGCGACGGCTGCCTAGCCAGACGAAAGCTACGTAAGCAAAGACCACAGTTGTGCCCGCTAGACCTATGCTAGTTTAGTTAGGGTGACCCTGGCCTAGGCCTTCCACTGTTGAGAAAGAGAAGTAGGCGCTACTGATGGCCGCGGTTTCACGGACCTAACCTTAGATACCGTCGGCCCAACCGTAAATGAAACCTTCGGGGACTAGGCGTTGCGCAATGGTACGGGGGTCGAGGCGTTTAGCTGAGTCACCTTGACCCAATGCTTGACAGCCTCAGGATGAACTACCGCGACACAGGACTATAGCGCAAATGGCTTAAGCTATTAAGCCTATGGCACCGCCTCCGCCGACGGAGCTACCGACGCTTACGTAACCAGCGCCTTCTGCCGACACTGGTCGAACCGCTTGACTGTGGCTGCGTCTGACGTTTGGCGCTTGACCTTTACTTCTTGCCGCTTCCATAATGCGTCCCGTGGTAGAAGGGACCGAGCGAATTGCCACTGTTGTAACCAGGTATGGACAGAGTCAAGGACAACTAGCCAACGCTATGAGACCCAAGAGCGAAGAGCTTACTACTGGGCCTTAGAATGGACTGCCCCTTATAAGGAAAGCCGCGGTTGGCGTAACTGGTCGCGCACGCGTTTCGTCAAGGTCTAGGACTAATATACTGTTGGAACCCGCGCATGTAGCTACACCGTTTGCCGCGCCTGCAGGGACCAGGACTCAGGATGCAGTGGCGCCTTCCACTATTGAAGTTACTGCTCCTTTGCTTGGCGAAATAATTATGTGGCGCGCTAGAACGTTGGATACAATTGATACTGCGTGACATAGTTGGGATAAAGTTACGCACGGAGGACTACGACCGCTACCCATAACCGATACTACTCCCGGACGGAAAGCCACTGCTTCTACTTCACCTATTCGTTTGGCCAAAACGGGACAAGCCACCAGGCTTGTAGGACAGTGAGGATCGACTTCACCATGACTTTCGAGACTTTCGCCAAGCGAAAGTCTTTAAGCGGTACTTGGGAGGACGTGGAGGGCTTTGGCAACGTCCAAACTATCTAACGCACGTTGCGGGCGGATGTAGCCTGCTTGTCCTTCCATTACTTCCTGTCTGGCAGAAGTTTGGGTAGCTCTTTGAAACGGTCATACAACTAAGACTAAATAATGTTTTTCACGCGCTTTTGTTGCAGTGCGTTTTGTTGTGGGTCTACCTGGCGCTATAGTGGGGAAACTTGCTAATGCTAGGTCATCTACGTCAACGCCTAACGCGCCAGCTAGTCGTTGTCGTCCAAATGCTTGTCGTCGTTTGCCTTCTACTCGTTTTGCTTGTCGTCGTCGTTGTCGCTCCGCCGTGCATAGAGGACGGTTACCGCATACGCCTCCCCAGAGGCTACTTGGGCCGGATACCACGGCCGTTGCGATGGCAACGTCCACGCACATGGTGGTAGGACTTTCGTAAGAAACTATGCTGGGTTTTCAATGGCATACAAAAATGTAGATGGCTGCTACCTTGGTTTGACCAAGTCTAGCTACATCTGCTCGTCAATTGCCAACTTCCGCTTGACTTGTTTGACACAAGTTTGTAAAGATAGCCAGCGTTGAACCGACCCCACTTAAACTTTAGTCTAATGTGTCTTAGCTAGTTTGACCCACTTCTTTATCGATAGCCTGACGACGCGCTCGTCTTTTTGCACATATGGCTTACAAAAAGCTACTGATAAGGGGATAAGCTACCATGGACACATTGATAA</t>
+          <t>TACCTTTTAATGTGGTTGTAAGGAAAGCTAAACCGGGGAGCGTTGCGGCGGAAACTACACGCTGACGCCTGTCGACAGGTCAGTGGACTTCGCAGAATGAGGCCACTACTACCATTGCAATGGTTGCCACTGCTTCGGGGAAAAGGTTGGTGCGACGACCCGTGAAAATGATTTCCGAACGGTTTGAGGGACGGAGACCGGAATGGGTGCCTGGGAAGACGCAAACTGCGGAAGCACAGACCACACTTGTGCCCGCTAAATCTGTGTTAGTTTAGTTAGGGCGACCCGGGTCTAGGCCTCCCTCTATTGAGCAAAAGTAGCAGGCGTTACTGGTGGCCGCGCTTCCACGGACCGAACCTTAGCTACCGCCGCCCTGACCGGAAATGCAACCTTCGGGGCCTAGGCGTCGGACACTGCTACGGCGGCCGCGGCGTCTAACTAAGGCAGCTTGACCCCATGCTCGAAAGACTTAGTATGAACTACCGGGAGACAGCGCTATAACGGAAGTGGCTTAAGCTGTTAAGTCTATGCCAGCGCCTTCGACGGCGGAGATACCGGCGTTTGCGCAACCAGCGGCTCCTGCCTACACTGGTCGAGCCGCTTAATTGCGGCTGCGTTTGTCGCTTAGCGCTCGACCTCTACTTTTTGCCACTTCCCTAATGGGTCCCATGGTAAAAGGCGCCAAGTGAATTACCACTATTGTAGCCAGGTATGGACAGAGTTAAGGACGACTATCCTACACTATGCGACCCAAGAGCGAAAAGGTTACTACTAGGACTTAGTATGGACTGACCGTTGTAAGCCAAACCCCGGTTAGCGTATCTAGTTGCGCAGGCTTTCCGTCAAGGCCTGGGACTAATGTACTGTTGCAACCCCCGCATGTAACTACATCGTTTGCCGCGCCTGCAAGCGCCAGCCCTTAGTATACACTGCCGGCTTCCGCTATTAAAATTACTGCTTCTCTGGTTGGCCAAGTAATTGTGTGGCGGACTAGAACGATGTATACACTTAATGCTACGCGAGATAGTCGGCATGAAATTGCGTACGAATGACTACGACCGCTACCCATAACCAATGCTACTTCCAGATGGCAAGCCGCTACTTCTGCTTCATCTATTCGTTTGCCCGAAACGCAACAAACCACCAGGCTTATAAGACAGAGACGACCGTCTTCAACACGATTTTCGCAATTTTCGACACGGAAAAGTCTTTAAGCGCTACTTGGGAGCGCGCGGAGGGCTTTGGCAACGGCCGAACTAACTGACGCAAGTCGCGGGCGGATGAAGGCTACTCGTTCTTCCATTACTTCCAGTCTGGCAAAAATTTGGTTAGCTTTTCGAAACGGTTATGCAGCTAAGCCTAAATGACGTTTTTCAGGGACTTTTGTTACAATGGGTTTTGTTGTGAGTCTACCTGGCGCTATAGTGAGGAGAGTTGCTAATACTAGGCCATCTGCGACAGCGGCTAACGCGCCAGCTAGTCGTCGTCGTCCACATACTTGTCGTCGTCTGGCTTCTGCTTGTCTTGCTTGTTGTTGTTGTCGTCGCGCCACCGTGGATAAATGACGGATACCGGATGCGGCTTCCGAGAGGCTACTTGGGGCGCATGCCGCGCCCTTTGCGCTGCCAGCGCCCGCGTACATGCTGCTAGAATTTTCGAAAGAAACTATGCTGGGTCTTTGACGGCATGCACAAATGGAGATGGCTACTACCATGGTTTGAGCAAGTCTAACTACATCTACTTGTTGACTGACACCTTCCGCTTGATTTGTTCGACACAAGGTTGTAGAGATATCCGGCGTTGAACCGGCCGCACTTAAACTTTAGTCTAATATGGCTTAGTTAATTTGAGCCCCTTCTTTATCGGTAACCAAATGACGGACTTGTCTTTTTGCACATGTGGCTTACAAAGAGTTACTGGTAGGGCGAGAAGCTACCGTGCACGCAGTGATAG</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>ATGGAAAATTACACCAATATCCCGTTCGACTTGGCGCCTCCTAACGCAGCTTTCGATGTCCCTTTACGCACTGCTGTTCAGTCCCCTGAGGCATCATATTCGGGTGACGATGGTAACGTGACTAACGGTGATGAAGCACGCTTTCCCACTACCCTGCTTGGCACCTTTACGAAAGGTCTGCCTAACTCACTGCCTCTGGCGCTGCCGACGGATCGGTCTGCTTTCGATGCATTCGTTTCTGGTGTCAACACGGGCGATCTGGATACGATCAAATCAATCCCACTGGGACCGGATCCGGAAGGTGACAACTCTTTCTCTTCATCCGCGATGACTACCGGCGCCAAAGTGCCTGGATTGGAATCTATGGCAGCCGGGTTGGCATTTACTTTGGAAGCCCCTGATCCGCAACGCGTTACCATGCCCCCAGCTCCGCAAATCGACTCAGTGGAACTGGGTTACGAACTGTCGGAGTCCTACTTGATGGCGCTGTGTCCTGATATCGCGTTTACCGAATTCGATAATTCGGATACCGTGGCGGAGGCGGCTGCCTCGATGGCTGCGAATGCATTGGTCGCGGAAGACGGCTGTGACCAGCTTGGCGAACTGACACCGACGCAGACTGCAAACCGCGAACTGGAAATGAAGAACGGCGAAGGTATTACGCAGGGCACCATCTTCCCTGGCTCGCTTAACGGTGACAACATTGGTCCATACCTGTCTCAGTTCCTGTTGATCGGTTGCGATACTCTGGGTTCTCGCTTCTCGAATGATGACCCGGAATCTTACCTGACGGGGAATATTCCTTTCGGCGCCAACCGCATTGACCAGCGCGTGCGCAAAGCAGTTCCAGATCCTGATTATATGACAACCTTGGGCGCGTACATCGATGTGGCAAACGGCGCGGACGTCCCTGGTCCTGAGTCCTACGTCACCGCGGAAGGTGATAACTTCAATGACGAGGAAACGAACCGCTTTATTAATACACCGCGCGATCTTGCAACCTATGTTAACTATGACGCACTGTATCAACCCTATTTCAATGCGTGCCTCCTGATGCTGGCGATGGGTATTGGCTATGATGAGGGCCTGCCTTTCGGTGACGAAGATGAAGTGGATAAGCAAACCGGTTTTGCCCTGTTCGGTGGTCCGAACATCCTGTCACTCCTAGCTGAAGTGGTACTGAAAGCTCTGAAAGCGGTTCGCTTTCAGAAATTCGCCATGAACCCTCCTGCACCTCCCGAAACCGTTGCAGGTTTGATAGATTGCGTGCAACGCCCGCCTACATCGGACGAACAGGAAGGTAATGAAGGACAGACCGTCTTCAAACCCATCGAGAAACTTTGCCAGTATGTTGATTCTGATTTATTACAAAAAGTGCGCGAAAACAACGTCACGCAAAACAACACCCAGATGGACCGCGATATCACCCCTTTGAACGATTACGATCCAGTAGATGCAGTTGCGGATTGCGCGGTCGATCAGCAACAGCAGGTTTACGAACAGCAGCAAACGGAAGATGAGCAAAACGAACAGCAGCAGCAACAGCGAGGCGGCACGTATCTCCTGCCAATGGCGTATGCGGAGGGGTCTCCGATGAACCCGGCCTATGGTGCCGGCAACGCTACCGTTGCAGGTGCGTGTACCACCATCCTGAAAGCATTCTTTGATACGACCCAAAAGTTACCGTATGTTTTTACATCTACCGACGATGGAACCAAACTGGTTCAGATCGATGTAGACGAGCAGTTAACGGTTGAAGGCGAACTGAACAAACTGTGTTCAAACATTTCTATCGGTCGCAACTTGGCTGGGGTGAATTTGAAATCAGATTACACAGAATCGATCAAACTGGGTGAAGAAATAGCTATCGGACTGCTGCGCGAGCAGAAAAACGTGTATACCGAATGTTTTTCGATGACTATTCCCCTATTCGATGGTACCTGTGTAACTATT</t>
+          <t>ATGGAAAATTACACCAACATTCCTTTCGATTTGGCCCCTCGCAACGCCGCCTTTGATGTGCGACTGCGGACAGCTGTCCAGTCACCTGAAGCGTCTTACTCCGGTGATGATGGTAACGTTACCAACGGTGACGAAGCCCCTTTTCCAACCACGCTGCTGGGCACTTTTACTAAAGGCTTGCCAAACTCCCTGCCTCTGGCCTTACCCACGGACCCTTCTGCGTTTGACGCCTTCGTGTCTGGTGTGAACACGGGCGATTTAGACACAATCAAATCAATCCCGCTGGGCCCAGATCCGGAGGGAGATAACTCGTTTTCATCGTCCGCAATGACCACCGGCGCGAAGGTGCCTGGCTTGGAATCGATGGCGGCGGGACTGGCCTTTACGTTGGAAGCCCCGGATCCGCAGCCTGTGACGATGCCGCCGGCGCCGCAGATTGATTCCGTCGAACTGGGGTACGAGCTTTCTGAATCATACTTGATGGCCCTCTGTCGCGATATTGCCTTCACCGAATTCGACAATTCAGATACGGTCGCGGAAGCTGCCGCCTCTATGGCCGCAAACGCGTTGGTCGCCGAGGACGGATGTGACCAGCTCGGCGAATTAACGCCGACGCAAACAGCGAATCGCGAGCTGGAGATGAAAAACGGTGAAGGGATTACCCAGGGTACCATTTTCCGCGGTTCACTTAATGGTGATAACATCGGTCCATACCTGTCTCAATTCCTGCTGATAGGATGTGATACGCTGGGTTCTCGCTTTTCCAATGATGATCCTGAATCATACCTGACTGGCAACATTCGGTTTGGGGCCAATCGCATAGATCAACGCGTCCGAAAGGCAGTTCCGGACCCTGATTACATGACAACGTTGGGGGCGTACATTGATGTAGCAAACGGCGCGGACGTTCGCGGTCGGGAATCATATGTGACGGCCGAAGGCGATAATTTTAATGACGAAGAGACCAACCGGTTCATTAACACACCGCCTGATCTTGCTACATATGTGAATTACGATGCGCTCTATCAGCCGTACTTTAACGCATGCTTACTGATGCTGGCGATGGGTATTGGTTACGATGAAGGTCTACCGTTCGGCGATGAAGACGAAGTAGATAAGCAAACGGGCTTTGCGTTGTTTGGTGGTCCGAATATTCTGTCTCTGCTGGCAGAAGTTGTGCTAAAAGCGTTAAAAGCTGTGCCTTTTCAGAAATTCGCGATGAACCCTCGCGCGCCTCCCGAAACCGTTGCCGGCTTGATTGACTGCGTTCAGCGCCCGCCTACTTCCGATGAGCAAGAAGGTAATGAAGGTCAGACCGTTTTTAAACCAATCGAAAAGCTTTGCCAATACGTCGATTCGGATTTACTGCAAAAAGTCCCTGAAAACAATGTTACCCAAAACAACACTCAGATGGACCGCGATATCACTCCTCTCAACGATTATGATCCGGTAGACGCTGTCGCCGATTGCGCGGTCGATCAGCAGCAGCAGGTGTATGAACAGCAGCAGACCGAAGACGAACAGAACGAACAACAACAACAGCAGCGCGGTGGCACCTATTTACTGCCTATGGCCTACGCCGAAGGCTCTCCGATGAACCCCGCGTACGGCGCGGGAAACGCGACGGTCGCGGGCGCATGTACGACGATCTTAAAAGCTTTCTTTGATACGACCCAGAAACTGCCGTACGTGTTTACCTCTACCGATGATGGTACCAAACTCGTTCAGATTGATGTAGATGAACAACTGACTGTGGAAGGCGAACTAAACAAGCTGTGTTCCAACATCTCTATAGGCCGCAACTTGGCCGGCGTGAATTTGAAATCAGATTATACCGAATCAATTAAACTCGGGGAAGAAATAGCCATTGGTTTACTGCCTGAACAGAAAAACGTGTACACCGAATGTTTCTCAATGACCATCCCGCTCTTCGATGGCACGTGCGTCACTATC</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>ATGGAAAATTACACCAATATC</t>
+          <t>ATGGAAAATTACACCAACAT</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>AATAGTTACACAGGTACC</t>
+          <t>GATAGTGACGCACGTG</t>
         </is>
       </c>
     </row>
@@ -1396,22 +1396,22 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>TACGTCAAAAAGTGGTTGTAGGGCAAACTGAACGGCGGAGCGTTAGCGCGGAAACTATAAGCGAACTGTTGAAGTCAGGTCAGAGCGCTGCGGTAAATGTGGCCGCTGCTACCGTTGCACTGATTGCCACTGCTTTGTGCGAAGGGCGACAGTAATGACCCAAGAAAGTGCTTCCCCGACGGGTTGCGAGACCTGTGGAGAGACGAGGACTTGGGAAGCAGTAAGCTACGCAAGCAAGCCCGATAGCTGTGACCACTGCACCTAAAGTATTTTTGGAATGGCGACCCAGGCCTAGGTTGCCCGCGCTTGTTGAAAAAGAGAAGACGCTACCGCAGCCCACGCTTGTGGGGACCGAACCTCAGATACCGGCGTCCAGAGCGCAAGTGGGACCTCCCCGGCCTACGCGTCGGACATTGGTACGGTGGCCGAGGCGTTTAGCTAAGCCATCTCGACCCGATGCTCTACAGTCTTCGCATAAACTACCGGGACACAGCGCTACACCGGAAATTACTGAAGCCCAGACGCCTGTAACATTTTCGTCGTCGACTCAGAGACCCGTTGTTAGGGAACGACTGTCATCTGGTCAGGGAGGTCGTCGTCCTCGTCGTTGTCGTCCACACGATGTTATTGTTGTTGTTGTTATTATTGAGATTAGACGAATGAGGCCGGCTCTGGGGAGCGGGACTTAAGCTCGACGGATTGCCATACCCCTAATGGTGTCTATGGCACAAGGGACCCCACGAGGTCCCACTACTATAGCCGGGGATAGAGAGTGTTAAGGACTAATAGCCAACACTATGCGACCCACCCAAAGGAGGATGGCTAGGCCGACGTATATAATGCCCGAACTAAGGAATACCAAGCTTGGGATAGCTGGTCGGACAAGGATTCCGCTGGGGCAGTGCGCTGATGTACTGGTGTAACCCACGAATGTAGCTGCACTGGTTGCCCCGACTGCAGGGACCAGGACTTAGGATGCAACGTGGTTGACCCGGATTGAAATTGCTACTTCTTTGTTTGTGAAAGTAATTGTGGGGCGGACTGGAACGATGTATACATTTGATACTACGGGAGATGGTTCGAATGAAATTGCGAACGAATGACGACGACCGGTAACCGCGCCTGAAGCTGCTACCGTATGGCAAGTGATTTAGTCTACAACACCTATTTGTTTGACCGAAACAAGACAACCCGCTTGGCTTGTAAGACAGAGACGAGCATCTTCACCAAGTCTTTAGAGACTTCCGGCAAGCGAAAGTCTTTAAATTGCAATTAGGAGCGTGGGGAGGGCTCTGGCACCGACCAAACCAACTAACACAATTTGCGGGCGCCGGATGGGGCCAGAGACAGCGCCGGCGGTGGAGCCTCCCGCGTCCGGTCTTGCCGAAGCTTTTTCAAGAGTTCGGCTAACTTCGCAATACAGCGATACAGCTGCTACTAGAGGAGTTGGGACATGGACTTTTATTGAAGTAGGTTTTGCTATGGGTCAACCTGCCACTATTGTTGGAGGGCGCCGCTTTGCTGAAGCTGGGACAGGACAGGAGTTGGTGACTATTAACGTTCAGTTTGGTTTTCGTCGTCGTCATAAGCGTTGTTTGGCGTCTTGTTGTTCTTGTCCTTGTCTTTCGTTAACCATGGAAAGACAATGGCTACCGGAAACGGCTTCCGAGGGGCTACTTACGCAGCATACCGCGACCATTGCGTTGCCACCGTCCGCGTACGTGCTGATATGACTTTCGGAAAAAATTGTGCTTGCTATGAGACGGGAAATGGAAATTTTGGAGTCGCTTGCCGTGTGGAGACCTTGTCCAGTTTACACTTGTCTTCGACGCGCACCCACTACTTGACTTGTTTGACACGAGATTGCAAAGGTAGCCCGGACTGAACCGTCCGCAGTTAAACGCGAGGCTAATGTGGCTCAGATATTTCGACCCCCTTCTCCAGCGCGACCCAGAAGACGCGCTCGTTCGCTTGTAGATGCACCTCGTTAAAAGTTACTGTCACGGTAACAAGCTGCCTCCGCAACTTCAGTAAAGTTTAGGATTT</t>
+          <t>TACGTCAAAAAATGTTTATAAGGCAAACTAAACGGTGGAGGATTGGGACGCAAACTATAGGCGGACTGCTGGAGTCAGGTCAGGGCGCTGCGTTAGATATGGCCGCTGCTACCGTTGCAATGCTTGCCCCTACTTTGCGCGAAAGGCGACAGAGACGAGCCTAGTAAATGGTTCCCAGACGGCTTGCGCGAACTGTGCAGAGACGACGATTTAGGAAGGAGAAAGCTGCGTAAGCAAGGACGTTAACTATGGCCGCTACAACTAAAGTAGTTCTGGAACGGCGACCCAGGACTAGGCTGGCCACGCTTGTTAAAGAAAAGTAGACGGTACCGCAGTCCACGGTTGTGCGCGCCCAACCTTAGCTACCGTCGACCGGATCGGAAATGGGAACTTCCAGGCCTACGGGTCGGACAGTGCTACGGAGGTCGCGGCGTTTAACTAAGCCACCTTGACCCGATACTTTACAGGCTTCGCATGAACTACCGGAATACGGGACTGCAACGTAAATTACTAAAACCAAGGCGTCTGTAGCAATTTCGACGGCGTCTCAGGAATCCATTGTTAGGCAACGAATGTCAACTAGTCAGAGAAGTCGTTGTCCTTGTTGTCGTCGTCCACACGATATTGTTATTGTTGTTGTTGTTGTTGAGGTTGGAAGACTGCGGCCGCCTCTGAGGAGGAGCGCTTAAGCTTGACGCGTTGCCCTACCCATAATGATGTCTATGACAGAAAGCGCCGCACGACGTTCCACTGCTATAACCCGGTATGGACAGCGTCAAAAATTAGTAGCCAACACTATGTGACCCGCCGAAGGGGGGATGGCTAGGTCGGCGAATATAATGACCGGACTAGGGAATGCCGAGTTTGGGATAACTGGTTGCGCAGGGATTTCGATGGGGCAGTGGACTAATATACTGCTGGAACCCGCGAATGTAACTACATTGCTTACCACGCCTACAGGCGCCAGGACTCAGAATGCATCGAGGCTGGCCAGGCTTAAAGTTACTGCTTCTTTGCTTATGCAAATAATTATGCGGCGGACTGGACCGATGCATACACTTAATACTGCGAAACATGGTCCGTATAAAGTTACGAACGGACAACAATGACCGGTAACCACGCCTGAAACTGCTACCTTAGGGCAAATGTTTCAGCCTGCATCATCTATTTGTCTGGCCAAAGCATGACAACCCCCTTGGGTTATATGACAGAAACGACCAGCTTCACCACGTTTTTAGCGACTTCCGTCATGCGAAAGTCTTTAAATTGCACTTGGGAGCCTGCGGAGGCCTTTGGCACCGGCCAAACCACCTAACGCATTTTGCGGGCGCTGGCTGCGGCCAAAGTCATCGCCGTCGGTGGAGTCTTCCGCGGCCGGTCTTGCCGAAACTTTTTCACGAATTTGGCTAGCTCCGGAACACGGGAATGCAGCTACTGCTAGAGAACTTGGCCCACGGACTCTTATTAAAGTAGGTCTTACTATGTGTCGATCTGCCGCTGTTGTTGGACGGTGGAGCGTTGCTAAAACTAGGCCACGACAGCAGGTGGTGGCTATTAACGTTTAGATTAGTTTTTGTCGTCGTTATAAGTGTCGTTTGGCGACTCGTTGTCCTTGTCCTCGTTTTTCGGTAACCATGAAAAGACGAAGGCTACCGCAAACGCCTCCCGAGTGGTTACTTACGTAGTATACCACGCCCCTTACGGTGCCATCGCCCACGTACGTGCTGGTAAGACTTTCGCAAAAAGTTGTGGTTACTGTGGGAAGGTAAATGCAAGTTCTGGAGACGGTTGCCGTGGGGAGAACTTGTCCACTTTACACTCGTCTTTGAGGCCCATCCGCTGCTTAACTTATTCAATACGAGTTTACAAAGATAACCCGCGCTGAACCGCCCACACTTGAACGGAAGGCTGATATGCCTTAGGTAATTCGAGCCGCTCCTTCAACGGGACCCCAATGACGGACTTGTCCGATTATAGATACAACTTGTCAAAAGTTACTGCCAGGGAAATAAACTACCGCCGCAACTCCACTAGAGCTTGGCCTTT</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>ATGCAGTTTTTCACCAACATCCCGTTTGACTTGCCGCCTCGCAATCGCGCCTTTGATATTCGCTTGACAACTTCAGTCCAGTCTCGCGACGCCATTTACACCGGCGACGATGGCAACGTGACTAACGGTGACGAAACACGCTTCCCGCTGTCATTACTGGGTTCTTTCACGAAGGGGCTGCCCAACGCTCTGGACACCTCTCTGCTCCTGAACCCTTCGTCATTCGATGCGTTCGTTCGGGCTATCGACACTGGTGACGTGGATTTCATAAAAACCTTACCGCTGGGTCCGGATCCAACGGGCGCGAACAACTTTTTCTCTTCTGCGATGGCGTCGGGTGCGAACACCCCTGGCTTGGAGTCTATGGCCGCAGGTCTCGCGTTCACCCTGGAGGGGCCGGATGCGCAGCCTGTAACCATGCCACCGGCTCCGCAAATCGATTCGGTAGAGCTGGGCTACGAGATGTCAGAAGCGTATTTGATGGCCCTGTGTCGCGATGTGGCCTTTAATGACTTCGGGTCTGCGGACATTGTAAAAGCAGCAGCTGAGTCTCTGGGCAACAATCCCTTGCTGACAGTAGACCAGTCCCTCCAGCAGCAGGAGCAGCAACAGCAGGTGTGCTACAATAACAACAACAACAATAATAACTCTAATCTGCTTACTCCGGCCGAGACCCCTCGCCCTGAATTCGAGCTGCCTAACGGTATGGGGATTACCACAGATACCGTGTTCCCTGGGGTGCTCCAGGGTGATGATATCGGCCCCTATCTCTCACAATTCCTGATTATCGGTTGTGATACGCTGGGTGGGTTTCCTCCTACCGATCCGGCTGCATATATTACGGGCTTGATTCCTTATGGTTCGAACCCTATCGACCAGCCTGTTCCTAAGGCGACCCCGTCACGCGACTACATGACCACATTGGGTGCTTACATCGACGTGACCAACGGGGCTGACGTCCCTGGTCCTGAATCCTACGTTGCACCAACTGGGCCTAACTTTAACGATGAAGAAACAAACACTTTCATTAACACCCCGCCTGACCTTGCTACATATGTAAACTATGATGCCCTCTACCAAGCTTACTTTAACGCTTGCTTACTGCTGCTGGCCATTGGCGCGGACTTCGACGATGGCATACCGTTCACTAAATCAGATGTTGTGGATAAACAAACTGGCTTTGTTCTGTTGGGCGAACCGAACATTCTGTCTCTGCTCGTAGAAGTGGTTCAGAAATCTCTGAAGGCCGTTCGCTTTCAGAAATTTAACGTTAATCCTCGCACCCCTCCCGAGACCGTGGCTGGTTTGGTTGATTGTGTTAAACGCCCGCGGCCTACCCCGGTCTCTGTCGCGGCCGCCACCTCGGAGGGCGCAGGCCAGAACGGCTTCGAAAAAGTTCTCAAGCCGATTGAAGCGTTATGTCGCTATGTCGACGATGATCTCCTCAACCCTGTACCTGAAAATAACTTCATCCAAAACGATACCCAGTTGGACGGTGATAACAACCTCCCGCGGCGAAACGACTTCGACCCTGTCCTGTCCTCAACCACTGATAATTGCAAGTCAAACCAAAAGCAGCAGCAGTATTCGCAACAAACCGCAGAACAACAAGAACAGGAACAGAAAGCAATTGGTACCTTTCTGTTACCGATGGCCTTTGCCGAAGGCTCCCCGATGAATGCGTCGTATGGCGCTGGTAACGCAACGGTGGCAGGCGCATGCACGACTATACTGAAAGCCTTTTTTAACACGAACGATACTCTGCCCTTTACCTTTAAAACCTCAGCGAACGGCACACCTCTGGAACAGGTCAAATGTGAACAGAAGCTGCGCGTGGGTGATGAACTGAACAAACTGTGCTCTAACGTTTCCATCGGGCCTGACTTGGCAGGCGTCAATTTGCGCTCCGATTACACCGAGTCTATAAAGCTGGGGGAAGAGGTCGCGCTGGGTCTTCTGCGCGAGCAAGCGAACATCTACGTGGAGCAATTTTCAATGACAGTGCCATTGTTCGACGGAGGCGTTGAAGTCATTTCAAATCCTAAA</t>
+          <t>ATGCAGTTTTTTACAAATATTCCGTTTGATTTGCCACCTCCTAACCCTGCGTTTGATATCCGCCTGACGACCTCAGTCCAGTCCCGCGACGCAATCTATACCGGCGACGATGGCAACGTTACGAACGGGGATGAAACGCGCTTTCCGCTGTCTCTGCTCGGATCATTTACCAAGGGTCTGCCGAACGCGCTTGACACGTCTCTGCTGCTAAATCCTTCCTCTTTCGACGCATTCGTTCCTGCAATTGATACCGGCGATGTTGATTTCATCAAGACCTTGCCGCTGGGTCCTGATCCGACCGGTGCGAACAATTTCTTTTCATCTGCCATGGCGTCAGGTGCCAACACGCGCGGGTTGGAATCGATGGCAGCTGGCCTAGCCTTTACCCTTGAAGGTCCGGATGCCCAGCCTGTCACGATGCCTCCAGCGCCGCAAATTGATTCGGTGGAACTGGGCTATGAAATGTCCGAAGCGTACTTGATGGCCTTATGCCCTGACGTTGCATTTAATGATTTTGGTTCCGCAGACATCGTTAAAGCTGCCGCAGAGTCCTTAGGTAACAATCCGTTGCTTACAGTTGATCAGTCTCTTCAGCAACAGGAACAACAGCAGCAGGTGTGCTATAACAATAACAACAACAACAACAACTCCAACCTTCTGACGCCGGCGGAGACTCCTCCTCGCGAATTCGAACTGCGCAACGGGATGGGTATTACTACAGATACTGTCTTTCGCGGCGTGCTGCAAGGTGACGATATTGGGCCATACCTGTCGCAGTTTTTAATCATCGGTTGTGATACACTGGGCGGCTTCCCCCCTACCGATCCAGCCGCTTATATTACTGGCCTGATCCCTTACGGCTCAAACCCTATTGACCAACGCGTCCCTAAAGCTACCCCGTCACCTGATTATATGACGACCTTGGGCGCTTACATTGATGTAACGAATGGTGCGGATGTCCGCGGTCCTGAGTCTTACGTAGCTCCGACCGGTCCGAATTTCAATGACGAAGAAACGAATACGTTTATTAATACGCCGCCTGACCTGGCTACGTATGTGAATTATGACGCTTTGTACCAGGCATATTTCAATGCTTGCCTGTTGTTACTGGCCATTGGTGCGGACTTTGACGATGGAATCCCGTTTACAAAGTCGGACGTAGTAGATAAACAGACCGGTTTCGTACTGTTGGGGGAACCCAATATACTGTCTTTGCTGGTCGAAGTGGTGCAAAAATCGCTGAAGGCAGTACGCTTTCAGAAATTTAACGTGAACCCTCGGACGCCTCCGGAAACCGTGGCCGGTTTGGTGGATTGCGTAAAACGCCCGCGACCGACGCCGGTTTCAGTAGCGGCAGCCACCTCAGAAGGCGCCGGCCAGAACGGCTTTGAAAAAGTGCTTAAACCGATCGAGGCCTTGTGCCCTTACGTCGATGACGATCTCTTGAACCGGGTGCCTGAGAATAATTTCATCCAGAATGATACACAGCTAGACGGCGACAACAACCTGCCACCTCGCAACGATTTTGATCCGGTGCTGTCGTCCACCACCGATAATTGCAAATCTAATCAAAAACAGCAGCAATATTCACAGCAAACCGCTGAGCAACAGGAACAGGAGCAAAAAGCCATTGGTACTTTTCTGCTTCCGATGGCGTTTGCGGAGGGCTCACCAATGAATGCATCATATGGTGCGGGGAATGCCACGGTAGCGGGTGCATGCACGACCATTCTGAAAGCGTTTTTCAACACCAATGACACCCTTCCATTTACGTTCAAGACCTCTGCCAACGGCACCCCTCTTGAACAGGTGAAATGTGAGCAGAAACTCCGGGTAGGCGACGAATTGAATAAGTTATGCTCAAATGTTTCTATTGGGCGCGACTTGGCGGGTGTGAACTTGCCTTCCGACTATACGGAATCCATTAAGCTCGGCGAGGAAGTTGCCCTGGGGTTACTGCCTGAACAGGCTAATATCTATGTTGAACAGTTTTCAATGACGGTCCCTTTATTTGATGGCGGCGTTGAGGTGATCTCGAACCGGAAA</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>ATGCAGTTTTTCACCAAC</t>
+          <t>ATGCAGTTTTTTACAAATATTCC</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>TTTAGGATTTGAAATGACTTCA</t>
+          <t>TTTCCGGTTCGAGATC</t>
         </is>
       </c>
     </row>
@@ -1438,22 +1438,22 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>GTCTGGACGAGATGCAGACTACTACGCCTACTAGGTTGGGGCGGCTTGCTTGCGCTGCTGCTTCGAAAACGTAGCGGACAACGCCGCCGGTTTGGACTTGAACTTCCCTGCCCGTGACACACAGTTTAATTGTTGCCTCTTTGGCTGGAACGACGATTTAAGTTGTTTAGGGACGGATTGCTGCTAGACCCAGTCCAGCTGCGCCTACGCAAGCGCCGCGAGCTTCTAACGTAGGACTTACCACTGGACAGGTAGACGCTTCTACAAGGCCACCCTTTGAGACTCCCGCTAGGACAACCAGCGGACCACTTGGGCTGCCGCCGGAAACGTTATCTGTAAAGGCCGGGTCGGAAGAGCCGCTGGTGGTAGGGCGGCCATGGCTGAAATGGCAGGGGGCTTGACCGCCGTGTCGACCGGCTTCACATAAACTACCGTAATCGCGGACTGCAAGGCAAATACGTTATGCCGTGACTGCTGTAGTGCCAATGCCGACGTCGCTTGGACCGCCCATACCTTCCGAAAGGCTTAAATCTACGACAGAGATAACCGAGACTACCATGGCATCTAGGCGAGAGCGTCAACAAGGCGCGATGGAAGCACCCGCACCTTTGACCGGGAAAATAAAGGGTCGAAGACCACTTGAGTAAATGCTAACTGAGTTAGTGGCAACTTGGCTTTGTTCTTTGAAAACGGGGCCTGCAGTTGATGTACCAGCTAAAGCTACTTAACAACTTGTAAGTCTTACCACCGGGCGGTCGCCCGGGGCTTGACGAACTGCTGCTCGACGGAAAGCACGCTTTACGCGGACTGAACCGAGCGCAGTGCAAGTGACTGTTATAGTTGTGGCTTCGCATAGGACCACGCGACTAAGACGACCCTAACCTGCGAAAATTGGGACGTCCACAATTGCCAGGGAAATAACTATAGCTAGGAGTCCGTCCCAAACAGTTAAAACCGTATAGATTAATAAAAGCGGACTAGCCGCGGCGTCTTGACCGTGTTGGAAGGAGCAACATAGTCTTCAACGTCCACTTAGCGAAACGAGCCGGCCTTCGCGACCCACCATGGGACTTGGACTGGTAGTTTCCACTTGACTTGCGACTGAAGCTAAATAGAGACGACCTTTTACGGCTTAATGACTTTGCTCAGCGTCGTTAATTGCGGCGTGTCTTGGGCTTATTACTTCATTGGATAAACGACGGCGTCCGCTAGGTCCTTCCGAGTGGCTGTTTGGGCAGAATGGGTAGGCCGTTGCGATGCGTCTTGCCGCGCAAGCGATGGCAAGACTTTCGCGATTAACCAGACCTAGGACCGCCACTAACGATAGGCCTGGGACAAATGGGACTACTGCTGCCGGACTTTGACTAGCTAAAGGGACCCAGCACGAACTGCAAGCTCCCGCTTTAGTTGTTTGACCGCCAGTTACAGCGCAAACCAGCTGTCTACGACCCATAATTAATGGCGAAGCTACCGTAAGTCCCAAACGACGACCCACTTTGATAGTGCCACGCGTGCGAATTGGTTCTTGAGTACTGGAAACGGCTTCTCAGCTGCAAACTTAAAGCCGACAAGTGGCCACTTCATTAATTTGATAAAGTCCTGCCCTGGAAATGCTAACTGCCGAAGTTCACGGGCCCGGACCAGATGTGTCCACACCTTTTAACACAAAGA</t>
+          <t>GTCTGTACGAGCTGAAGTCTACTACGACTGCTAGGGTGGGGAGGCTTACTTGCGCTACTACTTCGTAAGCGCAGCGCCCACCGGCGTCGATTTGGACTTGAACTTCCCTGCCCATGCCAAACGGTCTAATTGTTGCCCCTTTGGCTGGAACGTCGGTTTAAATTATTTAGTGACGGCTTACTACTAGACCCGGTCCATCTACGACTGCGCAAACGCCGTGACCTTCTAACATAAGACTTACCGCTAGACAGGTAGACACTTCTGCACGGCCAACCGTTAAGGCTTCCGCTGGGCCAGCCAGGAGAACAATTAGGCTGGCGCCGAAAACGCTAGCTATAGAGCCCGGGCCGAAAAAGACGATGATGTTAGGGGGGCCATGGCTGCAATGGCAGAGGGCTCGACCGCCGTGTCGACCGCCTTCATATGAACTACCGAGAACGTGGACTGCACGGTAAATACGTTATGCCGTGACTACTATAATGTCAATGTCGGCGACGCTTAGACCGGCCGTACCTCCCAAAGGGCTTAGACCTACGTCAGAGGTAGCCGAGGCTACCATGTCATCTGGGCAACAGAGTCGAAAAGGGACGGTGTAAACACCCGCAGCTTTGACCCGGTAAGTAAAGAGTCGAAGACCAATTAAGCAAATGGTAGCTGAGATAATGCCACCTTGGATTTGTCCTTTGGAAGCGAGGTCTACAGTTGATATACCAACTAAAACTGCTTAACGAGTTGTAAGTCTTGCCGCCGGGGGGCCGCCCGGGGCTTGACAACCTACTACTTGACGCTAAACACGGATTGCGCGCGCTAGACCGGGCGCAGTGGAAATGGCTATTGTAATTGTGGCTCCGAATAGGACCACGCGACTAGGAAGAGCCAAACCTACGTAAATTGGGACGCCCGCAATTGCCAGGTAAGTAGCTGTAGCTAGGAGTCCGTCCCAAACACTTAAAACCATAAAGGTTAATAAAAGCGGACTAGCCACGTCGCCTCGACCGCGTCGCCAGCAGAAACATGGTCTTTAACGTTCAGTTGGGAAAACGCGGAGGGCTCCGAGACCCACCTTGGAATTTGAACTGGTATTTCCCGCTTAATTTACGGCTAAAACTGGACAGGGAAGATCTTTTGCGCCTTGACGACTTTGCGCAACGGCGATAGTTACGCCGCGTTTTGGGCTTATTACTTCACTGGATGGACGACGGCGTCCGATAGGTCCTTCCAAGAGGCTGGTTGGGTAGCATGGGCAGACCATTGCGTTGTGTTTTGCCACGGAAACGGTGTCATGAATTCCGAGACTAACCCGACCTGGCGCCACCGCTGACGATGGGCCTGGGCCATATGGGCCTGCTGCTACCGGACTTTGACTAACTAAAGGCGCCGAGTACGAATTGTAAACTTCCACTCTAATTGTTTGACCGTCACTTGCAACGCAAGCCCGGAGTTTACGACCCATAGTTAATAGCGAAACTGCCGTAGGTTCCGGACAACGAGCCCCTCTGGTAATGGCAAGCGTGCAACTTAGTTCTTAATTACTGTAAACGTCTCCTTAGATGGAAGCTTAAGGGAGACAAGTGTCCGCTTCACTAGTTTGACAAAGTCCTGCCGTGGAAATGCTAACTACCAAAGTTCACGGGCCCGGACCATATATGGCCGCAGCTCTTAACGCATAGC</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>CAGACCTGCTCTACGTCTGATGATGCGGATGATCCAACCCCGCCGAACGAACGCGACGACGAAGCTTTTGCATCGCCTGTTGCGGCGGCCAAACCTGAACTTGAAGGGACGGGCACTGTGTGTCAAATTAACAACGGAGAAACCGACCTTGCTGCTAAATTCAACAAATCCCTGCCTAACGACGATCTGGGTCAGGTCGACGCGGATGCGTTCGCGGCGCTCGAAGATTGCATCCTGAATGGTGACCTGTCCATCTGCGAAGATGTTCCGGTGGGAAACTCTGAGGGCGATCCTGTTGGTCGCCTGGTGAACCCGACGGCGGCCTTTGCAATAGACATTTCCGGCCCAGCCTTCTCGGCGACCACCATCCCGCCGGTACCGACTTTACCGTCCCCCGAACTGGCGGCACAGCTGGCCGAAGTGTATTTGATGGCATTAGCGCCTGACGTTCCGTTTATGCAATACGGCACTGACGACATCACGGTTACGGCTGCAGCGAACCTGGCGGGTATGGAAGGCTTTCCGAATTTAGATGCTGTCTCTATTGGCTCTGATGGTACCGTAGATCCGCTCTCGCAGTTGTTCCGCGCTACCTTCGTGGGCGTGGAAACTGGCCCTTTTATTTCCCAGCTTCTGGTGAACTCATTTACGATTGACTCAATCACCGTTGAACCGAAACAAGAAACTTTTGCCCCGGACGTCAACTACATGGTCGATTTCGATGAATTGTTGAACATTCAGAATGGTGGCCCGCCAGCGGGCCCCGAACTGCTTGACGACGAGCTGCCTTTCGTGCGAAATGCGCCTGACTTGGCTCGCGTCACGTTCACTGACAATATCAACACCGAAGCGTATCCTGGTGCGCTGATTCTGCTGGGATTGGACGCTTTTAACCCTGCAGGTGTTAACGGTCCCTTTATTGATATCGATCCTCAGGCAGGGTTTGTCAATTTTGGCATATCTAATTATTTTCGCCTGATCGGCGCCGCAGAACTGGCACAACCTTCCTCGTTGTATCAGAAGTTGCAGGTGAATCGCTTTGCTCGGCCGGAAGCGCTGGGTGGTACCCTGAACCTGACCATCAAAGGTGAACTGAACGCTGACTTCGATTTATCTCTGCTGGAAAATGCCGAATTACTGAAACGAGTCGCAGCAATTAACGCCGCACAGAACCCGAATAATGAAGTAACCTATTTGCTGCCGCAGGCGATCCAGGAAGGCTCACCGACAAACCCGTCTTACCCATCCGGCAACGCTACGCAGAACGGCGCGTTCGCTACCGTTCTGAAAGCGCTAATTGGTCTGGATCCTGGCGGTGATTGCTATCCGGACCCTGTTTACCCTGATGACGACGGCCTGAAACTGATCGATTTCCCTGGGTCGTGCTTGACGTTCGAGGGCGAAATCAACAAACTGGCGGTCAATGTCGCGTTTGGTCGACAGATGCTGGGTATTAATTACCGCTTCGATGGCATTCAGGGTTTGCTGCTGGGTGAAACTATCACGGTGCGCACGCTTAACCAAGAACTCATGACCTTTGCCGAAGAGTCGACGTTTGAATTTCGGCTGTTCACCGGTGAAGTAATTAAACTATTTCAGGACGGGACCTTTACGATTGACGGCTTCAAGTGCCCGGGCCTGGTCTACACAGGTGTGGAAAATTGTGTTTCT</t>
+          <t>CAGACATGCTCGACTTCAGATGATGCTGACGATCCCACCCCTCCGAATGAACGCGATGATGAAGCATTCGCGTCGCGGGTGGCCGCAGCTAAACCTGAACTTGAAGGGACGGGTACGGTTTGCCAGATTAACAACGGGGAAACCGACCTTGCAGCCAAATTTAATAAATCACTGCCGAATGATGATCTGGGCCAGGTAGATGCTGACGCGTTTGCGGCACTGGAAGATTGTATTCTGAATGGCGATCTGTCCATCTGTGAAGACGTGCCGGTTGGCAATTCCGAAGGCGACCCGGTCGGTCCTCTTGTTAATCCGACCGCGGCTTTTGCGATCGATATCTCGGGCCCGGCTTTTTCTGCTACTACAATCCCCCCGGTACCGACGTTACCGTCTCCCGAGCTGGCGGCACAGCTGGCGGAAGTATACTTGATGGCTCTTGCACCTGACGTGCCATTTATGCAATACGGCACTGATGATATTACAGTTACAGCCGCTGCGAATCTGGCCGGCATGGAGGGTTTCCCGAATCTGGATGCAGTCTCCATCGGCTCCGATGGTACAGTAGACCCGTTGTCTCAGCTTTTCCCTGCCACATTTGTGGGCGTCGAAACTGGGCCATTCATTTCTCAGCTTCTGGTTAATTCGTTTACCATCGACTCTATTACGGTGGAACCTAAACAGGAAACCTTCGCTCCAGATGTCAACTATATGGTTGATTTTGACGAATTGCTCAACATTCAGAACGGCGGCCCCCCGGCGGGCCCCGAACTGTTGGATGATGAACTGCGATTTGTGCCTAACGCGCGCGATCTGGCCCGCGTCACCTTTACCGATAACATTAACACCGAGGCTTATCCTGGTGCGCTGATCCTTCTCGGTTTGGATGCATTTAACCCTGCGGGCGTTAACGGTCCATTCATCGACATCGATCCTCAGGCAGGGTTTGTGAATTTTGGTATTTCCAATTATTTTCGCCTGATCGGTGCAGCGGAGCTGGCGCAGCGGTCGTCTTTGTACCAGAAATTGCAAGTCAACCCTTTTGCGCCTCCCGAGGCTCTGGGTGGAACCTTAAACTTGACCATAAAGGGCGAATTAAATGCCGATTTTGACCTGTCCCTTCTAGAAAACGCGGAACTGCTGAAACGCGTTGCCGCTATCAATGCGGCGCAAAACCCGAATAATGAAGTGACCTACCTGCTGCCGCAGGCTATCCAGGAAGGTTCTCCGACCAACCCATCGTACCCGTCTGGTAACGCAACACAAAACGGTGCCTTTGCCACAGTACTTAAGGCTCTGATTGGGCTGGACCGCGGTGGCGACTGCTACCCGGACCCGGTATACCCGGACGACGATGGCCTGAAACTGATTGATTTCCGCGGCTCATGCTTAACATTTGAAGGTGAGATTAACAAACTGGCAGTGAACGTTGCGTTCGGGCCTCAAATGCTGGGTATCAATTATCGCTTTGACGGCATCCAAGGCCTGTTGCTCGGGGAGACCATTACCGTTCGCACGTTGAATCAAGAATTAATGACATTTGCAGAGGAATCTACCTTCGAATTCCCTCTGTTCACAGGCGAAGTGATCAAACTGTTTCAGGACGGCACCTTTACGATTGATGGTTTCAAGTGCCCGGGCCTGGTATATACCGGCGTCGAGAATTGCGTATCG</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>CAGACCTGCTCTACG</t>
+          <t>CAGACATGCTCGACTTC</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>AGAAACACAATTTTCCACAC</t>
+          <t>CGATACGCAATTCTCGA</t>
         </is>
       </c>
     </row>
@@ -1480,22 +1480,22 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>TACTACTTTCGAAGACCGCCGTAATAATGCCGTGACGAACGACGGAAGGGCGGCACAGAGAGAGTCTGGCAGTTGCTTAACCGTCTGTACGTCTGCGCGGGCGAGGAAAGACCCAGACACACAGGACAAGCGCTGTGGCACCTAAAGGACAGAGGATGGTTTGGACGCTTTTAGTGGAAGTTTGGAGCGTAGCCATAACGTCGGCCTCTTAACCGCCACCCCGGCTGCACGTTAGACTTATTACCCCTACTTCGATTGCATGGCGACAAGCTACCGGTCAAGTTGTTCAGGGACGGCTTGCTGCTACAACCCGCGCAATTGGGACTCCGGATAGTCGAGGACGACCTAACGTAACTTAGGTTGCTGTAATTGCAAACACTAGTCCAGGGAAGCCCGCAACTTAGACTACCAGGATTCAATCATTTGGGCAATCCGCCACCGCCCTTAGTCCATCTACCACGACTAAGGCTATTGTAAAAGTAATTTGTCGGCCTGTTAGAAGACAGGCTTGGAGACCGGCGTGTCGTCCGTCTTCACATAAACTACCGCGACGAAGCGCTATAGGGCAAAAGAGTCAAGCCATGGTTATTGTGGCATGTTTACCGGCGCCGATTGGACGTCCCAAAACTACGGAAATTGCCTGACAGATAAAGAGCGCTACGCCTACCGTTATAACTAGGCTACGTTCTAGAAAAGGCGTGGCTGAACGGCCCACACAGGAGACCAGGCTACCAGAGAGTCAAATACGACCGCTTGAAGCTGTAGCTACCATAACAACACCTTGGCTTTCGTTTTTGAGACCAGGGACTTTACCTCATATACTGCCCACAACTGTGCAACGAGTTGTATGTCTTACCCCCAGGCGGCCTTCTATGCGATAAACAGCTACTTGGAAACAAATAGGGATTGCCCGCGCTGGAGCGACGTGAGAGTAAATTACTGCAAGACATATGGCTTCGCAAGGCGTGGTAGGACTAGGAAAAATTGCTCAGCTAGGACCGACTTCGACCGGGCATACCGAGTAGATGGGCGGTCCTCCCGAAGTGTTGGGACCCATGGAGGTTAATGTAATTGCGCTACCGTCGACCGAGTAGGAGCTGGGCGTTGCGCAACATACGTTTTAACGTTCAGTTAGCGCACGACGGAGGACTTCGTATGCCCCCGGAGGATTTAAAGCAATAGTTGTTGGACTAGCTACTGCACGGCGACGGCCGCAGCTAGCATAGATTGTGCCTTAACAATTTACGTCACCTCAGTGACTTGGTCCGAGTCTTGCCGCCGTGGTTGGTCCAAAAGGAAGACGGGTACCGCCAACCCCTCCCCAGAGGACAGTTAGGCCGTATAGGCAGTCCATTGCGCTAGTTGGACCCACGCATAGACTGTCACGAGTTCCGCAAAGAGCCAAAACTTGACCCGGTCGCGACGAAGGGCAGTGGTTACTAAAGATTGCTACGTCCTTGGCTGGGATAGGGTAAACAGGGCAGGCTGCCACTAGCGCACCCTTGGACATAGTTGCTTCTACCACTTCTTCTTCACCCGGACTGGATACTTCCCCTCGACTTGTTTCACTGTAGCTTGCACCGGTAACCAGCGAGGTTGGACCCACAATTAAACGCGTACCTGCCCCAAAAACCACGACTCTACCCTCTCCGTCCGCGTTAAGCCGGAGACGTTGTCCTCGAGCCACCAGACGGTCTCCGAGCGCTGTGTCTCCCAGGCTAAGGCGGTCGTAGAATATTTAAGGGAAATATGAGACCATGATACTAGCTTGACAAGGGTCTATTGGCTATGTACGACCCACTAGTCTACACGTTTCCCAAAAAATGACCACTGCTAAAAACGCATGGTCGGCTGCTTCTTCTTTGGCGCCTTGACCTTCTAGACCACGAGCCGAGGCAACACCTAGTTTGGACACGACTTGAC</t>
+          <t>TACTACTTCCGGAGGCCACCGTAGTAATGGCGAGAGGACCGCCGCAAAGGCGGGACGGACAGGGTCTGCCAATTGCTTGACCGCCTGTACGTTTGCGCGGGCGACAACAGACCTAGACACACAGGACAGGCGCTGTGGCATCTGAAGGAAAGAGGCTGGTTTGCCCGCTTCTAATGCAAGTTCGGAGCGTAACCGTAGCGTCGCCCTCTTGAGCGGCAGCCAGGTTGGACATTAAACTTATTACCTCTACTTCGATTACACGGCAATAAACTGCCAGTCAAGTTGTTTAGGAACGGCTTGCTACTACAGCCGGCCCAGTTGGGTCTTCGGATAGTCGACGAGGACCTAACGTAACTCAGCTTACTGTAGTTGCACACGCTAGTCCACGGTAGGCCGCAACTTAGTCTACCAGGATTCGAGCAATTGGGAGACCCACCACCACCATTGGTCCACCTACCGCGTCTAAGGCTGTTGTAGAAGTAGTTCGTTGGCCTATTGAATGACAGGCTCGGAGACCGTCGCGTTGTCCGCCTTCAAATAAACTACCGCAACGACGGACTGTAAGGCAAAAGAGTCAAACCGTGGTTATTGTGCCAAGTCTACCGTCGCCGGTTAGAGGTCCCGAAACTGCGCAAGTTGCCGGAAAGATAAAGAGCCCTACGCCTGCCGTTGTAGCTGGGCTACGTTCTAGAGAAAGGATGACTGAACGGCCCGCAAAGTAGTCCGGGCTACCAGAGTGTCAAGTACGACCGCTTGAAGCTATAACTACCGTAGCACCACCTCGGCTTTCGTTTTTGGGACCACGGCCTTTACCTTATGTACTGACCGCAGCTATGGAACGAGTTGTAAGTCTTGCCACCAGGCGGCCTCCTATGGGAGAAGCACCTGCTTGGCGAGAAATAAGCGTTGCCGGCGCTAGAGCGCCGCAATAGCAAGTTGCTGCACGACATGTGGCTTCGAAAGGCTTGTTAAAATTAAAATAAGTTACTTAGGTAGGACCGGCTCCGGCCGGGAATACCAAGAAGATGGGGAGTTCTTCCGAAGTGTTGGGACCCGTGCAGGTTGATATAATTACGGTACCGGCGGCCAAGAAGAAGATGGGCTTTGCGGAACATACGTTTTAACGTCCAATTGGGACACGAAGGAGGACTTCGTATACCACCGGAAGACTTGAAGCATTAGTTGTTGGACTAGCTGCTGCAAGGAGACGGCCGGAGCTAGCACAGATTGTGGCTTGACGACTTGCGTCACCTCAGAGATTTGGTCCGGGTCTTGCCGCCCTGGTTGGTCCAGAAAAATGACGGCTACCGCCAGCCTCTTCCGAGAGGCCAGTTGGGTCGCATAGGAAGTCCGTTGCGCTAATTGGACCCGCGGATAGACTGTCAAGACTTTCGTAAAGACCCGAAACTCAACCCCGTCGGAACAAAAGGCAGGGGCTACTAAAGTTTGCTACGCCCGTGGCTAGCGTAAGGCAAACAAGGAAGACTACCACTGGCGCATCCATGGACGTAGTTGCTCCTACCACTTCTTCTCCACCCAGACTGGATGCTTCCGCTCGAATTATTTCATTGAAGGTTGCACCGTTAGCCAGCGAGATTGGACCCGCAATTGAACGGATACCTACCGCAGAAGCCGCGTCTTTACCCGCTTCGGCCACGCTAGGCGGCGAATGTCGTCCTCAACCCACCGAACGGCCTTCGGGCGCTGTGACTCCCCGGTTAAGGTGGCCGGAGTATATTTAAGGCTAACATGAGGCCGTGGTACTAGCTTGATAAGGGTCTGTTGGCGATATACGAGCCGCTAGTCTACACGTTTCCAAAGAAGTGGCCGCTACTAAAGACGCACGGGCGCCTGCTTCTTCTTTGCCGTCTTGAACTTCTGGACCATGAGCCAAGTCACCACCTGGTCTGGACACGACTTAAT</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>ATGATGAAAGCTTCTGGCGGCATTATTACGGCACTGCTTGCTGCCTTCCCGCCGTGTCTCTCTCAGACCGTCAACGAATTGGCAGACATGCAGACGCGCCCGCTCCTTTCTGGGTCTGTGTGTCCTGTTCGCGACACCGTGGATTTCCTGTCTCCTACCAAACCTGCGAAAATCACCTTCAAACCTCGCATCGGTATTGCAGCCGGAGAATTGGCGGTGGGGCCGACGTGCAATCTGAATAATGGGGATGAAGCTAACGTACCGCTGTTCGATGGCCAGTTCAACAAGTCCCTGCCGAACGACGATGTTGGGCGCGTTAACCCTGAGGCCTATCAGCTCCTGCTGGATTGCATTGAATCCAACGACATTAACGTTTGTGATCAGGTCCCTTCGGGCGTTGAATCTGATGGTCCTAAGTTAGTAAACCCGTTAGGCGGTGGCGGGAATCAGGTAGATGGTGCTGATTCCGATAACATTTTCATTAAACAGCCGGACAATCTTCTGTCCGAACCTCTGGCCGCACAGCAGGCAGAAGTGTATTTGATGGCGCTGCTTCGCGATATCCCGTTTTCTCAGTTCGGTACCAATAACACCGTACAAATGGCCGCGGCTAACCTGCAGGGTTTTGATGCCTTTAACGGACTGTCTATTTCTCGCGATGCGGATGGCAATATTGATCCGATGCAAGATCTTTTCCGCACCGACTTGCCGGGTGTGTCCTCTGGTCCGATGGTCTCTCAGTTTATGCTGGCGAACTTCGACATCGATGGTATTGTTGTGGAACCGAAAGCAAAAACTCTGGTCCCTGAAATGGAGTATATGACGGGTGTTGACACGTTGCTCAACATACAGAATGGGGGTCCGCCGGAAGATACGCTATTTGTCGATGAACCTTTGTTTATCCCTAACGGGCGCGACCTCGCTGCACTCTCATTTAATGACGTTCTGTATACCGAAGCGTTCCGCACCATCCTGATCCTTTTTAACGAGTCGATCCTGGCTGAAGCTGGCCCGTATGGCTCATCTACCCGCCAGGAGGGCTTCACAACCCTGGGTACCTCCAATTACATTAACGCGATGGCAGCTGGCTCATCCTCGACCCGCAACGCGTTGTATGCAAAATTGCAAGTCAATCGCGTGCTGCCTCCTGAAGCATACGGGGGCCTCCTAAATTTCGTTATCAACAACCTGATCGATGACGTGCCGCTGCCGGCGTCGATCGTATCTAACACGGAATTGTTAAATGCAGTGGAGTCACTGAACCAGGCTCAGAACGGCGGCACCAACCAGGTTTTCCTTCTGCCCATGGCGGTTGGGGAGGGGTCTCCTGTCAATCCGGCATATCCGTCAGGTAACGCGATCAACCTGGGTGCGTATCTGACAGTGCTCAAGGCGTTTCTCGGTTTTGAACTGGGCCAGCGCTGCTTCCCGTCACCAATGATTTCTAACGATGCAGGAACCGACCCTATCCCATTTGTCCCGTCCGACGGTGATCGCGTGGGAACCTGTATCAACGAAGATGGTGAAGAAGAAGTGGGCCTGACCTATGAAGGGGAGCTGAACAAAGTGACATCGAACGTGGCCATTGGTCGCTCCAACCTGGGTGTTAATTTGCGCATGGACGGGGTTTTTGGTGCTGAGATGGGAGAGGCAGGCGCAATTCGGCCTCTGCAACAGGAGCTCGGTGGTCTGCCAGAGGCTCGCGACACAGAGGGTCCGATTCCGCCAGCATCTTATAAATTCCCTTTATACTCTGGTACTATGATCGAACTGTTCCCAGATAACCGATACATGCTGGGTGATCAGATGTGCAAAGGGTTTTTTACTGGTGACGATTTTTGCGTACCAGCCGACGAAGAAGAAACCGCGGAACTGGAAGATCTGGTGCTCGGCTCCGTTGTGGATCAAACCTGTGCTGAACTG</t>
+          <t>ATGATGAAGGCCTCCGGTGGCATCATTACCGCTCTCCTGGCGGCGTTTCCGCCCTGCCTGTCCCAGACGGTTAACGAACTGGCGGACATGCAAACGCGCCCGCTGTTGTCTGGATCTGTGTGTCCTGTCCGCGACACCGTAGACTTCCTTTCTCCGACCAAACGGGCGAAGATTACGTTCAAGCCTCGCATTGGCATCGCAGCGGGAGAACTCGCCGTCGGTCCAACCTGTAATTTGAATAATGGAGATGAAGCTAATGTGCCGTTATTTGACGGTCAGTTCAACAAATCCTTGCCGAACGATGATGTCGGCCGGGTCAACCCAGAAGCCTATCAGCTGCTCCTGGATTGCATTGAGTCGAATGACATCAACGTGTGCGATCAGGTGCCATCCGGCGTTGAATCAGATGGTCCTAAGCTCGTTAACCCTCTGGGTGGTGGTGGTAACCAGGTGGATGGCGCAGATTCCGACAACATCTTCATCAAGCAACCGGATAACTTACTGTCCGAGCCTCTGGCAGCGCAACAGGCGGAAGTTTATTTGATGGCGTTGCTGCCTGACATTCCGTTTTCTCAGTTTGGCACCAATAACACGGTTCAGATGGCAGCGGCCAATCTCCAGGGCTTTGACGCGTTCAACGGCCTTTCTATTTCTCGGGATGCGGACGGCAACATCGACCCGATGCAAGATCTCTTTCCTACTGACTTGCCGGGCGTTTCATCAGGCCCGATGGTCTCACAGTTCATGCTGGCGAACTTCGATATTGATGGCATCGTGGTGGAGCCGAAAGCAAAAACCCTGGTGCCGGAAATGGAATACATGACTGGCGTCGATACCTTGCTCAACATTCAGAACGGTGGTCCGCCGGAGGATACCCTCTTCGTGGACGAACCGCTCTTTATTCGCAACGGCCGCGATCTCGCGGCGTTATCGTTCAACGACGTGCTGTACACCGAAGCTTTCCGAACAATTTTAATTTTATTCAATGAATCCATCCTGGCCGAGGCCGGCCCTTATGGTTCTTCTACCCCTCAAGAAGGCTTCACAACCCTGGGCACGTCCAACTATATTAATGCCATGGCCGCCGGTTCTTCTTCTACCCGAAACGCCTTGTATGCAAAATTGCAGGTTAACCCTGTGCTTCCTCCTGAAGCATATGGTGGCCTTCTGAACTTCGTAATCAACAACCTGATCGACGACGTTCCTCTGCCGGCCTCGATCGTGTCTAACACCGAACTGCTGAACGCAGTGGAGTCTCTAAACCAGGCCCAGAACGGCGGGACCAACCAGGTCTTTTTACTGCCGATGGCGGTCGGAGAAGGCTCTCCGGTCAACCCAGCGTATCCTTCAGGCAACGCGATTAACCTGGGCGCCTATCTGACAGTTCTGAAAGCATTTCTGGGCTTTGAGTTGGGGCAGCCTTGTTTTCCGTCCCCGATGATTTCAAACGATGCGGGCACCGATCGCATTCCGTTTGTTCCTTCTGATGGTGACCGCGTAGGTACCTGCATCAACGAGGATGGTGAAGAAGAGGTGGGTCTGACCTACGAAGGCGAGCTTAATAAAGTAACTTCCAACGTGGCAATCGGTCGCTCTAACCTGGGCGTTAACTTGCCTATGGATGGCGTCTTCGGCGCAGAAATGGGCGAAGCCGGTGCGATCCGCCGCTTACAGCAGGAGTTGGGTGGCTTGCCGGAAGCCCGCGACACTGAGGGGCCAATTCCACCGGCCTCATATAAATTCCGATTGTACTCCGGCACCATGATCGAACTATTCCCAGACAACCGCTATATGCTCGGCGATCAGATGTGCAAAGGTTTCTTCACCGGCGATGATTTCTGCGTGCCCGCGGACGAAGAAGAAACGGCAGAACTTGAAGACCTGGTACTCGGTTCAGTGGTGGACCAGACCTGTGCTGAATTA</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>ATGATGAAAGCTTCTGGC</t>
+          <t>ATGATGAAGGCCTCC</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>CAGTTCAGCACAGGTTT</t>
+          <t>TAATTCAGCACAGGTCT</t>
         </is>
       </c>
     </row>
@@ -1522,12 +1522,12 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>TACGACACGTTGCGCCGCCTGTGCTGAGGACCAAGCGGGTACGGCCTATGACCCCATGACGCCGAAGAGTGGAGGCTTGTCGGACGCTTTCCAAACGCGGCGGTTGACCTTCCTCTTTTTAGCGACCCAAAGTTGGGTAGCCTCTGGGGTATGTAATTTATAAATCTCCCGAGACTTTGGAACTTTTTTCACTTTGACGGGTGACTACCGTAAAGTCGCAGGTTCTAAGACCCGTTTTAGTACCGCGGACAAGGATAGCGCTGACGCGAACGCCACCAGGAACGGCGGGGTACGGACCGTAAACTACTCCAATGGCGAAGGCCACAGAAGGGACTTCTTTTGTTTTTGTGGCCACTCCCAGGATTGGACGTCTGGACGTGTTTGAGGCTGCTGCGCGACCTGGGATGGCGGGGGTTGGCGGGACTGTTACAACGCAAACGGAGAGCGGCGCTGCGTCGCGCTGGACTCGCGCTGCCGTGACCGTGCCAGACAGTCTAATGCTTGCCACTCTGGCTGGACCGCTGGTACAAGTTGTTTAGTAATGGCTTACTGCTTGACCCAGTCCATTGTCGTCTGCTAAAACGATAGAACCTCCTAACGTAGAATTTACCACTAAAGAGATAAACGCTTCTACATGGTCGCCCACTGGGACGTCCGGGAGACCACTTAGGCTGTCGCCGGAAGCGATAACTATAAAGCCCAGGGCGAAAGAGTCGTTGGTGGTAAGGAGGTCAGGGCTGAGACAGCAGTGGGCTCAACCGCCGTGTCGAACGGCTTGACATAAACTACCGTGAGCGGGCGCTGCATGGCAAATACGTTATACCGTGGCTACTCTAGTGTTGGTGCCGGCGCCGTTTAGACCGCCCATACCCACCAAAGGGCTTGGACCTGCGGCAAAGATAACCTAGTCTACCGTGGCACCTGGGTAAAAGCGTCAACAAGGGACGCTGGAAGCAGCCACACCTTTGTCCAGGTAAGCACAGCGTCAATAACCATTTGAGAAAATGGTAGCTACGGTAATGACACCTTGGATTTGTTCTCTGAAAGCGTGGTCTAGAATTGATATACCAACTGAAGCTACTCAACGACTTGTAGGTCTTGCCACCAGGCGGTCGCCCGGGGCTTCTTGAGCTGCTTCTTAATGCGAAGTAAGCGTTACGGGCGCTAAATCGTGGACATAGGAAACATCTATTGTAATTGTGACTTCGGATAGCGCCAAGGAATTAAGACAATCTTGACCCGCGCAAAAGCGGAGGACCGTAATTGCCAGGAAAATATCTAAGCCTAGGAGTCCGTCCGAAGCAATTAAAACCGTGTAGGTTGATAAAAGCGGACTAGCCACGGCGACTTGACCGTGTCGGACGAAGGACAATGGTTTTTAACGTCCAGTTGGCGAAACGTGGAGGCCTCCGGAACCCACCATGGGACTTATTATGCTAACGACCACTGGAACTGCGCCTAAAGCTGTAAAGAGACGACCTTTTACTACTCGACGAATTTGCGCACCGGCTCTAGTTGCGCCGCGTCTTAGGCTTGTTACTTCATTGTATAGACGACGGCGTCCGATAAGTCCAACCGAGGGGATGATTAGGAAGGATGGGGAGCCCGTTACGCTGCGTTTTACCGCGGAAACGTTGTCATGAGTTTCGGGAATATCCGGACCTGGCGCCGCCGCTCACGAAGGGATTGGGCCAAAAGGGTAGACTACTACCAAACCTTGATTAGTTAAAGCTTCCGCGCACGGACTGGATACTTCCGCTTTAATTATTTGAGCGTCAATTGCAACGTAAACCAGGAGTCTACGAGCCCTAGTTGATAGCTAAGCTACCATAAGTCCCAGACGACGACCCCCTTTGATAGTGTCACGCGTGAGACTTGGTCCTCGAATACTGCAAACGCCTTCTTCGCTGCAAACTCAAAGGAGACAAATGCCCGCTTCAATAGTTCAATAAGGTCCTGCCGTGGAAAAGATATCTACCGCTATACACAAGTCCGGACCAGATGTGTCCACACCGACTAACGGTTCGC</t>
+          <t>TACGACACGTTGCGGCGCCTATGCTGTGGACCTAGTGGTTACGGCCTGTGGCCGCAGGAGGGAGACGACTGTAGCCTTGTCGCGCGCTTTCCTAACGGAGCGGTCGATCTTCCACTTTTCAGCGAACCGAAATTGGGCAGACTTTGCGGCATGTAATTTATAGAGCTTCCAAGACTTTGGAACTTTTTTCATTTTGATGGCTGGCTGCCGTAGAGGCGAAGATTCTAAGAACCATTTTAGTACCGTGCGCAGGGATAACGCTGCCGCGACCGGCACCACGAACGTCGCGGCACAGACCGAAAACTACTCCAATGACGCAGTCCACACAAGGGCCTTCTTTTATTTTTGTGTCCCCTTCCTGCGTTGGAAGTCTGGACGTGCTTGAGGCTGCTACGCGACCTAGGTTGCCGGGGATTAGGAGCGCTATTGCAACGCAAACGGAGCGGAGGACTACGCCGTGGAGCGCTTGGACTACCATGCCCGTGGCACACGGTTTAGTGCTTACCGCTTTGCCTGGACCGCTGGTACAAATTGTTTAGAGACGGCTTGCTGCTTAATCCTGTCCAATGGCGTCTGCTGAAACGTTAGGACCTTCTAACGTAGGACTTGCCACTAAAGAGGTAAACACTTCTACAGGGCCGGCCACTAGGTCGTCCAGGAGAACAGTTAGGATGCCGCCGGAAGCGGTAGCTATAAAGGCCGGGCCGAAAAAGGCGCTGCTGGTAAGGCGGCCACGGCTGCAATAGTAGGGGGCTCGAGCGCCGCGTCGACCGCCTTGACATGAACTACCGCGACCGCGCGCTACATGGTAAATACGTTATGCCTTGGCTGCTCTATTGGTGGTGCCGACGTCGGTTAGAGCGCCCCTACCCACCGAAAGGCTTGGACCTACGCCAAAGTTAGCCGAGACTACCGTGGCACCTAGGCAAGAGAGTCGACAAAGGACGGTGGAAACAACCGCAACTTTGCCCAGGTAAACAAAGTGTTGACGACCACTTAAGGAAATGCTAACTACGCTAATGCCAACTTGGCTTTGTCCTTTGTAAGCGAGGTCTGGAGTTGATATACCAGCTAAAGCTACTTAACGACTTGTATGTCTTGCCACCGGGCGGTCGCCCGGGCCTCCTTGACCTGCTCCTTGACGGAAAGTAGGGATTGCGTGCTCTAGACCGAGGACAGAGAAAACACCTGTTGTAGTTGTGCCTTCGCATAGCTCCAAGCAACTAAGACAACCTCGATCCGCGAAAGAGTGGAGGCCCATAGTTGCCGGGCAAATATCTAAGTCTAGGAGTCCGCCCAAAGCATTTGAAGCCGTGGAGATTAATAAAAGCGAATTAACCGCGCCGCCTTAACCGTGTCGGACGTAGAACGATAGTCTTTAACGTTCACTTAGGAAAACGGGGAGGCCTTCGAGACCCACCGTGTGACTTATTGTGGTAGCGTCCTCTAGACCTACGTCTAAAACTGTAAAGAGACGACCTTTTACTACTTGACAACTTTGCGCAGCGTCTTTATTTACGCCGGGTCTTGGGCTTGTTGCTCCACTGGATGGACGAAGGTGTCCGCTAAGTTCAGCCGAGCGGCTGATTGGGCAGGATGGGCAGACCATTACGTTGCGTCTTGCCACGCAAGCGCTGTCAAGACTTTCGGGAGTAGCCAGACCTAGGACCCCCACTTACGAAAGGCTTGGGCCACAAAGGCAGCCTACTACCGGACCTCGACTAATTGAAACTCCCACGCACAGACTGCATGCTTCCGCTTTAGTTATTTGACCGGCACTTGCACCGCAAACCGGCGGTTTACAATCCTTATTTGATGGCGAAGCTGCCTTAAGTCCCAGACGACAATCCTCTTTGCTAATGGCAAGGATGGGAATTGGTTCTTAACTACTGGAAACGCCTCCTTCGTTGCAAGCTCAAAGCGAATAAATGCCCGCTCCAGTATTTCAACAAGGTCCTGCCGTGGAAGAGATAACTACCACTGTACACAAGGCCAAATCAGATATGGCCACAGCGACTGACGGTCCGC</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>ATGCTGTGCAACGCGGCGGACACGACTCCTGGTTCGCCCATGCCGGATACTGGGGTACTGCGGCTTCTCACCTCCGAACAGCCTGCGAAAGGTTTGCGCCGCCAACTGGAAGGAGAAAAATCGCTGGGTTTCAACCCATCGGAGACCCCATACATTAAATATTTAGAGGGCTCTGAAACCTTGAAAAAAGTGAAACTGCCCACTGATGGCATTTCAGCGTCCAAGATTCTGGGCAAAATCATGGCGCCTGTTCCTATCGCGACTGCGCTTGCGGTGGTCCTTGCCGCCCCATGCCTGGCATTTGATGAGGTTACCGCTTCCGGTGTCTTCCCTGAAGAAAACAAAAACACCGGTGAGGGTCCTAACCTGCAGACCTGCACAAACTCCGACGACGCGCTGGACCCTACCGCCCCCAACCGCCCTGACAATGTTGCGTTTGCCTCTCGCCGCGACGCAGCGCGACCTGAGCGCGACGGCACTGGCACGGTCTGTCAGATTACGAACGGTGAGACCGACCTGGCGACCATGTTCAACAAATCATTACCGAATGACGAACTGGGTCAGGTAACAGCAGACGATTTTGCTATCTTGGAGGATTGCATCTTAAATGGTGATTTCTCTATTTGCGAAGATGTACCAGCGGGTGACCCTGCAGGCCCTCTGGTGAATCCGACAGCGGCCTTCGCTATTGATATTTCGGGTCCCGCTTTCTCAGCAACCACCATTCCTCCAGTCCCGACTCTGTCGTCACCCGAGTTGGCGGCACAGCTTGCCGAACTGTATTTGATGGCACTCGCCCGCGACGTACCGTTTATGCAATATGGCACCGATGAGATCACAACCACGGCCGCGGCAAATCTGGCGGGTATGGGTGGTTTCCCGAACCTGGACGCCGTTTCTATTGGATCAGATGGCACCGTGGACCCATTTTCGCAGTTGTTCCCTGCGACCTTCGTCGGTGTGGAAACAGGTCCATTCGTGTCGCAGTTATTGGTAAACTCTTTTACCATCGATGCCATTACTGTGGAACCTAAACAAGAGACTTTCGCACCAGATCTTAACTATATGGTTGACTTCGATGAGTTGCTGAACATCCAGAACGGTGGTCCGCCAGCGGGCCCCGAAGAACTCGACGAAGAATTACGCTTCATTCGCAATGCCCGCGATTTAGCACCTGTATCCTTTGTAGATAACATTAACACTGAAGCCTATCGCGGTTCCTTAATTCTGTTAGAACTGGGCGCGTTTTCGCCTCCTGGCATTAACGGTCCTTTTATAGATTCGGATCCTCAGGCAGGCTTCGTTAATTTTGGCACATCCAACTATTTTCGCCTGATCGGTGCCGCTGAACTGGCACAGCCTGCTTCCTGTTACCAAAAATTGCAGGTCAACCGCTTTGCACCTCCGGAGGCCTTGGGTGGTACCCTGAATAATACGATTGCTGGTGACCTTGACGCGGATTTCGACATTTCTCTGCTGGAAAATGATGAGCTGCTTAAACGCGTGGCCGAGATCAACGCGGCGCAGAATCCGAACAATGAAGTAACATATCTGCTGCCGCAGGCTATTCAGGTTGGCTCCCCTACTAATCCTTCCTACCCCTCGGGCAATGCGACGCAAAATGGCGCCTTTGCAACAGTACTCAAAGCCCTTATAGGCCTGGACCGCGGCGGCGAGTGCTTCCCTAACCCGGTTTTCCCATCTGATGATGGTTTGGAACTAATCAATTTCGAAGGCGCGTGCCTGACCTATGAAGGCGAAATTAATAAACTCGCAGTTAACGTTGCATTTGGTCCTCAGATGCTCGGGATCAACTATCGATTCGATGGTATTCAGGGTCTGCTGCTGGGGGAAACTATCACAGTGCGCACTCTGAACCAGGAGCTTATGACGTTTGCGGAAGAAGCGACGTTTGAGTTTCCTCTGTTTACGGGCGAAGTTATCAAGTTATTCCAGGACGGCACCTTTTCTATAGATGGCGATATGTGTTCAGGCCTGGTCTACACAGGTGTGGCTGATTGCCAAGCG</t>
+          <t>ATGCTGTGCAACGCCGCGGATACGACACCTGGATCACCAATGCCGGACACCGGCGTCCTCCCTCTGCTGACATCGGAACAGCGCGCGAAAGGATTGCCTCGCCAGCTAGAAGGTGAAAAGTCGCTTGGCTTTAACCCGTCTGAAACGCCGTACATTAAATATCTCGAAGGTTCTGAAACCTTGAAAAAAGTAAAACTACCGACCGACGGCATCTCCGCTTCTAAGATTCTTGGTAAAATCATGGCACGCGTCCCTATTGCGACGGCGCTGGCCGTGGTGCTTGCAGCGCCGTGTCTGGCTTTTGATGAGGTTACTGCGTCAGGTGTGTTCCCGGAAGAAAATAAAAACACAGGGGAAGGACGCAACCTTCAGACCTGCACGAACTCCGACGATGCGCTGGATCCAACGGCCCCTAATCCTCGCGATAACGTTGCGTTTGCCTCGCCTCCTGATGCGGCACCTCGCGAACCTGATGGTACGGGCACCGTGTGCCAAATCACGAATGGCGAAACGGACCTGGCGACCATGTTTAACAAATCTCTGCCGAACGACGAATTAGGACAGGTTACCGCAGACGACTTTGCAATCCTGGAAGATTGCATCCTGAACGGTGATTTCTCCATTTGTGAAGATGTCCCGGCCGGTGATCCAGCAGGTCCTCTTGTCAATCCTACGGCGGCCTTCGCCATCGATATTTCCGGCCCGGCTTTTTCCGCGACGACCATTCCGCCGGTGCCGACGTTATCATCCCCCGAGCTCGCGGCGCAGCTGGCGGAACTGTACTTGATGGCGCTGGCGCGCGATGTACCATTTATGCAATACGGAACCGACGAGATAACCACCACGGCTGCAGCCAATCTCGCGGGGATGGGTGGCTTTCCGAACCTGGATGCGGTTTCAATCGGCTCTGATGGCACCGTGGATCCGTTCTCTCAGCTGTTTCCTGCCACCTTTGTTGGCGTTGAAACGGGTCCATTTGTTTCACAACTGCTGGTGAATTCCTTTACGATTGATGCGATTACGGTTGAACCGAAACAGGAAACATTCGCTCCAGACCTCAACTATATGGTCGATTTCGATGAATTGCTGAACATACAGAACGGTGGCCCGCCAGCGGGCCCGGAGGAACTGGACGAGGAACTGCCTTTCATCCCTAACGCACGAGATCTGGCTCCTGTCTCTTTTGTGGACAACATCAACACGGAAGCGTATCGAGGTTCGTTGATTCTGTTGGAGCTAGGCGCTTTCTCACCTCCGGGTATCAACGGCCCGTTTATAGATTCAGATCCTCAGGCGGGTTTCGTAAACTTCGGCACCTCTAATTATTTTCGCTTAATTGGCGCGGCGGAATTGGCACAGCCTGCATCTTGCTATCAGAAATTGCAAGTGAATCCTTTTGCCCCTCCGGAAGCTCTGGGTGGCACACTGAATAACACCATCGCAGGAGATCTGGATGCAGATTTTGACATTTCTCTGCTGGAAAATGATGAACTGTTGAAACGCGTCGCAGAAATAAATGCGGCCCAGAACCCGAACAACGAGGTGACCTACCTGCTTCCACAGGCGATTCAAGTCGGCTCGCCGACTAACCCGTCCTACCCGTCTGGTAATGCAACGCAGAACGGTGCGTTCGCGACAGTTCTGAAAGCCCTCATCGGTCTGGATCCTGGGGGTGAATGCTTTCCGAACCCGGTGTTTCCGTCGGATGATGGCCTGGAGCTGATTAACTTTGAGGGTGCGTGTCTGACGTACGAAGGCGAAATCAATAAACTGGCCGTGAACGTGGCGTTTGGCCGCCAAATGTTAGGAATAAACTACCGCTTCGACGGAATTCAGGGTCTGCTGTTAGGAGAAACGATTACCGTTCCTACCCTTAACCAAGAATTGATGACCTTTGCGGAGGAAGCAACGTTCGAGTTTCGCTTATTTACGGGCGAGGTCATAAAGTTGTTCCAGGACGGCACCTTCTCTATTGATGGTGACATGTGTTCCGGTTTAGTCTATACCGGTGTCGCTGACTGCCAGGCG</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -1537,7 +1537,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>CGCTTGGCAATCAG</t>
+          <t>CGCCTGGCAGTCA</t>
         </is>
       </c>
     </row>
@@ -1900,22 +1900,22 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>TACTTTCGAAAACAACCGTAACGTCGGGAAGACCGGCGCAGCGGTGGAACGGACCCGCGTTGGAGGTTGCTCCTCTTGGTTGGTTGCTTGGGCGAAGAAAGACCAAGGCACACAGCGCAGGCGCTAAGTGAACTAAAAGACAGGGGCTGGCTTGGACGTTTTCACTGCGACGTCTTTGCGCATCTGTGCCGGTTTCTTCTTAAGGTCCACCCAGGGTGCACGTTATAATGATTGCCGCTACTTTGATTGCAGGGGCTGAAGTAGCCAGTCAAGTTGTTTAGTAATGGTTTGCTATTCAAACCGTGGCAGAGGTTCTGGAGGATGGTTTTTGAGGACCTGACACAAAAAAGACGACTACACTTGCATACGCTAGTCCAAGGCAGACCACGTAGGCGAGCCCCACGGTTTTACTAGTTAGGCAACCCGCCGTGACGGTTGGTCCATCTACCCCGACTAAGGCTATTGCATAAGTATTGCTGGGGACTACCACAAGACAGCCTTCTCGACCGCCGCGTCTACCGTCTTCAAATGAACTACCGCGACTGGGCTCTATAAGGGAAAAGTCTCAAGCGATGGTTGAGAGAACATGCGCGCCGGCGGCTCTTGAACCTTGGAGACGGCCGGAAATTCCCAGACTTATAAGGCTTTAGACGCCCACCGTTTTAGCTAGGCCAAGTCCTGGACAAGGGATGGCTGAACGGCCCACATTGGCGCCCAGGTCAACAAAGCGTCGACGAAGAGAGGCTGAAGCGGTAGCTGTTATAGCAACAAGGAGGCTTCGTCCACTGGGACCAATTTCTTTACCTAATGTACTGCTGGAAGGTTCTAAACAATCTGCAAGTCTTACCTCGGAGATTTCAGTTCTGACTTAAGCATCTACTTCTATTCGGGGAGAAGTAGGCGTTGCCCGCCCTAGACCGCCGGAATCGCAAGTGCCTAGATGACATATGCCTTCGCAAAGGACGACGCAATCAGTACAAGGCGGTTCCGTAAGACAGAAGTCGTCTCCCCGGCATAAGGTGGAGCCTCGGAGTCCACCCAAAACGCTGAAAACCACTTGGCTTATAAGACTGGAGGGAACGTCGGAGCAGCAGGAGATGAGCCTTACGGAACATACGTTTCAACGTCCACTTAGGACAGGACGGAGGGCTCCGTATACCCCCGAATCAATTATTGTGGAACTGACCGGGAGAGTTATGGGGTAATGGCTTTCGATAGAATGTCTTATGGCTTGACGAGTTAGCGCAAGCGTGGTTGTTGCGCTTTACATTACCGCTGCCATTTCCGCCGTTACCACTACCATGGATAAATGACGGCTACCGGCAGCGTCTTCCAAGGGGTCAATTGGGCCGTATGGGCAGACCATTGCGTTAATTAGACCCACGTATATAGTGGTGGGACTTTCGGAAGGACCCAAAACTCAATCCAGTCGGAACGATGGACCCACTGGACCACCACAGGTTGCTACTCCCATGGTTTGCGTAACTTATGCAAGGAGGATTTCCGCTTTGGACATAACTGGTCTTGCCGGCGCTTCAAGTCCCGAACTGCATGCTTCCGCTTAACTTATTTCAACGCAGCTTACAATAGTATCCAGCGAGCTTGTAGCCGCAGTTAATAGGATACCTACCACACATGCCCCGCAATTACCCACTTTGCAGCCGTCAAGCCGGAGAAGTCGTTCTTGACGGCTTGGAGAGCCTTCGGGGACTGTGATTTCCAAGTTAGGGTGGCCGAAGCATGTTCAAAGCGGACATAAGACCCTTCCAAGACCTTGAAGACCGCTTTCTATAGAAGTTTGAACTACCGGCTTGTACATTTCCGGAAATGTGCCCACTACTAAAAACACTACTTTTAGTCCTACCGCCGTTGATAGACCTCTTGGACCAGTTGTTCCCTCCACTAAAACGTAAGTTACAACTCGAC</t>
+          <t>TACTTTCGCAAGCATCCGTAGCGACGCGACGACCGTCGGAGGGGCGGCACAGACCCCCGATGCAGGTTACTTCTTTTAGTCGGCTGTTTAGGCAACGACAGGCCCAGCCAAACGGCCCACGGACTAAGAGACCTGAAGAACAGAGGCTGCCTTGCCCGCTTTCAATGTGACGTTTTTGCTCAACTGTGGCGCTTTCTTCTCAAAGTCCAGCCGGGTTGGACGTTGTATTGATTGCCACTACTCTGATTGCATGGCCTAAAGTAACCCGTCAAGTTATTTAGGGACGGATTACTGTTCAAGCCCTGTCACAGATTTTGCAGAATGGTCTTTGAAGACCTGACACAGAAAAGCCGCCTGCAGTTACAAACACTAGTCCAAGGCAGCCCTCGAAGACGAGCGCCCCGATTCTACTAGTTAGGAAACCCGCCTTGCCGGTTGGTCCAACTGCCACGACTAAGGCTATTGCACAAATAGTGATGAGGTCTGCCGCAAGAAAGTCTTCTCGACCGCCGAGTTTACCGACTTCAAATAAACTACCGAGACTGCGGACTGTAAGGTAAGAGACTCAAGCGTTGCTTGAGCGACCACGCGCGGCGGCGTCTTTTGGACCTTGCCGACGGCCGCAAGTTTCCGGACTTGTAGGGTTTTAGACGCCCACCATTTTAACTGGGCCATGTCCTGAACAAGGGATGCCTAAACGGCCCGCAATGTCGACCTGGACAACACAGGGTCGAGGACAATAGACTGAAACGCTAGCTATTATATCACCAAGGCGGATTCGTCCATTGAGACCAATTTCTTTACCTAATATACTGGTGCAAGGTTCTAAACGACCTACATGTTTTGCCGCGCAGATTTCACTTTTGGCTTAAACAACTGCTTCTATTTGGCAACAAATAAGCCTTGCCAGGACTGGACCGCCGGAACCGAAAGTGGCTGGACGACATATGTCTTCGGAAAGGACGCCGCGACCATTACAAAGCGGTCCCGTAAGAGAGGAGTCGCCTTCCAGGCATAAGGTGCAGACTCGCGGTCCACCCGAAACGCTGTAAGCCGCTTGGCTTGTAAAACTGTAGGAACCGCCGCAGTAGAAGTAGCTGGGCGTTACGGAACATGCGATTTAACGTCCAGTTAGCGCACGAGGCGGGTCTCCGTATACCACCGGACCAATTGTTATGAGACTGCCCGGGAAACTTATGGGGCGACGGGTTTCGCTAAGACGTCTTGTGGCTTGACGACTTGGCGCAAGCGTGGTTGTTACGCTTCACATTACCGCTACCATTTCCACCGTTGCCGCTACCGTGGATGAACGACGGTTACCGTCAGCGGCTTCCAAGTGGACACTTAGGTCGGATAGGTAGGCCATTGCGCTAATTGGACCCACGGATATAATGATGGGACTTTCGTAAAGACCCGAAGCTTAACCCAGTCGGAACAATAGAGCCGCTAGACCATCAAAGTTTACTGCTTCCATGGTTTGGATAGCTTATACAGGGCGGATTTCCTCTTTGCACGTAGCTGGTCTTGCCAGGACTTCATGTCCCGGACTGGATACTTCCGCTTGACTTGTTTCAACGCAGATTGCACTAGTAGCCAGGAAGATTATAGCCGCACTTAATGGGATACCTACCCCATATGCCGCGCGAATACCCACTTTGGAGACGTCATGGAGGAGACGTTGTTCTCGAAGGTTTAGAAAGACTCCGGGCTCTGTGATTCCCAAGTTAGGGTGGCCGAAGTATATTTAAGGGAAATATGAGTCCGTTTCATGACCTCGATGACCGCTTCCTGTAGAAGTTTGAGCTGCCAGCCTGCACGTTTCCAGACATATGGCCACTACTAAAGACGCTACTCTTAGTTCTACCACCGTTGATGGACCTTTTAGAACAATTATTTCCGCCACTAAAACGCAAATTGCACCTTGAC</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>ATGAAAGCTTTTGTTGGCATTGCAGCCCTTCTGGCCGCGTCGCCACCTTGCCTGGGCGCAACCTCCAACGAGGAGAACCAACCAACGAACCCGCTTCTTTCTGGTTCCGTGTGTCGCGTCCGCGATTCACTTGATTTTCTGTCCCCGACCGAACCTGCAAAAGTGACGCTGCAGAAACGCGTAGACACGGCCAAAGAAGAATTCCAGGTGGGTCCCACGTGCAATATTACTAACGGCGATGAAACTAACGTCCCCGACTTCATCGGTCAGTTCAACAAATCATTACCAAACGATAAGTTTGGCACCGTCTCCAAGACCTCCTACCAAAAACTCCTGGACTGTGTTTTTTCTGCTGATGTGAACGTATGCGATCAGGTTCCGTCTGGTGCATCCGCTCGGGGTGCCAAAATGATCAATCCGTTGGGCGGCACTGCCAACCAGGTAGATGGGGCTGATTCCGATAACGTATTCATAACGACCCCTGATGGTGTTCTGTCGGAAGAGCTGGCGGCGCAGATGGCAGAAGTTTACTTGATGGCGCTGACCCGAGATATTCCCTTTTCAGAGTTCGCTACCAACTCTCTTGTACGCGCGGCCGCCGAGAACTTGGAACCTCTGCCGGCCTTTAAGGGTCTGAATATTCCGAAATCTGCGGGTGGCAAAATCGATCCGGTTCAGGACCTGTTCCCTACCGACTTGCCGGGTGTAACCGCGGGTCCAGTTGTTTCGCAGCTGCTTCTCTCCGACTTCGCCATCGACAATATCGTTGTTCCTCCGAAGCAGGTGACCCTGGTTAAAGAAATGGATTACATGACGACCTTCCAAGATTTGTTAGACGTTCAGAATGGAGCCTCTAAAGTCAAGACTGAATTCGTAGATGAAGATAAGCCCCTCTTCATCCGCAACGGGCGGGATCTGGCGGCCTTAGCGTTCACGGATCTACTGTATACGGAAGCGTTTCCTGCTGCGTTAGTCATGTTCCGCCAAGGCATTCTGTCTTCAGCAGAGGGGCCGTATTCCACCTCGGAGCCTCAGGTGGGTTTTGCGACTTTTGGTGAACCGAATATTCTGACCTCCCTTGCAGCCTCGTCGTCCTCTACTCGGAATGCCTTGTATGCAAAGTTGCAGGTGAATCCTGTCCTGCCTCCCGAGGCATATGGGGGCTTAGTTAATAACACCTTGACTGGCCCTCTCAATACCCCATTACCGAAAGCTATCTTACAGAATACCGAACTGCTCAATCGCGTTCGCACCAACAACGCGAAATGTAATGGCGACGGTAAAGGCGGCAATGGTGATGGTACCTATTTACTGCCGATGGCCGTCGCAGAAGGTTCCCCAGTTAACCCGGCATACCCGTCTGGTAACGCAATTAATCTGGGTGCATATATCACCACCCTGAAAGCCTTCCTGGGTTTTGAGTTAGGTCAGCCTTGCTACCTGGGTGACCTGGTGGTGTCCAACGATGAGGGTACCAAACGCATTGAATACGTTCCTCCTAAAGGCGAAACCTGTATTGACCAGAACGGCCGCGAAGTTCAGGGCTTGACGTACGAAGGCGAATTGAATAAAGTTGCGTCGAATGTTATCATAGGTCGCTCGAACATCGGCGTCAATTATCCTATGGATGGTGTGTACGGGGCGTTAATGGGTGAAACGTCGGCAGTTCGGCCTCTTCAGCAAGAACTGCCGAACCTCTCGGAAGCCCCTGACACTAAAGGTTCAATCCCACCGGCTTCGTACAAGTTTCGCCTGTATTCTGGGAAGGTTCTGGAACTTCTGGCGAAAGATATCTTCAAACTTGATGGCCGAACATGTAAAGGCCTTTACACGGGTGATGATTTTTGTGATGAAAATCAGGATGGCGGCAACTATCTGGAGAACCTGGTCAACAAGGGAGGTGATTTTGCATTCAATGTTGAGCTG</t>
+          <t>ATGAAAGCGTTCGTAGGCATCGCTGCGCTGCTGGCAGCCTCCCCGCCGTGTCTGGGGGCTACGTCCAATGAAGAAAATCAGCCGACAAATCCGTTGCTGTCCGGGTCGGTTTGCCGGGTGCCTGATTCTCTGGACTTCTTGTCTCCGACGGAACGGGCGAAAGTTACACTGCAAAAACGAGTTGACACCGCGAAAGAAGAGTTTCAGGTCGGCCCAACCTGCAACATAACTAACGGTGATGAGACTAACGTACCGGATTTCATTGGGCAGTTCAATAAATCCCTGCCTAATGACAAGTTCGGGACAGTGTCTAAAACGTCTTACCAGAAACTTCTGGACTGTGTCTTTTCGGCGGACGTCAATGTTTGTGATCAGGTTCCGTCGGGAGCTTCTGCTCGCGGGGCTAAGATGATCAATCCTTTGGGCGGAACGGCCAACCAGGTTGACGGTGCTGATTCCGATAACGTGTTTATCACTACTCCAGACGGCGTTCTTTCAGAAGAGCTGGCGGCTCAAATGGCTGAAGTTTATTTGATGGCTCTGACGCCTGACATTCCATTCTCTGAGTTCGCAACGAACTCGCTGGTGCGCGCCGCCGCAGAAAACCTGGAACGGCTGCCGGCGTTCAAAGGCCTGAACATCCCAAAATCTGCGGGTGGTAAAATTGACCCGGTACAGGACTTGTTCCCTACGGATTTGCCGGGCGTTACAGCTGGACCTGTTGTGTCCCAGCTCCTGTTATCTGACTTTGCGATCGATAATATAGTGGTTCCGCCTAAGCAGGTAACTCTGGTTAAAGAAATGGATTATATGACCACGTTCCAAGATTTGCTGGATGTACAAAACGGCGCGTCTAAAGTGAAAACCGAATTTGTTGACGAAGATAAACCGTTGTTTATTCGGAACGGTCCTGACCTGGCGGCCTTGGCTTTCACCGACCTGCTGTATACAGAAGCCTTTCCTGCGGCGCTGGTAATGTTTCGCCAGGGCATTCTCTCCTCAGCGGAAGGTCCGTATTCCACGTCTGAGCGCCAGGTGGGCTTTGCGACATTCGGCGAACCGAACATTTTGACATCCTTGGCGGCGTCATCTTCATCGACCCGCAATGCCTTGTACGCTAAATTGCAGGTCAATCGCGTGCTCCGCCCAGAGGCATATGGTGGCCTGGTTAACAATACTCTGACGGGCCCTTTGAATACCCCGCTGCCCAAAGCGATTCTGCAGAACACCGAACTGCTGAACCGCGTTCGCACCAACAATGCGAAGTGTAATGGCGATGGTAAAGGTGGCAACGGCGATGGCACCTACTTGCTGCCAATGGCAGTCGCCGAAGGTTCACCTGTGAATCCAGCCTATCCATCCGGTAACGCGATTAACCTGGGTGCCTATATTACTACCCTGAAAGCATTTCTGGGCTTCGAATTGGGTCAGCCTTGTTATCTCGGCGATCTGGTAGTTTCAAATGACGAAGGTACCAAACCTATCGAATATGTCCCGCCTAAAGGAGAAACGTGCATCGACCAGAACGGTCCTGAAGTACAGGGCCTGACCTATGAAGGCGAACTGAACAAAGTTGCGTCTAACGTGATCATCGGTCCTTCTAATATCGGCGTGAATTACCCTATGGATGGGGTATACGGCGCGCTTATGGGTGAAACCTCTGCAGTACCTCCTCTGCAACAAGAGCTTCCAAATCTTTCTGAGGCCCGAGACACTAAGGGTTCAATCCCACCGGCTTCATATAAATTCCCTTTATACTCAGGCAAAGTACTGGAGCTACTGGCGAAGGACATCTTCAAACTCGACGGTCGGACGTGCAAAGGTCTGTATACCGGTGATGATTTCTGCGATGAGAATCAAGATGGTGGCAACTACCTGGAAAATCTTGTTAATAAAGGCGGTGATTTTGCGTTTAACGTGGAACTG</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>ATGAAAGCTTTTGTTGGC</t>
+          <t>ATGAAAGCGTTCGTAGG</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>CAGCTCAACATTGAATGC</t>
+          <t>CAGTTCCACGTTAAACG</t>
         </is>
       </c>
     </row>
@@ -1942,22 +1942,22 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>TACCCGAGCCACTGGGGATAGGGGGACGGCTTTTAGCTGCTTGGTCTTCTTATATTGTGATTGATGTAAGACAAAAACTTGTTACATCCGGACCTCGACTTAGCGCAATGCTTGTGGCACCCGCCCGGCGAATGACCAGGTGGCAATAGACGCGGACGGGACCCGTACGAATTGGAGCGGTAATTACTACGCATGAAAAGTTAGACGGGTGGATGGCTAAAGTGGTGGAAAAACAGCGGCCTGTGCCTTTTGCGACGGATGGGAGACGGCAGTGGCTTACCCCGTTTACTGCGAGCGGTTCGACAACGGCCACGGCGCGACTTTTACGAAAGAAGTAATATATACTTTGGCCAACTTGTCGGATTGGGCTTGGGCCCACGGTTATAGAGACTGTTACGTATGCGCGTTGACCCGGACCACGAGCTGGCGAGCCAAGAGCTCCGAGGACCGCCACAGCTGGCCCTTAGGCGTAGCAAGTACAAGCCACTTCTGCACCGGCTACATAAGAAACGGGACAATTTGCTGGGAGGACCGCGGAGGGTTCTTCCGATGTTGGGCTGGGGCCCGGCGATATTTAAACTACTACTTGGCTGTTTGGGCCACCATAACTAAGGCCAACTGGGATTATTAGGATTACCGGGATTCTACGGCAAAGGAGTCATATTGCGCGGAAAGATACCGTTTTGGTGGTTTGCTAAGCGCTGAGTCAGTCTCTTAAAAGACCGTCTAGGAGGACCGAACGCCAGTTTGCGACTGCTTTGGCGTCTTATACTGCTGCGGCAGGGACAACGCTAACGCTACCCCCCGCGCGTCCGTGACTTGAGATGGTTTGGAAGCGGAAACGTTTGTCGGGTCCCAGACATAAACCGAATACTACCTAGCTTGGACTAACCGTGGGGTGGTGGAAAAATATTGGTTTAACAGGGAGCGTAGCGGCACTGTATATTTTTTCTTCTTCTGAATCGGTTAAGACTCCAGTTATTGCGCCTAAAACGGGCGGACAAACGCGACCAACTGCAGCGCACATGCCTGCGGCCGTAAAAGAGTAACTTTCTTTTTAACCTCAAGCTTAAAAACGGAGGCGACAGGCCACACGCTCTGCTACCAGGAGGTCTGTTGCCACTAGGGAAAAACGAGTGGGACCCGCGGGGTCGCTGGTTGTGGTTACTGTAGGGCAAATTTGGCGGCAAAGGACGCATAGGAAGTCCATTGCGTTGTAAACCGCCACGCCATAAGGTCTACCACGCGGGAATGATGTTGCCGGGACAGCCGTGGAACTTTCTACTGCTCGGCCTATTATAACGTTAACTATACTACTAAAGGCTCCTTGAATTACCACACTTGGGACTAAACGCGGTCGGCATACTAGGCTGGCGAGGCTAACTTCTAGTCGGTCCGTAACACGCGTGCGCGTAGCACGGATTGAAACTGAGGCGCAACCTTAATTACAAACTCTTACGTTAAAGAGGATATAAGAACCCGCACTTAAACGGAAAGCTGCGGCGACGACGTGGACTATAAAATTAGGGTTGGTGCTGGTTTCTGCACATACGCCAACTGTTATTGCCACGCTGACAGAAGGTCTTGCAGCTTCTATAGGGAATATGGTGCGCGCCGTGGGGACTTCTGGGGCTTCCGGAAAAAGGTTAACCGCCGCATGGGGAACCATAGCTTTAGCGACTGCTTTAAAAATTGTTGCCGAATTTTGGCTGGGGCGGTCTTTAAGTTGGATACGGCGTCCTTTGCGGCCACGTCTTTGGCCAACCCGTCGTCGGTCATTTTCCATACAACCTTCTCCTCGTCCGGGGACAACACTTTCTTCGGGGC</t>
+          <t>TACCCTAGACACTGGGGTTAAGGAGACGGCTTTTAGCTACTTGGCCTTCTTATATTGTGATTGATATAAGAGAAAAACTTGTTGCACCCGGACCTTAACTTGGGACATTGGTTGTGGCATCCGCCGGGCGAGTGTCCGGGTGGCGACAGTCGCGCGCGAGAACCGTACAACTTAGACCGGTAATTGCTACGCATGAAGAGATAAACGGGCGGTTGGCTAAAATGCTGCAAAGAAAGTGGCCTGTGGCTTTTGCGACGCATGGCGGACGGCAGGGGTTTACCCCGGTTGCTACGTGCGGTCCGACACCGGCCGCGTCGGAATTTTTACGACAGGAGTGACATGTACTTTGGCCACCTTGTCGGATTGGGCTTAGGCCCACGGTTATAAAGACTATTGCGTATACGAGTTGACCCGGACCAAGATCTGGGAAGTCAGGACCTCCGCGGCCCGCCGCACCTAGCGCTTAGCCGCAGTAAATACAAGCCACTCCTGCATCGTCTGCAAAAGAAACGAGACAATTTACTAGGCGGACCACGAAGTGTTCTTCCAATGTTGGGCTGGGGCCCCGCGATATTTAAACTGCTGCTTGGATGCTTGGGCCAGCACGAGTATGGTCAACTAGGCTTGTTGGGTTTGCCAGGCTTCTACGGCAAGGCGGTCATGTTGCGTGGCAAGATGCCGTTTTGGTGCTTTGCGAAACGCTGAGTCAGCCTTTTGAAAGAACGCCTGGGGGGACCCGACGCGAGGTTACGCCTACTTTGGCGGCTTATGCTACTACGTCAAGGACACCGGTAACGCTACCCGCCGCGAGTTCGGGACTTAAGTTGGTTTGCGAGGGGCAACGTCTGGCGGGTCCCGGAAATGAACCGCATACTGCCAAGCTTAGACTAACCGTGGGGAGGCGCGAAGATATTGGTCTAACACGGAGGATAACGTCAGTGGATGTTTTTTCTTCTTCTGGAACGGTTGAGACTTCACTTGTTACGGCTAAAGCGGGCGGATAAGCGGGACCATCTACAACGTACATGACTACGACCCTAAAAGAGCAACTTTCTTTTCAACCTCAAACTTAAAAACGCGGGAGACAGACCGCAGGGACTACTACCGGGAGGCCTATTGCCGCTAGGCAAAAACGACTGGAACCCTCGTGGTCGCTGATTGTGATTGCTGTAGGGCAAGTTCGGCGGCAAGGGACGAATAGGCAGACCGTTGCGCTGAAAACCTCCGCGGCAAAAGGTCTACCAAGCGGCGATAATATTGCCGGCCCACCCGTGGAACTTTCTACTACTCGGCCTGTTGTAGCGCTAGCTGTACTACTAGAGACTCCTTGACTTGCCACAGTTGGGACTAGACGCGGTTGGCATACTGGGCTGCCGCGGGTAGCTTCTAGTCGGCCCGTAGCAGGCGTGAGCGTATCATGCTTTAAAGCTGAGTCGAAACCTTAATTACAAACTTTTGCGATAAAGGGCGTAAAAAGAGCCGCAGTTGAACGCCAAACTGCGCCGCCGTCGGGCGCTATAGGACTAGGGCTGCTGTTGGTTCCTGCAGATACGACACCTATTGTTACCACGTTGGCACAAAGTCTTACACCTCCTATAAGCGATATGATGCGGACCGTGGGGACTCCTAGGACTTCCCGACAAGGGCTAGCCGCCACACGGCGACCCATAACTTTAACGCCTGCTCTAGAAATTATTGCCGGACTTTGGATGGGGCGGGCTCTAAGTTGGCTACGGGGTCCTCTGAGGTCATGTCTTTGGCCAGCCAGTCGTCGGCCATTTTCCGTACAACCTCCTTCTCGTCCGGGGACACCAGTTTCTTCGCGGG</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>ATGGGCTCGGTGACCCCTATCCCCCTGCCGAAAATCGACGAACCAGAAGAATATAACACTAACTACATTCTGTTTTTGAACAATGTAGGCCTGGAGCTGAATCGCGTTACGAACACCGTGGGCGGGCCGCTTACTGGTCCACCGTTATCTGCGCCTGCCCTGGGCATGCTTAACCTCGCCATTAATGATGCGTACTTTTCAATCTGCCCACCTACCGATTTCACCACCTTTTTGTCGCCGGACACGGAAAACGCTGCCTACCCTCTGCCGTCACCGAATGGGGCAAATGACGCTCGCCAAGCTGTTGCCGGTGCCGCGCTGAAAATGCTTTCTTCATTATATATGAAACCGGTTGAACAGCCTAACCCGAACCCGGGTGCCAATATCTCTGACAATGCATACGCGCAACTGGGCCTGGTGCTCGACCGCTCGGTTCTCGAGGCTCCTGGCGGTGTCGACCGGGAATCCGCATCGTTCATGTTCGGTGAAGACGTGGCCGATGTATTCTTTGCCCTGTTAAACGACCCTCCTGGCGCCTCCCAAGAAGGCTACAACCCGACCCCGGGCCGCTATAAATTTGATGATGAACCGACAAACCCGGTGGTATTGATTCCGGTTGACCCTAATAATCCTAATGGCCCTAAGATGCCGTTTCCTCAGTATAACGCGCCTTTCTATGGCAAAACCACCAAACGATTCGCGACTCAGTCAGAGAATTTTCTGGCAGATCCTCCTGGCTTGCGGTCAAACGCTGACGAAACCGCAGAATATGACGACGCCGTCCCTGTTGCGATTGCGATGGGGGGCGCGCAGGCACTGAACTCTACCAAACCTTCGCCTTTGCAAACAGCCCAGGGTCTGTATTTGGCTTATGATGGATCGAACCTGATTGGCACCCCACCACCTTTTTATAACCAAATTGTCCCTCGCATCGCCGTGACATATAAAAAAGAAGAAGACTTAGCCAATTCTGAGGTCAATAACGCGGATTTTGCCCGCCTGTTTGCGCTGGTTGACGTCGCGTGTACGGACGCCGGCATTTTCTCATTGAAAGAAAAATTGGAGTTCGAATTTTTGCCTCCGCTGTCCGGTGTGCGAGACGATGGTCCTCCAGACAACGGTGATCCCTTTTTGCTCACCCTGGGCGCCCCAGCGACCAACACCAATGACATCCCGTTTAAACCGCCGTTTCCTGCGTATCCTTCAGGTAACGCAACATTTGGCGGTGCGGTATTCCAGATGGTGCGCCCTTACTACAACGGCCCTGTCGGCACCTTGAAAGATGACGAGCCGGATAATATTGCAATTGATATGATGATTTCCGAGGAACTTAATGGTGTGAACCCTGATTTGCGCCAGCCGTATGATCCGACCGCTCCGATTGAAGATCAGCCAGGCATTGTGCGCACGCGCATCGTGCCTAACTTTGACTCCGCGTTGGAATTAATGTTTGAGAATGCAATTTCTCCTATATTCTTGGGCGTGAATTTGCCTTTCGACGCCGCTGCTGCACCTGATATTTTAATCCCAACCACGACCAAAGACGTGTATGCGGTTGACAATAACGGTGCGACTGTCTTCCAGAACGTCGAAGATATCCCTTATACCACGCGCGGCACCCCTGAAGACCCCGAAGGCCTTTTTCCAATTGGCGGCGTACCCCTTGGTATCGAAATCGCTGACGAAATTTTTAACAACGGCTTAAAACCGACCCCGCCAGAAATTCAACCTATGCCGCAGGAAACGCCGGTGCAGAAACCGGTTGGGCAGCAGCCAGTAAAAGGTATGTTGGAAGAGGAGCAGGCCCCTGTTGTGAAAGAAGCCCCG</t>
+          <t>ATGGGATCTGTGACCCCAATTCCTCTGCCGAAAATCGATGAACCGGAAGAATATAACACTAACTATATTCTCTTTTTGAACAACGTGGGCCTGGAATTGAACCCTGTAACCAACACCGTAGGCGGCCCGCTCACAGGCCCACCGCTGTCAGCGCGCGCTCTTGGCATGTTGAATCTGGCCATTAACGATGCGTACTTCTCTATTTGCCCGCCAACCGATTTTACGACGTTTCTTTCACCGGACACCGAAAACGCTGCGTACCGCCTGCCGTCCCCAAATGGGGCCAACGATGCACGCCAGGCTGTGGCCGGCGCAGCCTTAAAAATGCTGTCCTCACTGTACATGAAACCGGTGGAACAGCCTAACCCGAATCCGGGTGCCAATATTTCTGATAACGCATATGCTCAACTGGGCCTGGTTCTAGACCCTTCAGTCCTGGAGGCGCCGGGCGGCGTGGATCGCGAATCGGCGTCATTTATGTTCGGTGAGGACGTAGCAGACGTTTTCTTTGCTCTGTTAAATGATCCGCCTGGTGCTTCACAAGAAGGTTACAACCCGACCCCGGGGCGCTATAAATTTGACGACGAACCTACGAACCCGGTCGTGCTCATACCAGTTGATCCGAACAACCCAAACGGTCCGAAGATGCCGTTCCGCCAGTACAACGCACCGTTCTACGGCAAAACCACGAAACGCTTTGCGACTCAGTCGGAAAACTTTCTTGCGGACCCCCCTGGGCTGCGCTCCAATGCGGATGAAACCGCCGAATACGATGATGCAGTTCCTGTGGCCATTGCGATGGGCGGCGCTCAAGCCCTGAATTCAACCAAACGCTCCCCGTTGCAGACCGCCCAGGGCCTTTACTTGGCGTATGACGGTTCGAATCTGATTGGCACCCCTCCGCGCTTCTATAACCAGATTGTGCCTCCTATTGCAGTCACCTACAAAAAAGAAGAAGACCTTGCCAACTCTGAAGTGAACAATGCCGATTTCGCCCGCCTATTCGCCCTGGTAGATGTTGCATGTACTGATGCTGGGATTTTCTCGTTGAAAGAAAAGTTGGAGTTTGAATTTTTGCGCCCTCTGTCTGGCGTCCCTGATGATGGCCCTCCGGATAACGGCGATCCGTTTTTGCTGACCTTGGGAGCACCAGCGACTAACACTAACGACATCCCGTTCAAGCCGCCGTTCCCTGCTTATCCGTCTGGCAACGCGACTTTTGGAGGCGCCGTTTTCCAGATGGTTCGCCGCTATTATAACGGCCGGGTGGGCACCTTGAAAGATGATGAGCCGGACAACATCGCGATCGACATGATGATCTCTGAGGAACTGAACGGTGTCAACCCTGATCTGCGCCAACCGTATGACCCGACGGCGCCCATCGAAGATCAGCCGGGCATCGTCCGCACTCGCATAGTACGAAATTTCGACTCAGCTTTGGAATTAATGTTTGAAAACGCTATTTCCCGCATTTTTCTCGGCGTCAACTTGCGGTTTGACGCGGCGGCAGCCCGCGATATCCTGATCCCGACGACAACCAAGGACGTCTATGCTGTGGATAACAATGGTGCAACCGTGTTTCAGAATGTGGAGGATATTCGCTATACTACGCCTGGCACCCCTGAGGATCCTGAAGGGCTGTTCCCGATCGGCGGTGTGCCGCTGGGTATTGAAATTGCGGACGAGATCTTTAATAACGGCCTGAAACCTACCCCGCCCGAGATTCAACCGATGCCCCAGGAGACTCCAGTACAGAAACCGGTCGGTCAGCAGCCGGTAAAAGGCATGTTGGAGGAAGAGCAGGCCCCTGTGGTCAAAGAAGCGCCC</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>ATGGGCTCGGTGA</t>
+          <t>ATGGGATCTGTGACC</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>CGGGGCTTCTTTCA</t>
+          <t>GGGCGCTTCTTTGA</t>
         </is>
       </c>
     </row>
@@ -1984,22 +1984,22 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>TACTGCTAGCTGAAATGGGGCCACCTTGACGGTCATCACCTTCTTCTACGCCTTATGTTAAACTTGATGTAGGACAAGAACTTGTTGCATCCAAATCTTGAATTAGGACATTGCTTGTGTAAGCCACGCGAGTTTCGCCCGGGAGGCGACAGCGGCGGACGAGAACCGTACGAAGTTGACCGTCAGTTACTGCGTATGAAACGTTAATTAGGCAGTCGACCCAAATGGTGGAAAGACTGCGGGCCGCGTCTCCTACCTCGCATGGGAGACGGTCTAGGAAGAATGCGCTTTCTACGGGGAGTTCGACAACGTCCGCGCCGCTAACGGTACGACAGGTTTGACATATACTTCGGCTTTCATCACGGCGCGAGGGGCTAAAGATTATTACGCATACGTGTCGACGTTTTACATGACCTGTAGAGGCATTGCTTTCGCGGCCGCCGGACGCTAGGTCGGAGAAGAAGAAAGTAGAAGCCCTTTCGCCACCGGTGGCGACAAAAGCTAAATGACAAGTTGTTCCTTCCACGGCTAGTCAGGCCAATAAGTGGCTTTGGACCTGGTAAATTTAAATTGCTACTTGGCTGGTTGGGTCAGCTTGAGTAAGGTCATCTACGTTTGTAAGGCCTACCACTGTTTTACGGCGGAGGAGTCATATTGCGCGGTATAATACCGCTTTGGCGGTTCGGAAAGCCCTGGGTCTGGCTTTTATACGACCGGCTAGGTGGCCCATAGGGAACACGCCCTCTTCAACGTCTTATACTACTGCGTTAGGCCCTTCACATGCGGTACCCGCCACGCGGCCCAGAGTTGTGGTGCTTTGGATGAGGCTTAGTTTGCCACGTTCCGTACAAAAACCGTATGCTACCGGGCTTTGAGTAGCCATGGGGTGGCGCGGACATATTAGTCTAACACGGATTTTAGCGTCACTGCATGTTTTTTCTATTGCTAGACCATTTAAGACTTCAATTATTGCGCCTAAAACGTGGAAATGACCGGAATCAATTGCAGCGGTACTGTCTGCGCCCGTAAAAACGGAACTTTCTTTTTAACCTTAAACTTAAAAACGGAGGTGAGAGCCCACAAGCCCTACTACATGACGCCCTAGGTCTCCCGTTCCGAAGGTGACGACGTTAATTAAGCCCAAACCGAAGACGGGGCGTCAACGTTTTGAGACTACTTCGAGGAAAATTTGGCGGCAAGGGCCGAATAGGCAGACCATTGCGTTGGAAACCGCGACGCCGGAAAGTCTACCATGGATTCATAATGTTGCCAGGAGACCCATTCAACCGCTGGTGGAGCGGACTGTGGTAGCGCCAGCTTTACAAGCACAGTCTTCTCGACTTACCACACAGAGCCCTAGACAGATTGGGTATACTAGGCTTTGCGGGATAATGACTAGTTGGCCCTTAGCAGGGTTGGGGATACGGCGCGGCGAAGAGCAGGACGAACCTTTACTACAAGCTTTTGCGACACAGCGGATAGAAAGAGCCGCAATTGAACGGAAAGCTACGCCGTCGACCTGTTCTATAGGACTAGGGATGATGGTTTTTTCTGCACATACGCCACCTACTATTTCCGCGTCGTGACAAATTCTTGCACCTTCTATAAGGAATGTTCTGGTTCCCTTGTGCGTTCCCGTTATTTCCCGACAATGGCTAGCCCCCACAAGGTGACCCGTAGCTTTAGCGTTTGCTCTAGATATTATTATTCAACAGAGGATGAGGCGGACCGCTTGTTGGCTACGGCGTTGGCGGCGTCTTAGTTCCCGGTGGCGGATTTTTTCCGCTTGACCGTCTCCGCTTCCTACTTCTTGTCCGAGGCTACTACCTGCATCGCGGC</t>
+          <t>TACTGGTAGCTAAAATGGGGTCAACTTAACGGGCACCACCTTCTTCTGCGGCTCATGTTGAACTTAATATAAGACAAGAACTTGTTACAGCCCGACCTTGACTTAGCGCATTGGTTATGTAAGCCGCGCAATTTTCGACCGGGTGGAGACAGTGGTGCGCGAAATCCCTACAATGTCGATCGTCAGTTGCTGCGGATGAAACGCTAATTGGGTAGACGGCCAAAATGGTGTAAAGACTGGGGCCCCCGCCTCCTGCCCCGCATAGCGGACGGTCTGGGCAGGATACGCTTTCTGCGAGCGGTTCGCCAACGCCCGCGCCGCTAACGCTACAATAGGTTTGACATGTACTTTGGGTTCCACCACGGTGGAAGCGGCTAGAGCTTGTTGCGCATACGTGTCGAAGTCTTACAAGAACTATAAAGGCAATGGTTTCGAGGACGACGAACGCTAGGCCGTAGTAGAAGAAAGTAGAAGCCATTTCGGCATCGGTGGCGGCACAAACTAGACGACAAATTGTTTCTTCCGCGCCTAGTTAGTCCTATAAGTGGGTTTGGGCCAGGCAAGTTTAAATTACTGCTTGGCTGCTTGGGTCATCTCGAATAGGGTCAACTACGCTTATAAGGGCTACCGCTATTTTACGGCGCGGCGGTTATATTACGAGGCATGATGCCCCTCTGGCGATTTGCTAAACCTTGGGTTTGGCTTTTATACAACCGGCTGGGCGGGCCTTATGGAACGCGTCCACTCCACCGACTTATGCTACTGCGGTAGGGACTTCACATGCGCTACCCACCCCGCGGTCCCGACTTGTGCTGCTTTGCGTGCGGATTAGTCTGCCAGGTCCCATACAAGAACCGCATGCTACCCGGTTTTGACTAGCCATGGGGCGGCGCGAACATATTGGTCTAGCAAGGATTTTAACGACACTGTATATTCTTTCTGTTACTGAATCACTTGAGGCTCCAGTTATTACGACTGAAGCGCGGAAACGACCGCGACCACTTACACCGGTACTGTCTACGCCCCTAAAAACGTAACTTTCTCTTTAACCTTAAACTTAAAAACGCGGGCGACAGCCCGCAAGGACTGCTGCAAGACGCGCTAGGCCTTCCATTTCGGAGGTGTCGCCGATAGTTGAGCCCAGACCGCAGTCGCGGCGTCAACGTTTTGAGGCTGCTTCGAGGCAAGTTTGGGGGCAAAGGCCGAATAGGTAGACCGTTGCGATGAAAACCACGACGTCGGAAGGTCTACCATGGATTTATGATGTTACCAGCGGAGCCATTTAACCGTTGGTGAAGAGCGCTGTGTTAACGGCAACTTTACAAGCAAAGGCTTCTTGACTTGCCTCAAAGCGCGCTAGACAGGTTGGGCATACTGGGCTTTGCGGGCTAATGACTGGTTGGCCCCTATCAGGGCTGGGCTTACGGCGGAGCGAAGAGCAGCACGAACCTCTACTACAAGCTTTTGCGTCACAGAGCCTAGAAGAACCCGCAATTAAACGGAAAACTGCGTCGCCGGCCAGTCCTATAAAACTAGGGTTGATGGTTTTTCCTGCAGATACGCCAACTACTATTTCCGCGACGCAATAAGTTTTTACAACTTCTGTAAGCGATATTTTGGTTTCCATGGGGATTTCCGTTGTTTCCGGAGGAGGGATAGCCGCCCCAAGGAGACCCATAACTTTAGCGCTTGCTCTAAATGTTGTTGTTTAATAGGGGTTGGGGCGGCCCGCTTGTCGGCTACGGCGTTGGCGGTGTTTTAGTTCCAGGCGGCGCCTTCTTTCCGCTCGACCGCCTTCGTTTTCTACTTCTCGTCCGAGGCTACTACCTACACCGCGGC</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>ATGACGATCGACTTTACCCCGGTGGAACTGCCAGTAGTGGAAGAAGATGCGGAATACAATTTGAACTACATCCTGTTCTTGAACAACGTAGGTTTAGAACTTAATCCTGTAACGAACACATTCGGTGCGCTCAAAGCGGGCCCTCCGCTGTCGCCGCCTGCTCTTGGCATGCTTCAACTGGCAGTCAATGACGCATACTTTGCAATTAATCCGTCAGCTGGGTTTACCACCTTTCTGACGCCCGGCGCAGAGGATGGAGCGTACCCTCTGCCAGATCCTTCTTACGCGAAAGATGCCCCTCAAGCTGTTGCAGGCGCGGCGATTGCCATGCTGTCCAAACTGTATATGAAGCCGAAAGTAGTGCCGCGCTCCCCGATTTCTAATAATGCGTATGCACAGCTGCAAAATGTACTGGACATCTCCGTAACGAAAGCGCCGGCGGCCTGCGATCCAGCCTCTTCTTCTTTCATCTTCGGGAAAGCGGTGGCCACCGCTGTTTTCGATTTACTGTTCAACAAGGAAGGTGCCGATCAGTCCGGTTATTCACCGAAACCTGGACCATTTAAATTTAACGATGAACCGACCAACCCAGTCGAACTCATTCCAGTAGATGCAAACATTCCGGATGGTGACAAAATGCCGCCTCCTCAGTATAACGCGCCATATTATGGCGAAACCGCCAAGCCTTTCGGGACCCAGACCGAAAATATGCTGGCCGATCCACCGGGTATCCCTTGTGCGGGAGAAGTTGCAGAATATGATGACGCAATCCGGGAAGTGTACGCCATGGGCGGTGCGCCGGGTCTCAACACCACGAAACCTACTCCGAATCAAACGGTGCAAGGCATGTTTTTGGCATACGATGGCCCGAAACTCATCGGTACCCCACCGCGCCTGTATAATCAGATTGTGCCTAAAATCGCAGTGACGTACAAAAAAGATAACGATCTGGTAAATTCTGAAGTTAATAACGCGGATTTTGCACCTTTACTGGCCTTAGTTAACGTCGCCATGACAGACGCGGGCATTTTTGCCTTGAAAGAAAAATTGGAATTTGAATTTTTGCCTCCACTCTCGGGTGTTCGGGATGATGTACTGCGGGATCCAGAGGGCAAGGCTTCCACTGCTGCAATTAATTCGGGTTTGGCTTCTGCCCCGCAGTTGCAAAACTCTGATGAAGCTCCTTTTAAACCGCCGTTCCCGGCTTATCCGTCTGGTAACGCAACCTTTGGCGCTGCGGCCTTTCAGATGGTACCTAAGTATTACAACGGTCCTCTGGGTAAGTTGGCGACCACCTCGCCTGACACCATCGCGGTCGAAATGTTCGTGTCAGAAGAGCTGAATGGTGTGTCTCGGGATCTGTCTAACCCATATGATCCGAAACGCCCTATTACTGATCAACCGGGAATCGTCCCAACCCCTATGCCGCGCCGCTTCTCGTCCTGCTTGGAAATGATGTTCGAAAACGCTGTGTCGCCTATCTTTCTCGGCGTTAACTTGCCTTTCGATGCGGCAGCTGGACAAGATATCCTGATCCCTACTACCAAAAAAGACGTGTATGCGGTGGATGATAAAGGCGCAGCACTGTTTAAGAACGTGGAAGATATTCCTTACAAGACCAAGGGAACACGCAAGGGCAATAAAGGGCTGTTACCGATCGGGGGTGTTCCACTGGGCATCGAAATCGCAAACGAGATCTATAATAATAAGTTGTCTCCTACTCCGCCTGGCGAACAACCGATGCCGCAACCGCCGCAGAATCAAGGGCCACCGCCTAAAAAAGGCGAACTGGCAGAGGCGAAGGATGAAGAACAGGCTCCGATGATGGACGTAGCGCCG</t>
+          <t>ATGACCATCGATTTTACCCCAGTTGAATTGCCCGTGGTGGAAGAAGACGCCGAGTACAACTTGAATTATATTCTGTTCTTGAACAATGTCGGGCTGGAACTGAATCGCGTAACCAATACATTCGGCGCGTTAAAAGCTGGCCCACCTCTGTCACCACGCGCTTTAGGGATGTTACAGCTAGCAGTCAACGACGCCTACTTTGCGATTAACCCATCTGCCGGTTTTACCACATTTCTGACCCCGGGGGCGGAGGACGGGGCGTATCGCCTGCCAGACCCGTCCTATGCGAAAGACGCTCGCCAAGCGGTTGCGGGCGCGGCGATTGCGATGTTATCCAAACTGTACATGAAACCCAAGGTGGTGCCACCTTCGCCGATCTCGAACAACGCGTATGCACAGCTTCAGAATGTTCTTGATATTTCCGTTACCAAAGCTCCTGCTGCTTGCGATCCGGCATCATCTTCTTTCATCTTCGGTAAAGCCGTAGCCACCGCCGTGTTTGATCTGCTGTTTAACAAAGAAGGCGCGGATCAATCAGGATATTCACCCAAACCCGGTCCGTTCAAATTTAATGACGAACCGACGAACCCAGTAGAGCTTATCCCAGTTGATGCGAATATTCCCGATGGCGATAAAATGCCGCGCCGCCAATATAATGCTCCGTACTACGGGGAGACCGCTAAACGATTTGGAACCCAAACCGAAAATATGTTGGCCGACCCGCCCGGAATACCTTGCGCAGGTGAGGTGGCTGAATACGATGACGCCATCCCTGAAGTGTACGCGATGGGTGGGGCGCCAGGGCTGAACACGACGAAACGCACGCCTAATCAGACGGTCCAGGGTATGTTCTTGGCGTACGATGGGCCAAAACTGATCGGTACCCCGCCGCGCTTGTATAACCAGATCGTTCCTAAAATTGCTGTGACATATAAGAAAGACAATGACTTAGTGAACTCCGAGGTCAATAATGCTGACTTCGCGCCTTTGCTGGCGCTGGTGAATGTGGCCATGACAGATGCGGGGATTTTTGCATTGAAAGAGAAATTGGAATTTGAATTTTTGCGCCCGCTGTCGGGCGTTCCTGACGACGTTCTGCGCGATCCGGAAGGTAAAGCCTCCACAGCGGCTATCAACTCGGGTCTGGCGTCAGCGCCGCAGTTGCAAAACTCCGACGAAGCTCCGTTCAAACCCCCGTTTCCGGCTTATCCATCTGGCAACGCTACTTTTGGTGCTGCAGCCTTCCAGATGGTACCTAAATACTACAATGGTCGCCTCGGTAAATTGGCAACCACTTCTCGCGACACAATTGCCGTTGAAATGTTCGTTTCCGAAGAACTGAACGGAGTTTCGCGCGATCTGTCCAACCCGTATGACCCGAAACGCCCGATTACTGACCAACCGGGGATAGTCCCGACCCGAATGCCGCCTCGCTTCTCGTCGTGCTTGGAGATGATGTTCGAAAACGCAGTGTCTCGGATCTTCTTGGGCGTTAATTTGCCTTTTGACGCAGCGGCCGGTCAGGATATTTTGATCCCAACTACCAAAAAGGACGTCTATGCGGTTGATGATAAAGGCGCTGCGTTATTCAAAAATGTTGAAGACATTCGCTATAAAACCAAAGGTACCCCTAAAGGCAACAAAGGCCTCCTCCCTATCGGCGGGGTTCCTCTGGGTATTGAAATCGCGAACGAGATTTACAACAACAAATTATCCCCAACCCCGCCGGGCGAACAGCCGATGCCGCAACCGCCACAAAATCAAGGTCCGCCGCGGAAGAAAGGCGAGCTGGCGGAAGCAAAAGATGAAGAGCAGGCTCCGATGATGGATGTGGCGCCG</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>ATGACGATCGACTTTACC</t>
+          <t>ATGACCATCGATTTTACC</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>CGGCGCTACGTCC</t>
+          <t>CGGCGCCACATCC</t>
         </is>
       </c>
     </row>
@@ -2026,22 +2026,22 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>TACAGACCCTAAGGATAAAATGGAGGATGGCCACTTGGACGGCTTATGTTGTTATTGATATAAGACATAAACTTATTGGACCGTGACCTAGACTTGGCGGACAGATTGAGGGAGCGACGCTTAGGAGTCCAACCAGGACGTCGGAGAAGAGCTCACGACCCGCATGACTTAAACCGCTAGTTGCTACGCAAAAAACGATATTTAGGCGGACGACTACTTCGCAAATGGGGTATGAATGGCCTTGACGGCGGGTTGCTACCAGACTGCCTTCGCGGATGGCGGCATCGCCGCCGACGATAGTGCCAGGAACTCCGCGACATATGCTGGGGTAGGGGTAGCTAGCGAGCTTTTTGGTGAAAACGGGAAGCGGTCTACTAGAGCGTCAGGTAGCTGGGAAAAAGCTTGAATCTGCGCGGAGAGGGTCTTATGGTCAAACCACGCAGTTAGCGCGGACGTTAATAGCGCAACGACTAGGGCGGCAGTCTAGGTCCGCAACCGGTCCCGCGCATGGGAGGATTTCTACCCGGTATGTTTAAAGCTGGCCTTGGCTTGTTAGGGCACGCGGACTAAGGATAACTGGGTTTGTTGGGCTTGCCTGGTTTTGTTCGACACCGGCTTAGGATGCGCGGCAAGATGCCATTGCGCGGAGCTAAACGCCACGTTTGGCTGTTGTTAGACGAACGACTGGGCGGCCGGCCCCGTCTCGGACTTCTAGGTCACCTTCTATAACTGAGGGACAATATACGCTAGGCGAGTCCACGCGACGGCCTACTATTGGCGTTGGCGGGAAGTGGCCGCGTCAGTCACTGTCCTATGAAAAACCGCATGCTACCTTGGTTGGACTAGCCTTGCGGCGGTGCGGAGATGTTGGTCTACGACGCCTTTGAACGCAAGCTAGGAGGAGGCCTAGTCAGGCTATAGAGAAGGCTGCGATTGTGGCGGCTAAAACGGGGAGACAAGCGCGACACATTACGACGGTACAGCCTACGTCCGCAGAAACGCAACGCCCTTTTTATATGGAAGCTTAAAAACGGAGGCGAAAGGCCGTATGCTCTTTTGGGCAGTCCTGACCCGCTAGGCAAGAAGGTCTGGCATCCAAGCGGTCTCTGATTATTGTTGCCGTAATTGAAGTTTGGCGGTAAAGGCCGCATGGGTAGTCCATTACGATGAAAACCACCACGTTGGAAAGTCTACCGAGCGAATATAATGTTTGTCGGACTATTGGACCTGAAAGGCCTGCTACCACGTCTGCTATAAAGATAGCTTAAACACAGGCTGCTTGACTTGCCTTAATTAGCCCTGGACGCGCTTCTAATACTGCGCAGAGCGGGTTAGTGCCTTGTCCAGCCATGACACGGATGGGGACAAGGACAAGCCAAGCTTAGAAATAACAGGACGTAATTGCTATTACGTGACAGAGGACAAAAAGAGCCGCATTTGAACGGAAAACTACGAAAACGCCGTGTTCTACATAATCAAGGTTTGGGCTTGGTCCTCGGCAGCCTTCCGGGCATGGTCGATTTAGGACTACCTAGACTGTTTATATTTGGACGTCGTCTTCAATTCATGCTTCGGGCTCGATGAGCGAAGCTAGGACTTCCAGACAAAGGTTAACCTCCACAGGGCAACCCGGAGCCCTAGCGCCTACTTTAAAAGCGCCGTTTAAACTTTGGCTGGGGACTTCTTCGGGTCGGACCACCCCGACCGCAGAGAGTTTGGGTCAACGAGTTTCTAGTTCAATTTGTTTTTTGAGACCTACCCCGTTTACCAAGTTTGCCCTGATTC</t>
+          <t>TACAGTCCCTAAGGCTAGGACGGTGGCTGACCACTTGGACGCCTTATATTGTTATTAATGTAGGACATGAACTTGTTAGACCGTAACCTAGACTTAGCGGAAAGTTTGAGGGACCGACGATTAGGAGTTCACCCGGGCCGACGTAGAAGAGCGCAGGACCCACAGAATTTGAATCGGTAATTGCTACGGAAAAAACGTTAATTGGGGGGACGGCTACTCCGGAAATGTGGCATAAACGGGCTCAATGGTGGCTTGCTACCGGAATGTCTTCGCGGATGGCGTCAACGCCGACGGCGCTAATGCCAGAACCTCCGGGACATGTGGTGGGGCAGGGGCAGGTAACGCGGATTTTGGTGGAAACGCGATGGAGTTTACTAGAGCGTTAGCTAGCTAGGAAAGAGGTTGAATCTACGCGGAGACGGACTTATGGTCAAACCCCGGAGATAACGGGCGCGCTAATAACGGGACAACTAAGGGGGCAGCCTGGGCCCGCACCCCGTCCCGCGTATGGGAGGCTTTCTACCAGGCATATTTAAGGCCGGCCTCGGCTTGTTGGGGCATGGAGAGTAGGGCTAGCTAGGGTTATTAGGCTTACCGGGATTTGTTCGCCAACGCCTCAGCATGCGGGGTAAAATACCGTTGCGCGCGGCGAAGCGGCACGTCTGGCTATTATTAGACGAACGCCTAGGTGGACGTCCTCGCCTTGCCCTTCTAGGCCACCTCCTATAACTAAGTGAGGACATGCGATAAGCTAGCCCCCGCGACGGCCTACTATTGGGATTAGCCGCTAGAGGCCGTGTTAGCCAGTGACCAATAAAAAACCGAATACTACCATGGTTGGAGTAACCGTGGGGTGGCGGAAATATATTAGTCTACGACGCCTTTGACCGAAAGCTGGGAGGAGGCCTGGTTAGACTATAAAGTAGGCTACGTTTATGACGACTGAAGCGGGCGAATAAACGCGACACATTGCGGCGGTACAGACTGCGACCGCATAAGCGCAACGGACTTTTCATATGGAAGCTTAAGAACGCTGGTGACAGGCCTTAAGGACTTTTAGGCAGTCCGGACCCCCTGGGTAAGAAAGTCTGTCAGCCAAGGGGCCTCTGGTTATTGTTGCCATAATTAAAATTTGGCGGCAAGGGTCGTATAGGCAGACCATTACGATGTAAGCCCCCGCGGTGGAAAGTCTACCGGGGAGAGATGATGTTCGTCGGACTGTTGGACCTAAAAGGCCTGCTGCCCCGGCTACTGTAAAGATAGCTTAAACAAAGGCTGCTTGAGTTACCGTAATTGGCGCTGGACGGACTTCTAATGCTGCGCAGAGGAGGATAATGGCTTGTCCAGCCGTGGCAAGCCTGCGCTCACGGTCACGCGAAACTCAGCGAAAACAGCACGTAATTACTGTTGCGGGAGAGAGGACAAAAAGACCCACACTTGAACGGAAAGCTACGTAAGCGTCGCGTTCTACACGACCATGGTTTGGGCTTGGTCCTTGGAAGCCTTCCGGGTATAGTTAATTTGGGTCTACCGAGCCTATTCATGTTCGGCCGTCGTCTCCAGTTTATACTTCGCGCGCGCTGGGCGAAACTGGCCCTTCCCGACAAGGGCTAGCCACCTCAGGGCGACCCGAACCCGTAACGACTGCTTTATAAACGGCGTTTAGACTTTGGATGGGGCCTTCTTCGCGTCGGCCCCCCGCGCCCTCACAGGGTCTGGGTCAACGACTTCCTGGTCCAATTTGTCTTTTGCGACCTACCCCGTTTACCGAGTTTGCCGTGTTTT</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>ATGTCTGGGATTCCTATTTTACCTCCTACCGGTGAACCTGCCGAATACAACAATAACTATATTCTGTATTTGAATAACCTGGCACTGGATCTGAACCGCCTGTCTAACTCCCTCGCTGCGAATCCTCAGGTTGGTCCTGCAGCCTCTTCTCGAGTGCTGGGCGTACTGAATTTGGCGATCAACGATGCGTTTTTTGCTATAAATCCGCCTGCTGATGAAGCGTTTACCCCATACTTACCGGAACTGCCGCCCAACGATGGTCTGACGGAAGCGCCTACCGCCGTAGCGGCGGCTGCTATCACGGTCCTTGAGGCGCTGTATACGACCCCATCCCCATCGATCGCTCGAAAAACCACTTTTGCCCTTCGCCAGATGATCTCGCAGTCCATCGACCCTTTTTCGAACTTAGACGCGCCTCTCCCAGAATACCAGTTTGGTGCGTCAATCGCGCCTGCAATTATCGCGTTGCTGATCCCGCCGTCAGATCCAGGCGTTGGCCAGGGCGCGTACCCTCCTAAAGATGGGCCATACAAATTTCGACCGGAACCGAACAATCCCGTGCGCCTGATTCCTATTGACCCAAACAACCCGAACGGACCAAAACAAGCTGTGGCCGAATCCTACGCGCCGTTCTACGGTAACGCGCCTCGATTTGCGGTGCAAACCGACAACAATCTGCTTGCTGACCCGCCGGCCGGGGCAGAGCCTGAAGATCCAGTGGAAGATATTGACTCCCTGTTATATGCGATCCGCTCAGGTGCGCTGCCGGATGATAACCGCAACCGCCCTTCACCGGCGCAGTCAGTGACAGGATACTTTTTGGCGTACGATGGAACCAACCTGATCGGAACGCCGCCACGCCTCTACAACCAGATGCTGCGGAAACTTGCGTTCGATCCTCCTCCGGATCAGTCCGATATCTCTTCCGACGCTAACACCGCCGATTTTGCCCCTCTGTTCGCGCTGTGTAATGCTGCCATGTCGGATGCAGGCGTCTTTGCGTTGCGGGAAAAATATACCTTCGAATTTTTGCCTCCGCTTTCCGGCATACGAGAAAACCCGTCAGGACTGGGCGATCCGTTCTTCCAGACCGTAGGTTCGCCAGAGACTAATAACAACGGCATTAACTTCAAACCGCCATTTCCGGCGTACCCATCAGGTAATGCTACTTTTGGTGGTGCAACCTTTCAGATGGCTCGCTTATATTACAAACAGCCTGATAACCTGGACTTTCCGGACGATGGTGCAGACGATATTTCTATCGAATTTGTGTCCGACGAACTGAACGGAATTAATCGGGACCTGCGCGAAGATTATGACGCGTCTCGCCCAATCACGGAACAGGTCGGTACTGTGCCTACCCCTGTTCCTGTTCGGTTCGAATCTTTATTGTCCTGCATTAACGATAATGCACTGTCTCCTGTTTTTCTCGGCGTAAACTTGCCTTTTGATGCTTTTGCGGCACAAGATGTATTAGTTCCAAACCCGAACCAGGAGCCGTCGGAAGGCCCGTACCAGCTAAATCCTGATGGATCTGACAAATATAAACCTGCAGCAGAAGTTAAGTACGAAGCCCGAGCTACTCGCTTCGATCCTGAAGGTCTGTTTCCAATTGGAGGTGTCCCGTTGGGCCTCGGGATCGCGGATGAAATTTTCGCGGCAAATTTGAAACCGACCCCTGAAGAAGCCCAGCCTGGTGGGGCTGGCGTCTCTCAAACCCAGTTGCTCAAAGATCAAGTTAAACAAAAAACTCTGGATGGGGCAAATGGTTCAAACGGGACTAAG</t>
+          <t>ATGTCAGGGATTCCGATCCTGCCACCGACTGGTGAACCTGCGGAATATAACAATAATTACATCCTGTACTTGAACAATCTGGCATTGGATCTGAATCGCCTTTCAAACTCCCTGGCTGCTAATCCTCAAGTGGGCCCGGCTGCATCTTCTCGCGTCCTGGGTGTCTTAAACTTAGCCATTAACGATGCCTTTTTTGCAATTAACCCCCCTGCCGATGAGGCCTTTACACCGTATTTGCCCGAGTTACCACCGAACGATGGCCTTACAGAAGCGCCTACCGCAGTTGCGGCTGCCGCGATTACGGTCTTGGAGGCCCTGTACACCACCCCGTCCCCGTCCATTGCGCCTAAAACCACCTTTGCGCTACCTCAAATGATCTCGCAATCGATCGATCCTTTCTCCAACTTAGATGCGCCTCTGCCTGAATACCAGTTTGGGGCCTCTATTGCCCGCGCGATTATTGCCCTGTTGATTCCCCCGTCGGACCCGGGCGTGGGGCAGGGCGCATACCCTCCGAAAGATGGTCCGTATAAATTCCGGCCGGAGCCGAACAACCCCGTACCTCTCATCCCGATCGATCCCAATAATCCGAATGGCCCTAAACAAGCGGTTGCGGAGTCGTACGCCCCATTTTATGGCAACGCGCGCCGCTTCGCCGTGCAGACCGATAATAATCTGCTTGCGGATCCACCTGCAGGAGCGGAACGGGAAGATCCGGTGGAGGATATTGATTCACTCCTGTACGCTATTCGATCGGGGGCGCTGCCGGATGATAACCCTAATCGGCGATCTCCGGCACAATCGGTCACTGGTTATTTTTTGGCTTATGATGGTACCAACCTCATTGGCACCCCACCGCCTTTATATAATCAGATGCTGCGGAAACTGGCTTTCGACCCTCCTCCGGACCAATCTGATATTTCATCCGATGCAAATACTGCTGACTTCGCCCGCTTATTTGCGCTGTGTAACGCCGCCATGTCTGACGCTGGCGTATTCGCGTTGCCTGAAAAGTATACCTTCGAATTCTTGCGACCACTGTCCGGAATTCCTGAAAATCCGTCAGGCCTGGGGGACCCATTCTTTCAGACAGTCGGTTCCCCGGAGACCAATAACAACGGTATTAATTTTAAACCGCCGTTCCCAGCATATCCGTCTGGTAATGCTACATTCGGGGGCGCCACCTTTCAGATGGCCCCTCTCTACTACAAGCAGCCTGACAACCTGGATTTTCCGGACGACGGGGCCGATGACATTTCTATCGAATTTGTTTCCGACGAACTCAATGGCATTAACCGCGACCTGCCTGAAGATTACGACGCGTCTCCTCCTATTACCGAACAGGTCGGCACCGTTCGGACGCGAGTGCCAGTGCGCTTTGAGTCGCTTTTGTCGTGCATTAATGACAACGCCCTCTCTCCTGTTTTTCTGGGTGTGAACTTGCCTTTCGATGCATTCGCAGCGCAAGATGTGCTGGTACCAAACCCGAACCAGGAACCTTCGGAAGGCCCATATCAATTAAACCCAGATGGCTCGGATAAGTACAAGCCGGCAGCAGAGGTCAAATATGAAGCGCGCGCGACCCGCTTTGACCGGGAAGGGCTGTTCCCGATCGGTGGAGTCCCGCTGGGCTTGGGCATTGCTGACGAAATATTTGCCGCAAATCTGAAACCTACCCCGGAAGAAGCGCAGCCGGGGGGCGCGGGAGTGTCCCAGACCCAGTTGCTGAAGGACCAGGTTAAACAGAAAACGCTGGATGGGGCAAATGGCTCAAACGGCACAAAA</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>ATGTCTGGGATTCCTATT</t>
+          <t>ATGTCAGGGATTCCG</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>CTTAGTCCCGTTTGAAC</t>
+          <t>TTTTGTGCCGTTTGAG</t>
         </is>
       </c>
     </row>
@@ -2068,22 +2068,22 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>TACCGTTTGAAATGGGGCCAGGCGGACGGATTTCAGCTTCTTCTGCTCCACATATTGTTTTTGATATAAGAAATAAACTTATTGCAACCCGAACTAGAATTAGCCCATTGATTATGGGAGCCTCCAGGAGTCTGCCCTGGCGGCTAGAGACGCGGACGCAATCCATACGACGTCGACCGTTAGTTACTACGCATAAAATGCTAATTCGGCAGTCGACTAAAATGTTGCAAGAACTGGGGTTTACGTCTTTAGCTGCGAATGGGAGACGGTCTAGGCTGGTTGAGGCTACTGCGTGCGGTCCGTCACCGCCCGCGCCGCCAATGATACGACAGATACGACATATACGGAGGACGACTTTACGGGGGAGGCAGGGGATAAAGATTGCTATGTATACGGGTCAATCTTATATAATAGCTCAGGAGGTACTGTTTACGTGGTCCCCCTACGTTATGCCAGAGCATAAGCAAATTGAAACCGTTTCGCCACCGCTGCTTTAAGAAGCTAGAAGAAAAATTACTTCTTCCCCGTTTGGTTGCCCCTATATGCGGTTGGAAGCGGGGGAAATTTAAATTGCTACTTGGCTGATTAGGACACCTAGACCATGGCCTTCTACGCTTGCTCGGCCCACCGTTATAACAGGGCGCGGGAGTCATGTTGCGCGGTAAAATACCATGGGCGCGGTTTGGAAAGCGCTGAGTCTGGCTATTATAGTAGCGACTAGGAGGTCCGTAGGGAAGTCCCCGCCCGCTTCACTGCCTTATGCTGCTGCGGTAAGCGCTCCAAATACGCTACCCACCCCGACGTAGAGACTTGTGCTGCTTCGCGTGTGGGTTGGTCTGCCAGGTTCCATACAAGAACCGCATGCTACCACGTTTCAACTAACCATGCGGGGGGGGAGACATATTGGTTTAATAAGCGTTTTAGCGTCACCGGATGTTTGTTCTTCTATTGGACCGACTTAGGCTTTAGTTGTTGCGCCTGAAGCGGGCGGACGACCGCGAACACTTGCACCGATACCGCCTGCGCCCGTAAAAAAGAAACTTCCTTTTCAACGTCAAACTTAAAAACGCCGGCGACAGGCCGCAAGCGCGTCTGAGGGACGCGCTGGGTTTTAATCAACTAGCGCCACTAGGAAAAAACGACTGGGAACCGCGTGGACGATGATTGAGGCTGAGCGACGGAAAGTTTGGCGGCAAAGGTCGTATGGGAAGGCCGTTACGATGCAAGCCCCCACGTCGTAAGGTCTACCACGCGTTTATGATGTTACCGGCGGGCCCGGACCCAAGTAACCGTCTACTACTTGGCCTGTTGTAGCGCCAACTTAAACATAGGCTCCTCGACTTGCCCTAGAGCGGACTGGAGGCCGTCGGCTTACTAGGCTTTGCGCTGTAATGTCTGGTCGGACCATGGCACGCCTGTGCCGACGGGGGATTAAAAAGGAGAACGAACCTCTACTACAAACTTTTGCGCCACAGAGCGTAGAAAGACCCACACTTGAACGCGAAACTGCGCCGACGTCGGTTTCTGTATGACCAAGGCTGGTGCTTTTTTCTGCACATACGTCACCTACTATTCCCGCGTAGTGACAAATTTTTGCAACTCCTATAAGGAATAGCGTGCTTTAGCTGAGCGCTTCCAAAGCTTCCATTTATGGGGTAGCCACCGCACGGCGACCCGTAGCTTTAACGCTTGCTCTAGAAGCTATTACCTGAGCAGGGTTGTGGCGGCCTTGACGTCGGCCAACATGTCCCGTACGGCGTCGGTTGCGGCGTCGGCGGCGTCTTGGTTCCAGGCGGCGGATTTTACCTTTTTGACGGCTTCGGCTTTCTGCTTCTGGTCCAAGGCTACTACCTACAACTTGGA</t>
+          <t>TACCGCTTGAAATGGGGCCAGGGAAATGGATTCCATCTTCTCCTGCTTCACATATTATTTTTAATATAGGACATGAACTTGTTGCAGCCGGAGCTGGACTTGGCGCACTGATTATGGGACCCACCGGGCGTCTGGCCAGGAGGCTAGAGGCGAGCGCGTGACCCGTACAACGTTGACCGGTAATTACTGCGCATGAAATGCTAGTTTGGAAGACGTCTAAAATGGTGAAAAGACTGGGGTTTGCGGCTCTAGCTACGGATGGGAGACGGTCTAGGATGGTTGAGTCTGCTGCGCGGAGTCCGCCACCGCCCTCGCCGCCAATGATACGACAGTTACGACATGTACGCGGGCCGTCTTTACGGCGCCGGCAGCGGTTATAGATTACTATGGATACGTGTCGAGCTTATATAGTAACTTAGGAGCTACTGTTTGCGCGGTCCACCAACGTTGTGCCACAGAATGAGAAAGTTGAAGCCGTTCCGTCAGCGCTGGTTTAAAAAGCTGGACGACAAATTGCTTCTTCCGCGCTTGGTCGGACCAATATGCGGGTGGAAACGGGGCAAATTTAAGTTACTGCTCGGCTGGTTAGGGCACCTAGAACACGGCCTTCTACGGTTGCTTGGCCCTCCGTTATAGCAGGGCGCCGCGGTCATATTGCGCGGAAAGATGCCGTGGGGACGCTTTGGAAAACGGTGGGTCTGCCTGTTATAATAACGCCTGGGTGGCCCGTAAGGAAGGCCGCGCCCGCTTCAGTGGCTTATGCTACTACGCTAAGCGCTCCAGATGCGCTACCCACCACGTCGTAGAGACTTGTGGTGGTTTGGATGGGGTTTGGTTTGGCAGGTCCCGTACAAAAACCGCATGCTACCACGGTTTGACTAACCGTGCGGCGGAGGAGACATATTAGTCTAGTATGGATTTTAGCGCCATCGTATGTTTGTTCTTCTATTGGACCGCCTTAGACTCTAATTGTTACGCCTGAAACGCGGAGAAGACCGTGAGCAATTACAGCGCTACCGCCTGCGCCCATAAAAGAGAAACTTCCTCTTTAACGTCAAGCTTAAGAACGGAGGCAATAGACCACAAGGACGACTGAGAGACGCGCTAGGCTTTGACCACCTAGCGCCTCTGGGGAAAAACGACTGGGAGCCACGCGGCCGATGGTTAAGTCTAAGGGACGGTAAGTTCGGCGGCAAGGGACGCATGGGGAGGCCTTTGCGCTGCAAACCGCCACGCCGGAAGGTCTACCACGGATTTATGATATTACCCGCGGGACCAAATCCTAGCAACCGGCTACTGCTCGGCCTGTTGTAGCGGCACCTCAAACAGAGGCTCCTCGAATTGCCGTATAGAGGACTAAATGCGGTTGGCTTGCTAGGCTTTGGACTATAGTGGCTGGTCGGACCGTGACAGGGATGAGGAGACGGCGGATTAAAGAGAAGAACGAACCTCTACTACAAACTTTTGCGGCACAGGGGATATAAAGACCCGCAGTTAAACGCGAAACTACGCCGACGGCGTTTTCTATAGGACCACGGTTGATGGTTTTTTCTGCACATGCGGCAACTACTGTTCCCACGTAGCGACAAATTCTTGCAGCTTCTGTAGGCTATAGCGTGGTTCAGATGGGCGCTTCCCAAGCTTCCATTTATGGGTTAACCTCCGCATGGAGAGCCCTAGCTCTAGCGGTTACTCTAGAAGCTATTGCCTGAACAGGGTTGGGGCGGACTTAATGTCGGGCAGCACGTTCCATACGGCGTCGGATGGGGCGTCGGTGGCGTCTTAGTCCCAGGTGGCGGATTTTACCTTTTTAACGGTTTTGGCTTTCTACTTCTAGTTCACGGATACTACCTGCAGCTTGGA</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>ATGGCAAACTTTACCCCGGTCCGCCTGCCTAAAGTCGAAGAAGACGAGGTGTATAACAAAAACTATATTCTTTATTTGAATAACGTTGGGCTTGATCTTAATCGGGTAACTAATACCCTCGGAGGTCCTCAGACGGGACCGCCGATCTCTGCGCCTGCGTTAGGTATGCTGCAGCTGGCAATCAATGATGCGTATTTTACGATTAAGCCGTCAGCTGATTTTACAACGTTCTTGACCCCAAATGCAGAAATCGACGCTTACCCTCTGCCAGATCCGACCAACTCCGATGACGCACGCCAGGCAGTGGCGGGCGCGGCGGTTACTATGCTGTCTATGCTGTATATGCCTCCTGCTGAAATGCCCCCTCCGTCCCCTATTTCTAACGATACATATGCCCAGTTAGAATATATTATCGAGTCCTCCATGACAAATGCACCAGGGGGATGCAATACGGTCTCGTATTCGTTTAACTTTGGCAAAGCGGTGGCGACGAAATTCTTCGATCTTCTTTTTAATGAAGAAGGGGCAAACCAACGGGGATATACGCCAACCTTCGCCCCCTTTAAATTTAACGATGAACCGACTAATCCTGTGGATCTGGTACCGGAAGATGCGAACGAGCCGGGTGGCAATATTGTCCCGCGCCCTCAGTACAACGCGCCATTTTATGGTACCCGCGCCAAACCTTTCGCGACTCAGACCGATAATATCATCGCTGATCCTCCAGGCATCCCTTCAGGGGCGGGCGAAGTGACGGAATACGACGACGCCATTCGCGAGGTTTATGCGATGGGTGGGGCTGCATCTCTGAACACGACGAAGCGCACACCCAACCAGACGGTCCAAGGTATGTTCTTGGCGTACGATGGTGCAAAGTTGATTGGTACGCCCCCCCCTCTGTATAACCAAATTATTCGCAAAATCGCAGTGGCCTACAAACAAGAAGATAACCTGGCTGAATCCGAAATCAACAACGCGGACTTCGCCCGCCTGCTGGCGCTTGTGAACGTGGCTATGGCGGACGCGGGCATTTTTTCTTTGAAGGAAAAGTTGCAGTTTGAATTTTTGCGGCCGCTGTCCGGCGTTCGCGCAGACTCCCTGCGCGACCCAAAATTAGTTGATCGCGGTGATCCTTTTTTGCTGACCCTTGGCGCACCTGCTACTAACTCCGACTCGCTGCCTTTCAAACCGCCGTTTCCAGCATACCCTTCCGGCAATGCTACGTTCGGGGGTGCAGCATTCCAGATGGTGCGCAAATACTACAATGGCCGCCCGGGCCTGGGTTCATTGGCAGATGATGAACCGGACAACATCGCGGTTGAATTTGTATCCGAGGAGCTGAACGGGATCTCGCCTGACCTCCGGCAGCCGAATGATCCGAAACGCGACATTACAGACCAGCCTGGTACCGTGCGGACACGGCTGCCCCCTAATTTTTCCTCTTGCTTGGAGATGATGTTTGAAAACGCGGTGTCTCGCATCTTTCTGGGTGTGAACTTGCGCTTTGACGCGGCTGCAGCCAAAGACATACTGGTTCCGACCACGAAAAAAGACGTGTATGCAGTGGATGATAAGGGCGCATCACTGTTTAAAAACGTTGAGGATATTCCTTATCGCACGAAATCGACTCGCGAAGGTTTCGAAGGTAAATACCCCATCGGTGGCGTGCCGCTGGGCATCGAAATTGCGAACGAGATCTTCGATAATGGACTCGTCCCAACACCGCCGGAACTGCAGCCGGTTGTACAGGGCATGCCGCAGCCAACGCCGCAGCCGCCGCAGAACCAAGGTCCGCCGCCTAAAATGGAAAAACTGCCGAAGCCGAAAGACGAAGACCAGGTTCCGATGATGGATGTTGAACCT</t>
+          <t>ATGGCGAACTTTACCCCGGTCCCTTTACCTAAGGTAGAAGAGGACGAAGTGTATAATAAAAATTATATCCTGTACTTGAACAACGTCGGCCTCGACCTGAACCGCGTGACTAATACCCTGGGTGGCCCGCAGACCGGTCCTCCGATCTCCGCTCGCGCACTGGGCATGTTGCAACTGGCCATTAATGACGCGTACTTTACGATCAAACCTTCTGCAGATTTTACCACTTTTCTGACCCCAAACGCCGAGATCGATGCCTACCCTCTGCCAGATCCTACCAACTCAGACGACGCGCCTCAGGCGGTGGCGGGAGCGGCGGTTACTATGCTGTCAATGCTGTACATGCGCCCGGCAGAAATGCCGCGGCCGTCGCCAATATCTAATGATACCTATGCACAGCTCGAATATATCATTGAATCCTCGATGACAAACGCGCCAGGTGGTTGCAACACGGTGTCTTACTCTTTCAACTTCGGCAAGGCAGTCGCGACCAAATTTTTCGACCTGCTGTTTAACGAAGAAGGCGCGAACCAGCCTGGTTATACGCCCACCTTTGCCCCGTTTAAATTCAATGACGAGCCGACCAATCCCGTGGATCTTGTGCCGGAAGATGCCAACGAACCGGGAGGCAATATCGTCCCGCGGCGCCAGTATAACGCGCCTTTCTACGGCACCCCTGCGAAACCTTTTGCCACCCAGACGGACAATATTATTGCGGACCCACCGGGCATTCCTTCCGGCGCGGGCGAAGTCACCGAATACGATGATGCGATTCGCGAGGTCTACGCGATGGGTGGTGCAGCATCTCTGAACACCACCAAACCTACCCCAAACCAAACCGTCCAGGGCATGTTTTTGGCGTACGATGGTGCCAAACTGATTGGCACGCCGCCTCCTCTGTATAATCAGATCATACCTAAAATCGCGGTAGCATACAAACAAGAAGATAACCTGGCGGAATCTGAGATTAACAATGCGGACTTTGCGCCTCTTCTGGCACTCGTTAATGTCGCGATGGCGGACGCGGGTATTTTCTCTTTGAAGGAGAAATTGCAGTTCGAATTCTTGCCTCCGTTATCTGGTGTTCCTGCTGACTCTCTGCGCGATCCGAAACTGGTGGATCGCGGAGACCCCTTTTTGCTGACCCTCGGTGCGCCGGCTACCAATTCAGATTCCCTGCCATTCAAGCCGCCGTTCCCTGCGTACCCCTCCGGAAACGCGACGTTTGGCGGTGCGGCCTTCCAGATGGTGCCTAAATACTATAATGGGCGCCCTGGTTTAGGATCGTTGGCCGATGACGAGCCGGACAACATCGCCGTGGAGTTTGTCTCCGAGGAGCTTAACGGCATATCTCCTGATTTACGCCAACCGAACGATCCGAAACCTGATATCACCGACCAGCCTGGCACTGTCCCTACTCCTCTGCCGCCTAATTTCTCTTCTTGCTTGGAGATGATGTTTGAAAACGCCGTGTCCCCTATATTTCTGGGCGTCAATTTGCGCTTTGATGCGGCTGCCGCAAAAGATATCCTGGTGCCAACTACCAAAAAAGACGTGTACGCCGTTGATGACAAGGGTGCATCGCTGTTTAAGAACGTCGAAGACATCCGATATCGCACCAAGTCTACCCGCGAAGGGTTCGAAGGTAAATACCCAATTGGAGGCGTACCTCTCGGGATCGAGATCGCCAATGAGATCTTCGATAACGGACTTGTCCCAACCCCGCCTGAATTACAGCCCGTCGTGCAAGGTATGCCGCAGCCTACCCCGCAGCCACCGCAGAATCAGGGTCCACCGCCTAAAATGGAAAAATTGCCAAAACCGAAAGATGAAGATCAAGTGCCTATGATGGACGTCGAACCT</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>ATGGCAAACTTTACCC</t>
+          <t>ATGGCGAACTTTACCC</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>AGGTTCAACATCCATCA</t>
+          <t>AGGTTCGACGTCCATC</t>
         </is>
       </c>
     </row>
@@ -2110,22 +2110,22 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>TACTTTGCTTAGGAATGGGACCGCGACTGGGACCCGGACAACATAAGACCACACTAGAAACGGGTTTTTTTGGTCCTCCTCGGAGCGCCATGACTCTTACAACGAATGGTCAACCCATTTTACCGCGACCTACGTTGTCGTAGTCTATGCCTTGCGAAGTTTGGAGCGGGATGGTAGTGGAGGGCGATGGACCCCGACTAGAAGCACAGATAGAAACTACGGAACAGAGCGATACTGCTTAGGCGTTAGGGCCACATAGACTTACTACAGCTAGGAGCCGGTCGGTTGCTTGGATTGGAGTTTTTGTTTCTTTAGCGTTAAAGTATACGTCGTAAACCACGATACTTTCTCATAATAAAGAGACTATGGCTTTACAAAGGATTCGACTACCGGCTGGACCCGGACCTAGGCCTATTGTGGAGGTACCTAGGTTGCTGCGGGCTCCCGCAGCCTTTGGACCGTCGTTTCCGGTGATAGCTTCGAGGATTTTTGCTGCCTAGATTAGTCATGCCACTTCGTTTTCCACGGTTGCCGCTCGGCATAAGACTAATATGGTTGATAAGTGGCCACTTGTGGCGCCTACTTTTGTGGCTATAGTTAGGAAACGTCGGCTTTATGAAGAGGCTGCCATTTCCTCCGGTCATACGCGGCCCAACGGAGTGGGGCATGAACGTCTTTCACTTCGGCTAACGTGACTGGAGTCGCCTAGTTAAAGGAGGCCCAGGAGGAGGTGACCATCCCAGGTTTGTTGACTTTTTTCTCCACTTTCTTCACCATCTGGAAGTCCGCTTGGACAGGCTACTTCTTTTTCGCGAACATCTTAAATACGCGCTACCAGGAGTCAGCCAGGTCGTCCGGCCGTTAAACGACTTTAAGCGCGTCCTACAAAGTGGAGGACTATTGTTGTGGGACCTACTTCTGCATTTTTACATAAAGGACTGACTTTAATGGCGCTACCTGCGTAAATAGCGAAGCAACCTGAGATTTTACAAGATGCTGATGCGGGGAGGCATACGGAACCAATTACTTATAATATTCCTATTTTGCTAATTTCGCAACCGCCCTGGCCCGTTCCCACATTAGTTTTACTTCCCAGTTCTTAACGGAGGAATAAGCGGCCTATAGAAAGACACAGGAGGCAAAGGCAGTATGTGCAGGCCATTGAGGTGGTAGAGACCGCCGACACGCCTTCAAGAGGGAGACAAGTGGCCTAGGCTTTTGAAGCCACTTAGTCAGTTTGACCAGCGCCCGAGGTACTGACTCGACCTGAGTCGTTTGATACCGTTTTGCCAATGCTAATTGAAAGGCTGGAAGTGGCTCTGGCGGTTATACCGACCGTACAGGGCGCACTACCCACCCATGTTGTAGGTCCGACTATTGTAGCGCCCAGACGTTAACCCCGGACTGCAGCGTAGCGTTCGTAACTTCAAAATGTTATTTTTAGACCCGGTC</t>
+          <t>TACTTCGGATAAGACTGAAATCGGGACTGTGACCCGGAGGACATGAGCCCGCACTAGAAGCGTGTCTTCTTAGTCCTTCTTGGAGCTCCGTGACTTTTGCAGCGGATAGTCAACCCTTTTTACCGTGACCTACGGTGGCGTAGTCTGTGGCTTGCGAAATTTGGTGGAGGCTGGTAGTGGAGTGCGATGAATCCTGACTATAAGCATAGGTAGAAACTGCGGAACAGGGGAATACTGCTTAGACGCTAGGGCCATATAGACTTACTGCATCTGGGAGGAGGCCGCTTACTTGCGTTGAATTTTTTGTTTCTTTAACGGTAAAGGATGCGGCGGAAACCACGCTACTTTCTTATAATAAAGAGGCTGTGACTTTACAAGGGATTTGACTACCGGCTAAATCCTGACCTAGGCCTGTTGTGAAGCTACCTGGGTTGCTGCGGCCTTCCACATCCGTTGGAACGCCGTTTTCGGTGTTAGCTCCGAGCGTTTTTACTGCCAAGTTTAGTCATGCCGCTTCGATTCCCACGCTTACCACTTGGCATAAGACTGATATGGTTAATAAGCGGTCAATTGTGGCGGCTACTTTTGTGTCTATAATTAGGAAACGTTGGTTTTATAAAGAGGCTACCATTTCCACCAGTCATGCGTGGCCCGACGGACTGGGGCATAAACGTTTTTCACTTTGGTTAACGCGAGTGAAGACGTCTAGTCAAAGCGGGTCCAGGCGGCGGGAATCAGCCCAGGTTTGTTGACTTTTTCCTTCAGTTCCTTCAACACCTAGAGGTCCGGTTGGACAGACTACTTCTTTTTCGGGATCAGCTTAAGTACGGACTACCGGGTGTCAGACATGTTGTCCGTCCATTAAACGACTTTAAGCGCGTCCTACAGAGGGCGGGACTGTTGTTGTGCGACCTACTTCTACATTTTTACATAAAGAATTGTCTTTAATGTCGCTACCTGCGCAAGTAACGAAGAAACCTAAGATTCTACAAGATACTGATGCGCGCCGGTATACGTGAGCATTTACTTATAATGTTTCTATTTTGGTAATTCCGCAACCGCCCGGGCCCTTTCCCCCAGTATTTTTACTTTCCAGTCCTTAACGGAGGAATAAGAGGTCTATAGAAAGACACAGGTGGTAAGGGCAGGATATGGAGGCCGTTGAGGTGGTATAGACCGCCGACGCGTCTTCAAGACGCGGATAAATGCCCTAGACTTTTAAAACCGCTCAGTCACTTTGACCAACGTCCCAGATACTGCCTTGACCTAAGACGCTTAATGCCATTTTGGCACTGATAGTTGAAAGGCTGAAAATGTCTTTGGCGGTTGTACCGACCGTACAGGGGACAATACCCGCCGATGTTATAAGTCCGCCTGTTGTAACGGCCGAACGTCGACCCTGCGCTACACCGAAGCGTCCGCAACTTTAAAATGTTATTTTTGAATCCCGTC</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>ATGAAACGAATCCTTACCCTGGCGCTGACCCTGGGCCTGTTGTATTCTGGTGTGATCTTTGCCCAAAAAAACCAGGAGGAGCCTCGCGGTACTGAGAATGTTGCTTACCAGTTGGGTAAAATGGCGCTGGATGCAACAGCATCAGATACGGAACGCTTCAAACCTCGCCCTACCATCACCTCCCGCTACCTGGGGCTGATCTTCGTGTCTATCTTTGATGCCTTGTCTCGCTATGACGAATCCGCAATCCCGGTGTATCTGAATGATGTCGATCCTCGGCCAGCCAACGAACCTAACCTCAAAAACAAAGAAATCGCAATTTCATATGCAGCATTTGGTGCTATGAAAGAGTATTATTTCTCTGATACCGAAATGTTTCCTAAGCTGATGGCCGACCTGGGCCTGGATCCGGATAACACCTCCATGGATCCAACGACGCCCGAGGGCGTCGGAAACCTGGCAGCAAAGGCCACTATCGAAGCTCCTAAAAACGACGGATCTAATCAGTACGGTGAAGCAAAAGGTGCCAACGGCGAGCCGTATTCTGATTATACCAACTATTCACCGGTGAACACCGCGGATGAAAACACCGATATCAATCCTTTGCAGCCGAAATACTTCTCCGACGGTAAAGGAGGCCAGTATGCGCCGGGTTGCCTCACCCCGTACTTGCAGAAAGTGAAGCCGATTGCACTGACCTCAGCGGATCAATTTCCTCCGGGTCCTCCTCCACTGGTAGGGTCCAAACAACTGAAAAAAGAGGTGAAAGAAGTGGTAGACCTTCAGGCGAACCTGTCCGATGAAGAAAAAGCGCTTGTAGAATTTATGCGCGATGGTCCTCAGTCGGTCCAGCAGGCCGGCAATTTGCTGAAATTCGCGCAGGATGTTTCACCTCCTGATAACAACACCCTGGATGAAGACGTAAAAATGTATTTCCTGACTGAAATTACCGCGATGGACGCATTTATCGCTTCGTTGGACTCTAAAATGTTCTACGACTACGCCCCTCCGTATGCCTTGGTTAATGAATATTATAAGGATAAAACGATTAAAGCGTTGGCGGGACCGGGCAAGGGTGTAATCAAAATGAAGGGTCAAGAATTGCCTCCTTATTCGCCGGATATCTTTCTGTGTCCTCCGTTTCCGTCATACACGTCCGGTAACTCCACCATCTCTGGCGGCTGTGCGGAAGTTCTCCCTCTGTTCACCGGATCCGAAAACTTCGGTGAATCAGTCAAACTGGTCGCGGGCTCCATGACTGAGCTGGACTCAGCAAACTATGGCAAAACGGTTACGATTAACTTTCCGACCTTCACCGAGACCGCCAATATGGCTGGCATGTCCCGCGTGATGGGTGGGTACAACATCCAGGCTGATAACATCGCGGGTCTGCAATTGGGGCCTGACGTCGCATCGCAAGCATTGAAGTTTTACAATAAAAATCTGGGCCAG</t>
+          <t>ATGAAGCCTATTCTGACTTTAGCCCTGACACTGGGCCTCCTGTACTCGGGCGTGATCTTCGCACAGAAGAATCAGGAAGAACCTCGAGGCACTGAAAACGTCGCCTATCAGTTGGGAAAAATGGCACTGGATGCCACCGCATCAGACACCGAACGCTTTAAACCACCTCCGACCATCACCTCACGCTACTTAGGACTGATATTCGTATCCATCTTTGACGCCTTGTCCCCTTATGACGAATCTGCGATCCCGGTATATCTGAATGACGTAGACCCTCCTCCGGCGAATGAACGCAACTTAAAAAACAAAGAAATTGCCATTTCCTACGCCGCCTTTGGTGCGATGAAAGAATATTATTTCTCCGACACTGAAATGTTCCCTAAACTGATGGCCGATTTAGGACTGGATCCGGACAACACTTCGATGGACCCAACGACGCCGGAAGGTGTAGGCAACCTTGCGGCAAAAGCCACAATCGAGGCTCGCAAAAATGACGGTTCAAATCAGTACGGCGAAGCTAAGGGTGCGAATGGTGAACCGTATTCTGACTATACCAATTATTCGCCAGTTAACACCGCCGATGAAAACACAGATATTAATCCTTTGCAACCAAAATATTTCTCCGATGGTAAAGGTGGTCAGTACGCACCGGGCTGCCTGACCCCGTATTTGCAAAAAGTGAAACCAATTGCGCTCACTTCTGCAGATCAGTTTCGCCCAGGTCCGCCGCCCTTAGTCGGGTCCAAACAACTGAAAAAGGAAGTCAAGGAAGTTGTGGATCTCCAGGCCAACCTGTCTGATGAAGAAAAAGCCCTAGTCGAATTCATGCCTGATGGCCCACAGTCTGTACAACAGGCAGGTAATTTGCTGAAATTCGCGCAGGATGTCTCCCGCCCTGACAACAACACGCTGGATGAAGATGTAAAAATGTATTTCTTAACAGAAATTACAGCGATGGACGCGTTCATTGCTTCTTTGGATTCTAAGATGTTCTATGACTACGCGCGGCCATATGCACTCGTAAATGAATATTACAAAGATAAAACCATTAAGGCGTTGGCGGGCCCGGGAAAGGGGGTCATAAAAATGAAAGGTCAGGAATTGCCTCCTTATTCTCCAGATATCTTTCTGTGTCCACCATTCCCGTCCTATACCTCCGGCAACTCCACCATATCTGGCGGCTGCGCAGAAGTTCTGCGCCTATTTACGGGATCTGAAAATTTTGGCGAGTCAGTGAAACTGGTTGCAGGGTCTATGACGGAACTGGATTCTGCGAATTACGGTAAAACCGTGACTATCAACTTTCCGACTTTTACAGAAACCGCCAACATGGCTGGCATGTCCCCTGTTATGGGCGGCTACAATATTCAGGCGGACAACATTGCCGGCTTGCAGCTGGGACGCGATGTGGCTTCGCAGGCGTTGAAATTTTACAATAAAAACTTAGGGCAG</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>ATGAAACGAATCCTTACC</t>
+          <t>ATGAAGCCTATTCTGACTT</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>CTGGCCCAGATTTTTA</t>
+          <t>CTGCCCTAAGTTTTTATTG</t>
         </is>
       </c>
     </row>
@@ -2152,22 +2152,22 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>TACTTCTTTTAGAATTAACGAGAGTAAAGTAAACGCAAGCGCCAAAGCACGTTCCGAGGCGTTTTTCTTCTTGGCTAATTATAATGGGGTCTTCTTGAGCTGCGTAGATAACTAGGACACTGGCTTTAATACTAGTTGCTATAGAAGAGGGGCGGTCAACGCAGCGGATAAAAACGCATAGGATTGCACCGCCGCATGCTTTAACACCGCCGTTGATTACTATTGATGTTGAGCAATCGACCCGTTGACTTACCGGACTGCCGGTAGGGACTCGGGCTGTGGTGTTTTTGCTAGTTGATACTTGAACGCCGACACCAGCGTTTATACCTCGACAGATTTGCGAACTAAAAAAGTCTTCTGGGATACCTTAGGGATGCGCTAAGGGACATGTACCAGAACCTCCCGTTTTTAGGCCATAACAAGAGGCTAAGTTTTCGGATGCCCGACGTTCAGCGCCTATTATAACCACTTAACTACTTGTTCCTGTTGATACGAGTTTGGGCGTGGTACGGCTTTAAATGACACCTGCGGCTACTGGGCCCAGGAAACGTCGGCTGGGGCGGACGCATGTACCTACCTTAGCTTGGATTAAACTTGTTTTAGGGAGGGAAGCAAGACCTGAGCCGCCGGGTTAAGTTTGGTCAGGGCGGCGGCCGTATAAGTGACCTCCTTCTAAGTCGAAAAATGTTTCTTGACTTTCTCCAGATGCTACAGGGATTGTTTTAATGACTTCTTCCACTAAGTAGCCTCCTTTAGGTTTAACGAGCGAAAAACCTAACGTTAGGAATGCAGAGCCAATGGGGACCGTTGGACTACAAGCGATGATTCTTTTAGTGCGGACCACGCTTGAACTACCCATAGCGATTTTATCGCCGCGGATTTTGGTTGAGTCTAAAACGATTTTGCGACAAGCGGATGTGCTTCCGCAGTCACCGCTACCGCCTGCGTAAGTAAAGTACGAACCTACTCTTCATAGCGAGCTTAGACTAAGGAGGGCTCTGACAGTAATTGGTCTTGTAACTGCTGAGGAACTTCGGTCAGGAAGTTTGAGGCGGTAAGGGCCTTATGTGGAGTCCGTTGAGGCAACAGAGGCCGCGCCGTAGCCAACACGAATGTCTCCAGAAACCCCTATTGAAGAGGAAGCTACTACTATGTCTTCACGGGATACCGAATGGTTAAGCGAGCAAATTTAGAAAGTTCGTCCGCCGGCTACTTCGTCGATAGAGTGCGTACATGCCACCATAATTAATGGGACGACGCTAGCTTCAACCGCACTTTGTTCCAGGACTAGAGCCGTGAAAGCACCATTTGTTTGACTTGTACGAGAGACTGTTTTTTCAACGCGTCTTA</t>
+          <t>TACTTTTTTTAGGACTAGCGAGACTAGAGAAAACGTAAGCGCCACAGTACATTTCGTGGTGTCTTTCTTCTTGGCTAGTTATAATGGGGCCTTCTTGAACTACGGAGCTAGCTGGCTCACTGCCTTTAATACTAGTTGCTATAGAAAAGGGGCGGCCAACGGAGGGGATATAAGCGTATGGGATTACACCGCCGCATACTTTAGCACCGCCGCTGGTTACTATTGATATTGAGAGACCGCCCTGTTGACTTGCCGGACTGGCGATAGGGTCTTGGCCTATGGTGTTTTTGGTATTTAATGCTTGAACGACGTCACCACCGCTTGTACCTCGACAGGTTCGCGGACTAAAAAAGACTTCTGGCGTACCTTAGCGAGGGACTAAGGAACATATACCACAACCTCCCTTTTTTGGGACAAGAAAAGAGGCTAAGCTTCCGCATACCGGACGTCCAACGCCTATTATAGCCACTTAACTACTTGTTCCTATTGATGCGCGTTTGCGGATGATACGGATTTAAATGCCAACTACGCCTACTAGGCCCAGGAAACGTCGGGTGCGGCGGCCGTATATACCTGCCCTAACTTGGCTTAAACTTATTTTAAGCTGGTAAGCATAATCTAAGTCGACGTGTTAAGTTTGGCCACGGCGGAGGGCGGATGAGGGACCTCCTTCTGAGTCGAAAAATATTTCTTAACTTTCTCCAGATACTGCACGGATTGTTTTAATGGCTCCTTCCGCTAAGTAGGCTTCTTTAAGTCTAGCGAGCGAAAAACCTGACATTAGGGATGCAAAGGCATTGAGCCCCGTTAGACTACAAACGGTGCTTTTTTTAGTGTGGTCCACGTTTGAACTACCCCTAACGATTTTAGCGCCGAGCGTTTTGCTTAAGTCTGAAGCGCTTTTGTAACAAACGCATATGATTTCGGAGTCAGCGGTACCGCCTGCGCAAATAAAGTACAAACCTGCTTTTTATAGCCAGATTGAACTAAGGAGGCCTTTGTCAATAATTGGTTTTATAACTGCTGAGCAACTTTGGCCATGACGTTTGGGGTGGCAAAGGCCTCATATGGAGACCATTAAGGCAACATAGGCCACGGCGCAGCCAACACGAATGGCTCCACAAACCCCTATTAAAAAGCAAACTGCTACTATGGCTTCAAGGAATACCCGACGGCTAAGCTAGAAAATTTAGTAAGTTTGTCCGCCGCCTACTTCGCCGTTAGAGAGGATACATGCCACCGTAGTTAATAGCGCGCCGATAACTTCAGCCCCAGTTTGTTCCGGGACTAGACCCGTGGAAGCAACATTTGTTCGAATTATACGACAGCCTGTTTTTTCATCGCGTTTTG</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>ATGAAGAAAATCTTAATTGCTCTCATTTCATTTGCGTTCGCGGTTTCGTGCAAGGCTCCGCAAAAAGAAGAACCGATTAATATTACCCCAGAAGAACTCGACGCATCTATTGATCCTGTGACCGAAATTATGATCAACGATATCTTCTCCCCGCCAGTTGCGTCGCCTATTTTTGCGTATCCTAACGTGGCGGCGTACGAAATTGTGGCGGCAACTAATGATAACTACAACTCGTTAGCTGGGCAACTGAATGGCCTGACGGCCATCCCTGAGCCCGACACCACAAAAACGATCAACTATGAACTTGCGGCTGTGGTCGCAAATATGGAGCTGTCTAAACGCTTGATTTTTTCAGAAGACCCTATGGAATCCCTACGCGATTCCCTGTACATGGTCTTGGAGGGCAAAAATCCGGTATTGTTCTCCGATTCAAAAGCCTACGGGCTGCAAGTCGCGGATAATATTGGTGAATTGATGAACAAGGACAACTATGCTCAAACCCGCACCATGCCGAAATTTACTGTGGACGCCGATGACCCGGGTCCTTTGCAGCCGACCCCGCCTGCGTACATGGATGGAATCGAACCTAATTTGAACAAAATCCCTCCCTTCGTTCTGGACTCGGCGGCCCAATTCAAACCAGTCCCGCCGCCGGCATATTCACTGGAGGAAGATTCAGCTTTTTACAAAGAACTGAAAGAGGTCTACGATGTCCCTAACAAAATTACTGAAGAAGGTGATTCATCGGAGGAAATCCAAATTGCTCGCTTTTTGGATTGCAATCCTTACGTCTCGGTTACCCCTGGCAACCTGATGTTCGCTACTAAGAAAATCACGCCTGGTGCGAACTTGATGGGTATCGCTAAAATAGCGGCGCCTAAAACCAACTCAGATTTTGCTAAAACGCTGTTCGCCTACACGAAGGCGTCAGTGGCGATGGCGGACGCATTCATTTCATGCTTGGATGAGAAGTATCGCTCGAATCTGATTCCTCCCGAGACTGTCATTAACCAGAACATTGACGACTCCTTGAAGCCAGTCCTTCAAACTCCGCCATTCCCGGAATACACCTCAGGCAACTCCGTTGTCTCCGGCGCGGCATCGGTTGTGCTTACAGAGGTCTTTGGGGATAACTTCTCCTTCGATGATGATACAGAAGTGCCCTATGGCTTACCAATTCGCTCGTTTAAATCTTTCAAGCAGGCGGCCGATGAAGCAGCTATCTCACGCATGTACGGTGGTATTAATTACCCTGCTGCGATCGAAGTTGGCGTGAAACAAGGTCCTGATCTCGGCACTTTCGTGGTAAACAAACTGAACATGCTCTCTGACAAAAAAGTTGCGCAGAAT</t>
+          <t>ATGAAAAAAATCCTGATCGCTCTGATCTCTTTTGCATTCGCGGTGTCATGTAAAGCACCACAGAAAGAAGAACCGATCAATATTACCCCGGAAGAACTTGATGCCTCGATCGACCGAGTGACGGAAATTATGATCAACGATATCTTTTCCCCGCCGGTTGCCTCCCCTATATTCGCATACCCTAATGTGGCGGCGTATGAAATCGTGGCGGCGACCAATGATAACTATAACTCTCTGGCGGGACAACTGAACGGCCTGACCGCTATCCCAGAACCGGATACCACAAAAACCATAAATTACGAACTTGCTGCAGTGGTGGCGAACATGGAGCTGTCCAAGCGCCTGATTTTTTCTGAAGACCGCATGGAATCGCTCCCTGATTCCTTGTATATGGTGTTGGAGGGAAAAAACCCTGTTCTTTTCTCCGATTCGAAGGCGTATGGCCTGCAGGTTGCGGATAATATCGGTGAATTGATGAACAAGGATAACTACGCGCAAACGCCTACTATGCCTAAATTTACGGTTGATGCGGATGATCCGGGTCCTTTGCAGCCCACGCCGCCGGCATATATGGACGGGATTGAACCGAATTTGAATAAAATTCGACCATTCGTATTAGATTCAGCTGCACAATTCAAACCGGTGCCGCCTCCCGCCTACTCCCTGGAGGAAGACTCAGCTTTTTATAAAGAATTGAAAGAGGTCTATGACGTGCCTAACAAAATTACCGAGGAAGGCGATTCATCCGAAGAAATTCAGATCGCTCGCTTTTTGGACTGTAATCCCTACGTTTCCGTAACTCGGGGCAATCTGATGTTTGCCACGAAAAAAATCACACCAGGTGCAAACTTGATGGGGATTGCTAAAATCGCGGCTCGCAAAACGAATTCAGACTTCGCGAAAACATTGTTTGCGTATACTAAAGCCTCAGTCGCCATGGCGGACGCGTTTATTTCATGTTTGGACGAAAAATATCGGTCTAACTTGATTCCTCCGGAAACAGTTATTAACCAAAATATTGACGACTCGTTGAAACCGGTACTGCAAACCCCACCGTTTCCGGAGTATACCTCTGGTAATTCCGTTGTATCCGGTGCCGCGTCGGTTGTGCTTACCGAGGTGTTTGGGGATAATTTTTCGTTTGACGATGATACCGAAGTTCCTTATGGGCTGCCGATTCGATCTTTTAAATCATTCAAACAGGCGGCGGATGAAGCGGCAATCTCTCCTATGTACGGTGGCATCAATTATCGCGCGGCTATTGAAGTCGGGGTCAAACAAGGCCCTGATCTGGGCACCTTCGTTGTAAACAAGCTTAATATGCTGTCGGACAAAAAAGTAGCGCAAAAC</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>ATGAAGAAAATCTTAATTGCTCT</t>
+          <t>ATGAAAAAAATCCTGATCGC</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>ATTCTGCGCAACTTTTTTG</t>
+          <t>GTTTTGCGCTACTTTTTTG</t>
         </is>
       </c>
     </row>
@@ -2194,22 +2194,22 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>TACTTCGCGGAGAGGGGAAAGTAATAGCATACGTGGCACAATTACCACAGGACGCCGTGGTTGTTGCTGTTTCTTGCCGACCTATGGATAAAGCTCCCGCCAGATAGAGCGATGTTGGGACTTGACTGCTTGCAGTAACAGAGCCTATAAAAGTGGGGAGGGCACCGCAGAGCGTAGATACGGATGAGATTGTAACGCCGTATGCTCCCCTAAGCGAAGTACCTGAGGTGATTTGACAGGGACAGGAGAGCGGACTTGCCAGACTTTCTTGACAGATGGGGCCTGGGCAGTTTTTTAATAATAATGGGCGACCAAAGATAACACCGTAAATGCGTCCACCCCTTTAGCGACCAGAAACTGAATCTATTCCAACTCCGTTATTTTTTGTTCTACGAACCACTCCAATTTCTCTAGCCGTACCTAGTCCTCCATATGGCGTTAAGGTAGCTGAACCCACTCTGGGAGCGTAGACTTTAGGAACGAAACCGGCGCTTTCTACCGATAGAAGGAGCCTGTCGAGACGGCGGAATGAGACACAGGCTACTGGGACCGGCGAACGCGGGCTGTGGGGGTCTAATATACCTTCGTTATCTTGGCTTAAACTTATGGGATGCGGGTAAGCACAATCTGAGGCGCCGAGTCAAACTGGGCCCGGATGGCTGAGGCAAGCTAAGGCGCCTCCTAAGTGGAAAGATGTTTCTTCGGTACCTTCATATGCTTTGTCACCTTTTAGACCTGCTGCTATTCAATCTTCAACGCTTTAAAAACCTAACGTTGGGCTTGTAGAGATTGTGATTTCCATTGCACTACATGAAAGTCGTTGTTTAAAGTGGCCCTCCCTTAAACTACTTGTAACGACGGGTCTAGGAGCTCCTCGTCTTCCAACTACCGCACTTTCGTCGCCTCTGGTACAGATACGACCCGCATCGAGACCGTCTGCGGAAGTAGAGCACAAACCTGGTTTTCATGTTTAGCAGGAATTGGGCGGGACTTTGCATATAATTGTTGATATAGCTAGTCCTGAACCTCGGCTAGGACGTCTGGGGTCGCAAAGGTCTCTTATGGAGACCATTGAGCCACCGCAGAAGACGCCGCCGCTGACAGGACTGACCGCACAAACCACTACTGATGCGAAAACAACTACGCTGGCTTCACGGCATGCCGGAAGGCGGGGCTAGAAAAGTCAGGAAAAACGTCCGTCGTCTTCTCCGTCGATAGAGGGGAGAAATGCCCCCGTATTTGATAGCCGGCCGGTAACTCGAGCCCCAATTCGTCCCCGCGCGCCATCCGGGAAATCAGGACCTCGCTGACGGATTTCTCTTG</t>
+          <t>TACTTTGCGGACAGTGCGAAATAATAGCAGACGTGGCAAGACTACCAAAGGACGCCGTGGTTATTGCTGTTTCTTGCGAATCTATGTATGAAACTTCCTCCAGAAAGAGCGATGTTGGCGCTTGACTGGTTACATTAACACAGACTATAGAAATGGGGCGGCCACCGGAGAGCGTAAATACGAATAAGGTTATAACGTCGTATACTCCCGTAAGGAAAGTACCTAAGTTGGTTTAACAGAGACAGAAGGGCGGACTTGCCAGACTTTCTCGACAGTTGCGGCCTGGGCAGTTTTTTAATAATGATAGGCAACCAAAGTTAGCAGCGTAAGTGAGTCCAACCATTTAGAGAGCAAAAACTGGACCTGTTTCATCTTCGGTAGTTTTTGTTTTACGACCCACTTCAATTTCTTTAGCCATACCTGGTCCTCCACATAGCCTTAAGGTAGCTGGACCCCCTCTGGGACCGGAGACTTTAGGAGCGGAACCGCCGCTTTCTGCCAATAGACGCGGCGTGCCGTAACGGCGGAATGAGGCACAGCCTGCTGGGCCCGGGAAACGGAGGCTGGGGCGGCCTAATATACCTCCGATAACTTGGGTTGAACTTGTGGAATGCCGGAAAACACGACCTAAGGCGCCGCGTCAAGCTAGGCCCGGAGGGTTGTGGCAAGCTGAGACGACTTCTAAGAGGCAAAATGTTTCTTCGTTACCTTCATATACTTTGCCACCTTTTGGACCTGCTGCTATTTGACCTTCACCGGTTTAAGAACCTGACATTGGGCTTGTAAAGATTGTGGTTCCCGTTGCAGTACATAAAGGTCGTCGTCTAGAGAGGCCCACCGTTGAACTACTTGTAACGCCGCGTCTAGGACCTCCTTGTCTTCCAACTACCGCAGTTTCGGCGTCTTTGCTACAGCTACGACCCACAACGCGACCGACTGCGAAAGTAGAGTACAAACCTAGTTTTTATATTTAGCAGCGAGTGCGCTGGCCTTTGGATGTAGTTATTAATATAACTGGTCCTGAACCTTGGCTATGACGTCTGCGGCCGTAAAGGCCTTTTATGAAGCCCGTTAAGTCACCGGAGCAGACGGCGTCGATGGCACGACTGACCGCACAAACCACTACTAATGCGGAAGCAACTGCGTTGACTCCACGGCATACCGGAAGGTGGTGCGAGAAAGGTCAGTAAGAACGTCCGTCGACTCCTTCGACGCTAAAGTGGAGACATACCGCCGTAATTGATGGCGGGCCGGTAGCTTGACCCACACTTCGTCCCAGCGCGACAACCAGCGAACCACGACCTCGGAGACGCGTTTCTTTTA</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>ATGAAGCGCCTCTCCCCTTTCATTATCGTATGCACCGTGTTAATGGTGTCCTGCGGCACCAACAACGACAAAGAACGGCTGGATACCTATTTCGAGGGCGGTCTATCTCGCTACAACCCTGAACTGACGAACGTCATTGTCTCGGATATTTTCACCCCTCCCGTGGCGTCTCGCATCTATGCCTACTCTAACATTGCGGCATACGAGGGGATTCGCTTCATGGACTCCACTAAACTGTCCCTGTCCTCTCGCCTGAACGGTCTGAAAGAACTGTCTACCCCGGACCCGTCAAAAAATTATTATTACCCGCTGGTTTCTATTGTGGCATTTACGCAGGTGGGGAAATCGCTGGTCTTTGACTTAGATAAGGTTGAGGCAATAAAAAACAAGATGCTTGGTGAGGTTAAAGAGATCGGCATGGATCAGGAGGTATACCGCAATTCCATCGACTTGGGTGAGACCCTCGCATCTGAAATCCTTGCTTTGGCCGCGAAAGATGGCTATCTTCCTCGGACAGCTCTGCCGCCTTACTCTGTGTCCGATGACCCTGGCCGCTTGCGCCCGACACCCCCAGATTATATGGAAGCAATAGAACCGAATTTGAATACCCTACGCCCATTCGTGTTAGACTCCGCGGCTCAGTTTGACCCGGGCCTACCGACTCCGTTCGATTCCGCGGAGGATTCACCTTTCTACAAAGAAGCCATGGAAGTATACGAAACAGTGGAAAATCTGGACGACGATAAGTTAGAAGTTGCGAAATTTTTGGATTGCAACCCGAACATCTCTAACACTAAAGGTAACGTGATGTACTTTCAGCAACAAATTTCACCGGGAGGGAATTTGATGAACATTGCTGCCCAGATCCTCGAGGAGCAGAAGGTTGATGGCGTGAAAGCAGCGGAGACCATGTCTATGCTGGGCGTAGCTCTGGCAGACGCCTTCATCTCGTGTTTGGACCAAAAGTACAAATCGTCCTTAACCCGCCCTGAAACGTATATTAACAACTATATCGATCAGGACTTGGAGCCGATCCTGCAGACCCCAGCGTTTCCAGAGAATACCTCTGGTAACTCGGTGGCGTCTTCTGCGGCGGCGACTGTCCTGACTGGCGTGTTTGGTGATGACTACGCTTTTGTTGATGCGACCGAAGTGCCGTACGGCCTTCCGCCCCGATCTTTTCAGTCCTTTTTGCAGGCAGCAGAAGAGGCAGCTATCTCCCCTCTTTACGGGGGCATAAACTATCGGCCGGCCATTGAGCTCGGGGTTAAGCAGGGGCGCGCGGTAGGCCCTTTAGTCCTGGAGCGACTGCCTAAAGAGAAC</t>
+          <t>ATGAAACGCCTGTCACGCTTTATTATCGTCTGCACCGTTCTGATGGTTTCCTGCGGCACCAATAACGACAAAGAACGCTTAGATACATACTTTGAAGGAGGTCTTTCTCGCTACAACCGCGAACTGACCAATGTAATTGTGTCTGATATCTTTACCCCGCCGGTGGCCTCTCGCATTTATGCTTATTCCAATATTGCAGCATATGAGGGCATTCCTTTCATGGATTCAACCAAATTGTCTCTGTCTTCCCGCCTGAACGGTCTGAAAGAGCTGTCAACGCCGGACCCGTCAAAAAATTATTACTATCCGTTGGTTTCAATCGTCGCATTCACTCAGGTTGGTAAATCTCTCGTTTTTGACCTGGACAAAGTAGAAGCCATCAAAAACAAAATGCTGGGTGAAGTTAAAGAAATCGGTATGGACCAGGAGGTGTATCGGAATTCCATCGACCTGGGGGAGACCCTGGCCTCTGAAATCCTCGCCTTGGCGGCGAAAGACGGTTATCTGCGCCGCACGGCATTGCCGCCTTACTCCGTGTCGGACGACCCGGGCCCTTTGCCTCCGACCCCGCCGGATTATATGGAGGCTATTGAACCCAACTTGAACACCTTACGGCCTTTTGTGCTGGATTCCGCGGCGCAGTTCGATCCGGGCCTCCCAACACCGTTCGACTCTGCTGAAGATTCTCCGTTTTACAAAGAAGCAATGGAAGTATATGAAACGGTGGAAAACCTGGACGACGATAAACTGGAAGTGGCCAAATTCTTGGACTGTAACCCGAACATTTCTAACACCAAGGGCAACGTCATGTATTTCCAGCAGCAGATCTCTCCGGGTGGCAACTTGATGAACATTGCGGCGCAGATCCTGGAGGAACAGAAGGTTGATGGCGTCAAAGCCGCAGAAACGATGTCGATGCTGGGTGTTGCGCTGGCTGACGCTTTCATCTCATGTTTGGATCAAAAATATAAATCGTCGCTCACGCGACCGGAAACCTACATCAATAATTATATTGACCAGGACTTGGAACCGATACTGCAGACGCCGGCATTTCCGGAAAATACTTCGGGCAATTCAGTGGCCTCGTCTGCCGCAGCTACCGTGCTGACTGGCGTGTTTGGTGATGATTACGCCTTCGTTGACGCAACTGAGGTGCCGTATGGCCTTCCACCACGCTCTTTCCAGTCATTCTTGCAGGCAGCTGAGGAAGCTGCGATTTCACCTCTGTATGGCGGCATTAACTACCGCCCGGCCATCGAACTGGGTGTGAAGCAGGGTCGCGCTGTTGGTCGCTTGGTGCTGGAGCCTCTGCGCAAAGAAAAT</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>ATGAAGCGCCTCTC</t>
+          <t>ATGAAACGCCTGTCAC</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>GTTCTCTTTAGGCAGTC</t>
+          <t>ATTTTCTTTGCGCAGAGG</t>
         </is>
       </c>
     </row>
@@ -2236,22 +2236,22 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>TACTGCTGCAGCCCGTTATGAAGAAAAAGCCTGATGAGGGGCGCGGGAGGAAGTTACGAAGACCCCCCGGACCCGCCGCGCCGGCGAGACAGTCGCCGTCCGAAATGTCCATACCGGAGACGTAGGGGCGGACCGAGGCGCCCAAGATTCCGGCGCCGCTAGCTCAAGCTAAACCTATTTCTGTTGATATAATTTAACCGGGTCGGCTGACTACTTTTGCGACCCGTCAGCGGTTGCGACCGCTAGGACCCAGGCTACCTACAATGACAAAAGGACAACTATTTGGCGCATCAGAACAATCGGCGGAAACTGCGCGACCGGGGCATGTTGCTCTGCCGGCAGCCTCACATGAGCGTCTATGGAGCGGCTGGCAGGAGCCTCAGCCGATGCTTGGCGTTGGACTTGTAACGCCGTGACTTGCGGGTCTTACCACACAACTTTGGACATGACGGAGTCGTTCACCTAGTCGAAGGACTTGACTACTGTCGCGACCCGGACCTAGGCAGCCTGCTTTGGCTCTTGAACAGCAGTGGCCAACCCTAGCCGTTACACCGCCGTTTCTTGCGGAAGTTGCGCGAGTTTTTACTACCCTACTTAAAAGACCCAATACTTCCGGCGTTTATGTTGGGCGGAGGAAACCGCCTAATATGGCCAATACTCGGACAGTTATGCCGAAAATTCCAGTTATTGGGAAGAGCCAACGTTGGAGTCGACGTCCGGTTGTTACGGGCGGCGCGACCGCCGCCGGGCCCGCTGGACCCGTAAATACACTGGGTCTTAAAACACTGGGGGGTTTGCCGGGGATGCTTTCGCTTATATAAGGGACTGGGCAGGGCCAAGGGATAAGGCGCGGGACTTAAAAGACTGTTGTGGTTATGAGGACGAATATTTGGAAGGCACCTACTTTAATAACTGCGCAGCCGCTTAGACTTACTACTCGGATTTCGAGACCGCCTCTAATACCTCTTGTTTAATAACCCTTAGCCGTTGAGGAGGTAACAGTAGCGATTGTTTATGCTAGTCTTGTTGCTTTACCCGCAATTGCCGAACACGTTAAACTACAATCGTTTGCACGACCGATGGAAACTTGGAGAATAGCGACGCAACTTATTGTTCTGTGCCAAACTGCGACACGGAGGCCATTGGCGATAGGGATTGCAAATACCCTTGGGATTCTAAGGACGGAACCCACCACAGCCATACCCCTGGCAGCTATAAGGACGCAGGCTTAACAGAAGAATGGAAGGACACCCGCTATTAGGCCTTATAGGTAGACCAAGATGTAGTGACACAAGGCGCTGCAGAGTCCGTCGCGCCGCGATAAAACTGAGGCTACTCGAACTGAACTGCTAGTTGATGGGCCGACCGAGATGCCATCATCTTGGTCCCTATTGAGGCCCGTTCCTGAACAGGTAATTATATGGCTGCAACTGTCTAAAGTGGGGATGAACGCGGTGCAGAGGACATAACCCGCCGCATTTGAAAGTCTGGTGGCAACTAGGATGGTAACTAAAGCCTCTTGTCAAGCCCCTGGACCGTTTACTTAAGCAGGTTGCGTTACAGTTCCCGCTACACTTTCTA</t>
+          <t>TACTGGTGAAGCCCATTATGTAGAAAAAGTCTGATAAGGGGCGCCGCGGCGAGGTACGACGACCCGCCGAACCCACCACGTCGGCGGGACAGGCGGCGACCAAAGTGCCCGTACCGCAGCCGGAGAGGCGCGCCAAGACGACCAAGCTTCCGTCGGCGCTAGCTTAAACTGAATCTATTTCTATTGATGTAATTTAACCGAGTCGGCTGTCTGCTCTTGCGCCCAGTCAGCGGTTGAGACCGTTAGGACCCGGGCTACCTACACTGGCAGAAGGAAAACTAATTGGCGCACCAAAACGACCGCCGCAAACTACGCGAGCGAGGTATATTGCTTTGGCGTCAACCCCACATAAGTGTCTAGGGCGCGGCGGGCAGCAGTCTCAGACGGTGGTTGGGATTAGACTTATAACGTCGCGAGTTGCGAGTCTTGCCACATAACTTCGGACATGACGGAGTTGTCCACCTGGTTGAGGCGCTCGACTACTGGCGGGAGCCAGAGCTAGGTAGCCTGCTTTGGCTCTTAAACAGAAGAGGCCACCCATAGCCGTTACAACGCCGCTTTTTGCGTAAGTTGCGGGAATTTTTGCTACCATACTTGAAGGAACCGATACTCCCCGCGTTTATATTGGGTGGAGGCAACCGGCTGATGTGGCCGATGCTTGGCCATTTGTGACGCAAGTTTCAATTGTTAGGCAGTGGAAACGTCGGCGTCGACGTCCGCTTATTGCGGGGAGGACGTCCACCCCCGGGCCCACTAGACCCATAGATACATTGCGTCTTAAAGCACTGCGGCGTCTGGCGCGCTTGGTTTCGCTTATAAAAGGGACTGGGAAGGGGAAAAGGATAGGGGGGAGGTCTCAAGAGACTGTTGTGGTTATGTGCTCGGATATTTGCGAGGCATCTGCTCTAATAGCTGCGCAGCCGGTTGGACTTGCTACTTGGATTTCGAGAGCGTCTCTAGTACCTCTTGTTTAACAACCCATAGCCCTTAAGAAGCTAACACTAACGTTTGTTTATGCTAGTTTTATTGCTCTACCCACAGTTGCCCAACACATTGAACTACGACCGATTACAGGAGCGGTGTAAACTTGGCGACTAGCGCCGTAACTTGTTGTTTTGGGGAAAACTACGCCAAGCCGGACACTGGCGTTAGGCGTTGCACATACCGTTGGGATTCTAGGGACGCAACCCACCGCAACCGTACCCTTGTCAGCTATAGGCGCGAAGACTTAACAGCAGGATGGACGGCCAACCACTATTGGGCCTTATAGGCAGACCGAGGTGGAGGGACACGAGACGTTGCAGCGTTCGACGCGCGGCGATAAAGCTGAGTCTACTTGAGCTGAACTGGTAATTAATGGGCCGTCCAAGTTGCCACCACCTTGGTCCATAGTGCGGCCCCTTCCTAGACAGATAATTGTAGGGCTGGAACTGCCTGAAGTGGGCTTGGACACGCTGGAGTGGACACAACCCGCCTCACTTAAAGGTCTGGTGTCACCTAGGATGGTAACTAAAACCCCTTGTTAAGCCGCTAGAACGATTACTTAAACATGTCGCGTTACATTTCCCACTGCATTTTCTA</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>ATGACGACGTCGGGCAATACTTCTTTTTCGGACTACTCCCCGCGCCCTCCTTCAATGCTTCTGGGGGGCCTGGGCGGCGCGGCCGCTCTGTCAGCGGCAGGCTTTACAGGTATGGCCTCTGCATCCCCGCCTGGCTCCGCGGGTTCTAAGGCCGCGGCGATCGAGTTCGATTTGGATAAAGACAACTATATTAAATTGGCCCAGCCGACTGATGAAAACGCTGGGCAGTCGCCAACGCTGGCGATCCTGGGTCCGATGGATGTTACTGTTTTCCTGTTGATAAACCGCGTAGTCTTGTTAGCCGCCTTTGACGCGCTGGCCCCGTACAACGAGACGGCCGTCGGAGTGTACTCGCAGATACCTCGCCGACCGTCCTCGGAGTCGGCTACGAACCGCAACCTGAACATTGCGGCACTGAACGCCCAGAATGGTGTGTTGAAACCTGTACTGCCTCAGCAAGTGGATCAGCTTCCTGAACTGATGACAGCGCTGGGCCTGGATCCGTCGGACGAAACCGAGAACTTGTCGTCACCGGTTGGGATCGGCAATGTGGCGGCAAAGAACGCCTTCAACGCGCTCAAAAATGATGGGATGAATTTTCTGGGTTATGAAGGCCGCAAATACAACCCGCCTCCTTTGGCGGATTATACCGGTTATGAGCCTGTCAATACGGCTTTTAAGGTCAATAACCCTTCTCGGTTGCAACCTCAGCTGCAGGCCAACAATGCCCGCCGCGCTGGCGGCGGCCCGGGCGACCTGGGCATTTATGTGACCCAGAATTTTGTGACCCCCCAAACGGCCCCTACGAAAGCGAATATATTCCCTGACCCGTCCCGGTTCCCTATTCCGCGCCCTGAATTTTCTGACAACACCAATACTCCTGCTTATAAACCTTCCGTGGATGAAATTATTGACGCGTCGGCGAATCTGAATGATGAGCCTAAAGCTCTGGCGGAGATTATGGAGAACAAATTATTGGGAATCGGCAACTCCTCCATTGTCATCGCTAACAAATACGATCAGAACAACGAAATGGGCGTTAACGGCTTGTGCAATTTGATGTTAGCAAACGTGCTGGCTACCTTTGAACCTCTTATCGCTGCGTTGAATAACAAGACACGGTTTGACGCTGTGCCTCCGGTAACCGCTATCCCTAACGTTTATGGGAACCCTAAGATTCCTGCCTTGGGTGGTGTCGGTATGGGGACCGTCGATATTCCTGCGTCCGAATTGTCTTCTTACCTTCCTGTGGGCGATAATCCGGAATATCCATCTGGTTCTACATCACTGTGTTCCGCGACGTCTCAGGCAGCGCGGCGCTATTTTGACTCCGATGAGCTTGACTTGACGATCAACTACCCGGCTGGCTCTACGGTAGTAGAACCAGGGATAACTCCGGGCAAGGACTTGTCCATTAATATACCGACGTTGACAGATTTCACCCCTACTTGCGCCACGTCTCCTGTATTGGGCGGCGTAAACTTTCAGACCACCGTTGATCCTACCATTGATTTCGGAGAACAGTTCGGGGACCTGGCAAATGAATTCGTCCAACGCAATGTCAAGGGCGATGTGAAAGAT</t>
+          <t>ATGACCACTTCGGGTAATACATCTTTTTCAGACTATTCCCCGCGGCGCCGCTCCATGCTGCTGGGCGGCTTGGGTGGTGCAGCCGCCCTGTCCGCCGCTGGTTTCACGGGCATGGCGTCGGCCTCTCCGCGCGGTTCTGCTGGTTCGAAGGCAGCCGCGATCGAATTTGACTTAGATAAAGATAACTACATTAAATTGGCTCAGCCGACAGACGAGAACGCGGGTCAGTCGCCAACTCTGGCAATCCTGGGCCCGATGGATGTGACCGTCTTCCTTTTGATTAACCGCGTGGTTTTGCTGGCGGCGTTTGATGCGCTCGCTCCATATAACGAAACCGCAGTTGGGGTGTATTCACAGATCCCGCGCCGCCCGTCGTCAGAGTCTGCCACCAACCCTAATCTGAATATTGCAGCGCTCAACGCTCAGAACGGTGTATTGAAGCCTGTACTGCCTCAACAGGTGGACCAACTCCGCGAGCTGATGACCGCCCTCGGTCTCGATCCATCGGACGAAACCGAGAATTTGTCTTCTCCGGTGGGTATCGGCAATGTTGCGGCGAAAAACGCATTCAACGCCCTTAAAAACGATGGTATGAACTTCCTTGGCTATGAGGGGCGCAAATATAACCCACCTCCGTTGGCCGACTACACCGGCTACGAACCGGTAAACACTGCGTTCAAAGTTAACAATCCGTCACCTTTGCAGCCGCAGCTGCAGGCGAATAACGCCCCTCCTGCAGGTGGGGGCCCGGGTGATCTGGGTATCTATGTAACGCAGAATTTCGTGACGCCGCAGACCGCGCGAACCAAAGCGAATATTTTCCCTGACCCTTCCCCTTTTCCTATCCCCCCTCCAGAGTTCTCTGACAACACCAATACACGAGCCTATAAACGCTCCGTAGACGAGATTATCGACGCGTCGGCCAACCTGAACGATGAACCTAAAGCTCTCGCAGAGATCATGGAGAACAAATTGTTGGGTATCGGGAATTCTTCGATTGTGATTGCAAACAAATACGATCAAAATAACGAGATGGGTGTCAACGGGTTGTGTAACTTGATGCTGGCTAATGTCCTCGCCACATTTGAACCGCTGATCGCGGCATTGAACAACAAAACCCCTTTTGATGCGGTTCGGCCTGTGACCGCAATCCGCAACGTGTATGGCAACCCTAAGATCCCTGCGTTGGGTGGCGTTGGCATGGGAACAGTCGATATCCGCGCTTCTGAATTGTCGTCCTACCTGCCGGTTGGTGATAACCCGGAATATCCGTCTGGCTCCACCTCCCTGTGCTCTGCAACGTCGCAAGCTGCGCGCCGCTATTTCGACTCAGATGAACTCGACTTGACCATTAATTACCCGGCAGGTTCAACGGTGGTGGAACCAGGTATCACGCCGGGGAAGGATCTGTCTATTAACATCCCGACCTTGACGGACTTCACCCGAACCTGTGCGACCTCACCTGTGTTGGGCGGAGTGAATTTCCAGACCACAGTGGATCCTACCATTGATTTTGGGGAACAATTCGGCGATCTTGCTAATGAATTTGTACAGCGCAATGTAAAGGGTGACGTAAAAGAT</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>ATGACGACGTCGGG</t>
+          <t>ATGACCACTTCGGG</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>ATCTTTCACATCGCCCT</t>
+          <t>ATCTTTTACGTCACCCT</t>
         </is>
       </c>
     </row>
@@ -2278,22 +2278,22 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>TACCGGGGCCCACTGCATAGCAGTATATGGAACCACTGCTTAGAGGAAGTTTGAAGGAACAAGCTACGTAATCGCGGAATATTAGGCTGCCGTCAGCCGCAAATGAGGGCTTAGGGCGCGGCGGGTCGCCTTCTCAGACGGTGGTTGGCGTTGTTTTTGTAGCGGCCTGAGATACGCTACAAGGTCCAACACTTTCGCCGGAAATGGCTCGGACAAGGCCAGGACGCTGTCCGAGAGCCGCGTAACCCGGACCTAGGACTGCTACTCAGTGTCCTGGACAGCTGTCGGCATCCATAACCGTTATGTCGCCCGTTTCGACAGCGTCGACGCGCGTACCCACTACCATACTTGCGCGACCCGCCCTTTCTGGCGTGGTTATTACCGGTCGGCATACTTCTGATGTGGCCTATGGCTGGACAGTTGTGCCGCCTACTTGACCACCTGGGGAGGGGAAACGTTGGCCGTCACCTTGGATTAGCCGCTGCCTGGCTGCCACCGGGCCCGCTGTTTCCGTAGAAATGGCGCGTCGCGAAACGATGGGGAGTCGACCCCAATCACCGCGGCGTCTGGATGGCGCTAGGACGCGGAAAGTTTGACCGCCGAGGTCTGTTGAACCTGTTGTTACTACGCCCGCGGATGGGAGTCCGCCACCTACTTCACAACCGCCGGAGGCGTCCGAATTGGCTGCTTGTCTTTCACTTCCGGCTCAAAAAGCTCTTGTGTGGCGAGAGACAATGGAATAGAGGGGGACGCCGCCGATACCGGTTGCTAAACCTGGACCTACCAAACCGTGTTGACAAGAACCACACGAGCTGGCGCGGAAAGCTAAGGGACTAGCGCCGTAACTTATTGTTTGGACGGATACTATGACACGCCGGAAAGAGTCGCCACGCGTTGCAAATACCGAGTTTTGGACAGTGCCGAAACCCGCCGGGACCATTTCCGTGGCACCTTAGCTAAGGTCGTCTGCTTAACTGCCCGATGGACGGCCACCCCTTATTGGGCCTTATGGGCAGACCGAAATGGTGTGACTATCGACGTGTCCGAGTTCGACGGGCGAGAAAGGACCCGCTACTGCAAAACTTGAACTGGTTACGGAAGGGTCGTCCAAGGCCAGTCGCGCTTGGCCCTCGTCACGGCCGGAGCCTGAATCTTGAGTGCAACCGATGCAACTGACTAAAACTTTTGCTAACGCGATGGAGCGGACATAACCGGCCACGCTTAAAATGATTTTGGCGCCTCTGGAGAGACCGCAAACCTTGGGTCAAGCCGCTAGACCGTTTATGGAAGCATGTTGGATTATAGTTACCGCTACACTTCCTA</t>
+          <t>TACCGGGGCCCTCTACAGAGTAGCATGTGGAACCACTGGTTGGACGAAGTCTGAAGGAACAAGCTGCGTGACCGTGGGATGTTGGGCTGACGTCACCCTCAAATAAGCGGATATGGCGGAGGAGGCCGACTCCTCAGGCGCTGGTTGGGATTATTCTTGTAACGACCGGACATACGCTACAAAGTTCACCAATTCCGTCGTAAATGCCTTGGACAGGGCCATGAGGCCGTTCGTGATCCGCGAGACCCGAATCTAGGACTGCTGCTTAGTGTCCTGGACAGCTGGCGGCAGCCGTAGCCATTATGGCGTCCCTTTCGACAACGCCGACGTGCGTACCCGCTACCATACTTACGTGACCCTCCGTTCCTAGGATGGTTATTGCCGGTCGGCATGCTTCTAATGTGGCCGATAGGAGGCCACTTGTGACGACTACTTGAGCAGCTGGGCAGGGCGAACGTCGGGCGCCACCTTGGATTGGGAGGAGCGTGGCTACCACCAGGGCCGCTATTCCCGTATAAGTGCCGTGTCGGAAAACGCTGGGGTGTCGACCCCGACCACCGCGGGGTCTGGATGGGACTAGGTCGAGCGAAATTTGACCGACGAGGCCTATTAAACCTATTATTGCTGCGGCCACGGATAGGAGTCCGACAGCTACTTCATAACCGGCGTAGGCGTCCGGAGTGTCTGCTCGTCTTTCAGTTTCGCCTTAAGAAGCTTTTGTGTGGTGAGAGCCATTGAGACAGGGGCGCGCGCCGGCGCTACCGTTTACTGGATCTAGACCTGCCTAACCGTGTCGAAAAAGACCACACGAGGTGTCGGGGAAAACTAAGCAATTAACGACGGAACTTATTGTTCGGACGCATACTATGCCATGCGGGAAAGAGGCGGCACGCGTTACAGATGCCAAGATTTGGCCAATGTCGGAACCCACCAGGTCCGTTCCCCTGCCACCTTAGTTAGGGACGGCTGCTCAACTGGCCTATAGACGGCCACCCGTTGTTAGGCCTTATGGGCAGGCCGAAATGGTGGGATTAACGTCGGGTCCGAGTCCGGCGCGGAAGAAAGAATCCACTGCTGCAGGACTTAAACTGATTGCGAAAAGGCCGCCCAAGGCCGGTCGGACTCGGACCCCGGCATGGGCGGAGACTAGACCTCAATTGGAACCGTTGGAACTGACTGAAACTTTTACTGACACGGTGGAGCGCGCAAAACCGCCCACGCTTAAAGTGGTTTTGACGGCTTTGTAGTGACCGGAAACCCTGGGTCAAACCGCTGAATCGCTTATGAAAGCATGTTGCGTTATAGTTGCCACTACATTTCCTG</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>ATGGCCCCGGGTGACGTATCGTCATATACCTTGGTGACGAATCTCCTTCAAACTTCCTTGTTCGATGCATTAGCGCCTTATAATCCGACGGCAGTCGGCGTTTACTCCCGAATCCCGCGCCGCCCAGCGGAAGAGTCTGCCACCAACCGCAACAAAAACATCGCCGGACTCTATGCGATGTTCCAGGTTGTGAAAGCGGCCTTTACCGAGCCTGTTCCGGTCCTGCGACAGGCTCTCGGCGCATTGGGCCTGGATCCTGACGATGAGTCACAGGACCTGTCGACAGCCGTAGGTATTGGCAATACAGCGGGCAAAGCTGTCGCAGCTGCGCGCATGGGTGATGGTATGAACGCGCTGGGCGGGAAAGACCGCACCAATAATGGCCAGCCGTATGAAGACTACACCGGATACCGACCTGTCAACACGGCGGATGAACTGGTGGACCCCTCCCCTTTGCAACCGGCAGTGGAACCTAATCGGCGACGGACCGACGGTGGCCCGGGCGACAAAGGCATCTTTACCGCGCAGCGCTTTGCTACCCCTCAGCTGGGGTTAGTGGCGCCGCAGACCTACCGCGATCCTGCGCCTTTCAAACTGGCGGCTCCAGACAACTTGGACAACAATGATGCGGGCGCCTACCCTCAGGCGGTGGATGAAGTGTTGGCGGCCTCCGCAGGCTTAACCGACGAACAGAAAGTGAAGGCCGAGTTTTTCGAGAACACACCGCTCTCTGTTACCTTATCTCCCCCTGCGGCGGCTATGGCCAACGATTTGGACCTGGATGGTTTGGCACAACTGTTCTTGGTGTGCTCGACCGCGCCTTTCGATTCCCTGATCGCGGCATTGAATAACAAACCTGCCTATGATACTGTGCGGCCTTTCTCAGCGGTGCGCAACGTTTATGGCTCAAAACCTGTCACGGCTTTGGGCGGCCCTGGTAAAGGCACCGTGGAATCGATTCCAGCAGACGAATTGACGGGCTACCTGCCGGTGGGGAATAACCCGGAATACCCGTCTGGCTTTACCACACTGATAGCTGCACAGGCTCAAGCTGCCCGCTCTTTCCTGGGCGATGACGTTTTGAACTTGACCAATGCCTTCCCAGCAGGTTCCGGTCAGCGCGAACCGGGAGCAGTGCCGGCCTCGGACTTAGAACTCACGTTGGCTACGTTGACTGATTTTGAAAACGATTGCGCTACCTCGCCTGTATTGGCCGGTGCGAATTTTACTAAAACCGCGGAGACCTCTCTGGCGTTTGGAACCCAGTTCGGCGATCTGGCAAATACCTTCGTACAACCTAATATCAATGGCGATGTGAAGGAT</t>
+          <t>ATGGCCCCGGGAGATGTCTCATCGTACACCTTGGTGACCAACCTGCTTCAGACTTCCTTGTTCGACGCACTGGCACCCTACAACCCGACTGCAGTGGGAGTTTATTCGCCTATACCGCCTCCTCCGGCTGAGGAGTCCGCGACCAACCCTAATAAGAACATTGCTGGCCTGTATGCGATGTTTCAAGTGGTTAAGGCAGCATTTACGGAACCTGTCCCGGTACTCCGGCAAGCACTAGGCGCTCTGGGCTTAGATCCTGACGACGAATCACAGGACCTGTCGACCGCCGTCGGCATCGGTAATACCGCAGGGAAAGCTGTTGCGGCTGCACGCATGGGCGATGGTATGAATGCACTGGGAGGCAAGGATCCTACCAATAACGGCCAGCCGTACGAAGATTACACCGGCTATCCTCCGGTGAACACTGCTGATGAACTCGTCGACCCGTCCCGCTTGCAGCCCGCGGTGGAACCTAACCCTCCTCGCACCGATGGTGGTCCCGGCGATAAGGGCATATTCACGGCACAGCCTTTTGCGACCCCACAGCTGGGGCTGGTGGCGCCCCAGACCTACCCTGATCCAGCTCGCTTTAAACTGGCTGCTCCGGATAATTTGGATAATAACGACGCCGGTGCCTATCCTCAGGCTGTCGATGAAGTATTGGCCGCATCCGCAGGCCTCACAGACGAGCAGAAAGTCAAAGCGGAATTCTTCGAAAACACACCACTCTCGGTAACTCTGTCCCCGCGCGCGGCCGCGATGGCAAATGACCTAGATCTGGACGGATTGGCACAGCTTTTTCTGGTGTGCTCCACAGCCCCTTTTGATTCGTTAATTGCTGCCTTGAATAACAAGCCTGCGTATGATACGGTACGCCCTTTCTCCGCCGTGCGCAATGTCTACGGTTCTAAACCGGTTACAGCCTTGGGTGGTCCAGGCAAGGGGACGGTGGAATCAATCCCTGCCGACGAGTTGACCGGATATCTGCCGGTGGGCAACAATCCGGAATACCCGTCCGGCTTTACCACCCTAATTGCAGCCCAGGCTCAGGCCGCGCCTTCTTTCTTAGGTGACGACGTCCTGAATTTGACTAACGCTTTTCCGGCGGGTTCCGGCCAGCCTGAGCCTGGGGCCGTACCCGCCTCTGATCTGGAGTTAACCTTGGCAACCTTGACTGACTTTGAAAATGACTGTGCCACCTCGCGCGTTTTGGCGGGTGCGAATTTCACCAAAACTGCCGAAACATCACTGGCCTTTGGGACCCAGTTTGGCGACTTAGCGAATACTTTCGTACAACGCAATATCAACGGTGATGTAAAGGAC</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>ATGGCCCCGGGTG</t>
+          <t>ATGGCCCCGGGAG</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>ATCCTTCACATCGCCATTGATATTAGG</t>
+          <t>GTCCTTTACATCACCGTTGATATTGC</t>
         </is>
       </c>
     </row>
@@ -2320,22 +2320,22 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>TACTTGTAACGAACGTATTTGCGCGTCTTGCGCTAAAACAGGGCGGACGACGGCGGCTAGCACCGCCCGAACGGACTTGAGTACCAACGGGAACCGGATCTAGGCCTACTATTTAGGCTTCTACAATGGTGTGGACAGCCATAGCCATTACAACGCCGCTTTCGACAGAACTTGCACGACTTTTTGCTACCTTACTTGCACAACCCCTTGCTTCCACCAGCGTTTATGTTGGGCGGAGGCAACCGGCTGATGTGGCCGATGCAAGGCTGGTTATGGCGCAAATTTGACTTGTTGGGAAGGGGAAACGTTGGAGTCGACGTCCGCTTATTGCCGGCTGCGCGCCCGCCGCCAGGACCTCTAGACCCATAAATACACTGAGTCTTAAAGCAATGGGGTGTCTAACGACAATGGGACGGCTTGTAAAAATTTCTGGGCTGGCGTAAAGGTGACGGCGGAGGTCTAAAGTGGCTGTTGTGACTAGCGGGACGTATGTTTGCGAGGCACCTGCTCTATTAACTTCGTAGACGCCGGGACCTACTACTCGCGTTTCGCGAGCGCCTTTAGTACCTCTTATTCGACAACCCATAGCCCTTAAGGAGGTAACTTTATCCAGACTTTTTGCTGGTCTTGTTACTCGACCCACAATTGCCAAACCGTGTTAACTACGAAGTCTTGTAAGAACGCTGGAAGCTATGCGAGTAGCGCCGCAACCCGATGTTTGGATTTATGCTCCGCCACGCGGGCTAATGACGGCAAGGATTACACATACCGTTAGCGTTTTAGGGACGAAACCCGCCGCATCCCTACCCATGTCAACTACTATAGGGTCGATTGCTTAACCGACCAATAAACGGACACCCACTGTTAGGCCTCATGGGCAGACCGAGTTGATGGCAGCCAAGGCGTCGAAGGGTCCGTCGGGGAGGAAAAAAGCTGAGTCTGCTGGACTTAAACCTTAAACTAAAACTTCACCCGTTTAGATAACACCTTGGCCCGTAGTGTGGTCAACTTTTACAAGGACACAGAAAAGGCTGAAACTGTCTAAAGTTGTTTGCGACACGGATAAGCGGAGACCTACCGCCACATTTGAAGTTCTTTTGCCAACTTGGAAGCTACCGTAAACCACTTGTTAAGCCTCTAGACCGATTACTAAAGTAGGTCGCGTTGCAATTTCCGCTTCCACTGCCA</t>
+          <t>TACTTGTAACGTACGTATTTGCGTGTCTTGCGCTAAAACAGGGCCAATGAAGGTGGGTAACAACGCCCAGACGCCCTTGAGTACCACCGGAACCCTGACCTGGGACTGCTGTTTAGTCTTCTGCATTGCTGGGGTCACCCATAACCGTTGCATCGGCGCTTTCGTCAAAACTTGCATAACTTTTTACTGCCTTACTTGCAAGACCCATTACTCCCGCCGGCGTTCATATTAGGCGGAGGCAACCGGCTAATGTGTCCGATGCAGGGTTGCTTGTGGCGAAAGTTTGACTTGTTGGGAAGAGGAAACGTCGGCGTCGACGTCCGGTTGTTGCCCGCGGCTCGACCACCACCGGGACCGCTAGACCCGTAAATGCAGTGGGTCTTGAAACAATGGGGAGTCTAACGGCACTGGGATGGCTTATAAAAGTTTCTGGGATGCCGTAAGGGCAATGGCGGAGGGCTGAAATGCCTGTTGTGCCTGGCGGGACGCATATTCGCGAGACATCTGCTTTAATAACTCCGCAGGCGCCGGGAGCTGCTGCTTGGATTTCGCGACCGACTTTAGTACCTTTTATTCGACAACCCCTAACCGTTAAGAAGGTAACTTTAACCTAATTTTTTGCTAGTCTTATTGCTTGACCCCCATTTGCCAAACCGCGTCAACTACGACGTTTTGTATGAGCGGTGGAAGCTATGAGAATAACGCCGCAACCCGATGTTTGGATTTATGCTCCGGCAGGGAGGCTAGTGCCGCCAAGCGTTGCAAATGCCATTGGCTTTCTAAGGACGCAACCCGCCACATCCGTACCCATGGCACCTGCTATAGGGACGCTTGCTTAACCGCCCAATAAACGGGCATCCGCTATTGGGTCTTATAGGCAGCCCGAGGTGGTGGCACCCAAGACGGCGCAGTGTCCGACGGGCGGGAAAGAAACTAAGCCTACTGAATTTGAACCTCAAACTGAAGCTTCAGCCGTTTAGCTAACACCTTGGCCCTTAATGTGGCCATCTTTTGCACGGACAGAGGAAGGGGTGGAACTGCCTGAAGTTATTCGCGACGCGCATGAGCGCGGAACTACCCCCACAATTAAAATTTTTTTGTCACCTCGGAAGGTACCGAAAACCGCTCGTCAAACCACTGGAGCGCTTACTAAAGTAAGTTGGATTACACTTTCCCCTCCCACTACCA</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>ATGAACATTGCTTGCATAAACGCGCAGAACGCGATTTTGTCCCGCCTGCTGCCGCCGATCGTGGCGGGCTTGCCTGAACTCATGGTTGCCCTTGGCCTAGATCCGGATGATAAATCCGAAGATGTTACCACACCTGTCGGTATCGGTAATGTTGCGGCGAAAGCTGTCTTGAACGTGCTGAAAAACGATGGAATGAACGTGTTGGGGAACGAAGGTGGTCGCAAATACAACCCGCCTCCGTTGGCCGACTACACCGGCTACGTTCCGACCAATACCGCGTTTAAACTGAACAACCCTTCCCCTTTGCAACCTCAGCTGCAGGCGAATAACGGCCGACGCGCGGGCGGCGGTCCTGGAGATCTGGGTATTTATGTGACTCAGAATTTCGTTACCCCACAGATTGCTGTTACCCTGCCGAACATTTTTAAAGACCCGACCGCATTTCCACTGCCGCCTCCAGATTTCACCGACAACACTGATCGCCCTGCATACAAACGCTCCGTGGACGAGATAATTGAAGCATCTGCGGCCCTGGATGATGAGCGCAAAGCGCTCGCGGAAATCATGGAGAATAAGCTGTTGGGTATCGGGAATTCCTCCATTGAAATAGGTCTGAAAAACGACCAGAACAATGAGCTGGGTGTTAACGGTTTGGCACAATTGATGCTTCAGAACATTCTTGCGACCTTCGATACGCTCATCGCGGCGTTGGGCTACAAACCTAAATACGAGGCGGTGCGCCCGATTACTGCCGTTCCTAATGTGTATGGCAATCGCAAAATCCCTGCTTTGGGCGGCGTAGGGATGGGTACAGTTGATGATATCCCAGCTAACGAATTGGCTGGTTATTTGCCTGTGGGTGACAATCCGGAGTACCCGTCTGGCTCAACTACCGTCGGTTCCGCAGCTTCCCAGGCAGCCCCTCCTTTTTTCGACTCAGACGACCTGAATTTGGAATTTGATTTTGAAGTGGGCAAATCTATTGTGGAACCGGGCATCACACCAGTTGAAAATGTTCCTGTGTCTTTTCCGACTTTGACAGATTTCAACAAACGCTGTGCCTATTCGCCTCTGGATGGCGGTGTAAACTTCAAGAAAACGGTTGAACCTTCGATGGCATTTGGTGAACAATTCGGAGATCTGGCTAATGATTTCATCCAGCGCAACGTTAAAGGCGAAGGTGACGGT</t>
+          <t>ATGAACATTGCATGCATAAACGCACAGAACGCGATTTTGTCCCGGTTACTTCCACCCATTGTTGCGGGTCTGCGGGAACTCATGGTGGCCTTGGGACTGGACCCTGACGACAAATCAGAAGACGTAACGACCCCAGTGGGTATTGGCAACGTAGCCGCGAAAGCAGTTTTGAACGTATTGAAAAATGACGGAATGAACGTTCTGGGTAATGAGGGCGGCCGCAAGTATAATCCGCCTCCGTTGGCCGATTACACAGGCTACGTCCCAACGAACACCGCTTTCAAACTGAACAACCCTTCTCCTTTGCAGCCGCAGCTGCAGGCCAACAACGGGCGCCGAGCTGGTGGTGGCCCTGGCGATCTGGGCATTTACGTCACCCAGAACTTTGTTACCCCTCAGATTGCCGTGACCCTACCGAATATTTTCAAAGACCCTACGGCATTCCCGTTACCGCCTCCCGACTTTACGGACAACACGGACCGCCCTGCGTATAAGCGCTCTGTAGACGAAATTATTGAGGCGTCCGCGGCCCTCGACGACGAACCTAAAGCGCTGGCTGAAATCATGGAAAATAAGCTGTTGGGGATTGGCAATTCTTCCATTGAAATTGGATTAAAAAACGATCAGAATAACGAACTGGGGGTAAACGGTTTGGCGCAGTTGATGCTGCAAAACATACTCGCCACCTTCGATACTCTTATTGCGGCGTTGGGCTACAAACCTAAATACGAGGCCGTCCCTCCGATCACGGCGGTTCGCAACGTTTACGGTAACCGAAAGATTCCTGCGTTGGGCGGTGTAGGCATGGGTACCGTGGACGATATCCCTGCGAACGAATTGGCGGGTTATTTGCCCGTAGGCGATAACCCAGAATATCCGTCGGGCTCCACCACCGTGGGTTCTGCCGCGTCACAGGCTGCCCGCCCTTTCTTTGATTCGGATGACTTAAACTTGGAGTTTGACTTCGAAGTCGGCAAATCGATTGTGGAACCGGGAATTACACCGGTAGAAAACGTGCCTGTCTCCTTCCCCACCTTGACGGACTTCAATAAGCGCTGCGCGTACTCGCGCCTTGATGGGGGTGTTAATTTTAAAAAAACAGTGGAGCCTTCCATGGCTTTTGGCGAGCAGTTTGGTGACCTCGCGAATGATTTCATTCAACCTAATGTGAAAGGGGAGGGTGATGGT</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>ATGAACATTGCTTGCATAAA</t>
+          <t>ATGAACATTGCATGCATAAA</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>ACCGTCACCTTCG</t>
+          <t>ACCATCACCCTCC</t>
         </is>
       </c>
     </row>
@@ -2362,22 +2362,22 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>TACTTTTGGAGTCCGTTGTGCAGACGAAGACTGGACAGAGAACCAGCGGCGAGGAATGACAACCCGCCAAGAAGGCGCCGAGACTACGAGCGGGACGGCTTAGGCCGATTGCGCCCGTGGAGCCTTCTCGGCGGTTGTAAGCTGAAACTAGACCTATGTCTATTGATATAGTTTAACCAATTTGGCCGGTGACTGCTTGTCCGTAGTGTCAGCGGAGACAACCTCAGCCAGCCTAGGTACCTACACTGGCATTAGAACAACTACAGGGCGCAACCGTTGGACCGTCAAAAACTGCGCCAACGCGGGATATTGCTTTGCCGCCAGCCGCAAATGAGAGCGTAAGGCGCGGGAGGCAGAAGACTTAGACGGTGTTTGGGATTGTACTTGTAACGATATGACATATGAGTTGATTTGTGCAAACTTGGAGACGACGGCAACCCAGATGGACCGGGCCGCCCGAGGGACGCTCGCTACTACCAGCCGGACCCGGAACTAGGACTATTATTTAGACTTCTGGAATGGTGAGGTCACCCATAACCGTTGCAACGGAAATTCAGACACAACTTGCGAGAGTTTTTGCTACCATACTTACATAATCCGATACTTCCGCCAGCGTTCATATTGGGTGACGGCAACCGCCTAATGTGCCCGATACTTGGGCACTTATGTGGAAAGGGAAATTTGTTGGGAAGAGGAAACGTCGGCGTTGAGTTGCGATTATTGCCTGGAGCGGGTCCCCCCCCAGGCCCGCTGGACCCATAGATGCAGAGTGTCTTAAAGCAATGAGGCGTTTAACGAGACTGATTTGGCTTATAAAAGTGGCTAGGCCGAGTTAAAGGTAACCGCCGCGGGTTTTTGAGGCTATTGTGGGGAGGTGCGCTAATATTTGGAAGCCATCTGCTTTAGAATCTCCGGAGACGCAGGGACTTACTACTTGCGTTTCGAAATCGCCTTCACTACCTGTTATTCGACAACCCATAACCGATGTGCAGCTGACATTAACCGGGATTTATACTACTTTTATTACTTTACCCACACAAGCCGAACCGACGCAACAGGGACGTTTTGAAGAATCGGTGGAAGCTACGCGACTAGCGCCAGAACGCGTTGTTTGCCTTTATACTGTGGCAAGGAGGCCATAGGCGACAGGGATTGCACATGCCATTAAGATTTCACTGCCGAAACCCGCCTCGACCATACCCATGCCAATTGCTATAGGCCCGTTGGCTTAACTACGGCATGGACGGATGGCCCCTGTTAGGCCTCATGGGAAGACCAAGGTGGAGAGACACGCGCCGACCGCGTGTCTGCCGTGCGGCGATAAAATTGAGGCTTCTCGACCTAAACTGAGACCTTAAATTACGCCCATGTAGACGACAACTTGGACTTTGATGCGGCCGGTTCTTGGACGTCGACTTAAAGTTGTGCAACCGACTTAAATTATTTCGAACGCGACTCAGGGGACAGAACCCGCCACACTTAAAAGCGTTCTGACATGTCGTCAGCGACTAAATACCGCTTGTCAAGCCACTAAACCGTTTGCTCAAACAGTTGGCGTTACACTTTCCCTTATAGTTTTGGCTGTGGGCTTTA</t>
+          <t>TACTTTTGCAGCCCATTATGGAGGCGCAGACTAGAAAGTGACCCAGGAGCCAGGAATGAGGACCCACCCAGAAGCCGGCGCGACTACGACCGGGATGGTTTAGGCCGGTTGCGTCCGTGGAGACTCCTTGGGGGTTGGAAGCTAAAACTGAACCTATGCCTATTGATGTAATTTAACCAGTTTGGTCGCTGTCTACTTGTCCGAAGAGTTAGTGGGAACAACCTCAGGCATCCTAGGTACCTACATTGGCAATAAAACAACTACAGTGGACACCCGTTAGACCGTCAGAAGCTGCGTCACCGGGGCATATTGCTTTGCCGGCATCCGCACATAAGAGGATAGGGCGGAGCGGGCAGAAGACTTAGGCGATGCTTGGGATTGTACTTGTAGCGTTAGGACATGTGGGTCGAATTGTGGAAGCTCGGAGACGACGGCGAACCCGACGGACCGGGCCGACCGAGGGAAGCGCGGTACTACCACCCAGACCCGAACCTAGGCCTATTATTTAGCCTTCTGGAGTGCTGGGGTCACCCGTAGCCGTTGCACCGAAAGTTTAGACAAAACTTACGGAATTTTTTACTACCGTACTTGCAAAACCCGATGCTTCCCCCAGCGTTTATATTGGGCGACGGTAACCGGCTAATATGTCCAATGCTCGGCCAATTGTGAGGCAAAGCGGACTTGTTAGGCAGCGGAAACGTCGGTGTCAATTTGCGGTTATTGCCGGCGGCGGGCCCACCGCCTGGTCCACTAGACCCGTAAATGCAAAGGGTTTTGAAACAGTGTGGAGTCTAGCGCGAGTGGTTTGGCTTGTAAAAATGGCTAGGCCGTGTTAAGGGCAATCGGCGTGGCTTTTTAAGGCTGTTGTGCGGAGGCGCGCTGATATTTGCTAGCCAACTGCTCTAGAACCTTCGCAGCCGAAGAGACTTGCTGCTTGGATTTCGTGACCGCCTTCAATACCTATTATTCGAAAACCCATAGCCAATGTGTAGATGACAGTAGCCCGGATTTATGCTACTTTTATTGCTCTACCCCCAGAAACCGAACCGTCGAAACAGGGACGTTTTGAAAGAACGCTGCAAGCTGCGCGACTAGCGTCAAAACGCTTTGTTTGCGTTCATACTATGGCACGCGGGACAAAGGCGGCAAGCCTTGCAGATACCATTGAGCTTCCATTGGCGTAACCCGCCACGTCCGTACCCGTGCCACTTACTGTAAGCCCGGTGTCTTAACTACGGAATAGACGGTTGGCCGCTGTTGGGCCTTATGGGTAGCCCGAGGTGCAGAAACACACGTCGCCCGCGTGTCTGGCGAGGAGCGATGAAATTGAGCCTTCTCGACCTGAACTGGGAACTTAAGTTACGACCATGGAGACGCCATCTTGGCCTTTGGTGGGGTCGATTCTTAAACGTCGACTTAAAATTGTGAAACCGTCTTAAATTATTTCGTACGCGGCTTAGAGCGCACAACCCGCCACACTTGAAAGCGTTTTGACACGTTGTCAGTGATTAGATGCCCCTTGTTAAGCCCCTAAATCGATTGCTTAAACAATTAGGATTACATTTTCCCTTATAGTTTTGACTATGTGGATTA</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>ATGAAAACCTCAGGCAACACGTCTGCTTCTGACCTGTCTCTTGGTCGCCGCTCCTTACTGTTGGGCGGTTCTTCCGCGGCTCTGATGCTCGCCCTGCCGAATCCGGCTAACGCGGGCACCTCGGAAGAGCCGCCAACATTCGACTTTGATCTGGATACAGATAACTATATCAAATTGGTTAAACCGGCCACTGACGAACAGGCATCACAGTCGCCTCTGTTGGAGTCGGTCGGATCCATGGATGTGACCGTAATCTTGTTGATGTCCCGCGTTGGCAACCTGGCAGTTTTTGACGCGGTTGCGCCCTATAACGAAACGGCGGTCGGCGTTTACTCTCGCATTCCGCGCCCTCCGTCTTCTGAATCTGCCACAAACCCTAACATGAACATTGCTATACTGTATACTCAACTAAACACGTTTGAACCTCTGCTGCCGTTGGGTCTACCTGGCCCGGCGGGCTCCCTGCGAGCGATGATGGTCGGCCTGGGCCTTGATCCTGATAATAAATCTGAAGACCTTACCACTCCAGTGGGTATTGGCAACGTTGCCTTTAAGTCTGTGTTGAACGCTCTCAAAAACGATGGTATGAATGTATTAGGCTATGAAGGCGGTCGCAAGTATAACCCACTGCCGTTGGCGGATTACACGGGCTATGAACCCGTGAATACACCTTTCCCTTTAAACAACCCTTCTCCTTTGCAGCCGCAACTCAACGCTAATAACGGACCTCGCCCAGGGGGGGGTCCGGGCGACCTGGGTATCTACGTCTCACAGAATTTCGTTACTCCGCAAATTGCTCTGACTAAACCGAATATTTTCACCGATCCGGCTCAATTTCCATTGGCGGCGCCCAAAAACTCCGATAACACCCCTCCACGCGATTATAAACCTTCGGTAGACGAAATCTTAGAGGCCTCTGCGTCCCTGAATGATGAACGCAAAGCTTTAGCGGAAGTGATGGACAATAAGCTGTTGGGTATTGGCTACACGTCGACTGTAATTGGCCCTAAATATGATGAAAATAATGAAATGGGTGTGTTCGGCTTGGCTGCGTTGTCCCTGCAAAACTTCTTAGCCACCTTCGATGCGCTGATCGCGGTCTTGCGCAACAAACGGAAATATGACACCGTTCCTCCGGTATCCGCTGTCCCTAACGTGTACGGTAATTCTAAAGTGACGGCTTTGGGCGGAGCTGGTATGGGTACGGTTAACGATATCCGGGCAACCGAATTGATGCCGTACCTGCCTACCGGGGACAATCCGGAGTACCCTTCTGGTTCCACCTCTCTGTGCGCGGCTGGCGCACAGACGGCACGCCGCTATTTTAACTCCGAAGAGCTGGATTTGACTCTGGAATTTAATGCGGGTACATCTGCTGTTGAACCTGAAACTACGCCGGCCAAGAACCTGCAGCTGAATTTCAACACGTTGGCTGAATTTAATAAAGCTTGCGCTGAGTCCCCTGTCTTGGGCGGTGTGAATTTTCGCAAGACTGTACAGCAGTCGCTGATTTATGGCGAACAGTTCGGTGATTTGGCAAACGAGTTTGTCAACCGCAATGTGAAAGGGAATATCAAAACCGACACCCGAAAT</t>
+          <t>ATGAAAACGTCGGGTAATACCTCCGCGTCTGATCTTTCACTGGGTCCTCGGTCCTTACTCCTGGGTGGGTCTTCGGCCGCGCTGATGCTGGCCCTACCAAATCCGGCCAACGCAGGCACCTCTGAGGAACCCCCAACCTTCGATTTTGACTTGGATACGGATAACTACATTAAATTGGTCAAACCAGCGACAGATGAACAGGCTTCTCAATCACCCTTGTTGGAGTCCGTAGGATCCATGGATGTAACCGTTATTTTGTTGATGTCACCTGTGGGCAATCTGGCAGTCTTCGACGCAGTGGCCCCGTATAACGAAACGGCCGTAGGCGTGTATTCTCCTATCCCGCCTCGCCCGTCTTCTGAATCCGCTACGAACCCTAACATGAACATCGCAATCCTGTACACCCAGCTTAACACCTTCGAGCCTCTGCTGCCGCTTGGGCTGCCTGGCCCGGCTGGCTCCCTTCGCGCCATGATGGTGGGTCTGGGCTTGGATCCGGATAATAAATCGGAAGACCTCACGACCCCAGTGGGCATCGGCAACGTGGCTTTCAAATCTGTTTTGAATGCCTTAAAAAATGATGGCATGAACGTTTTGGGCTACGAAGGGGGTCGCAAATATAACCCGCTGCCATTGGCCGATTATACAGGTTACGAGCCGGTTAACACTCCGTTTCGCCTGAACAATCCGTCGCCTTTGCAGCCACAGTTAAACGCCAATAACGGCCGCCGCCCGGGTGGCGGACCAGGTGATCTGGGCATTTACGTTTCCCAAAACTTTGTCACACCTCAGATCGCGCTCACCAAACCGAACATTTTTACCGATCCGGCACAATTCCCGTTAGCCGCACCGAAAAATTCCGACAACACGCCTCCGCGCGACTATAAACGATCGGTTGACGAGATCTTGGAAGCGTCGGCTTCTCTGAACGACGAACCTAAAGCACTGGCGGAAGTTATGGATAATAAGCTTTTGGGTATCGGTTACACATCTACTGTCATCGGGCCTAAATACGATGAAAATAACGAGATGGGGGTCTTTGGCTTGGCAGCTTTGTCCCTGCAAAACTTTCTTGCGACGTTCGACGCGCTGATCGCAGTTTTGCGAAACAAACGCAAGTATGATACCGTGCGCCCTGTTTCCGCCGTTCGGAACGTCTATGGTAACTCGAAGGTAACCGCATTGGGCGGTGCAGGCATGGGCACGGTGAATGACATTCGGGCCACAGAATTGATGCCTTATCTGCCAACCGGCGACAACCCGGAATACCCATCGGGCTCCACGTCTTTGTGTGCAGCGGGCGCACAGACCGCTCCTCGCTACTTTAACTCGGAAGAGCTGGACTTGACCCTTGAATTCAATGCTGGTACCTCTGCGGTAGAACCGGAAACCACCCCAGCTAAGAATTTGCAGCTGAATTTTAACACTTTGGCAGAATTTAATAAAGCATGCGCCGAATCTCGCGTGTTGGGCGGTGTGAACTTTCGCAAAACTGTGCAACAGTCACTAATCTACGGGGAACAATTCGGGGATTTAGCTAACGAATTTGTTAATCCTAATGTAAAAGGGAATATCAAAACTGATACACCTAAT</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>ATGAAAACCTCAGGCAA</t>
+          <t>ATGAAAACGTCGGGTA</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>ATTTCGGGTGTCGG</t>
+          <t>ATTAGGTGTATCAGTTTTGATA</t>
         </is>
       </c>
     </row>
@@ -2404,22 +2404,22 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>TACTGATGAAGACTCGCGAGTAGTCACAGGCTAAAGAGTGGTGGAGCGGGAAGCGATGAATAACCTAGGCGGAGACGGCGACGCGAGCGTTGGAATCCAAGTTGACCCTGACGACGCCGGCGGCCGCGCCGGCTACTTGGCGGTTGACAACTAAAGCTAAAGCTATTACCGTTGAAATAGGCGCTAGAGTAATAATGGGCGCGTCCGCCACACAAAGGCCTTCTCCCGCAGTAACCAGGATACCTACGGAGTCAAATATAGAACTAGTGGAGGGACAAGGTTGAGAGAAACAAACTACGGGAACGAGGCATATTGGGTTGGCGGCACCCGTAGTTGAGGGCGTAGCGCGGAGGAGGTCGGCCCCTTCGTCGGTGGTTAGGATTGTTTTTATAGCGCCCTAACATGCGGCGCGACGCGCAAAACCTCCCCCATAAGCTTCTCGGACAGGGTCAATACGGACGTCCAAAATGCCGGCGCCCGGACCTAGGCCTGCTGGCGAGCCTCCTAGGATGCTGCGGGTAGCCATAGCCGTTGTAGCGCCCATTTCGGCAACAAGCGCGGGCGCGCTTGCTGCCATACTTGTTGGAGCCGTTGCAACCTGGATTTATGTTGCCGTTTGGTATGCTTCTAATATGTCCAATAGTCGGTCATTTAAGCGGCATATTTAATCACTTAGGCAGGTTTAACGTCGGCCGGAACTTAGGTTTGGTCGGAGCGCAACCACCGCCGGGCCCTCTATTTCCTTAGAACCATTAAGTCCGCAAACAATGCGGCGTCAACCGCGACCACTTCGGAATGTGGATGGCGTTGGGACCGGTCAAATGCCAAGGACATGGCCTATTGAGGTGGTTGTGGTTGCAGGCGTTTATGTTTGTCAGACAGCTAGTCTAAGAACTCCGAAGGCGGTGAGAATGGCTGCTCTTCTTTGAGTACCGACTTAACAAACTATTGTTCGAGCGTCCCTAGCGTGACCGTGGTAGGCGACGACGAAATAGTTTACTAGACCTGGACCTACCAAACACGTTGGAGATACGGCAATGCCGCAATCGCGGAGATCTACTGGACTAACGCCGAAACTTGAACTTTTGGTTTAAGTTAAGACACGCGGGCAAGTGTCGGCAATTGTTGCACATACCGGCCTTTTTTTAAAGACGGAACCCGCCTCAACCGTTTCCCTGGCAGTTACTATACGGCCGTTTGCTTAACAGAAGTATGGACGGGCAGCCACTGTTGGGCCTTATGTAGAGCCCGAGTTGCTGGGACACAAGCCGGCTTCGGGTTCGGCGCGCGGCCAAGGACCCGCTGCTGCAGGAGCTAAACTGAATAAGAAAAGGTCGACCCAGCCCAAATTGGCTCGGCCCAAATCAGGGCCGTTTTCTATGTCTTGACTTGAACCTATGGAACTGAGCCAAGTGGGGACTAACACGTCTAAGCGCGCAAAACCCGCCACAATTAAAAGTCTGCTGTCAACTAGGAAGATAGCTTAACCCCCGCGTCAAGCCACTAGCCCGCTTGGTCAAGAATGTTGGATTATAATTCCCGCTTCAGAGC</t>
+          <t>TACTGCTGTAGGCTCGGAAGAAGTCACAGTCTAAAAAGAGGCGCGGGAGCCAGTGACAACTAGCCAAGGCGCAGGCGCCGTCGGGACCGGTGCAATCCGAGCTGGCCGTGGCGACGGCGTCGGCCACGCCGACTGCTTGGCGGGTGGCACCTAAAACTAAAACTATTACCATTGAAGTAGGGACTGAACTAGTAGTGCGGACGGCCACCACACAAGGGACTTCTTCCGCAGTAGCCGGGCTACCTGCGAAGCCATATGTAAAACTAGTGGAGGGACAAAGTCAATAGTAACAAGCTACGCGAACGGGGCATGTTAGGCTGTCGCCAGCCTTAATTGAGCGCGTAGCGGGCGGGAGGCCGGCCACTTCGGCGATGGTTAGGATTGTTTTTGTAACGGCCAGACATACGGCGCGACGGACACGACCTTCCACACAAGCTTCTCGCGCAAGGACATTACGGACGCCCGAAATGCCGGCGTCCAAATCTGGGCCTGCTAGCCAGTCTTCTAGGATGGTGAGGATAACCCTAGCCCTTGTAACGCCCCTTTCGTCATCAGGGACGCGCGCGTTTGCTACCGTACTTGTTAGACCCATTGCAACCGGCGTTCATGTTACCATTCGGCATACTCCTGATGTGGCCAATGGTCGGCCAATTGAGGGGCATATTTAATCAATTAGGCAGCTTTAACGTCGGCCGTGACTTGGGCTTGGTCGGAGGACAGCCGCCGCCGGGCCCTCTATTCCCATAGAACCAATAGGTCCGGAAACAGTGTGGTGTCGAACGCGAACACTTTGGCATATGGATGGGATTAGGCCCGGTCAAATGCCAAGGCCAGGGACTATTGAGCTGCTTGTGATTACAGGGATTTATGTTTGTCAGGCAGCTAGTCTAGGAGCTCCGGAGCCGCTGAAATTGGCTGCTCTTTTTCAACTACCGGCTTAACAAGCTATTATTTGACCGTCCGTAGCGAGACCGTGGCAGCCGCCGGCGTGATAGTTTGCTAGACCTGAACCTACCGAACACATTGAATATGCGGCACTGGCGCGAGCGAGCGGACCTACTGGACTAACGGCGAAACTTGAACTTCTGGTTTAAGTTAAGGCAAGCGGGCAAGTGTCGCCACTTGTTACATATGCCAGGATTTTTTTAGAGTCGCAACCCTCCACACCCGTTTCCGTGCCAATTACTATACGGCCGCTTGCTTAACAGCAGCATAGACGGGCACCCGCTATTAGGCCTTATGTAGAGTCCTAGGTGGTGGGAAACAAGCCGACTTCGCGTCCGTCGCGGAGCGAAAGACCCACTACTACAAAACCTAAACTGGATGAGGAAGGGCCGACCAAGCCCAGACTGCCTTGGACCGGACCACGGCCGGTTCCTATGCCTTGACTTGAACCTATGCAACTGCGCGAAATGGGGACTAACGCGGCTGAGGGCGCAGAACCCGCCACAATTAAAAGTCTGCTGGCAACTAGCGAGGTAACTTAACCCACGCGTCAAGCCACTGGGACGATTAGTCAAAGAAGTCGCGTTGTAATTTCCGCTCCACAGC</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>ATGACTACTTCTGAGCGCTCATCAGTGTCCGATTTCTCACCACCTCGCCCTTCGCTACTTATTGGATCCGCCTCTGCCGCTGCGCTCGCAACCTTAGGTTCAACTGGGACTGCTGCGGCCGCCGGCGCGGCCGATGAACCGCCAACTGTTGATTTCGATTTCGATAATGGCAACTTTATCCGCGATCTCATTATTACCCGCGCAGGCGGTGTGTTTCCGGAAGAGGGCGTCATTGGTCCTATGGATGCCTCAGTTTATATCTTGATCACCTCCCTGTTCCAACTCTCTTTGTTTGATGCCCTTGCTCCGTATAACCCAACCGCCGTGGGCATCAACTCCCGCATCGCGCCTCCTCCAGCCGGGGAAGCAGCCACCAATCCTAACAAAAATATCGCGGGATTGTACGCCGCGCTGCGCGTTTTGGAGGGGGTATTCGAAGAGCCTGTCCCAGTTATGCCTGCAGGTTTTACGGCCGCGGGCCTGGATCCGGACGACCGCTCGGAGGATCCTACGACGCCCATCGGTATCGGCAACATCGCGGGTAAAGCCGTTGTTCGCGCCCGCGCGAACGACGGTATGAACAACCTCGGCAACGTTGGACCTAAATACAACGGCAAACCATACGAAGATTATACAGGTTATCAGCCAGTAAATTCGCCGTATAAATTAGTGAATCCGTCCAAATTGCAGCCGGCCTTGAATCCAAACCAGCCTCGCGTTGGTGGCGGCCCGGGAGATAAAGGAATCTTGGTAATTCAGGCGTTTGTTACGCCGCAGTTGGCGCTGGTGAAGCCTTACACCTACCGCAACCCTGGCCAGTTTACGGTTCCTGTACCGGATAACTCCACCAACACCAACGTCCGCAAATACAAACAGTCTGTCGATCAGATTCTTGAGGCTTCCGCCACTCTTACCGACGAGAAGAAACTCATGGCTGAATTGTTTGATAACAAGCTCGCAGGGATCGCACTGGCACCATCCGCTGCTGCTTTATCAAATGATCTGGACCTGGATGGTTTGTGCAACCTCTATGCCGTTACGGCGTTAGCGCCTCTAGATGACCTGATTGCGGCTTTGAACTTGAAAACCAAATTCAATTCTGTGCGCCCGTTCACAGCCGTTAACAACGTGTATGGCCGGAAAAAAATTTCTGCCTTGGGCGGAGTTGGCAAAGGGACCGTCAATGATATGCCGGCAAACGAATTGTCTTCATACCTGCCCGTCGGTGACAACCCGGAATACATCTCGGGCTCAACGACCCTGTGTTCGGCCGAAGCCCAAGCCGCGCGCCGGTTCCTGGGCGACGACGTCCTCGATTTGACTTATTCTTTTCCAGCTGGGTCGGGTTTAACCGAGCCGGGTTTAGTCCCGGCAAAAGATACAGAACTGAACTTGGATACCTTGACTCGGTTCACCCCTGATTGTGCAGATTCGCGCGTTTTGGGCGGTGTTAATTTTCAGACGACAGTTGATCCTTCTATCGAATTGGGGGCGCAGTTCGGTGATCGGGCGAACCAGTTCTTACAACCTAATATTAAGGGCGAAGTCTCG</t>
+          <t>ATGACGACATCCGAGCCTTCTTCAGTGTCAGATTTTTCTCCGCGCCCTCGGTCACTGTTGATCGGTTCCGCGTCCGCGGCAGCCCTGGCCACGTTAGGCTCGACCGGCACCGCTGCCGCAGCCGGTGCGGCTGACGAACCGCCCACCGTGGATTTTGATTTTGATAATGGTAACTTCATCCCTGACTTGATCATCACGCCTGCCGGTGGTGTGTTCCCTGAAGAAGGCGTCATCGGCCCGATGGACGCTTCGGTATACATTTTGATCACCTCCCTGTTTCAGTTATCATTGTTCGATGCGCTTGCCCCGTACAATCCGACAGCGGTCGGAATTAACTCGCGCATCGCCCGCCCTCCGGCCGGTGAAGCCGCTACCAATCCTAACAAAAACATTGCCGGTCTGTATGCCGCGCTGCCTGTGCTGGAAGGTGTGTTCGAAGAGCGCGTTCCTGTAATGCCTGCGGGCTTTACGGCCGCAGGTTTAGACCCGGACGATCGGTCAGAAGATCCTACCACTCCTATTGGGATCGGGAACATTGCGGGGAAAGCAGTAGTCCCTGCGCGCGCAAACGATGGCATGAACAATCTGGGTAACGTTGGCCGCAAGTACAATGGTAAGCCGTATGAGGACTACACCGGTTACCAGCCGGTTAACTCCCCGTATAAATTAGTTAATCCGTCGAAATTGCAGCCGGCACTGAACCCGAACCAGCCTCCTGTCGGCGGCGGCCCGGGAGATAAGGGTATCTTGGTTATCCAGGCCTTTGTCACACCACAGCTTGCGCTTGTGAAACCGTATACCTACCCTAATCCGGGCCAGTTTACGGTTCCGGTCCCTGATAACTCGACGAACACTAATGTCCCTAAATACAAACAGTCCGTCGATCAGATCCTCGAGGCCTCGGCGACTTTAACCGACGAGAAAAAGTTGATGGCCGAATTGTTCGATAATAAACTGGCAGGCATCGCTCTGGCACCGTCGGCGGCCGCACTATCAAACGATCTGGACTTGGATGGCTTGTGTAACTTATACGCCGTGACCGCGCTCGCTCGCCTGGATGACCTGATTGCCGCTTTGAACTTGAAGACCAAATTCAATTCCGTTCGCCCGTTCACAGCGGTGAACAATGTATACGGTCCTAAAAAAATCTCAGCGTTGGGAGGTGTGGGCAAAGGCACGGTTAATGATATGCCGGCGAACGAATTGTCGTCGTATCTGCCCGTGGGCGATAATCCGGAATACATCTCAGGATCCACCACCCTTTGTTCGGCTGAAGCGCAGGCAGCGCCTCGCTTTCTGGGTGATGATGTTTTGGATTTGACCTACTCCTTCCCGGCTGGTTCGGGTCTGACGGAACCTGGCCTGGTGCCGGCCAAGGATACGGAACTGAACTTGGATACGTTGACGCGCTTTACCCCTGATTGCGCCGACTCCCGCGTCTTGGGCGGTGTTAATTTTCAGACGACCGTTGATCGCTCCATTGAATTGGGTGCGCAGTTCGGTGACCCTGCTAATCAGTTTCTTCAGCGCAACATTAAAGGCGAGGTGTCG</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>ATGACTACTTCTGAGCG</t>
+          <t>ATGACGACATCCGAG</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>CGAGACTTCGCCC</t>
+          <t>CGACACCTCGCCT</t>
         </is>
       </c>
     </row>

</xml_diff>